<commit_message>
Deleted permission of 'user_delete_self' and revised some specification docs.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/RequirementDefinition.xlsx
+++ b/skrum_docs/02_SpecificationDocs/RequirementDefinition.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nohr/OneDrive/Skrum/06_プロダクト開発/プロダクト資料/01_要件定義/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nohr/Dev/skrum/skrum_docs/02_SpecificationDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="更新履歴" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="239">
   <si>
     <t>ユーザ権限</t>
     <rPh sb="3" eb="5">
@@ -2461,6 +2461,32 @@
     </rPh>
     <rPh sb="12" eb="14">
       <t>サクj</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>管理者ユーザと一般ユーザの自ユーザ削除を不可に変更。</t>
+    <rPh sb="0" eb="3">
+      <t>カn</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>イッp</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ジブn</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>サk</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>フk</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ヘンコ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2510,7 +2536,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2526,6 +2552,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3677,7 +3709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3822,6 +3854,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3994,8 +4035,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3654906" y="15109408"/>
-          <a:ext cx="2001854" cy="2001725"/>
+          <a:off x="3691035" y="15261253"/>
+          <a:ext cx="2022928" cy="2022669"/>
           <a:chOff x="3479800" y="21310600"/>
           <a:chExt cx="1981200" cy="1981200"/>
         </a:xfrm>
@@ -4113,8 +4154,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6811562" y="15109408"/>
-          <a:ext cx="1998903" cy="2001725"/>
+          <a:off x="6880808" y="15261253"/>
+          <a:ext cx="2016968" cy="2022669"/>
           <a:chOff x="6743700" y="21310600"/>
           <a:chExt cx="1981200" cy="1981200"/>
         </a:xfrm>
@@ -5547,10 +5588,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
+      <c r="B7" s="83">
+        <v>42937</v>
+      </c>
+      <c r="C7" s="82" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="82" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="82" t="s">
+        <v>238</v>
+      </c>
       <c r="F7" s="82"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -6111,7 +6160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ243"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="99" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="98" workbookViewId="0">
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
@@ -6121,15 +6170,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="146"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="149"/>
       <c r="H1" s="55"/>
       <c r="I1" s="52" t="s">
         <v>81</v>
@@ -6140,53 +6189,53 @@
       <c r="M1" s="53"/>
       <c r="N1" s="53"/>
       <c r="O1" s="54"/>
-      <c r="P1" s="153" t="s">
+      <c r="P1" s="156" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" s="154"/>
-      <c r="R1" s="154"/>
-      <c r="S1" s="154"/>
-      <c r="T1" s="154"/>
-      <c r="U1" s="154"/>
-      <c r="V1" s="154"/>
-      <c r="W1" s="154"/>
-      <c r="X1" s="154"/>
-      <c r="Y1" s="154"/>
-      <c r="Z1" s="155"/>
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="157"/>
+      <c r="W1" s="157"/>
+      <c r="X1" s="157"/>
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="158"/>
       <c r="AA1" s="52" t="s">
         <v>76</v>
       </c>
       <c r="AB1" s="50"/>
       <c r="AC1" s="51"/>
-      <c r="AD1" s="150">
+      <c r="AD1" s="153">
         <v>42760</v>
       </c>
-      <c r="AE1" s="151"/>
-      <c r="AF1" s="151"/>
-      <c r="AG1" s="151"/>
-      <c r="AH1" s="152"/>
+      <c r="AE1" s="154"/>
+      <c r="AF1" s="154"/>
+      <c r="AG1" s="154"/>
+      <c r="AH1" s="155"/>
       <c r="AI1" s="52" t="s">
         <v>78</v>
       </c>
       <c r="AJ1" s="53"/>
       <c r="AK1" s="54"/>
-      <c r="AL1" s="141" t="s">
+      <c r="AL1" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="AM1" s="142"/>
-      <c r="AN1" s="142"/>
-      <c r="AO1" s="142"/>
-      <c r="AP1" s="143"/>
+      <c r="AM1" s="145"/>
+      <c r="AN1" s="145"/>
+      <c r="AO1" s="145"/>
+      <c r="AP1" s="146"/>
       <c r="AQ1" s="2"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A2" s="147"/>
-      <c r="B2" s="148"/>
-      <c r="C2" s="148"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="148"/>
-      <c r="G2" s="149"/>
+      <c r="A2" s="150"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="152"/>
       <c r="H2" s="56"/>
       <c r="I2" s="52" t="s">
         <v>82</v>
@@ -6197,41 +6246,41 @@
       <c r="M2" s="53"/>
       <c r="N2" s="53"/>
       <c r="O2" s="54"/>
-      <c r="P2" s="153"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="154"/>
-      <c r="S2" s="154"/>
-      <c r="T2" s="154"/>
-      <c r="U2" s="154"/>
-      <c r="V2" s="154"/>
-      <c r="W2" s="154"/>
-      <c r="X2" s="154"/>
-      <c r="Y2" s="154"/>
-      <c r="Z2" s="155"/>
+      <c r="P2" s="156"/>
+      <c r="Q2" s="157"/>
+      <c r="R2" s="157"/>
+      <c r="S2" s="157"/>
+      <c r="T2" s="157"/>
+      <c r="U2" s="157"/>
+      <c r="V2" s="157"/>
+      <c r="W2" s="157"/>
+      <c r="X2" s="157"/>
+      <c r="Y2" s="157"/>
+      <c r="Z2" s="158"/>
       <c r="AA2" s="52" t="s">
         <v>77</v>
       </c>
       <c r="AB2" s="50"/>
       <c r="AC2" s="51"/>
-      <c r="AD2" s="150">
+      <c r="AD2" s="153">
         <v>42929</v>
       </c>
-      <c r="AE2" s="151"/>
-      <c r="AF2" s="151"/>
-      <c r="AG2" s="151"/>
-      <c r="AH2" s="152"/>
+      <c r="AE2" s="154"/>
+      <c r="AF2" s="154"/>
+      <c r="AG2" s="154"/>
+      <c r="AH2" s="155"/>
       <c r="AI2" s="52" t="s">
         <v>79</v>
       </c>
       <c r="AJ2" s="53"/>
       <c r="AK2" s="54"/>
-      <c r="AL2" s="141" t="s">
+      <c r="AL2" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="AM2" s="142"/>
-      <c r="AN2" s="142"/>
-      <c r="AO2" s="142"/>
-      <c r="AP2" s="143"/>
+      <c r="AM2" s="145"/>
+      <c r="AN2" s="145"/>
+      <c r="AO2" s="145"/>
+      <c r="AP2" s="146"/>
       <c r="AQ2" s="2"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
@@ -6758,27 +6807,27 @@
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="42"/>
-      <c r="L18" s="135" t="s">
+      <c r="L18" s="138" t="s">
         <v>54</v>
       </c>
-      <c r="M18" s="136"/>
-      <c r="N18" s="136"/>
-      <c r="O18" s="136"/>
-      <c r="P18" s="136"/>
-      <c r="Q18" s="136"/>
-      <c r="R18" s="136"/>
-      <c r="S18" s="136"/>
-      <c r="T18" s="136"/>
-      <c r="U18" s="136"/>
-      <c r="V18" s="136"/>
-      <c r="W18" s="136"/>
-      <c r="X18" s="136"/>
-      <c r="Y18" s="136"/>
-      <c r="Z18" s="136"/>
-      <c r="AA18" s="136"/>
-      <c r="AB18" s="136"/>
-      <c r="AC18" s="136"/>
-      <c r="AD18" s="137"/>
+      <c r="M18" s="139"/>
+      <c r="N18" s="139"/>
+      <c r="O18" s="139"/>
+      <c r="P18" s="139"/>
+      <c r="Q18" s="139"/>
+      <c r="R18" s="139"/>
+      <c r="S18" s="139"/>
+      <c r="T18" s="139"/>
+      <c r="U18" s="139"/>
+      <c r="V18" s="139"/>
+      <c r="W18" s="139"/>
+      <c r="X18" s="139"/>
+      <c r="Y18" s="139"/>
+      <c r="Z18" s="139"/>
+      <c r="AA18" s="139"/>
+      <c r="AB18" s="139"/>
+      <c r="AC18" s="139"/>
+      <c r="AD18" s="140"/>
       <c r="AE18" s="2"/>
       <c r="AP18" s="5"/>
       <c r="AQ18" s="2"/>
@@ -6794,27 +6843,27 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="42"/>
-      <c r="L19" s="135" t="s">
+      <c r="L19" s="138" t="s">
         <v>55</v>
       </c>
-      <c r="M19" s="136"/>
-      <c r="N19" s="136"/>
-      <c r="O19" s="136"/>
-      <c r="P19" s="136"/>
-      <c r="Q19" s="136"/>
-      <c r="R19" s="136"/>
-      <c r="S19" s="136"/>
-      <c r="T19" s="136"/>
-      <c r="U19" s="136"/>
-      <c r="V19" s="136"/>
-      <c r="W19" s="136"/>
-      <c r="X19" s="136"/>
-      <c r="Y19" s="136"/>
-      <c r="Z19" s="136"/>
-      <c r="AA19" s="136"/>
-      <c r="AB19" s="136"/>
-      <c r="AC19" s="136"/>
-      <c r="AD19" s="137"/>
+      <c r="M19" s="139"/>
+      <c r="N19" s="139"/>
+      <c r="O19" s="139"/>
+      <c r="P19" s="139"/>
+      <c r="Q19" s="139"/>
+      <c r="R19" s="139"/>
+      <c r="S19" s="139"/>
+      <c r="T19" s="139"/>
+      <c r="U19" s="139"/>
+      <c r="V19" s="139"/>
+      <c r="W19" s="139"/>
+      <c r="X19" s="139"/>
+      <c r="Y19" s="139"/>
+      <c r="Z19" s="139"/>
+      <c r="AA19" s="139"/>
+      <c r="AB19" s="139"/>
+      <c r="AC19" s="139"/>
+      <c r="AD19" s="140"/>
       <c r="AE19" s="2"/>
       <c r="AP19" s="5"/>
       <c r="AQ19" s="2"/>
@@ -6830,27 +6879,27 @@
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
       <c r="K20" s="43"/>
-      <c r="L20" s="135" t="s">
+      <c r="L20" s="138" t="s">
         <v>56</v>
       </c>
-      <c r="M20" s="136"/>
-      <c r="N20" s="136"/>
-      <c r="O20" s="136"/>
-      <c r="P20" s="136"/>
-      <c r="Q20" s="136"/>
-      <c r="R20" s="136"/>
-      <c r="S20" s="136"/>
-      <c r="T20" s="136"/>
-      <c r="U20" s="136"/>
-      <c r="V20" s="136"/>
-      <c r="W20" s="136"/>
-      <c r="X20" s="136"/>
-      <c r="Y20" s="136"/>
-      <c r="Z20" s="136"/>
-      <c r="AA20" s="136"/>
-      <c r="AB20" s="136"/>
-      <c r="AC20" s="136"/>
-      <c r="AD20" s="137"/>
+      <c r="M20" s="139"/>
+      <c r="N20" s="139"/>
+      <c r="O20" s="139"/>
+      <c r="P20" s="139"/>
+      <c r="Q20" s="139"/>
+      <c r="R20" s="139"/>
+      <c r="S20" s="139"/>
+      <c r="T20" s="139"/>
+      <c r="U20" s="139"/>
+      <c r="V20" s="139"/>
+      <c r="W20" s="139"/>
+      <c r="X20" s="139"/>
+      <c r="Y20" s="139"/>
+      <c r="Z20" s="139"/>
+      <c r="AA20" s="139"/>
+      <c r="AB20" s="139"/>
+      <c r="AC20" s="139"/>
+      <c r="AD20" s="140"/>
       <c r="AE20" s="2"/>
       <c r="AP20" s="5"/>
       <c r="AQ20" s="2"/>
@@ -7270,27 +7319,27 @@
       <c r="I38" s="61"/>
       <c r="J38" s="61"/>
       <c r="K38" s="62"/>
-      <c r="L38" s="132" t="s">
+      <c r="L38" s="135" t="s">
         <v>60</v>
       </c>
-      <c r="M38" s="133"/>
-      <c r="N38" s="133"/>
-      <c r="O38" s="133"/>
-      <c r="P38" s="133"/>
-      <c r="Q38" s="133"/>
-      <c r="R38" s="133"/>
-      <c r="S38" s="133"/>
-      <c r="T38" s="133"/>
-      <c r="U38" s="133"/>
-      <c r="V38" s="133"/>
-      <c r="W38" s="133"/>
-      <c r="X38" s="133"/>
-      <c r="Y38" s="133"/>
-      <c r="Z38" s="133"/>
-      <c r="AA38" s="133"/>
-      <c r="AB38" s="133"/>
-      <c r="AC38" s="133"/>
-      <c r="AD38" s="134"/>
+      <c r="M38" s="136"/>
+      <c r="N38" s="136"/>
+      <c r="O38" s="136"/>
+      <c r="P38" s="136"/>
+      <c r="Q38" s="136"/>
+      <c r="R38" s="136"/>
+      <c r="S38" s="136"/>
+      <c r="T38" s="136"/>
+      <c r="U38" s="136"/>
+      <c r="V38" s="136"/>
+      <c r="W38" s="136"/>
+      <c r="X38" s="136"/>
+      <c r="Y38" s="136"/>
+      <c r="Z38" s="136"/>
+      <c r="AA38" s="136"/>
+      <c r="AB38" s="136"/>
+      <c r="AC38" s="136"/>
+      <c r="AD38" s="137"/>
       <c r="AE38" s="2"/>
       <c r="AP38" s="5"/>
       <c r="AQ38" s="2"/>
@@ -7306,27 +7355,27 @@
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="13"/>
-      <c r="L39" s="135" t="s">
+      <c r="L39" s="138" t="s">
         <v>57</v>
       </c>
-      <c r="M39" s="136"/>
-      <c r="N39" s="136"/>
-      <c r="O39" s="136"/>
-      <c r="P39" s="136"/>
-      <c r="Q39" s="136"/>
-      <c r="R39" s="136"/>
-      <c r="S39" s="136"/>
-      <c r="T39" s="136"/>
-      <c r="U39" s="136"/>
-      <c r="V39" s="136"/>
-      <c r="W39" s="136"/>
-      <c r="X39" s="136"/>
-      <c r="Y39" s="136"/>
-      <c r="Z39" s="136"/>
-      <c r="AA39" s="136"/>
-      <c r="AB39" s="136"/>
-      <c r="AC39" s="136"/>
-      <c r="AD39" s="137"/>
+      <c r="M39" s="139"/>
+      <c r="N39" s="139"/>
+      <c r="O39" s="139"/>
+      <c r="P39" s="139"/>
+      <c r="Q39" s="139"/>
+      <c r="R39" s="139"/>
+      <c r="S39" s="139"/>
+      <c r="T39" s="139"/>
+      <c r="U39" s="139"/>
+      <c r="V39" s="139"/>
+      <c r="W39" s="139"/>
+      <c r="X39" s="139"/>
+      <c r="Y39" s="139"/>
+      <c r="Z39" s="139"/>
+      <c r="AA39" s="139"/>
+      <c r="AB39" s="139"/>
+      <c r="AC39" s="139"/>
+      <c r="AD39" s="140"/>
       <c r="AE39" s="2"/>
       <c r="AP39" s="5"/>
       <c r="AQ39" s="2"/>
@@ -7342,27 +7391,27 @@
       <c r="I40" s="40"/>
       <c r="J40" s="40"/>
       <c r="K40" s="41"/>
-      <c r="L40" s="135" t="s">
+      <c r="L40" s="138" t="s">
         <v>71</v>
       </c>
-      <c r="M40" s="136"/>
-      <c r="N40" s="136"/>
-      <c r="O40" s="136"/>
-      <c r="P40" s="136"/>
-      <c r="Q40" s="136"/>
-      <c r="R40" s="136"/>
-      <c r="S40" s="136"/>
-      <c r="T40" s="136"/>
-      <c r="U40" s="136"/>
-      <c r="V40" s="136"/>
-      <c r="W40" s="136"/>
-      <c r="X40" s="136"/>
-      <c r="Y40" s="136"/>
-      <c r="Z40" s="136"/>
-      <c r="AA40" s="136"/>
-      <c r="AB40" s="136"/>
-      <c r="AC40" s="136"/>
-      <c r="AD40" s="137"/>
+      <c r="M40" s="139"/>
+      <c r="N40" s="139"/>
+      <c r="O40" s="139"/>
+      <c r="P40" s="139"/>
+      <c r="Q40" s="139"/>
+      <c r="R40" s="139"/>
+      <c r="S40" s="139"/>
+      <c r="T40" s="139"/>
+      <c r="U40" s="139"/>
+      <c r="V40" s="139"/>
+      <c r="W40" s="139"/>
+      <c r="X40" s="139"/>
+      <c r="Y40" s="139"/>
+      <c r="Z40" s="139"/>
+      <c r="AA40" s="139"/>
+      <c r="AB40" s="139"/>
+      <c r="AC40" s="139"/>
+      <c r="AD40" s="140"/>
       <c r="AE40" s="2"/>
       <c r="AP40" s="5"/>
       <c r="AQ40" s="2"/>
@@ -7378,27 +7427,27 @@
       <c r="I41" s="40"/>
       <c r="J41" s="40"/>
       <c r="K41" s="41"/>
-      <c r="L41" s="135" t="s">
+      <c r="L41" s="138" t="s">
         <v>208</v>
       </c>
-      <c r="M41" s="136"/>
-      <c r="N41" s="136"/>
-      <c r="O41" s="136"/>
-      <c r="P41" s="136"/>
-      <c r="Q41" s="136"/>
-      <c r="R41" s="136"/>
-      <c r="S41" s="136"/>
-      <c r="T41" s="136"/>
-      <c r="U41" s="136"/>
-      <c r="V41" s="136"/>
-      <c r="W41" s="136"/>
-      <c r="X41" s="136"/>
-      <c r="Y41" s="136"/>
-      <c r="Z41" s="136"/>
-      <c r="AA41" s="136"/>
-      <c r="AB41" s="136"/>
-      <c r="AC41" s="136"/>
-      <c r="AD41" s="137"/>
+      <c r="M41" s="139"/>
+      <c r="N41" s="139"/>
+      <c r="O41" s="139"/>
+      <c r="P41" s="139"/>
+      <c r="Q41" s="139"/>
+      <c r="R41" s="139"/>
+      <c r="S41" s="139"/>
+      <c r="T41" s="139"/>
+      <c r="U41" s="139"/>
+      <c r="V41" s="139"/>
+      <c r="W41" s="139"/>
+      <c r="X41" s="139"/>
+      <c r="Y41" s="139"/>
+      <c r="Z41" s="139"/>
+      <c r="AA41" s="139"/>
+      <c r="AB41" s="139"/>
+      <c r="AC41" s="139"/>
+      <c r="AD41" s="140"/>
       <c r="AE41" s="2"/>
       <c r="AP41" s="5"/>
       <c r="AQ41" s="2"/>
@@ -7414,27 +7463,27 @@
       <c r="I42" s="40"/>
       <c r="J42" s="40"/>
       <c r="K42" s="41"/>
-      <c r="L42" s="135" t="s">
+      <c r="L42" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="M42" s="136"/>
-      <c r="N42" s="136"/>
-      <c r="O42" s="136"/>
-      <c r="P42" s="136"/>
-      <c r="Q42" s="136"/>
-      <c r="R42" s="136"/>
-      <c r="S42" s="136"/>
-      <c r="T42" s="136"/>
-      <c r="U42" s="136"/>
-      <c r="V42" s="136"/>
-      <c r="W42" s="136"/>
-      <c r="X42" s="136"/>
-      <c r="Y42" s="136"/>
-      <c r="Z42" s="136"/>
-      <c r="AA42" s="136"/>
-      <c r="AB42" s="136"/>
-      <c r="AC42" s="136"/>
-      <c r="AD42" s="137"/>
+      <c r="M42" s="139"/>
+      <c r="N42" s="139"/>
+      <c r="O42" s="139"/>
+      <c r="P42" s="139"/>
+      <c r="Q42" s="139"/>
+      <c r="R42" s="139"/>
+      <c r="S42" s="139"/>
+      <c r="T42" s="139"/>
+      <c r="U42" s="139"/>
+      <c r="V42" s="139"/>
+      <c r="W42" s="139"/>
+      <c r="X42" s="139"/>
+      <c r="Y42" s="139"/>
+      <c r="Z42" s="139"/>
+      <c r="AA42" s="139"/>
+      <c r="AB42" s="139"/>
+      <c r="AC42" s="139"/>
+      <c r="AD42" s="140"/>
       <c r="AE42" s="2"/>
       <c r="AP42" s="5"/>
       <c r="AQ42" s="2"/>
@@ -7450,27 +7499,27 @@
       <c r="I43" s="40"/>
       <c r="J43" s="40"/>
       <c r="K43" s="41"/>
-      <c r="L43" s="135" t="s">
+      <c r="L43" s="138" t="s">
         <v>69</v>
       </c>
-      <c r="M43" s="136"/>
-      <c r="N43" s="136"/>
-      <c r="O43" s="136"/>
-      <c r="P43" s="136"/>
-      <c r="Q43" s="136"/>
-      <c r="R43" s="136"/>
-      <c r="S43" s="136"/>
-      <c r="T43" s="136"/>
-      <c r="U43" s="136"/>
-      <c r="V43" s="136"/>
-      <c r="W43" s="136"/>
-      <c r="X43" s="136"/>
-      <c r="Y43" s="136"/>
-      <c r="Z43" s="136"/>
-      <c r="AA43" s="136"/>
-      <c r="AB43" s="136"/>
-      <c r="AC43" s="136"/>
-      <c r="AD43" s="137"/>
+      <c r="M43" s="139"/>
+      <c r="N43" s="139"/>
+      <c r="O43" s="139"/>
+      <c r="P43" s="139"/>
+      <c r="Q43" s="139"/>
+      <c r="R43" s="139"/>
+      <c r="S43" s="139"/>
+      <c r="T43" s="139"/>
+      <c r="U43" s="139"/>
+      <c r="V43" s="139"/>
+      <c r="W43" s="139"/>
+      <c r="X43" s="139"/>
+      <c r="Y43" s="139"/>
+      <c r="Z43" s="139"/>
+      <c r="AA43" s="139"/>
+      <c r="AB43" s="139"/>
+      <c r="AC43" s="139"/>
+      <c r="AD43" s="140"/>
       <c r="AE43" s="2"/>
       <c r="AP43" s="5"/>
       <c r="AQ43" s="2"/>
@@ -7545,27 +7594,27 @@
       <c r="I46" s="61"/>
       <c r="J46" s="61"/>
       <c r="K46" s="62"/>
-      <c r="L46" s="132" t="s">
+      <c r="L46" s="135" t="s">
         <v>60</v>
       </c>
-      <c r="M46" s="133"/>
-      <c r="N46" s="133"/>
-      <c r="O46" s="133"/>
-      <c r="P46" s="133"/>
-      <c r="Q46" s="133"/>
-      <c r="R46" s="133"/>
-      <c r="S46" s="133"/>
-      <c r="T46" s="133"/>
-      <c r="U46" s="133"/>
-      <c r="V46" s="133"/>
-      <c r="W46" s="133"/>
-      <c r="X46" s="133"/>
-      <c r="Y46" s="133"/>
-      <c r="Z46" s="133"/>
-      <c r="AA46" s="133"/>
-      <c r="AB46" s="133"/>
-      <c r="AC46" s="133"/>
-      <c r="AD46" s="134"/>
+      <c r="M46" s="136"/>
+      <c r="N46" s="136"/>
+      <c r="O46" s="136"/>
+      <c r="P46" s="136"/>
+      <c r="Q46" s="136"/>
+      <c r="R46" s="136"/>
+      <c r="S46" s="136"/>
+      <c r="T46" s="136"/>
+      <c r="U46" s="136"/>
+      <c r="V46" s="136"/>
+      <c r="W46" s="136"/>
+      <c r="X46" s="136"/>
+      <c r="Y46" s="136"/>
+      <c r="Z46" s="136"/>
+      <c r="AA46" s="136"/>
+      <c r="AB46" s="136"/>
+      <c r="AC46" s="136"/>
+      <c r="AD46" s="137"/>
       <c r="AP46" s="5"/>
       <c r="AQ46" s="2"/>
     </row>
@@ -7579,27 +7628,27 @@
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
       <c r="K47" s="13"/>
-      <c r="L47" s="135" t="s">
+      <c r="L47" s="138" t="s">
         <v>57</v>
       </c>
-      <c r="M47" s="136"/>
-      <c r="N47" s="136"/>
-      <c r="O47" s="136"/>
-      <c r="P47" s="136"/>
-      <c r="Q47" s="136"/>
-      <c r="R47" s="136"/>
-      <c r="S47" s="136"/>
-      <c r="T47" s="136"/>
-      <c r="U47" s="136"/>
-      <c r="V47" s="136"/>
-      <c r="W47" s="136"/>
-      <c r="X47" s="136"/>
-      <c r="Y47" s="136"/>
-      <c r="Z47" s="136"/>
-      <c r="AA47" s="136"/>
-      <c r="AB47" s="136"/>
-      <c r="AC47" s="136"/>
-      <c r="AD47" s="137"/>
+      <c r="M47" s="139"/>
+      <c r="N47" s="139"/>
+      <c r="O47" s="139"/>
+      <c r="P47" s="139"/>
+      <c r="Q47" s="139"/>
+      <c r="R47" s="139"/>
+      <c r="S47" s="139"/>
+      <c r="T47" s="139"/>
+      <c r="U47" s="139"/>
+      <c r="V47" s="139"/>
+      <c r="W47" s="139"/>
+      <c r="X47" s="139"/>
+      <c r="Y47" s="139"/>
+      <c r="Z47" s="139"/>
+      <c r="AA47" s="139"/>
+      <c r="AB47" s="139"/>
+      <c r="AC47" s="139"/>
+      <c r="AD47" s="140"/>
       <c r="AP47" s="5"/>
       <c r="AQ47" s="2"/>
     </row>
@@ -7613,27 +7662,27 @@
       <c r="I48" s="40"/>
       <c r="J48" s="40"/>
       <c r="K48" s="41"/>
-      <c r="L48" s="135" t="s">
+      <c r="L48" s="138" t="s">
         <v>73</v>
       </c>
-      <c r="M48" s="136"/>
-      <c r="N48" s="136"/>
-      <c r="O48" s="136"/>
-      <c r="P48" s="136"/>
-      <c r="Q48" s="136"/>
-      <c r="R48" s="136"/>
-      <c r="S48" s="136"/>
-      <c r="T48" s="136"/>
-      <c r="U48" s="136"/>
-      <c r="V48" s="136"/>
-      <c r="W48" s="136"/>
-      <c r="X48" s="136"/>
-      <c r="Y48" s="136"/>
-      <c r="Z48" s="136"/>
-      <c r="AA48" s="136"/>
-      <c r="AB48" s="136"/>
-      <c r="AC48" s="136"/>
-      <c r="AD48" s="137"/>
+      <c r="M48" s="139"/>
+      <c r="N48" s="139"/>
+      <c r="O48" s="139"/>
+      <c r="P48" s="139"/>
+      <c r="Q48" s="139"/>
+      <c r="R48" s="139"/>
+      <c r="S48" s="139"/>
+      <c r="T48" s="139"/>
+      <c r="U48" s="139"/>
+      <c r="V48" s="139"/>
+      <c r="W48" s="139"/>
+      <c r="X48" s="139"/>
+      <c r="Y48" s="139"/>
+      <c r="Z48" s="139"/>
+      <c r="AA48" s="139"/>
+      <c r="AB48" s="139"/>
+      <c r="AC48" s="139"/>
+      <c r="AD48" s="140"/>
       <c r="AP48" s="5"/>
       <c r="AQ48" s="2"/>
     </row>
@@ -10236,30 +10285,30 @@
       <c r="P123" s="61"/>
       <c r="Q123" s="61"/>
       <c r="R123" s="62"/>
-      <c r="S123" s="132" t="s">
+      <c r="S123" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="T123" s="133"/>
-      <c r="U123" s="133"/>
-      <c r="V123" s="133"/>
-      <c r="W123" s="133"/>
-      <c r="X123" s="134"/>
-      <c r="Y123" s="132" t="s">
+      <c r="T123" s="136"/>
+      <c r="U123" s="136"/>
+      <c r="V123" s="136"/>
+      <c r="W123" s="136"/>
+      <c r="X123" s="137"/>
+      <c r="Y123" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="Z123" s="133"/>
-      <c r="AA123" s="133"/>
-      <c r="AB123" s="133"/>
-      <c r="AC123" s="133"/>
-      <c r="AD123" s="134"/>
-      <c r="AE123" s="132" t="s">
+      <c r="Z123" s="136"/>
+      <c r="AA123" s="136"/>
+      <c r="AB123" s="136"/>
+      <c r="AC123" s="136"/>
+      <c r="AD123" s="137"/>
+      <c r="AE123" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="AF123" s="133"/>
-      <c r="AG123" s="133"/>
-      <c r="AH123" s="133"/>
-      <c r="AI123" s="133"/>
-      <c r="AJ123" s="134"/>
+      <c r="AF123" s="136"/>
+      <c r="AG123" s="136"/>
+      <c r="AH123" s="136"/>
+      <c r="AI123" s="136"/>
+      <c r="AJ123" s="137"/>
       <c r="AP123" s="5"/>
       <c r="AQ123" s="2"/>
     </row>
@@ -10281,30 +10330,30 @@
       <c r="P124" s="12"/>
       <c r="Q124" s="12"/>
       <c r="R124" s="13"/>
-      <c r="S124" s="135" t="s">
+      <c r="S124" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="T124" s="136"/>
-      <c r="U124" s="136"/>
-      <c r="V124" s="136"/>
-      <c r="W124" s="136"/>
-      <c r="X124" s="137"/>
-      <c r="Y124" s="135" t="s">
+      <c r="T124" s="139"/>
+      <c r="U124" s="139"/>
+      <c r="V124" s="139"/>
+      <c r="W124" s="139"/>
+      <c r="X124" s="140"/>
+      <c r="Y124" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="Z124" s="136"/>
-      <c r="AA124" s="136"/>
-      <c r="AB124" s="136"/>
-      <c r="AC124" s="136"/>
-      <c r="AD124" s="137"/>
-      <c r="AE124" s="135" t="s">
+      <c r="Z124" s="139"/>
+      <c r="AA124" s="139"/>
+      <c r="AB124" s="139"/>
+      <c r="AC124" s="139"/>
+      <c r="AD124" s="140"/>
+      <c r="AE124" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="AF124" s="136"/>
-      <c r="AG124" s="136"/>
-      <c r="AH124" s="136"/>
-      <c r="AI124" s="136"/>
-      <c r="AJ124" s="137"/>
+      <c r="AF124" s="139"/>
+      <c r="AG124" s="139"/>
+      <c r="AH124" s="139"/>
+      <c r="AI124" s="139"/>
+      <c r="AJ124" s="140"/>
       <c r="AP124" s="5"/>
       <c r="AQ124" s="2"/>
     </row>
@@ -10365,30 +10414,30 @@
       <c r="P126" s="19"/>
       <c r="Q126" s="19"/>
       <c r="R126" s="20"/>
-      <c r="S126" s="138" t="s">
+      <c r="S126" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="T126" s="139"/>
-      <c r="U126" s="139"/>
-      <c r="V126" s="139"/>
-      <c r="W126" s="139"/>
-      <c r="X126" s="140"/>
-      <c r="Y126" s="138" t="s">
+      <c r="T126" s="142"/>
+      <c r="U126" s="142"/>
+      <c r="V126" s="142"/>
+      <c r="W126" s="142"/>
+      <c r="X126" s="143"/>
+      <c r="Y126" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="Z126" s="139"/>
-      <c r="AA126" s="139"/>
-      <c r="AB126" s="139"/>
-      <c r="AC126" s="139"/>
-      <c r="AD126" s="140"/>
-      <c r="AE126" s="138" t="s">
+      <c r="Z126" s="142"/>
+      <c r="AA126" s="142"/>
+      <c r="AB126" s="142"/>
+      <c r="AC126" s="142"/>
+      <c r="AD126" s="143"/>
+      <c r="AE126" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="AF126" s="139"/>
-      <c r="AG126" s="139"/>
-      <c r="AH126" s="139"/>
-      <c r="AI126" s="139"/>
-      <c r="AJ126" s="140"/>
+      <c r="AF126" s="142"/>
+      <c r="AG126" s="142"/>
+      <c r="AH126" s="142"/>
+      <c r="AI126" s="142"/>
+      <c r="AJ126" s="143"/>
       <c r="AP126" s="5"/>
       <c r="AQ126" s="2"/>
     </row>
@@ -11085,22 +11134,22 @@
       <c r="V142" s="124"/>
       <c r="W142" s="124"/>
       <c r="X142" s="125"/>
-      <c r="Y142" s="120" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z142" s="121"/>
-      <c r="AA142" s="121"/>
-      <c r="AB142" s="121"/>
-      <c r="AC142" s="121"/>
-      <c r="AD142" s="122"/>
-      <c r="AE142" s="120" t="s">
-        <v>179</v>
-      </c>
-      <c r="AF142" s="121"/>
-      <c r="AG142" s="121"/>
-      <c r="AH142" s="121"/>
-      <c r="AI142" s="121"/>
-      <c r="AJ142" s="122"/>
+      <c r="Y142" s="126" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z142" s="127"/>
+      <c r="AA142" s="127"/>
+      <c r="AB142" s="127"/>
+      <c r="AC142" s="127"/>
+      <c r="AD142" s="128"/>
+      <c r="AE142" s="126" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF142" s="127"/>
+      <c r="AG142" s="127"/>
+      <c r="AH142" s="127"/>
+      <c r="AI142" s="127"/>
+      <c r="AJ142" s="128"/>
       <c r="AP142" s="5"/>
       <c r="AQ142" s="2"/>
     </row>
@@ -12505,30 +12554,30 @@
       <c r="P174" s="27"/>
       <c r="Q174" s="27"/>
       <c r="R174" s="28"/>
-      <c r="S174" s="126" t="s">
+      <c r="S174" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="T174" s="127"/>
-      <c r="U174" s="127"/>
-      <c r="V174" s="127"/>
-      <c r="W174" s="127"/>
-      <c r="X174" s="128"/>
-      <c r="Y174" s="129" t="s">
+      <c r="T174" s="130"/>
+      <c r="U174" s="130"/>
+      <c r="V174" s="130"/>
+      <c r="W174" s="130"/>
+      <c r="X174" s="131"/>
+      <c r="Y174" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="Z174" s="130"/>
-      <c r="AA174" s="130"/>
-      <c r="AB174" s="130"/>
-      <c r="AC174" s="130"/>
-      <c r="AD174" s="131"/>
-      <c r="AE174" s="129" t="s">
+      <c r="Z174" s="133"/>
+      <c r="AA174" s="133"/>
+      <c r="AB174" s="133"/>
+      <c r="AC174" s="133"/>
+      <c r="AD174" s="134"/>
+      <c r="AE174" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="AF174" s="130"/>
-      <c r="AG174" s="130"/>
-      <c r="AH174" s="130"/>
-      <c r="AI174" s="130"/>
-      <c r="AJ174" s="131"/>
+      <c r="AF174" s="133"/>
+      <c r="AG174" s="133"/>
+      <c r="AH174" s="133"/>
+      <c r="AI174" s="133"/>
+      <c r="AJ174" s="134"/>
       <c r="AP174" s="5"/>
       <c r="AQ174" s="2"/>
     </row>

</xml_diff>

<commit_message>
MAIL - Changed DB schema.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/RequirementDefinition.xlsx
+++ b/skrum_docs/02_SpecificationDocs/RequirementDefinition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="更新履歴" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="261">
   <si>
     <t>ユーザ権限</t>
     <rPh sb="3" eb="5">
@@ -2503,6 +2503,198 @@
     </rPh>
     <rPh sb="7" eb="9">
       <t>ヘンコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メール設定を追加。</t>
+    <rPh sb="3" eb="5">
+      <t>セッテ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ツイk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メール通知設定</t>
+    <rPh sb="3" eb="5">
+      <t>ツウt</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>項目</t>
+    <rPh sb="0" eb="2">
+      <t>コウモk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>進捗登録リマインダー</t>
+    <rPh sb="0" eb="4">
+      <t>シンチョk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>レポート</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skrumからのお知らせ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skrumからの重要なお知らせやサービスの更新情報</t>
+    <rPh sb="8" eb="10">
+      <t>ジュ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>コウs</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジョウh</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>所属部署/チームのメンバーの目標進捗率が一定の値に達した時</t>
+    <rPh sb="0" eb="2">
+      <t>ショゾk</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ブsh</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>モクヒョ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>シンチョk</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>リt</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>イッt</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>アタイn</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>タッs</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>所属部署/チームのメンバーがタイムラインに投稿した時</t>
+    <rPh sb="0" eb="2">
+      <t>ショゾk</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ブsh</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>トウコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>所属部署/チームのメンバーの進捗状況レポート</t>
+    <rPh sb="0" eb="2">
+      <t>ショゾk</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ブsh</t>
+    </rPh>
+    <rPh sb="14" eb="18">
+      <t>シンチョk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>所属部署/チームの進捗状況レポート</t>
+    <rPh sb="0" eb="2">
+      <t>ショゾk</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>シンチョk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <rPh sb="0" eb="2">
+      <t>メイsh</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイミング</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>適時</t>
+    <rPh sb="0" eb="2">
+      <t>テk</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>毎日</t>
+    <rPh sb="0" eb="2">
+      <t>マイニt</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>週一回（金曜日）</t>
+    <rPh sb="0" eb="3">
+      <t>シュ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>キンヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>権限</t>
+    <rPh sb="0" eb="2">
+      <t>ケンゲn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>スーパー管理者</t>
+    <rPh sb="4" eb="7">
+      <t>カンr</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（10%ごと）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フィードバック対象者自動抽出レポート</t>
+    <rPh sb="7" eb="10">
+      <t>タイsh</t>
+    </rPh>
+    <rPh sb="10" eb="14">
+      <t>ジド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>週一回（月曜日）</t>
+    <rPh sb="0" eb="3">
+      <t>シュ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ゲツ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>キンヨウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2552,7 +2744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2577,8 +2769,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="88">
+  <borders count="89">
     <border>
       <left/>
       <right/>
@@ -3721,11 +3919,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3854,6 +4061,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3881,76 +4160,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5204,6 +5456,131 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>51835</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>129590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>38877</xdr:colOff>
+      <xdr:row>233</xdr:row>
+      <xdr:rowOff>246224</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="四角形吹き出し 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11676223" y="60001019"/>
+          <a:ext cx="1477348" cy="635001"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -72183"/>
+            <a:gd name="adj2" fmla="val -43622"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>48725</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>139440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>35767</xdr:colOff>
+      <xdr:row>233</xdr:row>
+      <xdr:rowOff>256074</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="四角形吹き出し 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11673113" y="60010869"/>
+          <a:ext cx="1477348" cy="635001"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -73060"/>
+            <a:gd name="adj2" fmla="val 29847"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
+            <a:t>まずはこの</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400"/>
+            <a:t>2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
+            <a:t>つだけ。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5472,7 +5849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5642,10 +6019,18 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
+      <c r="B9" s="83">
+        <v>42947</v>
+      </c>
+      <c r="C9" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="82" t="s">
+        <v>240</v>
+      </c>
       <c r="F9" s="82"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -6182,9 +6567,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ244"/>
+  <dimension ref="A1:AQ258"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="98" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" workbookViewId="0">
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
@@ -6194,15 +6579,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="125"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="149"/>
       <c r="H1" s="55"/>
       <c r="I1" s="52" t="s">
         <v>79</v>
@@ -6213,53 +6598,53 @@
       <c r="M1" s="53"/>
       <c r="N1" s="53"/>
       <c r="O1" s="54"/>
-      <c r="P1" s="132" t="s">
+      <c r="P1" s="156" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" s="133"/>
-      <c r="R1" s="133"/>
-      <c r="S1" s="133"/>
-      <c r="T1" s="133"/>
-      <c r="U1" s="133"/>
-      <c r="V1" s="133"/>
-      <c r="W1" s="133"/>
-      <c r="X1" s="133"/>
-      <c r="Y1" s="133"/>
-      <c r="Z1" s="134"/>
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="157"/>
+      <c r="W1" s="157"/>
+      <c r="X1" s="157"/>
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="158"/>
       <c r="AA1" s="52" t="s">
         <v>74</v>
       </c>
       <c r="AB1" s="50"/>
       <c r="AC1" s="51"/>
-      <c r="AD1" s="129">
+      <c r="AD1" s="153">
         <v>42760</v>
       </c>
-      <c r="AE1" s="130"/>
-      <c r="AF1" s="130"/>
-      <c r="AG1" s="130"/>
-      <c r="AH1" s="131"/>
+      <c r="AE1" s="154"/>
+      <c r="AF1" s="154"/>
+      <c r="AG1" s="154"/>
+      <c r="AH1" s="155"/>
       <c r="AI1" s="52" t="s">
         <v>76</v>
       </c>
       <c r="AJ1" s="53"/>
       <c r="AK1" s="54"/>
-      <c r="AL1" s="120" t="s">
+      <c r="AL1" s="144" t="s">
         <v>78</v>
       </c>
-      <c r="AM1" s="121"/>
-      <c r="AN1" s="121"/>
-      <c r="AO1" s="121"/>
-      <c r="AP1" s="122"/>
+      <c r="AM1" s="145"/>
+      <c r="AN1" s="145"/>
+      <c r="AO1" s="145"/>
+      <c r="AP1" s="146"/>
       <c r="AQ1" s="2"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A2" s="126"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="128"/>
+      <c r="A2" s="150"/>
+      <c r="B2" s="151"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="152"/>
       <c r="H2" s="56"/>
       <c r="I2" s="52" t="s">
         <v>80</v>
@@ -6270,41 +6655,41 @@
       <c r="M2" s="53"/>
       <c r="N2" s="53"/>
       <c r="O2" s="54"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="133"/>
-      <c r="R2" s="133"/>
-      <c r="S2" s="133"/>
-      <c r="T2" s="133"/>
-      <c r="U2" s="133"/>
-      <c r="V2" s="133"/>
-      <c r="W2" s="133"/>
-      <c r="X2" s="133"/>
-      <c r="Y2" s="133"/>
-      <c r="Z2" s="134"/>
+      <c r="P2" s="156"/>
+      <c r="Q2" s="157"/>
+      <c r="R2" s="157"/>
+      <c r="S2" s="157"/>
+      <c r="T2" s="157"/>
+      <c r="U2" s="157"/>
+      <c r="V2" s="157"/>
+      <c r="W2" s="157"/>
+      <c r="X2" s="157"/>
+      <c r="Y2" s="157"/>
+      <c r="Z2" s="158"/>
       <c r="AA2" s="52" t="s">
         <v>75</v>
       </c>
       <c r="AB2" s="50"/>
       <c r="AC2" s="51"/>
-      <c r="AD2" s="129">
-        <v>42929</v>
-      </c>
-      <c r="AE2" s="130"/>
-      <c r="AF2" s="130"/>
-      <c r="AG2" s="130"/>
-      <c r="AH2" s="131"/>
+      <c r="AD2" s="153">
+        <v>42947</v>
+      </c>
+      <c r="AE2" s="154"/>
+      <c r="AF2" s="154"/>
+      <c r="AG2" s="154"/>
+      <c r="AH2" s="155"/>
       <c r="AI2" s="52" t="s">
         <v>77</v>
       </c>
       <c r="AJ2" s="53"/>
       <c r="AK2" s="54"/>
-      <c r="AL2" s="120" t="s">
+      <c r="AL2" s="144" t="s">
         <v>78</v>
       </c>
-      <c r="AM2" s="121"/>
-      <c r="AN2" s="121"/>
-      <c r="AO2" s="121"/>
-      <c r="AP2" s="122"/>
+      <c r="AM2" s="145"/>
+      <c r="AN2" s="145"/>
+      <c r="AO2" s="145"/>
+      <c r="AP2" s="146"/>
       <c r="AQ2" s="2"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
@@ -10472,30 +10857,30 @@
       <c r="P127" s="19"/>
       <c r="Q127" s="19"/>
       <c r="R127" s="20"/>
-      <c r="S127" s="147" t="s">
+      <c r="S127" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="T127" s="148"/>
-      <c r="U127" s="148"/>
-      <c r="V127" s="148"/>
-      <c r="W127" s="148"/>
-      <c r="X127" s="149"/>
-      <c r="Y127" s="147" t="s">
+      <c r="T127" s="142"/>
+      <c r="U127" s="142"/>
+      <c r="V127" s="142"/>
+      <c r="W127" s="142"/>
+      <c r="X127" s="143"/>
+      <c r="Y127" s="141" t="s">
         <v>14</v>
       </c>
-      <c r="Z127" s="148"/>
-      <c r="AA127" s="148"/>
-      <c r="AB127" s="148"/>
-      <c r="AC127" s="148"/>
-      <c r="AD127" s="149"/>
-      <c r="AE127" s="147" t="s">
+      <c r="Z127" s="142"/>
+      <c r="AA127" s="142"/>
+      <c r="AB127" s="142"/>
+      <c r="AC127" s="142"/>
+      <c r="AD127" s="143"/>
+      <c r="AE127" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="AF127" s="148"/>
-      <c r="AG127" s="148"/>
-      <c r="AH127" s="148"/>
-      <c r="AI127" s="148"/>
-      <c r="AJ127" s="149"/>
+      <c r="AF127" s="142"/>
+      <c r="AG127" s="142"/>
+      <c r="AH127" s="142"/>
+      <c r="AI127" s="142"/>
+      <c r="AJ127" s="143"/>
       <c r="AP127" s="5"/>
       <c r="AQ127" s="2"/>
     </row>
@@ -10517,30 +10902,30 @@
       <c r="P128" s="22"/>
       <c r="Q128" s="22"/>
       <c r="R128" s="23"/>
-      <c r="S128" s="144" t="s">
+      <c r="S128" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T128" s="145"/>
-      <c r="U128" s="145"/>
-      <c r="V128" s="145"/>
-      <c r="W128" s="145"/>
-      <c r="X128" s="146"/>
-      <c r="Y128" s="144" t="s">
+      <c r="T128" s="121"/>
+      <c r="U128" s="121"/>
+      <c r="V128" s="121"/>
+      <c r="W128" s="121"/>
+      <c r="X128" s="122"/>
+      <c r="Y128" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="Z128" s="145"/>
-      <c r="AA128" s="145"/>
-      <c r="AB128" s="145"/>
-      <c r="AC128" s="145"/>
-      <c r="AD128" s="146"/>
-      <c r="AE128" s="144" t="s">
+      <c r="Z128" s="121"/>
+      <c r="AA128" s="121"/>
+      <c r="AB128" s="121"/>
+      <c r="AC128" s="121"/>
+      <c r="AD128" s="122"/>
+      <c r="AE128" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF128" s="145"/>
-      <c r="AG128" s="145"/>
-      <c r="AH128" s="145"/>
-      <c r="AI128" s="145"/>
-      <c r="AJ128" s="146"/>
+      <c r="AF128" s="121"/>
+      <c r="AG128" s="121"/>
+      <c r="AH128" s="121"/>
+      <c r="AI128" s="121"/>
+      <c r="AJ128" s="122"/>
       <c r="AP128" s="5"/>
       <c r="AQ128" s="2"/>
     </row>
@@ -10564,30 +10949,30 @@
       <c r="P129" s="22"/>
       <c r="Q129" s="22"/>
       <c r="R129" s="23"/>
-      <c r="S129" s="144" t="s">
+      <c r="S129" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T129" s="145"/>
-      <c r="U129" s="145"/>
-      <c r="V129" s="145"/>
-      <c r="W129" s="145"/>
-      <c r="X129" s="146"/>
-      <c r="Y129" s="144" t="s">
+      <c r="T129" s="121"/>
+      <c r="U129" s="121"/>
+      <c r="V129" s="121"/>
+      <c r="W129" s="121"/>
+      <c r="X129" s="122"/>
+      <c r="Y129" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="Z129" s="145"/>
-      <c r="AA129" s="145"/>
-      <c r="AB129" s="145"/>
-      <c r="AC129" s="145"/>
-      <c r="AD129" s="146"/>
-      <c r="AE129" s="144" t="s">
+      <c r="Z129" s="121"/>
+      <c r="AA129" s="121"/>
+      <c r="AB129" s="121"/>
+      <c r="AC129" s="121"/>
+      <c r="AD129" s="122"/>
+      <c r="AE129" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF129" s="145"/>
-      <c r="AG129" s="145"/>
-      <c r="AH129" s="145"/>
-      <c r="AI129" s="145"/>
-      <c r="AJ129" s="146"/>
+      <c r="AF129" s="121"/>
+      <c r="AG129" s="121"/>
+      <c r="AH129" s="121"/>
+      <c r="AI129" s="121"/>
+      <c r="AJ129" s="122"/>
       <c r="AP129" s="5"/>
       <c r="AQ129" s="2"/>
     </row>
@@ -10605,30 +10990,30 @@
       <c r="P130" s="22"/>
       <c r="Q130" s="22"/>
       <c r="R130" s="23"/>
-      <c r="S130" s="144" t="s">
+      <c r="S130" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T130" s="145"/>
-      <c r="U130" s="145"/>
-      <c r="V130" s="145"/>
-      <c r="W130" s="145"/>
-      <c r="X130" s="146"/>
-      <c r="Y130" s="144" t="s">
+      <c r="T130" s="121"/>
+      <c r="U130" s="121"/>
+      <c r="V130" s="121"/>
+      <c r="W130" s="121"/>
+      <c r="X130" s="122"/>
+      <c r="Y130" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z130" s="145"/>
-      <c r="AA130" s="145"/>
-      <c r="AB130" s="145"/>
-      <c r="AC130" s="145"/>
-      <c r="AD130" s="146"/>
-      <c r="AE130" s="144" t="s">
+      <c r="Z130" s="121"/>
+      <c r="AA130" s="121"/>
+      <c r="AB130" s="121"/>
+      <c r="AC130" s="121"/>
+      <c r="AD130" s="122"/>
+      <c r="AE130" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF130" s="145"/>
-      <c r="AG130" s="145"/>
-      <c r="AH130" s="145"/>
-      <c r="AI130" s="145"/>
-      <c r="AJ130" s="146"/>
+      <c r="AF130" s="121"/>
+      <c r="AG130" s="121"/>
+      <c r="AH130" s="121"/>
+      <c r="AI130" s="121"/>
+      <c r="AJ130" s="122"/>
       <c r="AP130" s="5"/>
       <c r="AQ130" s="2"/>
     </row>
@@ -10650,30 +11035,30 @@
       <c r="P131" s="22"/>
       <c r="Q131" s="22"/>
       <c r="R131" s="23"/>
-      <c r="S131" s="144" t="s">
+      <c r="S131" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T131" s="145"/>
-      <c r="U131" s="145"/>
-      <c r="V131" s="145"/>
-      <c r="W131" s="145"/>
-      <c r="X131" s="146"/>
-      <c r="Y131" s="144" t="s">
+      <c r="T131" s="121"/>
+      <c r="U131" s="121"/>
+      <c r="V131" s="121"/>
+      <c r="W131" s="121"/>
+      <c r="X131" s="122"/>
+      <c r="Y131" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z131" s="145"/>
-      <c r="AA131" s="145"/>
-      <c r="AB131" s="145"/>
-      <c r="AC131" s="145"/>
-      <c r="AD131" s="146"/>
-      <c r="AE131" s="144" t="s">
+      <c r="Z131" s="121"/>
+      <c r="AA131" s="121"/>
+      <c r="AB131" s="121"/>
+      <c r="AC131" s="121"/>
+      <c r="AD131" s="122"/>
+      <c r="AE131" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF131" s="145"/>
-      <c r="AG131" s="145"/>
-      <c r="AH131" s="145"/>
-      <c r="AI131" s="145"/>
-      <c r="AJ131" s="146"/>
+      <c r="AF131" s="121"/>
+      <c r="AG131" s="121"/>
+      <c r="AH131" s="121"/>
+      <c r="AI131" s="121"/>
+      <c r="AJ131" s="122"/>
       <c r="AP131" s="5"/>
       <c r="AQ131" s="2"/>
     </row>
@@ -10697,30 +11082,30 @@
       <c r="P132" s="22"/>
       <c r="Q132" s="22"/>
       <c r="R132" s="25"/>
-      <c r="S132" s="144" t="s">
+      <c r="S132" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T132" s="145"/>
-      <c r="U132" s="145"/>
-      <c r="V132" s="145"/>
-      <c r="W132" s="145"/>
-      <c r="X132" s="146"/>
-      <c r="Y132" s="144" t="s">
+      <c r="T132" s="121"/>
+      <c r="U132" s="121"/>
+      <c r="V132" s="121"/>
+      <c r="W132" s="121"/>
+      <c r="X132" s="122"/>
+      <c r="Y132" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="Z132" s="145"/>
-      <c r="AA132" s="145"/>
-      <c r="AB132" s="145"/>
-      <c r="AC132" s="145"/>
-      <c r="AD132" s="146"/>
-      <c r="AE132" s="144" t="s">
+      <c r="Z132" s="121"/>
+      <c r="AA132" s="121"/>
+      <c r="AB132" s="121"/>
+      <c r="AC132" s="121"/>
+      <c r="AD132" s="122"/>
+      <c r="AE132" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF132" s="145"/>
-      <c r="AG132" s="145"/>
-      <c r="AH132" s="145"/>
-      <c r="AI132" s="145"/>
-      <c r="AJ132" s="146"/>
+      <c r="AF132" s="121"/>
+      <c r="AG132" s="121"/>
+      <c r="AH132" s="121"/>
+      <c r="AI132" s="121"/>
+      <c r="AJ132" s="122"/>
       <c r="AP132" s="5"/>
       <c r="AQ132" s="2"/>
     </row>
@@ -10738,30 +11123,30 @@
       <c r="P133" s="22"/>
       <c r="Q133" s="22"/>
       <c r="R133" s="25"/>
-      <c r="S133" s="144" t="s">
+      <c r="S133" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T133" s="145"/>
-      <c r="U133" s="145"/>
-      <c r="V133" s="145"/>
-      <c r="W133" s="145"/>
-      <c r="X133" s="146"/>
-      <c r="Y133" s="144" t="s">
+      <c r="T133" s="121"/>
+      <c r="U133" s="121"/>
+      <c r="V133" s="121"/>
+      <c r="W133" s="121"/>
+      <c r="X133" s="122"/>
+      <c r="Y133" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z133" s="145"/>
-      <c r="AA133" s="145"/>
-      <c r="AB133" s="145"/>
-      <c r="AC133" s="145"/>
-      <c r="AD133" s="146"/>
-      <c r="AE133" s="144" t="s">
+      <c r="Z133" s="121"/>
+      <c r="AA133" s="121"/>
+      <c r="AB133" s="121"/>
+      <c r="AC133" s="121"/>
+      <c r="AD133" s="122"/>
+      <c r="AE133" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF133" s="145"/>
-      <c r="AG133" s="145"/>
-      <c r="AH133" s="145"/>
-      <c r="AI133" s="145"/>
-      <c r="AJ133" s="146"/>
+      <c r="AF133" s="121"/>
+      <c r="AG133" s="121"/>
+      <c r="AH133" s="121"/>
+      <c r="AI133" s="121"/>
+      <c r="AJ133" s="122"/>
       <c r="AP133" s="5"/>
       <c r="AQ133" s="2"/>
     </row>
@@ -10783,30 +11168,30 @@
       <c r="P134" s="22"/>
       <c r="Q134" s="22"/>
       <c r="R134" s="25"/>
-      <c r="S134" s="144" t="s">
+      <c r="S134" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T134" s="145"/>
-      <c r="U134" s="145"/>
-      <c r="V134" s="145"/>
-      <c r="W134" s="145"/>
-      <c r="X134" s="146"/>
-      <c r="Y134" s="144" t="s">
+      <c r="T134" s="121"/>
+      <c r="U134" s="121"/>
+      <c r="V134" s="121"/>
+      <c r="W134" s="121"/>
+      <c r="X134" s="122"/>
+      <c r="Y134" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z134" s="145"/>
-      <c r="AA134" s="145"/>
-      <c r="AB134" s="145"/>
-      <c r="AC134" s="145"/>
-      <c r="AD134" s="146"/>
-      <c r="AE134" s="144" t="s">
+      <c r="Z134" s="121"/>
+      <c r="AA134" s="121"/>
+      <c r="AB134" s="121"/>
+      <c r="AC134" s="121"/>
+      <c r="AD134" s="122"/>
+      <c r="AE134" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF134" s="145"/>
-      <c r="AG134" s="145"/>
-      <c r="AH134" s="145"/>
-      <c r="AI134" s="145"/>
-      <c r="AJ134" s="146"/>
+      <c r="AF134" s="121"/>
+      <c r="AG134" s="121"/>
+      <c r="AH134" s="121"/>
+      <c r="AI134" s="121"/>
+      <c r="AJ134" s="122"/>
       <c r="AP134" s="5"/>
       <c r="AQ134" s="2"/>
     </row>
@@ -10828,30 +11213,30 @@
       <c r="P135" s="22"/>
       <c r="Q135" s="22"/>
       <c r="R135" s="25"/>
-      <c r="S135" s="144" t="s">
+      <c r="S135" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T135" s="145"/>
-      <c r="U135" s="145"/>
-      <c r="V135" s="145"/>
-      <c r="W135" s="145"/>
-      <c r="X135" s="146"/>
-      <c r="Y135" s="144" t="s">
+      <c r="T135" s="121"/>
+      <c r="U135" s="121"/>
+      <c r="V135" s="121"/>
+      <c r="W135" s="121"/>
+      <c r="X135" s="122"/>
+      <c r="Y135" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z135" s="145"/>
-      <c r="AA135" s="145"/>
-      <c r="AB135" s="145"/>
-      <c r="AC135" s="145"/>
-      <c r="AD135" s="146"/>
-      <c r="AE135" s="141" t="s">
+      <c r="Z135" s="121"/>
+      <c r="AA135" s="121"/>
+      <c r="AB135" s="121"/>
+      <c r="AC135" s="121"/>
+      <c r="AD135" s="122"/>
+      <c r="AE135" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="AF135" s="142"/>
-      <c r="AG135" s="142"/>
-      <c r="AH135" s="142"/>
-      <c r="AI135" s="142"/>
-      <c r="AJ135" s="143"/>
+      <c r="AF135" s="124"/>
+      <c r="AG135" s="124"/>
+      <c r="AH135" s="124"/>
+      <c r="AI135" s="124"/>
+      <c r="AJ135" s="125"/>
       <c r="AP135" s="5"/>
       <c r="AQ135" s="2"/>
     </row>
@@ -10875,30 +11260,30 @@
       <c r="P136" s="22"/>
       <c r="Q136" s="22"/>
       <c r="R136" s="25"/>
-      <c r="S136" s="144" t="s">
+      <c r="S136" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T136" s="145"/>
-      <c r="U136" s="145"/>
-      <c r="V136" s="145"/>
-      <c r="W136" s="145"/>
-      <c r="X136" s="146"/>
-      <c r="Y136" s="144" t="s">
+      <c r="T136" s="121"/>
+      <c r="U136" s="121"/>
+      <c r="V136" s="121"/>
+      <c r="W136" s="121"/>
+      <c r="X136" s="122"/>
+      <c r="Y136" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="Z136" s="145"/>
-      <c r="AA136" s="145"/>
-      <c r="AB136" s="145"/>
-      <c r="AC136" s="145"/>
-      <c r="AD136" s="146"/>
-      <c r="AE136" s="144" t="s">
+      <c r="Z136" s="121"/>
+      <c r="AA136" s="121"/>
+      <c r="AB136" s="121"/>
+      <c r="AC136" s="121"/>
+      <c r="AD136" s="122"/>
+      <c r="AE136" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF136" s="145"/>
-      <c r="AG136" s="145"/>
-      <c r="AH136" s="145"/>
-      <c r="AI136" s="145"/>
-      <c r="AJ136" s="146"/>
+      <c r="AF136" s="121"/>
+      <c r="AG136" s="121"/>
+      <c r="AH136" s="121"/>
+      <c r="AI136" s="121"/>
+      <c r="AJ136" s="122"/>
       <c r="AP136" s="5"/>
       <c r="AQ136" s="2"/>
     </row>
@@ -10916,30 +11301,30 @@
       <c r="P137" s="22"/>
       <c r="Q137" s="22"/>
       <c r="R137" s="25"/>
-      <c r="S137" s="144" t="s">
+      <c r="S137" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T137" s="145"/>
-      <c r="U137" s="145"/>
-      <c r="V137" s="145"/>
-      <c r="W137" s="145"/>
-      <c r="X137" s="146"/>
-      <c r="Y137" s="144" t="s">
+      <c r="T137" s="121"/>
+      <c r="U137" s="121"/>
+      <c r="V137" s="121"/>
+      <c r="W137" s="121"/>
+      <c r="X137" s="122"/>
+      <c r="Y137" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z137" s="145"/>
-      <c r="AA137" s="145"/>
-      <c r="AB137" s="145"/>
-      <c r="AC137" s="145"/>
-      <c r="AD137" s="146"/>
-      <c r="AE137" s="144" t="s">
+      <c r="Z137" s="121"/>
+      <c r="AA137" s="121"/>
+      <c r="AB137" s="121"/>
+      <c r="AC137" s="121"/>
+      <c r="AD137" s="122"/>
+      <c r="AE137" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF137" s="145"/>
-      <c r="AG137" s="145"/>
-      <c r="AH137" s="145"/>
-      <c r="AI137" s="145"/>
-      <c r="AJ137" s="146"/>
+      <c r="AF137" s="121"/>
+      <c r="AG137" s="121"/>
+      <c r="AH137" s="121"/>
+      <c r="AI137" s="121"/>
+      <c r="AJ137" s="122"/>
       <c r="AP137" s="5"/>
       <c r="AQ137" s="2"/>
     </row>
@@ -10961,30 +11346,30 @@
       <c r="P138" s="22"/>
       <c r="Q138" s="22"/>
       <c r="R138" s="25"/>
-      <c r="S138" s="144" t="s">
+      <c r="S138" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T138" s="145"/>
-      <c r="U138" s="145"/>
-      <c r="V138" s="145"/>
-      <c r="W138" s="145"/>
-      <c r="X138" s="146"/>
-      <c r="Y138" s="144" t="s">
+      <c r="T138" s="121"/>
+      <c r="U138" s="121"/>
+      <c r="V138" s="121"/>
+      <c r="W138" s="121"/>
+      <c r="X138" s="122"/>
+      <c r="Y138" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z138" s="145"/>
-      <c r="AA138" s="145"/>
-      <c r="AB138" s="145"/>
-      <c r="AC138" s="145"/>
-      <c r="AD138" s="146"/>
-      <c r="AE138" s="144" t="s">
+      <c r="Z138" s="121"/>
+      <c r="AA138" s="121"/>
+      <c r="AB138" s="121"/>
+      <c r="AC138" s="121"/>
+      <c r="AD138" s="122"/>
+      <c r="AE138" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF138" s="145"/>
-      <c r="AG138" s="145"/>
-      <c r="AH138" s="145"/>
-      <c r="AI138" s="145"/>
-      <c r="AJ138" s="146"/>
+      <c r="AF138" s="121"/>
+      <c r="AG138" s="121"/>
+      <c r="AH138" s="121"/>
+      <c r="AI138" s="121"/>
+      <c r="AJ138" s="122"/>
       <c r="AP138" s="5"/>
       <c r="AQ138" s="2"/>
     </row>
@@ -11006,30 +11391,30 @@
       <c r="P139" s="22"/>
       <c r="Q139" s="22"/>
       <c r="R139" s="25"/>
-      <c r="S139" s="144" t="s">
+      <c r="S139" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T139" s="145"/>
-      <c r="U139" s="145"/>
-      <c r="V139" s="145"/>
-      <c r="W139" s="145"/>
-      <c r="X139" s="146"/>
-      <c r="Y139" s="144" t="s">
+      <c r="T139" s="121"/>
+      <c r="U139" s="121"/>
+      <c r="V139" s="121"/>
+      <c r="W139" s="121"/>
+      <c r="X139" s="122"/>
+      <c r="Y139" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z139" s="145"/>
-      <c r="AA139" s="145"/>
-      <c r="AB139" s="145"/>
-      <c r="AC139" s="145"/>
-      <c r="AD139" s="146"/>
-      <c r="AE139" s="141" t="s">
+      <c r="Z139" s="121"/>
+      <c r="AA139" s="121"/>
+      <c r="AB139" s="121"/>
+      <c r="AC139" s="121"/>
+      <c r="AD139" s="122"/>
+      <c r="AE139" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="AF139" s="142"/>
-      <c r="AG139" s="142"/>
-      <c r="AH139" s="142"/>
-      <c r="AI139" s="142"/>
-      <c r="AJ139" s="143"/>
+      <c r="AF139" s="124"/>
+      <c r="AG139" s="124"/>
+      <c r="AH139" s="124"/>
+      <c r="AI139" s="124"/>
+      <c r="AJ139" s="125"/>
       <c r="AP139" s="5"/>
       <c r="AQ139" s="2"/>
     </row>
@@ -11053,30 +11438,30 @@
       <c r="P140" s="22"/>
       <c r="Q140" s="22"/>
       <c r="R140" s="25"/>
-      <c r="S140" s="144" t="s">
+      <c r="S140" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T140" s="145"/>
-      <c r="U140" s="145"/>
-      <c r="V140" s="145"/>
-      <c r="W140" s="145"/>
-      <c r="X140" s="146"/>
-      <c r="Y140" s="144" t="s">
+      <c r="T140" s="121"/>
+      <c r="U140" s="121"/>
+      <c r="V140" s="121"/>
+      <c r="W140" s="121"/>
+      <c r="X140" s="122"/>
+      <c r="Y140" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="Z140" s="145"/>
-      <c r="AA140" s="145"/>
-      <c r="AB140" s="145"/>
-      <c r="AC140" s="145"/>
-      <c r="AD140" s="146"/>
-      <c r="AE140" s="144" t="s">
+      <c r="Z140" s="121"/>
+      <c r="AA140" s="121"/>
+      <c r="AB140" s="121"/>
+      <c r="AC140" s="121"/>
+      <c r="AD140" s="122"/>
+      <c r="AE140" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF140" s="145"/>
-      <c r="AG140" s="145"/>
-      <c r="AH140" s="145"/>
-      <c r="AI140" s="145"/>
-      <c r="AJ140" s="146"/>
+      <c r="AF140" s="121"/>
+      <c r="AG140" s="121"/>
+      <c r="AH140" s="121"/>
+      <c r="AI140" s="121"/>
+      <c r="AJ140" s="122"/>
       <c r="AP140" s="5"/>
       <c r="AQ140" s="2"/>
     </row>
@@ -11094,30 +11479,30 @@
       <c r="P141" s="22"/>
       <c r="Q141" s="22"/>
       <c r="R141" s="25"/>
-      <c r="S141" s="144" t="s">
+      <c r="S141" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T141" s="145"/>
-      <c r="U141" s="145"/>
-      <c r="V141" s="145"/>
-      <c r="W141" s="145"/>
-      <c r="X141" s="146"/>
-      <c r="Y141" s="144" t="s">
+      <c r="T141" s="121"/>
+      <c r="U141" s="121"/>
+      <c r="V141" s="121"/>
+      <c r="W141" s="121"/>
+      <c r="X141" s="122"/>
+      <c r="Y141" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z141" s="145"/>
-      <c r="AA141" s="145"/>
-      <c r="AB141" s="145"/>
-      <c r="AC141" s="145"/>
-      <c r="AD141" s="146"/>
-      <c r="AE141" s="144" t="s">
+      <c r="Z141" s="121"/>
+      <c r="AA141" s="121"/>
+      <c r="AB141" s="121"/>
+      <c r="AC141" s="121"/>
+      <c r="AD141" s="122"/>
+      <c r="AE141" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF141" s="145"/>
-      <c r="AG141" s="145"/>
-      <c r="AH141" s="145"/>
-      <c r="AI141" s="145"/>
-      <c r="AJ141" s="146"/>
+      <c r="AF141" s="121"/>
+      <c r="AG141" s="121"/>
+      <c r="AH141" s="121"/>
+      <c r="AI141" s="121"/>
+      <c r="AJ141" s="122"/>
       <c r="AP141" s="5"/>
       <c r="AQ141" s="2"/>
     </row>
@@ -11139,30 +11524,30 @@
       <c r="P142" s="22"/>
       <c r="Q142" s="22"/>
       <c r="R142" s="25"/>
-      <c r="S142" s="144" t="s">
+      <c r="S142" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="T142" s="145"/>
-      <c r="U142" s="145"/>
-      <c r="V142" s="145"/>
-      <c r="W142" s="145"/>
-      <c r="X142" s="146"/>
-      <c r="Y142" s="144" t="s">
+      <c r="T142" s="121"/>
+      <c r="U142" s="121"/>
+      <c r="V142" s="121"/>
+      <c r="W142" s="121"/>
+      <c r="X142" s="122"/>
+      <c r="Y142" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z142" s="145"/>
-      <c r="AA142" s="145"/>
-      <c r="AB142" s="145"/>
-      <c r="AC142" s="145"/>
-      <c r="AD142" s="146"/>
-      <c r="AE142" s="144" t="s">
+      <c r="Z142" s="121"/>
+      <c r="AA142" s="121"/>
+      <c r="AB142" s="121"/>
+      <c r="AC142" s="121"/>
+      <c r="AD142" s="122"/>
+      <c r="AE142" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF142" s="145"/>
-      <c r="AG142" s="145"/>
-      <c r="AH142" s="145"/>
-      <c r="AI142" s="145"/>
-      <c r="AJ142" s="146"/>
+      <c r="AF142" s="121"/>
+      <c r="AG142" s="121"/>
+      <c r="AH142" s="121"/>
+      <c r="AI142" s="121"/>
+      <c r="AJ142" s="122"/>
       <c r="AP142" s="5"/>
       <c r="AQ142" s="2"/>
     </row>
@@ -11184,30 +11569,30 @@
       <c r="P143" s="88"/>
       <c r="Q143" s="88"/>
       <c r="R143" s="89"/>
-      <c r="S143" s="141" t="s">
+      <c r="S143" s="123" t="s">
         <v>43</v>
       </c>
-      <c r="T143" s="142"/>
-      <c r="U143" s="142"/>
-      <c r="V143" s="142"/>
-      <c r="W143" s="142"/>
-      <c r="X143" s="143"/>
-      <c r="Y143" s="156" t="s">
+      <c r="T143" s="124"/>
+      <c r="U143" s="124"/>
+      <c r="V143" s="124"/>
+      <c r="W143" s="124"/>
+      <c r="X143" s="125"/>
+      <c r="Y143" s="126" t="s">
         <v>235</v>
       </c>
-      <c r="Z143" s="157"/>
-      <c r="AA143" s="157"/>
-      <c r="AB143" s="157"/>
-      <c r="AC143" s="157"/>
-      <c r="AD143" s="158"/>
-      <c r="AE143" s="156" t="s">
+      <c r="Z143" s="127"/>
+      <c r="AA143" s="127"/>
+      <c r="AB143" s="127"/>
+      <c r="AC143" s="127"/>
+      <c r="AD143" s="128"/>
+      <c r="AE143" s="126" t="s">
         <v>235</v>
       </c>
-      <c r="AF143" s="157"/>
-      <c r="AG143" s="157"/>
-      <c r="AH143" s="157"/>
-      <c r="AI143" s="157"/>
-      <c r="AJ143" s="158"/>
+      <c r="AF143" s="127"/>
+      <c r="AG143" s="127"/>
+      <c r="AH143" s="127"/>
+      <c r="AI143" s="127"/>
+      <c r="AJ143" s="128"/>
       <c r="AP143" s="5"/>
       <c r="AQ143" s="2"/>
     </row>
@@ -11231,30 +11616,30 @@
       <c r="P144" s="85"/>
       <c r="Q144" s="85"/>
       <c r="R144" s="86"/>
-      <c r="S144" s="141" t="s">
+      <c r="S144" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T144" s="142"/>
-      <c r="U144" s="142"/>
-      <c r="V144" s="142"/>
-      <c r="W144" s="142"/>
-      <c r="X144" s="143"/>
-      <c r="Y144" s="144" t="s">
+      <c r="T144" s="124"/>
+      <c r="U144" s="124"/>
+      <c r="V144" s="124"/>
+      <c r="W144" s="124"/>
+      <c r="X144" s="125"/>
+      <c r="Y144" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="Z144" s="145"/>
-      <c r="AA144" s="145"/>
-      <c r="AB144" s="145"/>
-      <c r="AC144" s="145"/>
-      <c r="AD144" s="146"/>
-      <c r="AE144" s="144" t="s">
+      <c r="Z144" s="121"/>
+      <c r="AA144" s="121"/>
+      <c r="AB144" s="121"/>
+      <c r="AC144" s="121"/>
+      <c r="AD144" s="122"/>
+      <c r="AE144" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF144" s="145"/>
-      <c r="AG144" s="145"/>
-      <c r="AH144" s="145"/>
-      <c r="AI144" s="145"/>
-      <c r="AJ144" s="146"/>
+      <c r="AF144" s="121"/>
+      <c r="AG144" s="121"/>
+      <c r="AH144" s="121"/>
+      <c r="AI144" s="121"/>
+      <c r="AJ144" s="122"/>
       <c r="AP144" s="5"/>
       <c r="AQ144" s="2"/>
     </row>
@@ -11272,30 +11657,30 @@
       <c r="P145" s="22"/>
       <c r="Q145" s="22"/>
       <c r="R145" s="25"/>
-      <c r="S145" s="141" t="s">
+      <c r="S145" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T145" s="142"/>
-      <c r="U145" s="142"/>
-      <c r="V145" s="142"/>
-      <c r="W145" s="142"/>
-      <c r="X145" s="143"/>
-      <c r="Y145" s="141" t="s">
+      <c r="T145" s="124"/>
+      <c r="U145" s="124"/>
+      <c r="V145" s="124"/>
+      <c r="W145" s="124"/>
+      <c r="X145" s="125"/>
+      <c r="Y145" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z145" s="142"/>
-      <c r="AA145" s="142"/>
-      <c r="AB145" s="142"/>
-      <c r="AC145" s="142"/>
-      <c r="AD145" s="143"/>
-      <c r="AE145" s="144" t="s">
+      <c r="Z145" s="124"/>
+      <c r="AA145" s="124"/>
+      <c r="AB145" s="124"/>
+      <c r="AC145" s="124"/>
+      <c r="AD145" s="125"/>
+      <c r="AE145" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF145" s="145"/>
-      <c r="AG145" s="145"/>
-      <c r="AH145" s="145"/>
-      <c r="AI145" s="145"/>
-      <c r="AJ145" s="146"/>
+      <c r="AF145" s="121"/>
+      <c r="AG145" s="121"/>
+      <c r="AH145" s="121"/>
+      <c r="AI145" s="121"/>
+      <c r="AJ145" s="122"/>
       <c r="AP145" s="5"/>
       <c r="AQ145" s="2"/>
     </row>
@@ -11317,30 +11702,30 @@
       <c r="P146" s="22"/>
       <c r="Q146" s="22"/>
       <c r="R146" s="25"/>
-      <c r="S146" s="141" t="s">
+      <c r="S146" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T146" s="142"/>
-      <c r="U146" s="142"/>
-      <c r="V146" s="142"/>
-      <c r="W146" s="142"/>
-      <c r="X146" s="143"/>
-      <c r="Y146" s="141" t="s">
+      <c r="T146" s="124"/>
+      <c r="U146" s="124"/>
+      <c r="V146" s="124"/>
+      <c r="W146" s="124"/>
+      <c r="X146" s="125"/>
+      <c r="Y146" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z146" s="142"/>
-      <c r="AA146" s="142"/>
-      <c r="AB146" s="142"/>
-      <c r="AC146" s="142"/>
-      <c r="AD146" s="143"/>
-      <c r="AE146" s="144" t="s">
+      <c r="Z146" s="124"/>
+      <c r="AA146" s="124"/>
+      <c r="AB146" s="124"/>
+      <c r="AC146" s="124"/>
+      <c r="AD146" s="125"/>
+      <c r="AE146" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF146" s="145"/>
-      <c r="AG146" s="145"/>
-      <c r="AH146" s="145"/>
-      <c r="AI146" s="145"/>
-      <c r="AJ146" s="146"/>
+      <c r="AF146" s="121"/>
+      <c r="AG146" s="121"/>
+      <c r="AH146" s="121"/>
+      <c r="AI146" s="121"/>
+      <c r="AJ146" s="122"/>
       <c r="AP146" s="5"/>
       <c r="AQ146" s="2"/>
     </row>
@@ -11364,30 +11749,30 @@
       <c r="P147" s="22"/>
       <c r="Q147" s="22"/>
       <c r="R147" s="25"/>
-      <c r="S147" s="141" t="s">
+      <c r="S147" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T147" s="142"/>
-      <c r="U147" s="142"/>
-      <c r="V147" s="142"/>
-      <c r="W147" s="142"/>
-      <c r="X147" s="143"/>
-      <c r="Y147" s="141" t="s">
+      <c r="T147" s="124"/>
+      <c r="U147" s="124"/>
+      <c r="V147" s="124"/>
+      <c r="W147" s="124"/>
+      <c r="X147" s="125"/>
+      <c r="Y147" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z147" s="142"/>
-      <c r="AA147" s="142"/>
-      <c r="AB147" s="142"/>
-      <c r="AC147" s="142"/>
-      <c r="AD147" s="143"/>
-      <c r="AE147" s="144" t="s">
+      <c r="Z147" s="124"/>
+      <c r="AA147" s="124"/>
+      <c r="AB147" s="124"/>
+      <c r="AC147" s="124"/>
+      <c r="AD147" s="125"/>
+      <c r="AE147" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="AF147" s="145"/>
-      <c r="AG147" s="145"/>
-      <c r="AH147" s="145"/>
-      <c r="AI147" s="145"/>
-      <c r="AJ147" s="146"/>
+      <c r="AF147" s="121"/>
+      <c r="AG147" s="121"/>
+      <c r="AH147" s="121"/>
+      <c r="AI147" s="121"/>
+      <c r="AJ147" s="122"/>
       <c r="AP147" s="5"/>
       <c r="AQ147" s="2"/>
     </row>
@@ -11405,30 +11790,30 @@
       <c r="P148" s="22"/>
       <c r="Q148" s="22"/>
       <c r="R148" s="25"/>
-      <c r="S148" s="141" t="s">
+      <c r="S148" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T148" s="142"/>
-      <c r="U148" s="142"/>
-      <c r="V148" s="142"/>
-      <c r="W148" s="142"/>
-      <c r="X148" s="143"/>
-      <c r="Y148" s="141" t="s">
+      <c r="T148" s="124"/>
+      <c r="U148" s="124"/>
+      <c r="V148" s="124"/>
+      <c r="W148" s="124"/>
+      <c r="X148" s="125"/>
+      <c r="Y148" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z148" s="142"/>
-      <c r="AA148" s="142"/>
-      <c r="AB148" s="142"/>
-      <c r="AC148" s="142"/>
-      <c r="AD148" s="143"/>
-      <c r="AE148" s="144" t="s">
+      <c r="Z148" s="124"/>
+      <c r="AA148" s="124"/>
+      <c r="AB148" s="124"/>
+      <c r="AC148" s="124"/>
+      <c r="AD148" s="125"/>
+      <c r="AE148" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF148" s="145"/>
-      <c r="AG148" s="145"/>
-      <c r="AH148" s="145"/>
-      <c r="AI148" s="145"/>
-      <c r="AJ148" s="146"/>
+      <c r="AF148" s="121"/>
+      <c r="AG148" s="121"/>
+      <c r="AH148" s="121"/>
+      <c r="AI148" s="121"/>
+      <c r="AJ148" s="122"/>
       <c r="AP148" s="5"/>
       <c r="AQ148" s="2"/>
     </row>
@@ -11450,30 +11835,30 @@
       <c r="P149" s="22"/>
       <c r="Q149" s="22"/>
       <c r="R149" s="25"/>
-      <c r="S149" s="141" t="s">
+      <c r="S149" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T149" s="142"/>
-      <c r="U149" s="142"/>
-      <c r="V149" s="142"/>
-      <c r="W149" s="142"/>
-      <c r="X149" s="143"/>
-      <c r="Y149" s="141" t="s">
+      <c r="T149" s="124"/>
+      <c r="U149" s="124"/>
+      <c r="V149" s="124"/>
+      <c r="W149" s="124"/>
+      <c r="X149" s="125"/>
+      <c r="Y149" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z149" s="142"/>
-      <c r="AA149" s="142"/>
-      <c r="AB149" s="142"/>
-      <c r="AC149" s="142"/>
-      <c r="AD149" s="143"/>
-      <c r="AE149" s="144" t="s">
+      <c r="Z149" s="124"/>
+      <c r="AA149" s="124"/>
+      <c r="AB149" s="124"/>
+      <c r="AC149" s="124"/>
+      <c r="AD149" s="125"/>
+      <c r="AE149" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF149" s="145"/>
-      <c r="AG149" s="145"/>
-      <c r="AH149" s="145"/>
-      <c r="AI149" s="145"/>
-      <c r="AJ149" s="146"/>
+      <c r="AF149" s="121"/>
+      <c r="AG149" s="121"/>
+      <c r="AH149" s="121"/>
+      <c r="AI149" s="121"/>
+      <c r="AJ149" s="122"/>
       <c r="AP149" s="5"/>
       <c r="AQ149" s="2"/>
     </row>
@@ -11497,30 +11882,30 @@
       <c r="P150" s="22"/>
       <c r="Q150" s="22"/>
       <c r="R150" s="25"/>
-      <c r="S150" s="141" t="s">
+      <c r="S150" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T150" s="142"/>
-      <c r="U150" s="142"/>
-      <c r="V150" s="142"/>
-      <c r="W150" s="142"/>
-      <c r="X150" s="143"/>
-      <c r="Y150" s="141" t="s">
+      <c r="T150" s="124"/>
+      <c r="U150" s="124"/>
+      <c r="V150" s="124"/>
+      <c r="W150" s="124"/>
+      <c r="X150" s="125"/>
+      <c r="Y150" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z150" s="142"/>
-      <c r="AA150" s="142"/>
-      <c r="AB150" s="142"/>
-      <c r="AC150" s="142"/>
-      <c r="AD150" s="143"/>
-      <c r="AE150" s="144" t="s">
+      <c r="Z150" s="124"/>
+      <c r="AA150" s="124"/>
+      <c r="AB150" s="124"/>
+      <c r="AC150" s="124"/>
+      <c r="AD150" s="125"/>
+      <c r="AE150" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF150" s="145"/>
-      <c r="AG150" s="145"/>
-      <c r="AH150" s="145"/>
-      <c r="AI150" s="145"/>
-      <c r="AJ150" s="146"/>
+      <c r="AF150" s="121"/>
+      <c r="AG150" s="121"/>
+      <c r="AH150" s="121"/>
+      <c r="AI150" s="121"/>
+      <c r="AJ150" s="122"/>
       <c r="AP150" s="5"/>
       <c r="AQ150" s="2"/>
     </row>
@@ -11540,30 +11925,30 @@
       <c r="P151" s="22"/>
       <c r="Q151" s="22"/>
       <c r="R151" s="25"/>
-      <c r="S151" s="141" t="s">
+      <c r="S151" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T151" s="142"/>
-      <c r="U151" s="142"/>
-      <c r="V151" s="142"/>
-      <c r="W151" s="142"/>
-      <c r="X151" s="143"/>
-      <c r="Y151" s="141" t="s">
+      <c r="T151" s="124"/>
+      <c r="U151" s="124"/>
+      <c r="V151" s="124"/>
+      <c r="W151" s="124"/>
+      <c r="X151" s="125"/>
+      <c r="Y151" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z151" s="142"/>
-      <c r="AA151" s="142"/>
-      <c r="AB151" s="142"/>
-      <c r="AC151" s="142"/>
-      <c r="AD151" s="143"/>
-      <c r="AE151" s="144" t="s">
+      <c r="Z151" s="124"/>
+      <c r="AA151" s="124"/>
+      <c r="AB151" s="124"/>
+      <c r="AC151" s="124"/>
+      <c r="AD151" s="125"/>
+      <c r="AE151" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF151" s="145"/>
-      <c r="AG151" s="145"/>
-      <c r="AH151" s="145"/>
-      <c r="AI151" s="145"/>
-      <c r="AJ151" s="146"/>
+      <c r="AF151" s="121"/>
+      <c r="AG151" s="121"/>
+      <c r="AH151" s="121"/>
+      <c r="AI151" s="121"/>
+      <c r="AJ151" s="122"/>
       <c r="AP151" s="5"/>
       <c r="AQ151" s="2"/>
     </row>
@@ -11585,30 +11970,30 @@
       <c r="P152" s="22"/>
       <c r="Q152" s="22"/>
       <c r="R152" s="25"/>
-      <c r="S152" s="141" t="s">
+      <c r="S152" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T152" s="142"/>
-      <c r="U152" s="142"/>
-      <c r="V152" s="142"/>
-      <c r="W152" s="142"/>
-      <c r="X152" s="143"/>
-      <c r="Y152" s="141" t="s">
+      <c r="T152" s="124"/>
+      <c r="U152" s="124"/>
+      <c r="V152" s="124"/>
+      <c r="W152" s="124"/>
+      <c r="X152" s="125"/>
+      <c r="Y152" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z152" s="142"/>
-      <c r="AA152" s="142"/>
-      <c r="AB152" s="142"/>
-      <c r="AC152" s="142"/>
-      <c r="AD152" s="143"/>
-      <c r="AE152" s="144" t="s">
+      <c r="Z152" s="124"/>
+      <c r="AA152" s="124"/>
+      <c r="AB152" s="124"/>
+      <c r="AC152" s="124"/>
+      <c r="AD152" s="125"/>
+      <c r="AE152" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF152" s="145"/>
-      <c r="AG152" s="145"/>
-      <c r="AH152" s="145"/>
-      <c r="AI152" s="145"/>
-      <c r="AJ152" s="146"/>
+      <c r="AF152" s="121"/>
+      <c r="AG152" s="121"/>
+      <c r="AH152" s="121"/>
+      <c r="AI152" s="121"/>
+      <c r="AJ152" s="122"/>
       <c r="AP152" s="5"/>
       <c r="AQ152" s="2"/>
     </row>
@@ -11632,30 +12017,30 @@
       <c r="P153" s="22"/>
       <c r="Q153" s="22"/>
       <c r="R153" s="25"/>
-      <c r="S153" s="141" t="s">
+      <c r="S153" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T153" s="142"/>
-      <c r="U153" s="142"/>
-      <c r="V153" s="142"/>
-      <c r="W153" s="142"/>
-      <c r="X153" s="143"/>
-      <c r="Y153" s="141" t="s">
+      <c r="T153" s="124"/>
+      <c r="U153" s="124"/>
+      <c r="V153" s="124"/>
+      <c r="W153" s="124"/>
+      <c r="X153" s="125"/>
+      <c r="Y153" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z153" s="142"/>
-      <c r="AA153" s="142"/>
-      <c r="AB153" s="142"/>
-      <c r="AC153" s="142"/>
-      <c r="AD153" s="143"/>
-      <c r="AE153" s="144" t="s">
+      <c r="Z153" s="124"/>
+      <c r="AA153" s="124"/>
+      <c r="AB153" s="124"/>
+      <c r="AC153" s="124"/>
+      <c r="AD153" s="125"/>
+      <c r="AE153" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF153" s="145"/>
-      <c r="AG153" s="145"/>
-      <c r="AH153" s="145"/>
-      <c r="AI153" s="145"/>
-      <c r="AJ153" s="146"/>
+      <c r="AF153" s="121"/>
+      <c r="AG153" s="121"/>
+      <c r="AH153" s="121"/>
+      <c r="AI153" s="121"/>
+      <c r="AJ153" s="122"/>
       <c r="AP153" s="5"/>
       <c r="AQ153" s="2"/>
     </row>
@@ -11675,30 +12060,30 @@
       <c r="P154" s="22"/>
       <c r="Q154" s="22"/>
       <c r="R154" s="25"/>
-      <c r="S154" s="141" t="s">
+      <c r="S154" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T154" s="142"/>
-      <c r="U154" s="142"/>
-      <c r="V154" s="142"/>
-      <c r="W154" s="142"/>
-      <c r="X154" s="143"/>
-      <c r="Y154" s="141" t="s">
+      <c r="T154" s="124"/>
+      <c r="U154" s="124"/>
+      <c r="V154" s="124"/>
+      <c r="W154" s="124"/>
+      <c r="X154" s="125"/>
+      <c r="Y154" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z154" s="142"/>
-      <c r="AA154" s="142"/>
-      <c r="AB154" s="142"/>
-      <c r="AC154" s="142"/>
-      <c r="AD154" s="143"/>
-      <c r="AE154" s="144" t="s">
+      <c r="Z154" s="124"/>
+      <c r="AA154" s="124"/>
+      <c r="AB154" s="124"/>
+      <c r="AC154" s="124"/>
+      <c r="AD154" s="125"/>
+      <c r="AE154" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF154" s="145"/>
-      <c r="AG154" s="145"/>
-      <c r="AH154" s="145"/>
-      <c r="AI154" s="145"/>
-      <c r="AJ154" s="146"/>
+      <c r="AF154" s="121"/>
+      <c r="AG154" s="121"/>
+      <c r="AH154" s="121"/>
+      <c r="AI154" s="121"/>
+      <c r="AJ154" s="122"/>
       <c r="AP154" s="5"/>
       <c r="AQ154" s="2"/>
     </row>
@@ -11720,30 +12105,30 @@
       <c r="P155" s="22"/>
       <c r="Q155" s="22"/>
       <c r="R155" s="25"/>
-      <c r="S155" s="141" t="s">
+      <c r="S155" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T155" s="142"/>
-      <c r="U155" s="142"/>
-      <c r="V155" s="142"/>
-      <c r="W155" s="142"/>
-      <c r="X155" s="143"/>
-      <c r="Y155" s="141" t="s">
+      <c r="T155" s="124"/>
+      <c r="U155" s="124"/>
+      <c r="V155" s="124"/>
+      <c r="W155" s="124"/>
+      <c r="X155" s="125"/>
+      <c r="Y155" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z155" s="142"/>
-      <c r="AA155" s="142"/>
-      <c r="AB155" s="142"/>
-      <c r="AC155" s="142"/>
-      <c r="AD155" s="143"/>
-      <c r="AE155" s="144" t="s">
+      <c r="Z155" s="124"/>
+      <c r="AA155" s="124"/>
+      <c r="AB155" s="124"/>
+      <c r="AC155" s="124"/>
+      <c r="AD155" s="125"/>
+      <c r="AE155" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF155" s="145"/>
-      <c r="AG155" s="145"/>
-      <c r="AH155" s="145"/>
-      <c r="AI155" s="145"/>
-      <c r="AJ155" s="146"/>
+      <c r="AF155" s="121"/>
+      <c r="AG155" s="121"/>
+      <c r="AH155" s="121"/>
+      <c r="AI155" s="121"/>
+      <c r="AJ155" s="122"/>
       <c r="AP155" s="5"/>
       <c r="AQ155" s="2"/>
     </row>
@@ -11767,30 +12152,30 @@
       <c r="P156" s="22"/>
       <c r="Q156" s="22"/>
       <c r="R156" s="25"/>
-      <c r="S156" s="141" t="s">
+      <c r="S156" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T156" s="142"/>
-      <c r="U156" s="142"/>
-      <c r="V156" s="142"/>
-      <c r="W156" s="142"/>
-      <c r="X156" s="143"/>
-      <c r="Y156" s="141" t="s">
+      <c r="T156" s="124"/>
+      <c r="U156" s="124"/>
+      <c r="V156" s="124"/>
+      <c r="W156" s="124"/>
+      <c r="X156" s="125"/>
+      <c r="Y156" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z156" s="142"/>
-      <c r="AA156" s="142"/>
-      <c r="AB156" s="142"/>
-      <c r="AC156" s="142"/>
-      <c r="AD156" s="143"/>
-      <c r="AE156" s="144" t="s">
+      <c r="Z156" s="124"/>
+      <c r="AA156" s="124"/>
+      <c r="AB156" s="124"/>
+      <c r="AC156" s="124"/>
+      <c r="AD156" s="125"/>
+      <c r="AE156" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF156" s="145"/>
-      <c r="AG156" s="145"/>
-      <c r="AH156" s="145"/>
-      <c r="AI156" s="145"/>
-      <c r="AJ156" s="146"/>
+      <c r="AF156" s="121"/>
+      <c r="AG156" s="121"/>
+      <c r="AH156" s="121"/>
+      <c r="AI156" s="121"/>
+      <c r="AJ156" s="122"/>
       <c r="AP156" s="5"/>
       <c r="AQ156" s="2"/>
     </row>
@@ -11808,30 +12193,30 @@
       <c r="P157" s="22"/>
       <c r="Q157" s="22"/>
       <c r="R157" s="25"/>
-      <c r="S157" s="141" t="s">
+      <c r="S157" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T157" s="142"/>
-      <c r="U157" s="142"/>
-      <c r="V157" s="142"/>
-      <c r="W157" s="142"/>
-      <c r="X157" s="143"/>
-      <c r="Y157" s="141" t="s">
+      <c r="T157" s="124"/>
+      <c r="U157" s="124"/>
+      <c r="V157" s="124"/>
+      <c r="W157" s="124"/>
+      <c r="X157" s="125"/>
+      <c r="Y157" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z157" s="142"/>
-      <c r="AA157" s="142"/>
-      <c r="AB157" s="142"/>
-      <c r="AC157" s="142"/>
-      <c r="AD157" s="143"/>
-      <c r="AE157" s="144" t="s">
+      <c r="Z157" s="124"/>
+      <c r="AA157" s="124"/>
+      <c r="AB157" s="124"/>
+      <c r="AC157" s="124"/>
+      <c r="AD157" s="125"/>
+      <c r="AE157" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF157" s="145"/>
-      <c r="AG157" s="145"/>
-      <c r="AH157" s="145"/>
-      <c r="AI157" s="145"/>
-      <c r="AJ157" s="146"/>
+      <c r="AF157" s="121"/>
+      <c r="AG157" s="121"/>
+      <c r="AH157" s="121"/>
+      <c r="AI157" s="121"/>
+      <c r="AJ157" s="122"/>
       <c r="AP157" s="5"/>
       <c r="AQ157" s="2"/>
     </row>
@@ -11853,30 +12238,30 @@
       <c r="P158" s="22"/>
       <c r="Q158" s="22"/>
       <c r="R158" s="25"/>
-      <c r="S158" s="141" t="s">
+      <c r="S158" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T158" s="142"/>
-      <c r="U158" s="142"/>
-      <c r="V158" s="142"/>
-      <c r="W158" s="142"/>
-      <c r="X158" s="143"/>
-      <c r="Y158" s="141" t="s">
+      <c r="T158" s="124"/>
+      <c r="U158" s="124"/>
+      <c r="V158" s="124"/>
+      <c r="W158" s="124"/>
+      <c r="X158" s="125"/>
+      <c r="Y158" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z158" s="142"/>
-      <c r="AA158" s="142"/>
-      <c r="AB158" s="142"/>
-      <c r="AC158" s="142"/>
-      <c r="AD158" s="143"/>
-      <c r="AE158" s="144" t="s">
+      <c r="Z158" s="124"/>
+      <c r="AA158" s="124"/>
+      <c r="AB158" s="124"/>
+      <c r="AC158" s="124"/>
+      <c r="AD158" s="125"/>
+      <c r="AE158" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF158" s="145"/>
-      <c r="AG158" s="145"/>
-      <c r="AH158" s="145"/>
-      <c r="AI158" s="145"/>
-      <c r="AJ158" s="146"/>
+      <c r="AF158" s="121"/>
+      <c r="AG158" s="121"/>
+      <c r="AH158" s="121"/>
+      <c r="AI158" s="121"/>
+      <c r="AJ158" s="122"/>
       <c r="AP158" s="5"/>
       <c r="AQ158" s="2"/>
     </row>
@@ -11898,30 +12283,30 @@
       <c r="P159" s="88"/>
       <c r="Q159" s="88"/>
       <c r="R159" s="89"/>
-      <c r="S159" s="141" t="s">
+      <c r="S159" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T159" s="142"/>
-      <c r="U159" s="142"/>
-      <c r="V159" s="142"/>
-      <c r="W159" s="142"/>
-      <c r="X159" s="143"/>
-      <c r="Y159" s="141" t="s">
+      <c r="T159" s="124"/>
+      <c r="U159" s="124"/>
+      <c r="V159" s="124"/>
+      <c r="W159" s="124"/>
+      <c r="X159" s="125"/>
+      <c r="Y159" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z159" s="142"/>
-      <c r="AA159" s="142"/>
-      <c r="AB159" s="142"/>
-      <c r="AC159" s="142"/>
-      <c r="AD159" s="143"/>
-      <c r="AE159" s="144" t="s">
+      <c r="Z159" s="124"/>
+      <c r="AA159" s="124"/>
+      <c r="AB159" s="124"/>
+      <c r="AC159" s="124"/>
+      <c r="AD159" s="125"/>
+      <c r="AE159" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF159" s="145"/>
-      <c r="AG159" s="145"/>
-      <c r="AH159" s="145"/>
-      <c r="AI159" s="145"/>
-      <c r="AJ159" s="146"/>
+      <c r="AF159" s="121"/>
+      <c r="AG159" s="121"/>
+      <c r="AH159" s="121"/>
+      <c r="AI159" s="121"/>
+      <c r="AJ159" s="122"/>
       <c r="AP159" s="5"/>
       <c r="AQ159" s="2"/>
     </row>
@@ -11943,30 +12328,30 @@
       <c r="P160" s="88"/>
       <c r="Q160" s="88"/>
       <c r="R160" s="89"/>
-      <c r="S160" s="141" t="s">
+      <c r="S160" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T160" s="142"/>
-      <c r="U160" s="142"/>
-      <c r="V160" s="142"/>
-      <c r="W160" s="142"/>
-      <c r="X160" s="143"/>
-      <c r="Y160" s="141" t="s">
+      <c r="T160" s="124"/>
+      <c r="U160" s="124"/>
+      <c r="V160" s="124"/>
+      <c r="W160" s="124"/>
+      <c r="X160" s="125"/>
+      <c r="Y160" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="Z160" s="142"/>
-      <c r="AA160" s="142"/>
-      <c r="AB160" s="142"/>
-      <c r="AC160" s="142"/>
-      <c r="AD160" s="143"/>
-      <c r="AE160" s="144" t="s">
+      <c r="Z160" s="124"/>
+      <c r="AA160" s="124"/>
+      <c r="AB160" s="124"/>
+      <c r="AC160" s="124"/>
+      <c r="AD160" s="125"/>
+      <c r="AE160" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF160" s="145"/>
-      <c r="AG160" s="145"/>
-      <c r="AH160" s="145"/>
-      <c r="AI160" s="145"/>
-      <c r="AJ160" s="146"/>
+      <c r="AF160" s="121"/>
+      <c r="AG160" s="121"/>
+      <c r="AH160" s="121"/>
+      <c r="AI160" s="121"/>
+      <c r="AJ160" s="122"/>
       <c r="AP160" s="5"/>
       <c r="AQ160" s="2"/>
     </row>
@@ -11990,30 +12375,30 @@
       <c r="P161" s="85"/>
       <c r="Q161" s="85"/>
       <c r="R161" s="86"/>
-      <c r="S161" s="141" t="s">
+      <c r="S161" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T161" s="142"/>
-      <c r="U161" s="142"/>
-      <c r="V161" s="142"/>
-      <c r="W161" s="142"/>
-      <c r="X161" s="143"/>
-      <c r="Y161" s="144" t="s">
+      <c r="T161" s="124"/>
+      <c r="U161" s="124"/>
+      <c r="V161" s="124"/>
+      <c r="W161" s="124"/>
+      <c r="X161" s="125"/>
+      <c r="Y161" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="Z161" s="145"/>
-      <c r="AA161" s="145"/>
-      <c r="AB161" s="145"/>
-      <c r="AC161" s="145"/>
-      <c r="AD161" s="146"/>
-      <c r="AE161" s="144" t="s">
+      <c r="Z161" s="121"/>
+      <c r="AA161" s="121"/>
+      <c r="AB161" s="121"/>
+      <c r="AC161" s="121"/>
+      <c r="AD161" s="122"/>
+      <c r="AE161" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF161" s="145"/>
-      <c r="AG161" s="145"/>
-      <c r="AH161" s="145"/>
-      <c r="AI161" s="145"/>
-      <c r="AJ161" s="146"/>
+      <c r="AF161" s="121"/>
+      <c r="AG161" s="121"/>
+      <c r="AH161" s="121"/>
+      <c r="AI161" s="121"/>
+      <c r="AJ161" s="122"/>
       <c r="AP161" s="5"/>
       <c r="AQ161" s="2"/>
     </row>
@@ -12031,30 +12416,30 @@
       <c r="P162" s="22"/>
       <c r="Q162" s="22"/>
       <c r="R162" s="25"/>
-      <c r="S162" s="141" t="s">
+      <c r="S162" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T162" s="142"/>
-      <c r="U162" s="142"/>
-      <c r="V162" s="142"/>
-      <c r="W162" s="142"/>
-      <c r="X162" s="143"/>
-      <c r="Y162" s="144" t="s">
+      <c r="T162" s="124"/>
+      <c r="U162" s="124"/>
+      <c r="V162" s="124"/>
+      <c r="W162" s="124"/>
+      <c r="X162" s="125"/>
+      <c r="Y162" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z162" s="145"/>
-      <c r="AA162" s="145"/>
-      <c r="AB162" s="145"/>
-      <c r="AC162" s="145"/>
-      <c r="AD162" s="146"/>
-      <c r="AE162" s="144" t="s">
+      <c r="Z162" s="121"/>
+      <c r="AA162" s="121"/>
+      <c r="AB162" s="121"/>
+      <c r="AC162" s="121"/>
+      <c r="AD162" s="122"/>
+      <c r="AE162" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF162" s="145"/>
-      <c r="AG162" s="145"/>
-      <c r="AH162" s="145"/>
-      <c r="AI162" s="145"/>
-      <c r="AJ162" s="146"/>
+      <c r="AF162" s="121"/>
+      <c r="AG162" s="121"/>
+      <c r="AH162" s="121"/>
+      <c r="AI162" s="121"/>
+      <c r="AJ162" s="122"/>
       <c r="AP162" s="5"/>
       <c r="AQ162" s="2"/>
     </row>
@@ -12076,30 +12461,30 @@
       <c r="P163" s="22"/>
       <c r="Q163" s="22"/>
       <c r="R163" s="25"/>
-      <c r="S163" s="141" t="s">
+      <c r="S163" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T163" s="142"/>
-      <c r="U163" s="142"/>
-      <c r="V163" s="142"/>
-      <c r="W163" s="142"/>
-      <c r="X163" s="143"/>
-      <c r="Y163" s="144" t="s">
+      <c r="T163" s="124"/>
+      <c r="U163" s="124"/>
+      <c r="V163" s="124"/>
+      <c r="W163" s="124"/>
+      <c r="X163" s="125"/>
+      <c r="Y163" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z163" s="145"/>
-      <c r="AA163" s="145"/>
-      <c r="AB163" s="145"/>
-      <c r="AC163" s="145"/>
-      <c r="AD163" s="146"/>
-      <c r="AE163" s="144" t="s">
+      <c r="Z163" s="121"/>
+      <c r="AA163" s="121"/>
+      <c r="AB163" s="121"/>
+      <c r="AC163" s="121"/>
+      <c r="AD163" s="122"/>
+      <c r="AE163" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF163" s="145"/>
-      <c r="AG163" s="145"/>
-      <c r="AH163" s="145"/>
-      <c r="AI163" s="145"/>
-      <c r="AJ163" s="146"/>
+      <c r="AF163" s="121"/>
+      <c r="AG163" s="121"/>
+      <c r="AH163" s="121"/>
+      <c r="AI163" s="121"/>
+      <c r="AJ163" s="122"/>
       <c r="AP163" s="5"/>
       <c r="AQ163" s="2"/>
     </row>
@@ -12121,30 +12506,30 @@
       <c r="P164" s="88"/>
       <c r="Q164" s="88"/>
       <c r="R164" s="89"/>
-      <c r="S164" s="141" t="s">
+      <c r="S164" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T164" s="142"/>
-      <c r="U164" s="142"/>
-      <c r="V164" s="142"/>
-      <c r="W164" s="142"/>
-      <c r="X164" s="143"/>
-      <c r="Y164" s="144" t="s">
+      <c r="T164" s="124"/>
+      <c r="U164" s="124"/>
+      <c r="V164" s="124"/>
+      <c r="W164" s="124"/>
+      <c r="X164" s="125"/>
+      <c r="Y164" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z164" s="145"/>
-      <c r="AA164" s="145"/>
-      <c r="AB164" s="145"/>
-      <c r="AC164" s="145"/>
-      <c r="AD164" s="146"/>
-      <c r="AE164" s="144" t="s">
+      <c r="Z164" s="121"/>
+      <c r="AA164" s="121"/>
+      <c r="AB164" s="121"/>
+      <c r="AC164" s="121"/>
+      <c r="AD164" s="122"/>
+      <c r="AE164" s="120" t="s">
         <v>177</v>
       </c>
-      <c r="AF164" s="145"/>
-      <c r="AG164" s="145"/>
-      <c r="AH164" s="145"/>
-      <c r="AI164" s="145"/>
-      <c r="AJ164" s="146"/>
+      <c r="AF164" s="121"/>
+      <c r="AG164" s="121"/>
+      <c r="AH164" s="121"/>
+      <c r="AI164" s="121"/>
+      <c r="AJ164" s="122"/>
       <c r="AP164" s="5"/>
       <c r="AQ164" s="2"/>
     </row>
@@ -12168,30 +12553,30 @@
       <c r="P165" s="85"/>
       <c r="Q165" s="85"/>
       <c r="R165" s="86"/>
-      <c r="S165" s="141" t="s">
+      <c r="S165" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T165" s="142"/>
-      <c r="U165" s="142"/>
-      <c r="V165" s="142"/>
-      <c r="W165" s="142"/>
-      <c r="X165" s="143"/>
-      <c r="Y165" s="144" t="s">
+      <c r="T165" s="124"/>
+      <c r="U165" s="124"/>
+      <c r="V165" s="124"/>
+      <c r="W165" s="124"/>
+      <c r="X165" s="125"/>
+      <c r="Y165" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="Z165" s="145"/>
-      <c r="AA165" s="145"/>
-      <c r="AB165" s="145"/>
-      <c r="AC165" s="145"/>
-      <c r="AD165" s="146"/>
-      <c r="AE165" s="144" t="s">
+      <c r="Z165" s="121"/>
+      <c r="AA165" s="121"/>
+      <c r="AB165" s="121"/>
+      <c r="AC165" s="121"/>
+      <c r="AD165" s="122"/>
+      <c r="AE165" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF165" s="145"/>
-      <c r="AG165" s="145"/>
-      <c r="AH165" s="145"/>
-      <c r="AI165" s="145"/>
-      <c r="AJ165" s="146"/>
+      <c r="AF165" s="121"/>
+      <c r="AG165" s="121"/>
+      <c r="AH165" s="121"/>
+      <c r="AI165" s="121"/>
+      <c r="AJ165" s="122"/>
       <c r="AP165" s="5"/>
       <c r="AQ165" s="2"/>
     </row>
@@ -12209,30 +12594,30 @@
       <c r="P166" s="22"/>
       <c r="Q166" s="22"/>
       <c r="R166" s="25"/>
-      <c r="S166" s="141" t="s">
+      <c r="S166" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T166" s="142"/>
-      <c r="U166" s="142"/>
-      <c r="V166" s="142"/>
-      <c r="W166" s="142"/>
-      <c r="X166" s="143"/>
-      <c r="Y166" s="144" t="s">
+      <c r="T166" s="124"/>
+      <c r="U166" s="124"/>
+      <c r="V166" s="124"/>
+      <c r="W166" s="124"/>
+      <c r="X166" s="125"/>
+      <c r="Y166" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z166" s="145"/>
-      <c r="AA166" s="145"/>
-      <c r="AB166" s="145"/>
-      <c r="AC166" s="145"/>
-      <c r="AD166" s="146"/>
-      <c r="AE166" s="144" t="s">
+      <c r="Z166" s="121"/>
+      <c r="AA166" s="121"/>
+      <c r="AB166" s="121"/>
+      <c r="AC166" s="121"/>
+      <c r="AD166" s="122"/>
+      <c r="AE166" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF166" s="145"/>
-      <c r="AG166" s="145"/>
-      <c r="AH166" s="145"/>
-      <c r="AI166" s="145"/>
-      <c r="AJ166" s="146"/>
+      <c r="AF166" s="121"/>
+      <c r="AG166" s="121"/>
+      <c r="AH166" s="121"/>
+      <c r="AI166" s="121"/>
+      <c r="AJ166" s="122"/>
       <c r="AP166" s="5"/>
       <c r="AQ166" s="2"/>
     </row>
@@ -12254,30 +12639,30 @@
       <c r="P167" s="22"/>
       <c r="Q167" s="22"/>
       <c r="R167" s="25"/>
-      <c r="S167" s="141" t="s">
+      <c r="S167" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T167" s="142"/>
-      <c r="U167" s="142"/>
-      <c r="V167" s="142"/>
-      <c r="W167" s="142"/>
-      <c r="X167" s="143"/>
-      <c r="Y167" s="144" t="s">
+      <c r="T167" s="124"/>
+      <c r="U167" s="124"/>
+      <c r="V167" s="124"/>
+      <c r="W167" s="124"/>
+      <c r="X167" s="125"/>
+      <c r="Y167" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z167" s="145"/>
-      <c r="AA167" s="145"/>
-      <c r="AB167" s="145"/>
-      <c r="AC167" s="145"/>
-      <c r="AD167" s="146"/>
-      <c r="AE167" s="144" t="s">
+      <c r="Z167" s="121"/>
+      <c r="AA167" s="121"/>
+      <c r="AB167" s="121"/>
+      <c r="AC167" s="121"/>
+      <c r="AD167" s="122"/>
+      <c r="AE167" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF167" s="145"/>
-      <c r="AG167" s="145"/>
-      <c r="AH167" s="145"/>
-      <c r="AI167" s="145"/>
-      <c r="AJ167" s="146"/>
+      <c r="AF167" s="121"/>
+      <c r="AG167" s="121"/>
+      <c r="AH167" s="121"/>
+      <c r="AI167" s="121"/>
+      <c r="AJ167" s="122"/>
       <c r="AP167" s="5"/>
       <c r="AQ167" s="2"/>
     </row>
@@ -12299,30 +12684,30 @@
       <c r="P168" s="88"/>
       <c r="Q168" s="88"/>
       <c r="R168" s="89"/>
-      <c r="S168" s="141" t="s">
+      <c r="S168" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T168" s="142"/>
-      <c r="U168" s="142"/>
-      <c r="V168" s="142"/>
-      <c r="W168" s="142"/>
-      <c r="X168" s="143"/>
-      <c r="Y168" s="144" t="s">
+      <c r="T168" s="124"/>
+      <c r="U168" s="124"/>
+      <c r="V168" s="124"/>
+      <c r="W168" s="124"/>
+      <c r="X168" s="125"/>
+      <c r="Y168" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z168" s="145"/>
-      <c r="AA168" s="145"/>
-      <c r="AB168" s="145"/>
-      <c r="AC168" s="145"/>
-      <c r="AD168" s="146"/>
-      <c r="AE168" s="144" t="s">
+      <c r="Z168" s="121"/>
+      <c r="AA168" s="121"/>
+      <c r="AB168" s="121"/>
+      <c r="AC168" s="121"/>
+      <c r="AD168" s="122"/>
+      <c r="AE168" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="AF168" s="145"/>
-      <c r="AG168" s="145"/>
-      <c r="AH168" s="145"/>
-      <c r="AI168" s="145"/>
-      <c r="AJ168" s="146"/>
+      <c r="AF168" s="121"/>
+      <c r="AG168" s="121"/>
+      <c r="AH168" s="121"/>
+      <c r="AI168" s="121"/>
+      <c r="AJ168" s="122"/>
       <c r="AP168" s="5"/>
       <c r="AQ168" s="2"/>
     </row>
@@ -12346,30 +12731,30 @@
       <c r="P169" s="85"/>
       <c r="Q169" s="85"/>
       <c r="R169" s="86"/>
-      <c r="S169" s="141" t="s">
+      <c r="S169" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T169" s="142"/>
-      <c r="U169" s="142"/>
-      <c r="V169" s="142"/>
-      <c r="W169" s="142"/>
-      <c r="X169" s="143"/>
-      <c r="Y169" s="144" t="s">
+      <c r="T169" s="124"/>
+      <c r="U169" s="124"/>
+      <c r="V169" s="124"/>
+      <c r="W169" s="124"/>
+      <c r="X169" s="125"/>
+      <c r="Y169" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="Z169" s="145"/>
-      <c r="AA169" s="145"/>
-      <c r="AB169" s="145"/>
-      <c r="AC169" s="145"/>
-      <c r="AD169" s="146"/>
-      <c r="AE169" s="144" t="s">
+      <c r="Z169" s="121"/>
+      <c r="AA169" s="121"/>
+      <c r="AB169" s="121"/>
+      <c r="AC169" s="121"/>
+      <c r="AD169" s="122"/>
+      <c r="AE169" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF169" s="145"/>
-      <c r="AG169" s="145"/>
-      <c r="AH169" s="145"/>
-      <c r="AI169" s="145"/>
-      <c r="AJ169" s="146"/>
+      <c r="AF169" s="121"/>
+      <c r="AG169" s="121"/>
+      <c r="AH169" s="121"/>
+      <c r="AI169" s="121"/>
+      <c r="AJ169" s="122"/>
       <c r="AP169" s="5"/>
       <c r="AQ169" s="2"/>
     </row>
@@ -12387,30 +12772,30 @@
       <c r="P170" s="22"/>
       <c r="Q170" s="22"/>
       <c r="R170" s="25"/>
-      <c r="S170" s="141" t="s">
+      <c r="S170" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T170" s="142"/>
-      <c r="U170" s="142"/>
-      <c r="V170" s="142"/>
-      <c r="W170" s="142"/>
-      <c r="X170" s="143"/>
-      <c r="Y170" s="144" t="s">
+      <c r="T170" s="124"/>
+      <c r="U170" s="124"/>
+      <c r="V170" s="124"/>
+      <c r="W170" s="124"/>
+      <c r="X170" s="125"/>
+      <c r="Y170" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z170" s="145"/>
-      <c r="AA170" s="145"/>
-      <c r="AB170" s="145"/>
-      <c r="AC170" s="145"/>
-      <c r="AD170" s="146"/>
-      <c r="AE170" s="144" t="s">
+      <c r="Z170" s="121"/>
+      <c r="AA170" s="121"/>
+      <c r="AB170" s="121"/>
+      <c r="AC170" s="121"/>
+      <c r="AD170" s="122"/>
+      <c r="AE170" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF170" s="145"/>
-      <c r="AG170" s="145"/>
-      <c r="AH170" s="145"/>
-      <c r="AI170" s="145"/>
-      <c r="AJ170" s="146"/>
+      <c r="AF170" s="121"/>
+      <c r="AG170" s="121"/>
+      <c r="AH170" s="121"/>
+      <c r="AI170" s="121"/>
+      <c r="AJ170" s="122"/>
       <c r="AP170" s="5"/>
       <c r="AQ170" s="2"/>
     </row>
@@ -12432,30 +12817,30 @@
       <c r="P171" s="22"/>
       <c r="Q171" s="22"/>
       <c r="R171" s="25"/>
-      <c r="S171" s="141" t="s">
+      <c r="S171" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T171" s="142"/>
-      <c r="U171" s="142"/>
-      <c r="V171" s="142"/>
-      <c r="W171" s="142"/>
-      <c r="X171" s="143"/>
-      <c r="Y171" s="144" t="s">
+      <c r="T171" s="124"/>
+      <c r="U171" s="124"/>
+      <c r="V171" s="124"/>
+      <c r="W171" s="124"/>
+      <c r="X171" s="125"/>
+      <c r="Y171" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z171" s="145"/>
-      <c r="AA171" s="145"/>
-      <c r="AB171" s="145"/>
-      <c r="AC171" s="145"/>
-      <c r="AD171" s="146"/>
-      <c r="AE171" s="144" t="s">
+      <c r="Z171" s="121"/>
+      <c r="AA171" s="121"/>
+      <c r="AB171" s="121"/>
+      <c r="AC171" s="121"/>
+      <c r="AD171" s="122"/>
+      <c r="AE171" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF171" s="145"/>
-      <c r="AG171" s="145"/>
-      <c r="AH171" s="145"/>
-      <c r="AI171" s="145"/>
-      <c r="AJ171" s="146"/>
+      <c r="AF171" s="121"/>
+      <c r="AG171" s="121"/>
+      <c r="AH171" s="121"/>
+      <c r="AI171" s="121"/>
+      <c r="AJ171" s="122"/>
       <c r="AP171" s="5"/>
       <c r="AQ171" s="2"/>
     </row>
@@ -12477,30 +12862,30 @@
       <c r="P172" s="22"/>
       <c r="Q172" s="22"/>
       <c r="R172" s="25"/>
-      <c r="S172" s="141" t="s">
+      <c r="S172" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T172" s="142"/>
-      <c r="U172" s="142"/>
-      <c r="V172" s="142"/>
-      <c r="W172" s="142"/>
-      <c r="X172" s="143"/>
-      <c r="Y172" s="144" t="s">
+      <c r="T172" s="124"/>
+      <c r="U172" s="124"/>
+      <c r="V172" s="124"/>
+      <c r="W172" s="124"/>
+      <c r="X172" s="125"/>
+      <c r="Y172" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="Z172" s="145"/>
-      <c r="AA172" s="145"/>
-      <c r="AB172" s="145"/>
-      <c r="AC172" s="145"/>
-      <c r="AD172" s="146"/>
-      <c r="AE172" s="144" t="s">
+      <c r="Z172" s="121"/>
+      <c r="AA172" s="121"/>
+      <c r="AB172" s="121"/>
+      <c r="AC172" s="121"/>
+      <c r="AD172" s="122"/>
+      <c r="AE172" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF172" s="145"/>
-      <c r="AG172" s="145"/>
-      <c r="AH172" s="145"/>
-      <c r="AI172" s="145"/>
-      <c r="AJ172" s="146"/>
+      <c r="AF172" s="121"/>
+      <c r="AG172" s="121"/>
+      <c r="AH172" s="121"/>
+      <c r="AI172" s="121"/>
+      <c r="AJ172" s="122"/>
       <c r="AP172" s="5"/>
       <c r="AQ172" s="2"/>
     </row>
@@ -12522,30 +12907,30 @@
       <c r="P173" s="22"/>
       <c r="Q173" s="22"/>
       <c r="R173" s="25"/>
-      <c r="S173" s="141" t="s">
+      <c r="S173" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T173" s="142"/>
-      <c r="U173" s="142"/>
-      <c r="V173" s="142"/>
-      <c r="W173" s="142"/>
-      <c r="X173" s="143"/>
-      <c r="Y173" s="144" t="s">
+      <c r="T173" s="124"/>
+      <c r="U173" s="124"/>
+      <c r="V173" s="124"/>
+      <c r="W173" s="124"/>
+      <c r="X173" s="125"/>
+      <c r="Y173" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="Z173" s="145"/>
-      <c r="AA173" s="145"/>
-      <c r="AB173" s="145"/>
-      <c r="AC173" s="145"/>
-      <c r="AD173" s="146"/>
-      <c r="AE173" s="144" t="s">
+      <c r="Z173" s="121"/>
+      <c r="AA173" s="121"/>
+      <c r="AB173" s="121"/>
+      <c r="AC173" s="121"/>
+      <c r="AD173" s="122"/>
+      <c r="AE173" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF173" s="145"/>
-      <c r="AG173" s="145"/>
-      <c r="AH173" s="145"/>
-      <c r="AI173" s="145"/>
-      <c r="AJ173" s="146"/>
+      <c r="AF173" s="121"/>
+      <c r="AG173" s="121"/>
+      <c r="AH173" s="121"/>
+      <c r="AI173" s="121"/>
+      <c r="AJ173" s="122"/>
       <c r="AP173" s="5"/>
       <c r="AQ173" s="2"/>
     </row>
@@ -12567,30 +12952,30 @@
       <c r="P174" s="22"/>
       <c r="Q174" s="22"/>
       <c r="R174" s="25"/>
-      <c r="S174" s="141" t="s">
+      <c r="S174" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="T174" s="142"/>
-      <c r="U174" s="142"/>
-      <c r="V174" s="142"/>
-      <c r="W174" s="142"/>
-      <c r="X174" s="143"/>
-      <c r="Y174" s="144" t="s">
+      <c r="T174" s="124"/>
+      <c r="U174" s="124"/>
+      <c r="V174" s="124"/>
+      <c r="W174" s="124"/>
+      <c r="X174" s="125"/>
+      <c r="Y174" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="Z174" s="145"/>
-      <c r="AA174" s="145"/>
-      <c r="AB174" s="145"/>
-      <c r="AC174" s="145"/>
-      <c r="AD174" s="146"/>
-      <c r="AE174" s="144" t="s">
+      <c r="Z174" s="121"/>
+      <c r="AA174" s="121"/>
+      <c r="AB174" s="121"/>
+      <c r="AC174" s="121"/>
+      <c r="AD174" s="122"/>
+      <c r="AE174" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AF174" s="145"/>
-      <c r="AG174" s="145"/>
-      <c r="AH174" s="145"/>
-      <c r="AI174" s="145"/>
-      <c r="AJ174" s="146"/>
+      <c r="AF174" s="121"/>
+      <c r="AG174" s="121"/>
+      <c r="AH174" s="121"/>
+      <c r="AI174" s="121"/>
+      <c r="AJ174" s="122"/>
       <c r="AP174" s="5"/>
       <c r="AQ174" s="2"/>
     </row>
@@ -12612,30 +12997,30 @@
       <c r="P175" s="27"/>
       <c r="Q175" s="27"/>
       <c r="R175" s="28"/>
-      <c r="S175" s="150" t="s">
+      <c r="S175" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="T175" s="151"/>
-      <c r="U175" s="151"/>
-      <c r="V175" s="151"/>
-      <c r="W175" s="151"/>
-      <c r="X175" s="152"/>
-      <c r="Y175" s="153" t="s">
+      <c r="T175" s="130"/>
+      <c r="U175" s="130"/>
+      <c r="V175" s="130"/>
+      <c r="W175" s="130"/>
+      <c r="X175" s="131"/>
+      <c r="Y175" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="Z175" s="154"/>
-      <c r="AA175" s="154"/>
-      <c r="AB175" s="154"/>
-      <c r="AC175" s="154"/>
-      <c r="AD175" s="155"/>
-      <c r="AE175" s="153" t="s">
+      <c r="Z175" s="133"/>
+      <c r="AA175" s="133"/>
+      <c r="AB175" s="133"/>
+      <c r="AC175" s="133"/>
+      <c r="AD175" s="134"/>
+      <c r="AE175" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="AF175" s="154"/>
-      <c r="AG175" s="154"/>
-      <c r="AH175" s="154"/>
-      <c r="AI175" s="154"/>
-      <c r="AJ175" s="155"/>
+      <c r="AF175" s="133"/>
+      <c r="AG175" s="133"/>
+      <c r="AH175" s="133"/>
+      <c r="AI175" s="133"/>
+      <c r="AJ175" s="134"/>
       <c r="AP175" s="5"/>
       <c r="AQ175" s="2"/>
     </row>
@@ -14501,37 +14886,41 @@
     </row>
     <row r="223" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A223" s="4"/>
-      <c r="F223" s="105"/>
-      <c r="G223" s="16"/>
-      <c r="H223" s="16"/>
-      <c r="I223" s="16"/>
-      <c r="J223" s="104"/>
-      <c r="K223" s="105"/>
-      <c r="L223" s="16"/>
-      <c r="M223" s="16"/>
-      <c r="N223" s="104"/>
-      <c r="O223" s="16"/>
-      <c r="P223" s="16"/>
-      <c r="Q223" s="105"/>
-      <c r="R223" s="16"/>
-      <c r="S223" s="16"/>
-      <c r="T223" s="16"/>
-      <c r="U223" s="16"/>
-      <c r="V223" s="16"/>
-      <c r="W223" s="16"/>
-      <c r="X223" s="16"/>
-      <c r="Y223" s="16"/>
-      <c r="Z223" s="16"/>
-      <c r="AA223" s="16"/>
-      <c r="AB223" s="16"/>
-      <c r="AC223" s="16"/>
-      <c r="AD223" s="16"/>
-      <c r="AE223" s="16"/>
-      <c r="AF223" s="16"/>
-      <c r="AG223" s="16"/>
-      <c r="AH223" s="16"/>
-      <c r="AI223" s="16"/>
-      <c r="AJ223" s="104"/>
+      <c r="F223" s="107"/>
+      <c r="G223" s="107"/>
+      <c r="H223" s="107"/>
+      <c r="I223" s="107"/>
+      <c r="J223" s="107"/>
+      <c r="K223" s="107"/>
+      <c r="L223" s="107"/>
+      <c r="M223" s="107"/>
+      <c r="N223" s="107"/>
+      <c r="O223" s="107"/>
+      <c r="P223" s="107"/>
+      <c r="Q223" s="107"/>
+      <c r="R223" s="107"/>
+      <c r="S223" s="107"/>
+      <c r="T223" s="107"/>
+      <c r="U223" s="107"/>
+      <c r="V223" s="107"/>
+      <c r="W223" s="107"/>
+      <c r="X223" s="107"/>
+      <c r="Y223" s="107"/>
+      <c r="Z223" s="107"/>
+      <c r="AA223" s="107"/>
+      <c r="AB223" s="107"/>
+      <c r="AC223" s="107"/>
+      <c r="AD223" s="107"/>
+      <c r="AE223" s="107"/>
+      <c r="AF223" s="107"/>
+      <c r="AG223" s="107"/>
+      <c r="AH223" s="107"/>
+      <c r="AI223" s="107"/>
+      <c r="AJ223" s="107"/>
+      <c r="AK223" s="107"/>
+      <c r="AL223" s="107"/>
+      <c r="AM223" s="107"/>
+      <c r="AN223" s="2"/>
       <c r="AP223" s="5"/>
       <c r="AQ223" s="2"/>
     </row>
@@ -14541,247 +14930,1104 @@
         <v>11</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>154</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="F224" s="107"/>
+      <c r="G224" s="107"/>
+      <c r="H224" s="107"/>
+      <c r="I224" s="107"/>
+      <c r="J224" s="107"/>
+      <c r="K224" s="107"/>
+      <c r="L224" s="107"/>
+      <c r="M224" s="107"/>
+      <c r="N224" s="107"/>
+      <c r="O224" s="107"/>
+      <c r="P224" s="107"/>
+      <c r="Q224" s="107"/>
+      <c r="R224" s="107"/>
+      <c r="S224" s="107"/>
+      <c r="T224" s="107"/>
+      <c r="U224" s="107"/>
+      <c r="V224" s="107"/>
+      <c r="W224" s="107"/>
+      <c r="X224" s="107"/>
+      <c r="Y224" s="107"/>
+      <c r="Z224" s="107"/>
+      <c r="AA224" s="107"/>
+      <c r="AB224" s="107"/>
+      <c r="AC224" s="107"/>
+      <c r="AD224" s="107"/>
+      <c r="AE224" s="107"/>
+      <c r="AF224" s="107"/>
+      <c r="AG224" s="107"/>
+      <c r="AH224" s="107"/>
+      <c r="AI224" s="107"/>
+      <c r="AJ224" s="107"/>
+      <c r="AK224" s="107"/>
+      <c r="AL224" s="107"/>
+      <c r="AM224" s="107"/>
+      <c r="AN224" s="2"/>
       <c r="AP224" s="5"/>
       <c r="AQ224" s="2"/>
     </row>
     <row r="225" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A225" s="4"/>
-      <c r="C225" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D225" s="1" t="s">
-        <v>162</v>
-      </c>
+      <c r="C225" s="10"/>
+      <c r="D225" s="10"/>
+      <c r="E225" s="10"/>
+      <c r="F225" s="107"/>
+      <c r="G225" s="107"/>
+      <c r="H225" s="107"/>
+      <c r="I225" s="107"/>
+      <c r="J225" s="107"/>
+      <c r="K225" s="107"/>
+      <c r="L225" s="107"/>
+      <c r="M225" s="107"/>
+      <c r="N225" s="107"/>
+      <c r="O225" s="107"/>
+      <c r="P225" s="107"/>
+      <c r="Q225" s="107"/>
+      <c r="R225" s="107"/>
+      <c r="S225" s="107"/>
+      <c r="T225" s="107"/>
+      <c r="U225" s="107"/>
+      <c r="V225" s="107"/>
+      <c r="W225" s="107"/>
+      <c r="X225" s="107"/>
+      <c r="Y225" s="107"/>
+      <c r="Z225" s="107"/>
+      <c r="AA225" s="107"/>
+      <c r="AB225" s="107"/>
+      <c r="AC225" s="107"/>
+      <c r="AD225" s="107"/>
+      <c r="AE225" s="107"/>
+      <c r="AF225" s="107"/>
+      <c r="AG225" s="107"/>
+      <c r="AH225" s="107"/>
+      <c r="AI225" s="107"/>
+      <c r="AJ225" s="107"/>
+      <c r="AK225" s="107"/>
+      <c r="AL225" s="107"/>
+      <c r="AM225" s="107"/>
+      <c r="AN225" s="2"/>
       <c r="AP225" s="5"/>
       <c r="AQ225" s="2"/>
     </row>
     <row r="226" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A226" s="4"/>
-      <c r="C226" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D226" s="1" t="s">
-        <v>160</v>
-      </c>
+      <c r="B226" s="9"/>
+      <c r="C226" s="69" t="s">
+        <v>242</v>
+      </c>
+      <c r="D226" s="70"/>
+      <c r="E226" s="70"/>
+      <c r="F226" s="70"/>
+      <c r="G226" s="70"/>
+      <c r="H226" s="71"/>
+      <c r="I226" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="J226" s="70"/>
+      <c r="K226" s="70"/>
+      <c r="L226" s="70"/>
+      <c r="M226" s="70"/>
+      <c r="N226" s="70"/>
+      <c r="O226" s="70"/>
+      <c r="P226" s="70"/>
+      <c r="Q226" s="70"/>
+      <c r="R226" s="70"/>
+      <c r="S226" s="70"/>
+      <c r="T226" s="70"/>
+      <c r="U226" s="70"/>
+      <c r="V226" s="70"/>
+      <c r="W226" s="70"/>
+      <c r="X226" s="70"/>
+      <c r="Y226" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z226" s="70"/>
+      <c r="AA226" s="70"/>
+      <c r="AB226" s="70"/>
+      <c r="AC226" s="71"/>
+      <c r="AD226" s="135" t="s">
+        <v>256</v>
+      </c>
+      <c r="AE226" s="136"/>
+      <c r="AF226" s="136"/>
+      <c r="AG226" s="136"/>
+      <c r="AH226" s="136"/>
+      <c r="AI226" s="136"/>
+      <c r="AJ226" s="136"/>
+      <c r="AK226" s="136"/>
+      <c r="AL226" s="137"/>
+      <c r="AM226" s="107"/>
+      <c r="AN226" s="2"/>
       <c r="AP226" s="5"/>
       <c r="AQ226" s="2"/>
     </row>
     <row r="227" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A227" s="4"/>
-      <c r="C227" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="B227" s="9"/>
+      <c r="C227" s="72"/>
+      <c r="D227" s="73"/>
+      <c r="E227" s="73"/>
+      <c r="F227" s="73"/>
+      <c r="G227" s="73"/>
+      <c r="H227" s="74"/>
+      <c r="I227" s="73"/>
+      <c r="J227" s="73"/>
+      <c r="K227" s="73"/>
+      <c r="L227" s="73"/>
+      <c r="M227" s="73"/>
+      <c r="N227" s="73"/>
+      <c r="O227" s="73"/>
+      <c r="P227" s="73"/>
+      <c r="Q227" s="73"/>
+      <c r="R227" s="73"/>
+      <c r="S227" s="73"/>
+      <c r="T227" s="73"/>
+      <c r="U227" s="73"/>
+      <c r="V227" s="73"/>
+      <c r="W227" s="73"/>
+      <c r="X227" s="73"/>
+      <c r="Y227" s="72"/>
+      <c r="Z227" s="73"/>
+      <c r="AA227" s="73"/>
+      <c r="AB227" s="73"/>
+      <c r="AC227" s="74"/>
+      <c r="AD227" s="60" t="s">
+        <v>257</v>
+      </c>
+      <c r="AE227" s="61"/>
+      <c r="AF227" s="61"/>
+      <c r="AG227" s="62"/>
+      <c r="AH227" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI227" s="62"/>
+      <c r="AJ227" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK227" s="61"/>
+      <c r="AL227" s="62"/>
+      <c r="AM227" s="107"/>
+      <c r="AN227" s="2"/>
       <c r="AP227" s="5"/>
       <c r="AQ227" s="2"/>
     </row>
     <row r="228" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A228" s="4"/>
-      <c r="C228" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D228" s="1" t="s">
-        <v>163</v>
-      </c>
+      <c r="B228" s="9"/>
+      <c r="C228" s="108" t="s">
+        <v>111</v>
+      </c>
+      <c r="D228" s="109"/>
+      <c r="E228" s="109"/>
+      <c r="F228" s="115"/>
+      <c r="G228" s="115"/>
+      <c r="H228" s="112"/>
+      <c r="I228" s="108" t="s">
+        <v>247</v>
+      </c>
+      <c r="J228" s="115"/>
+      <c r="K228" s="115"/>
+      <c r="L228" s="115"/>
+      <c r="M228" s="115"/>
+      <c r="N228" s="115"/>
+      <c r="O228" s="115"/>
+      <c r="P228" s="115"/>
+      <c r="Q228" s="115"/>
+      <c r="R228" s="115"/>
+      <c r="S228" s="115"/>
+      <c r="T228" s="115"/>
+      <c r="U228" s="115"/>
+      <c r="V228" s="115"/>
+      <c r="W228" s="115"/>
+      <c r="X228" s="115"/>
+      <c r="Y228" s="161" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z228" s="115"/>
+      <c r="AA228" s="115"/>
+      <c r="AB228" s="115"/>
+      <c r="AC228" s="119"/>
+      <c r="AD228" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE228" s="165"/>
+      <c r="AF228" s="165"/>
+      <c r="AG228" s="167"/>
+      <c r="AH228" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI228" s="167"/>
+      <c r="AJ228" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK228" s="165"/>
+      <c r="AL228" s="167"/>
+      <c r="AM228" s="107"/>
+      <c r="AN228" s="2"/>
       <c r="AP228" s="5"/>
       <c r="AQ228" s="2"/>
     </row>
     <row r="229" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A229" s="4"/>
-      <c r="D229" s="1" t="s">
-        <v>164</v>
-      </c>
+      <c r="B229" s="9"/>
+      <c r="C229" s="99"/>
+      <c r="D229" s="16"/>
+      <c r="E229" s="16"/>
+      <c r="F229" s="107"/>
+      <c r="G229" s="107"/>
+      <c r="H229" s="17"/>
+      <c r="I229" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="J229" s="114"/>
+      <c r="K229" s="114"/>
+      <c r="L229" s="114"/>
+      <c r="M229" s="114"/>
+      <c r="N229" s="114"/>
+      <c r="O229" s="114"/>
+      <c r="P229" s="114"/>
+      <c r="Q229" s="114"/>
+      <c r="R229" s="114"/>
+      <c r="S229" s="114"/>
+      <c r="T229" s="114"/>
+      <c r="U229" s="114"/>
+      <c r="V229" s="114"/>
+      <c r="W229" s="114"/>
+      <c r="X229" s="114"/>
+      <c r="Y229" s="162"/>
+      <c r="Z229" s="114"/>
+      <c r="AA229" s="114"/>
+      <c r="AB229" s="114"/>
+      <c r="AC229" s="118"/>
+      <c r="AD229" s="168"/>
+      <c r="AE229" s="169"/>
+      <c r="AF229" s="169"/>
+      <c r="AG229" s="170"/>
+      <c r="AH229" s="168"/>
+      <c r="AI229" s="170"/>
+      <c r="AJ229" s="168"/>
+      <c r="AK229" s="169"/>
+      <c r="AL229" s="170"/>
+      <c r="AM229" s="107"/>
+      <c r="AN229" s="2"/>
       <c r="AP229" s="5"/>
       <c r="AQ229" s="2"/>
     </row>
     <row r="230" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A230" s="4"/>
+      <c r="B230" s="9"/>
+      <c r="C230" s="99"/>
+      <c r="D230" s="16"/>
+      <c r="E230" s="16"/>
+      <c r="F230" s="107"/>
+      <c r="G230" s="107"/>
+      <c r="H230" s="17"/>
+      <c r="I230" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="J230" s="113"/>
+      <c r="K230" s="113"/>
+      <c r="L230" s="113"/>
+      <c r="M230" s="113"/>
+      <c r="N230" s="113"/>
+      <c r="O230" s="113"/>
+      <c r="P230" s="113"/>
+      <c r="Q230" s="113"/>
+      <c r="R230" s="113"/>
+      <c r="S230" s="113"/>
+      <c r="T230" s="113"/>
+      <c r="U230" s="113"/>
+      <c r="V230" s="113"/>
+      <c r="W230" s="113"/>
+      <c r="X230" s="113"/>
+      <c r="Y230" s="163" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z230" s="113"/>
+      <c r="AA230" s="113"/>
+      <c r="AB230" s="113"/>
+      <c r="AC230" s="117"/>
+      <c r="AD230" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE230" s="165"/>
+      <c r="AF230" s="165"/>
+      <c r="AG230" s="167"/>
+      <c r="AH230" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI230" s="167"/>
+      <c r="AJ230" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK230" s="165"/>
+      <c r="AL230" s="167"/>
+      <c r="AM230" s="107"/>
+      <c r="AN230" s="2"/>
       <c r="AP230" s="5"/>
       <c r="AQ230" s="2"/>
     </row>
     <row r="231" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A231" s="4"/>
+      <c r="B231" s="9"/>
+      <c r="C231" s="39"/>
+      <c r="D231" s="40"/>
+      <c r="E231" s="40"/>
+      <c r="F231" s="114"/>
+      <c r="G231" s="114"/>
+      <c r="H231" s="41"/>
+      <c r="I231" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="J231" s="113"/>
+      <c r="K231" s="113"/>
+      <c r="L231" s="113"/>
+      <c r="M231" s="113"/>
+      <c r="N231" s="113"/>
+      <c r="O231" s="113"/>
+      <c r="P231" s="113"/>
+      <c r="Q231" s="113"/>
+      <c r="R231" s="113"/>
+      <c r="S231" s="113"/>
+      <c r="T231" s="113"/>
+      <c r="U231" s="113"/>
+      <c r="V231" s="113"/>
+      <c r="W231" s="113"/>
+      <c r="X231" s="113"/>
+      <c r="Y231" s="164" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z231" s="113"/>
+      <c r="AA231" s="113"/>
+      <c r="AB231" s="113"/>
+      <c r="AC231" s="117"/>
+      <c r="AD231" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE231" s="165"/>
+      <c r="AF231" s="165"/>
+      <c r="AG231" s="167"/>
+      <c r="AH231" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI231" s="167"/>
+      <c r="AJ231" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK231" s="165"/>
+      <c r="AL231" s="167"/>
+      <c r="AM231" s="107"/>
+      <c r="AN231" s="2"/>
       <c r="AP231" s="5"/>
       <c r="AQ231" s="2"/>
     </row>
     <row r="232" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A232" s="4"/>
-      <c r="B232" s="1">
-        <v>12</v>
-      </c>
-      <c r="C232" s="1" t="s">
-        <v>157</v>
-      </c>
+      <c r="B232" s="9"/>
+      <c r="C232" s="108" t="s">
+        <v>244</v>
+      </c>
+      <c r="D232" s="109"/>
+      <c r="E232" s="109"/>
+      <c r="F232" s="115"/>
+      <c r="G232" s="115"/>
+      <c r="H232" s="112"/>
+      <c r="I232" s="171" t="s">
+        <v>249</v>
+      </c>
+      <c r="J232" s="171"/>
+      <c r="K232" s="171"/>
+      <c r="L232" s="171"/>
+      <c r="M232" s="171"/>
+      <c r="N232" s="171"/>
+      <c r="O232" s="171"/>
+      <c r="P232" s="171"/>
+      <c r="Q232" s="171"/>
+      <c r="R232" s="171"/>
+      <c r="S232" s="171"/>
+      <c r="T232" s="171"/>
+      <c r="U232" s="171"/>
+      <c r="V232" s="171"/>
+      <c r="W232" s="171"/>
+      <c r="X232" s="171"/>
+      <c r="Y232" s="172" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z232" s="171"/>
+      <c r="AA232" s="171"/>
+      <c r="AB232" s="171"/>
+      <c r="AC232" s="173"/>
+      <c r="AD232" s="174" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE232" s="175"/>
+      <c r="AF232" s="175"/>
+      <c r="AG232" s="176"/>
+      <c r="AH232" s="174" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI232" s="176"/>
+      <c r="AJ232" s="174" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK232" s="175"/>
+      <c r="AL232" s="176"/>
+      <c r="AM232" s="107"/>
+      <c r="AN232" s="2"/>
       <c r="AP232" s="5"/>
       <c r="AQ232" s="2"/>
     </row>
     <row r="233" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A233" s="4"/>
-      <c r="C233" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D233" s="1" t="s">
-        <v>165</v>
-      </c>
+      <c r="B233" s="9"/>
+      <c r="C233" s="99"/>
+      <c r="D233" s="16"/>
+      <c r="E233" s="16"/>
+      <c r="F233" s="107"/>
+      <c r="G233" s="107"/>
+      <c r="H233" s="159"/>
+      <c r="I233" s="160" t="s">
+        <v>250</v>
+      </c>
+      <c r="J233" s="113"/>
+      <c r="K233" s="113"/>
+      <c r="L233" s="113"/>
+      <c r="M233" s="113"/>
+      <c r="N233" s="113"/>
+      <c r="O233" s="113"/>
+      <c r="P233" s="113"/>
+      <c r="Q233" s="113"/>
+      <c r="R233" s="113"/>
+      <c r="S233" s="113"/>
+      <c r="T233" s="113"/>
+      <c r="U233" s="113"/>
+      <c r="V233" s="113"/>
+      <c r="W233" s="113"/>
+      <c r="X233" s="113"/>
+      <c r="Y233" s="164" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z233" s="113"/>
+      <c r="AA233" s="113"/>
+      <c r="AB233" s="113"/>
+      <c r="AC233" s="117"/>
+      <c r="AD233" s="166" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE233" s="165"/>
+      <c r="AF233" s="165"/>
+      <c r="AG233" s="167"/>
+      <c r="AH233" s="166" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI233" s="167"/>
+      <c r="AJ233" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK233" s="165"/>
+      <c r="AL233" s="167"/>
+      <c r="AM233" s="107"/>
+      <c r="AN233" s="2"/>
       <c r="AP233" s="5"/>
       <c r="AQ233" s="2"/>
     </row>
     <row r="234" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A234" s="4"/>
-      <c r="C234" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>166</v>
-      </c>
+      <c r="B234" s="9"/>
+      <c r="C234" s="39"/>
+      <c r="D234" s="40"/>
+      <c r="E234" s="40"/>
+      <c r="F234" s="114"/>
+      <c r="G234" s="114"/>
+      <c r="H234" s="118"/>
+      <c r="I234" s="171" t="s">
+        <v>259</v>
+      </c>
+      <c r="J234" s="171"/>
+      <c r="K234" s="171"/>
+      <c r="L234" s="171"/>
+      <c r="M234" s="171"/>
+      <c r="N234" s="171"/>
+      <c r="O234" s="171"/>
+      <c r="P234" s="171"/>
+      <c r="Q234" s="171"/>
+      <c r="R234" s="171"/>
+      <c r="S234" s="171"/>
+      <c r="T234" s="171"/>
+      <c r="U234" s="171"/>
+      <c r="V234" s="171"/>
+      <c r="W234" s="171"/>
+      <c r="X234" s="171"/>
+      <c r="Y234" s="172" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z234" s="171"/>
+      <c r="AA234" s="171"/>
+      <c r="AB234" s="171"/>
+      <c r="AC234" s="173"/>
+      <c r="AD234" s="177" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE234" s="178"/>
+      <c r="AF234" s="178"/>
+      <c r="AG234" s="179"/>
+      <c r="AH234" s="177" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI234" s="179"/>
+      <c r="AJ234" s="174" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK234" s="175"/>
+      <c r="AL234" s="176"/>
+      <c r="AM234" s="107"/>
+      <c r="AN234" s="2"/>
       <c r="AP234" s="5"/>
       <c r="AQ234" s="2"/>
     </row>
     <row r="235" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A235" s="4"/>
+      <c r="B235" s="9"/>
+      <c r="C235" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D235" s="12"/>
+      <c r="E235" s="12"/>
+      <c r="F235" s="113"/>
+      <c r="G235" s="113"/>
+      <c r="H235" s="117"/>
+      <c r="I235" s="160" t="s">
+        <v>246</v>
+      </c>
+      <c r="J235" s="113"/>
+      <c r="K235" s="113"/>
+      <c r="L235" s="113"/>
+      <c r="M235" s="113"/>
+      <c r="N235" s="113"/>
+      <c r="O235" s="113"/>
+      <c r="P235" s="113"/>
+      <c r="Q235" s="113"/>
+      <c r="R235" s="113"/>
+      <c r="S235" s="113"/>
+      <c r="T235" s="113"/>
+      <c r="U235" s="113"/>
+      <c r="V235" s="113"/>
+      <c r="W235" s="113"/>
+      <c r="X235" s="113"/>
+      <c r="Y235" s="164" t="s">
+        <v>253</v>
+      </c>
+      <c r="Z235" s="113"/>
+      <c r="AA235" s="113"/>
+      <c r="AB235" s="113"/>
+      <c r="AC235" s="117"/>
+      <c r="AD235" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE235" s="139"/>
+      <c r="AF235" s="139"/>
+      <c r="AG235" s="140"/>
+      <c r="AH235" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI235" s="140"/>
+      <c r="AJ235" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK235" s="139"/>
+      <c r="AL235" s="140"/>
+      <c r="AM235" s="107"/>
+      <c r="AN235" s="2"/>
       <c r="AP235" s="5"/>
       <c r="AQ235" s="2"/>
     </row>
     <row r="236" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A236" s="4"/>
+      <c r="C236" s="3"/>
+      <c r="D236" s="3"/>
+      <c r="E236" s="3"/>
+      <c r="F236" s="107"/>
+      <c r="G236" s="107"/>
+      <c r="H236" s="107"/>
+      <c r="I236" s="107"/>
+      <c r="J236" s="107"/>
+      <c r="K236" s="107"/>
+      <c r="L236" s="107"/>
+      <c r="M236" s="107"/>
+      <c r="N236" s="107"/>
+      <c r="O236" s="107"/>
+      <c r="P236" s="107"/>
+      <c r="Q236" s="107"/>
+      <c r="R236" s="107"/>
+      <c r="S236" s="107"/>
+      <c r="T236" s="107"/>
+      <c r="U236" s="107"/>
+      <c r="V236" s="107"/>
+      <c r="W236" s="107"/>
+      <c r="X236" s="107"/>
+      <c r="Y236" s="107"/>
+      <c r="Z236" s="107"/>
+      <c r="AA236" s="107"/>
+      <c r="AB236" s="107"/>
+      <c r="AC236" s="107"/>
+      <c r="AD236" s="107"/>
+      <c r="AE236" s="107"/>
+      <c r="AF236" s="107"/>
+      <c r="AG236" s="107"/>
+      <c r="AH236" s="107"/>
+      <c r="AI236" s="107"/>
+      <c r="AJ236" s="107"/>
+      <c r="AK236" s="107"/>
+      <c r="AL236" s="107"/>
+      <c r="AM236" s="107"/>
+      <c r="AN236" s="2"/>
       <c r="AP236" s="5"/>
       <c r="AQ236" s="2"/>
     </row>
     <row r="237" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A237" s="4"/>
+      <c r="F237" s="107"/>
+      <c r="G237" s="107"/>
+      <c r="H237" s="107"/>
+      <c r="I237" s="107"/>
+      <c r="J237" s="107"/>
+      <c r="K237" s="107"/>
+      <c r="L237" s="107"/>
+      <c r="M237" s="107"/>
+      <c r="N237" s="107"/>
+      <c r="O237" s="107"/>
+      <c r="P237" s="107"/>
+      <c r="Q237" s="107"/>
+      <c r="R237" s="107"/>
+      <c r="S237" s="107"/>
+      <c r="T237" s="107"/>
+      <c r="U237" s="107"/>
+      <c r="V237" s="107"/>
+      <c r="W237" s="107"/>
+      <c r="X237" s="107"/>
+      <c r="Y237" s="107"/>
+      <c r="Z237" s="107"/>
+      <c r="AA237" s="107"/>
+      <c r="AB237" s="107"/>
+      <c r="AC237" s="107"/>
+      <c r="AD237" s="107"/>
+      <c r="AE237" s="107"/>
+      <c r="AF237" s="107"/>
+      <c r="AG237" s="107"/>
+      <c r="AH237" s="107"/>
+      <c r="AI237" s="107"/>
+      <c r="AJ237" s="107"/>
+      <c r="AK237" s="107"/>
+      <c r="AL237" s="107"/>
+      <c r="AM237" s="107"/>
+      <c r="AN237" s="2"/>
       <c r="AP237" s="5"/>
       <c r="AQ237" s="2"/>
     </row>
     <row r="238" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A238" s="4"/>
+      <c r="B238" s="1">
+        <v>12</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="AP238" s="5"/>
       <c r="AQ238" s="2"/>
     </row>
     <row r="239" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A239" s="4"/>
+      <c r="C239" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="AP239" s="5"/>
       <c r="AQ239" s="2"/>
     </row>
     <row r="240" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A240" s="4"/>
+      <c r="C240" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="AP240" s="5"/>
       <c r="AQ240" s="2"/>
     </row>
     <row r="241" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A241" s="4"/>
+      <c r="C241" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="AP241" s="5"/>
       <c r="AQ241" s="2"/>
     </row>
     <row r="242" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A242" s="4"/>
+      <c r="C242" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="AP242" s="5"/>
       <c r="AQ242" s="2"/>
     </row>
     <row r="243" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A243" s="6"/>
-      <c r="B243" s="7"/>
-      <c r="C243" s="7"/>
-      <c r="D243" s="7"/>
-      <c r="E243" s="7"/>
-      <c r="F243" s="7"/>
-      <c r="G243" s="7"/>
-      <c r="H243" s="7"/>
-      <c r="I243" s="7"/>
-      <c r="J243" s="7"/>
-      <c r="K243" s="7"/>
-      <c r="L243" s="7"/>
-      <c r="M243" s="7"/>
-      <c r="N243" s="7"/>
-      <c r="O243" s="7"/>
-      <c r="P243" s="7"/>
-      <c r="Q243" s="7"/>
-      <c r="R243" s="7"/>
-      <c r="S243" s="7"/>
-      <c r="T243" s="7"/>
-      <c r="U243" s="7"/>
-      <c r="V243" s="7"/>
-      <c r="W243" s="7"/>
-      <c r="X243" s="7"/>
-      <c r="Y243" s="7"/>
-      <c r="Z243" s="7"/>
-      <c r="AA243" s="7"/>
-      <c r="AB243" s="7"/>
-      <c r="AC243" s="7"/>
-      <c r="AD243" s="7"/>
-      <c r="AE243" s="7"/>
-      <c r="AF243" s="7"/>
-      <c r="AG243" s="7"/>
-      <c r="AH243" s="7"/>
-      <c r="AI243" s="7"/>
-      <c r="AJ243" s="7"/>
-      <c r="AK243" s="7"/>
-      <c r="AL243" s="7"/>
-      <c r="AM243" s="7"/>
-      <c r="AN243" s="7"/>
-      <c r="AO243" s="7"/>
-      <c r="AP243" s="8"/>
+      <c r="A243" s="4"/>
+      <c r="D243" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AP243" s="5"/>
       <c r="AQ243" s="2"/>
     </row>
     <row r="244" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A244" s="3"/>
-      <c r="B244" s="3"/>
-      <c r="C244" s="3"/>
-      <c r="D244" s="3"/>
-      <c r="E244" s="3"/>
-      <c r="F244" s="3"/>
-      <c r="G244" s="3"/>
-      <c r="H244" s="3"/>
-      <c r="I244" s="3"/>
-      <c r="J244" s="3"/>
-      <c r="K244" s="3"/>
-      <c r="L244" s="3"/>
-      <c r="M244" s="3"/>
-      <c r="N244" s="3"/>
-      <c r="O244" s="3"/>
-      <c r="P244" s="3"/>
-      <c r="Q244" s="3"/>
-      <c r="R244" s="3"/>
-      <c r="S244" s="3"/>
-      <c r="T244" s="3"/>
-      <c r="U244" s="3"/>
-      <c r="V244" s="3"/>
-      <c r="W244" s="3"/>
-      <c r="X244" s="3"/>
-      <c r="Y244" s="3"/>
-      <c r="Z244" s="3"/>
-      <c r="AA244" s="3"/>
-      <c r="AB244" s="3"/>
-      <c r="AC244" s="3"/>
-      <c r="AD244" s="3"/>
-      <c r="AE244" s="3"/>
-      <c r="AF244" s="3"/>
-      <c r="AG244" s="3"/>
-      <c r="AH244" s="3"/>
-      <c r="AI244" s="3"/>
-      <c r="AJ244" s="3"/>
-      <c r="AK244" s="3"/>
-      <c r="AL244" s="3"/>
-      <c r="AM244" s="3"/>
-      <c r="AN244" s="3"/>
-      <c r="AO244" s="3"/>
-      <c r="AP244" s="3"/>
+      <c r="A244" s="4"/>
+      <c r="AP244" s="5"/>
+      <c r="AQ244" s="2"/>
+    </row>
+    <row r="245" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A245" s="4"/>
+      <c r="AP245" s="5"/>
+      <c r="AQ245" s="2"/>
+    </row>
+    <row r="246" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A246" s="4"/>
+      <c r="B246" s="1">
+        <v>13</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AP246" s="5"/>
+      <c r="AQ246" s="2"/>
+    </row>
+    <row r="247" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A247" s="4"/>
+      <c r="C247" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AP247" s="5"/>
+      <c r="AQ247" s="2"/>
+    </row>
+    <row r="248" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A248" s="4"/>
+      <c r="C248" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP248" s="5"/>
+      <c r="AQ248" s="2"/>
+    </row>
+    <row r="249" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A249" s="4"/>
+      <c r="AP249" s="5"/>
+      <c r="AQ249" s="2"/>
+    </row>
+    <row r="250" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A250" s="4"/>
+      <c r="AP250" s="5"/>
+      <c r="AQ250" s="2"/>
+    </row>
+    <row r="251" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A251" s="4"/>
+      <c r="AP251" s="5"/>
+      <c r="AQ251" s="2"/>
+    </row>
+    <row r="252" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A252" s="4"/>
+      <c r="AP252" s="5"/>
+      <c r="AQ252" s="2"/>
+    </row>
+    <row r="253" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A253" s="4"/>
+      <c r="AP253" s="5"/>
+      <c r="AQ253" s="2"/>
+    </row>
+    <row r="254" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A254" s="4"/>
+      <c r="AP254" s="5"/>
+      <c r="AQ254" s="2"/>
+    </row>
+    <row r="255" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A255" s="4"/>
+      <c r="AP255" s="5"/>
+      <c r="AQ255" s="2"/>
+    </row>
+    <row r="256" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A256" s="4"/>
+      <c r="AP256" s="5"/>
+      <c r="AQ256" s="2"/>
+    </row>
+    <row r="257" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A257" s="6"/>
+      <c r="B257" s="7"/>
+      <c r="C257" s="7"/>
+      <c r="D257" s="7"/>
+      <c r="E257" s="7"/>
+      <c r="F257" s="7"/>
+      <c r="G257" s="7"/>
+      <c r="H257" s="7"/>
+      <c r="I257" s="7"/>
+      <c r="J257" s="7"/>
+      <c r="K257" s="7"/>
+      <c r="L257" s="7"/>
+      <c r="M257" s="7"/>
+      <c r="N257" s="7"/>
+      <c r="O257" s="7"/>
+      <c r="P257" s="7"/>
+      <c r="Q257" s="7"/>
+      <c r="R257" s="7"/>
+      <c r="S257" s="7"/>
+      <c r="T257" s="7"/>
+      <c r="U257" s="7"/>
+      <c r="V257" s="7"/>
+      <c r="W257" s="7"/>
+      <c r="X257" s="7"/>
+      <c r="Y257" s="7"/>
+      <c r="Z257" s="7"/>
+      <c r="AA257" s="7"/>
+      <c r="AB257" s="7"/>
+      <c r="AC257" s="7"/>
+      <c r="AD257" s="7"/>
+      <c r="AE257" s="7"/>
+      <c r="AF257" s="7"/>
+      <c r="AG257" s="7"/>
+      <c r="AH257" s="7"/>
+      <c r="AI257" s="7"/>
+      <c r="AJ257" s="7"/>
+      <c r="AK257" s="7"/>
+      <c r="AL257" s="7"/>
+      <c r="AM257" s="7"/>
+      <c r="AN257" s="7"/>
+      <c r="AO257" s="7"/>
+      <c r="AP257" s="8"/>
+      <c r="AQ257" s="2"/>
+    </row>
+    <row r="258" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A258" s="3"/>
+      <c r="B258" s="3"/>
+      <c r="C258" s="3"/>
+      <c r="D258" s="3"/>
+      <c r="E258" s="3"/>
+      <c r="F258" s="3"/>
+      <c r="G258" s="3"/>
+      <c r="H258" s="3"/>
+      <c r="I258" s="3"/>
+      <c r="J258" s="3"/>
+      <c r="K258" s="3"/>
+      <c r="L258" s="3"/>
+      <c r="M258" s="3"/>
+      <c r="N258" s="3"/>
+      <c r="O258" s="3"/>
+      <c r="P258" s="3"/>
+      <c r="Q258" s="3"/>
+      <c r="R258" s="3"/>
+      <c r="S258" s="3"/>
+      <c r="T258" s="3"/>
+      <c r="U258" s="3"/>
+      <c r="V258" s="3"/>
+      <c r="W258" s="3"/>
+      <c r="X258" s="3"/>
+      <c r="Y258" s="3"/>
+      <c r="Z258" s="3"/>
+      <c r="AA258" s="3"/>
+      <c r="AB258" s="3"/>
+      <c r="AC258" s="3"/>
+      <c r="AD258" s="3"/>
+      <c r="AE258" s="3"/>
+      <c r="AF258" s="3"/>
+      <c r="AG258" s="3"/>
+      <c r="AH258" s="3"/>
+      <c r="AI258" s="3"/>
+      <c r="AJ258" s="3"/>
+      <c r="AK258" s="3"/>
+      <c r="AL258" s="3"/>
+      <c r="AM258" s="3"/>
+      <c r="AN258" s="3"/>
+      <c r="AO258" s="3"/>
+      <c r="AP258" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="172">
-    <mergeCell ref="Y174:AD174"/>
-    <mergeCell ref="Y159:AD159"/>
-    <mergeCell ref="Y160:AD160"/>
-    <mergeCell ref="Y161:AD161"/>
-    <mergeCell ref="Y162:AD162"/>
-    <mergeCell ref="Y163:AD163"/>
-    <mergeCell ref="Y164:AD164"/>
-    <mergeCell ref="Y165:AD165"/>
-    <mergeCell ref="Y166:AD166"/>
-    <mergeCell ref="Y167:AD167"/>
+  <mergeCells count="197">
+    <mergeCell ref="AJ234:AL234"/>
+    <mergeCell ref="AD226:AL226"/>
+    <mergeCell ref="AD228:AG228"/>
+    <mergeCell ref="AD229:AG229"/>
+    <mergeCell ref="AD230:AG230"/>
+    <mergeCell ref="AD231:AG231"/>
+    <mergeCell ref="AD232:AG232"/>
+    <mergeCell ref="AD233:AG233"/>
+    <mergeCell ref="AD235:AG235"/>
+    <mergeCell ref="AH228:AI228"/>
+    <mergeCell ref="AH229:AI229"/>
+    <mergeCell ref="AH230:AI230"/>
+    <mergeCell ref="AH231:AI231"/>
+    <mergeCell ref="AH232:AI232"/>
+    <mergeCell ref="AH233:AI233"/>
+    <mergeCell ref="AH235:AI235"/>
+    <mergeCell ref="AJ228:AL228"/>
+    <mergeCell ref="AJ229:AL229"/>
+    <mergeCell ref="AJ230:AL230"/>
+    <mergeCell ref="AJ231:AL231"/>
+    <mergeCell ref="AJ232:AL232"/>
+    <mergeCell ref="AJ233:AL233"/>
+    <mergeCell ref="AJ235:AL235"/>
+    <mergeCell ref="AD234:AG234"/>
+    <mergeCell ref="AH234:AI234"/>
+    <mergeCell ref="AL1:AP1"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="AL2:AP2"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="AD2:AH2"/>
+    <mergeCell ref="P1:Z1"/>
+    <mergeCell ref="P2:Z2"/>
+    <mergeCell ref="L47:AD47"/>
+    <mergeCell ref="L48:AD48"/>
+    <mergeCell ref="L18:AD18"/>
+    <mergeCell ref="L19:AD19"/>
+    <mergeCell ref="L20:AD20"/>
+    <mergeCell ref="L40:AD40"/>
+    <mergeCell ref="L41:AD41"/>
+    <mergeCell ref="L43:AD43"/>
+    <mergeCell ref="L39:AD39"/>
+    <mergeCell ref="L42:AD42"/>
+    <mergeCell ref="Y156:AD156"/>
+    <mergeCell ref="Y157:AD157"/>
+    <mergeCell ref="Y158:AD158"/>
+    <mergeCell ref="S142:X142"/>
+    <mergeCell ref="S143:X143"/>
+    <mergeCell ref="S144:X144"/>
+    <mergeCell ref="S145:X145"/>
+    <mergeCell ref="S146:X146"/>
+    <mergeCell ref="S147:X147"/>
+    <mergeCell ref="S148:X148"/>
+    <mergeCell ref="S149:X149"/>
+    <mergeCell ref="S150:X150"/>
+    <mergeCell ref="S151:X151"/>
+    <mergeCell ref="S152:X152"/>
+    <mergeCell ref="S153:X153"/>
+    <mergeCell ref="S154:X154"/>
+    <mergeCell ref="S155:X155"/>
+    <mergeCell ref="S156:X156"/>
+    <mergeCell ref="S157:X157"/>
+    <mergeCell ref="S158:X158"/>
+    <mergeCell ref="AE148:AJ148"/>
+    <mergeCell ref="AE149:AJ149"/>
+    <mergeCell ref="AE150:AJ150"/>
+    <mergeCell ref="L44:AD44"/>
+    <mergeCell ref="Y151:AD151"/>
+    <mergeCell ref="Y152:AD152"/>
+    <mergeCell ref="Y153:AD153"/>
+    <mergeCell ref="Y154:AD154"/>
+    <mergeCell ref="Y155:AD155"/>
+    <mergeCell ref="S129:X129"/>
+    <mergeCell ref="S130:X130"/>
+    <mergeCell ref="S131:X131"/>
+    <mergeCell ref="S132:X132"/>
+    <mergeCell ref="S133:X133"/>
+    <mergeCell ref="S134:X134"/>
+    <mergeCell ref="S135:X135"/>
+    <mergeCell ref="S136:X136"/>
+    <mergeCell ref="S137:X137"/>
+    <mergeCell ref="S138:X138"/>
+    <mergeCell ref="S139:X139"/>
+    <mergeCell ref="S140:X140"/>
+    <mergeCell ref="S141:X141"/>
+    <mergeCell ref="S125:X125"/>
+    <mergeCell ref="L49:AD49"/>
+    <mergeCell ref="AE160:AJ160"/>
+    <mergeCell ref="AE151:AJ151"/>
+    <mergeCell ref="AE152:AJ152"/>
+    <mergeCell ref="AE153:AJ153"/>
+    <mergeCell ref="AE154:AJ154"/>
+    <mergeCell ref="AE155:AJ155"/>
+    <mergeCell ref="AE156:AJ156"/>
+    <mergeCell ref="AE157:AJ157"/>
+    <mergeCell ref="AE158:AJ158"/>
+    <mergeCell ref="AE159:AJ159"/>
+    <mergeCell ref="AE166:AJ166"/>
+    <mergeCell ref="AE167:AJ167"/>
+    <mergeCell ref="AE168:AJ168"/>
+    <mergeCell ref="AE169:AJ169"/>
+    <mergeCell ref="Y168:AD168"/>
+    <mergeCell ref="Y169:AD169"/>
+    <mergeCell ref="AE161:AJ161"/>
+    <mergeCell ref="AE162:AJ162"/>
+    <mergeCell ref="AE163:AJ163"/>
+    <mergeCell ref="AE164:AJ164"/>
+    <mergeCell ref="AE165:AJ165"/>
+    <mergeCell ref="AE170:AJ170"/>
+    <mergeCell ref="AE171:AJ171"/>
+    <mergeCell ref="AE172:AJ172"/>
+    <mergeCell ref="Y170:AD170"/>
+    <mergeCell ref="Y171:AD171"/>
+    <mergeCell ref="Y172:AD172"/>
+    <mergeCell ref="S167:X167"/>
+    <mergeCell ref="S168:X168"/>
+    <mergeCell ref="S169:X169"/>
+    <mergeCell ref="S124:X124"/>
+    <mergeCell ref="Y124:AD124"/>
+    <mergeCell ref="Y125:AD125"/>
+    <mergeCell ref="AE124:AJ124"/>
+    <mergeCell ref="AE125:AJ125"/>
+    <mergeCell ref="S127:X127"/>
+    <mergeCell ref="S128:X128"/>
+    <mergeCell ref="Y127:AD127"/>
+    <mergeCell ref="Y128:AD128"/>
+    <mergeCell ref="AE127:AJ127"/>
+    <mergeCell ref="AE128:AJ128"/>
+    <mergeCell ref="S159:X159"/>
+    <mergeCell ref="S160:X160"/>
+    <mergeCell ref="S161:X161"/>
+    <mergeCell ref="S162:X162"/>
+    <mergeCell ref="S163:X163"/>
+    <mergeCell ref="S164:X164"/>
+    <mergeCell ref="S165:X165"/>
+    <mergeCell ref="S166:X166"/>
+    <mergeCell ref="S173:X173"/>
+    <mergeCell ref="S170:X170"/>
+    <mergeCell ref="S171:X171"/>
+    <mergeCell ref="S172:X172"/>
+    <mergeCell ref="S174:X174"/>
+    <mergeCell ref="S175:X175"/>
+    <mergeCell ref="Y175:AD175"/>
+    <mergeCell ref="AE175:AJ175"/>
+    <mergeCell ref="AE129:AJ129"/>
+    <mergeCell ref="AE130:AJ130"/>
+    <mergeCell ref="AE131:AJ131"/>
+    <mergeCell ref="AE132:AJ132"/>
+    <mergeCell ref="AE133:AJ133"/>
+    <mergeCell ref="AE134:AJ134"/>
+    <mergeCell ref="AE135:AJ135"/>
+    <mergeCell ref="AE136:AJ136"/>
+    <mergeCell ref="AE137:AJ137"/>
+    <mergeCell ref="AE138:AJ138"/>
+    <mergeCell ref="AE139:AJ139"/>
+    <mergeCell ref="AE140:AJ140"/>
+    <mergeCell ref="AE141:AJ141"/>
+    <mergeCell ref="AE142:AJ142"/>
+    <mergeCell ref="AE143:AJ143"/>
+    <mergeCell ref="AE144:AJ144"/>
+    <mergeCell ref="AE145:AJ145"/>
+    <mergeCell ref="AE146:AJ146"/>
+    <mergeCell ref="AE147:AJ147"/>
+    <mergeCell ref="AE173:AJ173"/>
     <mergeCell ref="AE174:AJ174"/>
     <mergeCell ref="Y129:AD129"/>
     <mergeCell ref="Y130:AD130"/>
@@ -14806,144 +16052,16 @@
     <mergeCell ref="Y149:AD149"/>
     <mergeCell ref="Y150:AD150"/>
     <mergeCell ref="Y173:AD173"/>
-    <mergeCell ref="S174:X174"/>
-    <mergeCell ref="S175:X175"/>
-    <mergeCell ref="Y175:AD175"/>
-    <mergeCell ref="AE175:AJ175"/>
-    <mergeCell ref="AE129:AJ129"/>
-    <mergeCell ref="AE130:AJ130"/>
-    <mergeCell ref="AE131:AJ131"/>
-    <mergeCell ref="AE132:AJ132"/>
-    <mergeCell ref="AE133:AJ133"/>
-    <mergeCell ref="AE134:AJ134"/>
-    <mergeCell ref="AE135:AJ135"/>
-    <mergeCell ref="AE136:AJ136"/>
-    <mergeCell ref="AE137:AJ137"/>
-    <mergeCell ref="AE138:AJ138"/>
-    <mergeCell ref="AE139:AJ139"/>
-    <mergeCell ref="AE140:AJ140"/>
-    <mergeCell ref="AE141:AJ141"/>
-    <mergeCell ref="AE142:AJ142"/>
-    <mergeCell ref="AE143:AJ143"/>
-    <mergeCell ref="AE144:AJ144"/>
-    <mergeCell ref="AE145:AJ145"/>
-    <mergeCell ref="AE146:AJ146"/>
-    <mergeCell ref="AE147:AJ147"/>
-    <mergeCell ref="AE173:AJ173"/>
-    <mergeCell ref="S159:X159"/>
-    <mergeCell ref="S160:X160"/>
-    <mergeCell ref="S161:X161"/>
-    <mergeCell ref="S162:X162"/>
-    <mergeCell ref="S163:X163"/>
-    <mergeCell ref="S164:X164"/>
-    <mergeCell ref="S165:X165"/>
-    <mergeCell ref="S166:X166"/>
-    <mergeCell ref="S173:X173"/>
-    <mergeCell ref="S170:X170"/>
-    <mergeCell ref="S171:X171"/>
-    <mergeCell ref="S172:X172"/>
-    <mergeCell ref="S124:X124"/>
-    <mergeCell ref="Y124:AD124"/>
-    <mergeCell ref="Y125:AD125"/>
-    <mergeCell ref="AE124:AJ124"/>
-    <mergeCell ref="AE125:AJ125"/>
-    <mergeCell ref="S127:X127"/>
-    <mergeCell ref="S128:X128"/>
-    <mergeCell ref="Y127:AD127"/>
-    <mergeCell ref="Y128:AD128"/>
-    <mergeCell ref="AE127:AJ127"/>
-    <mergeCell ref="AE128:AJ128"/>
-    <mergeCell ref="AE170:AJ170"/>
-    <mergeCell ref="AE171:AJ171"/>
-    <mergeCell ref="AE172:AJ172"/>
-    <mergeCell ref="Y170:AD170"/>
-    <mergeCell ref="Y171:AD171"/>
-    <mergeCell ref="Y172:AD172"/>
-    <mergeCell ref="S167:X167"/>
-    <mergeCell ref="S168:X168"/>
-    <mergeCell ref="S169:X169"/>
-    <mergeCell ref="AE166:AJ166"/>
-    <mergeCell ref="AE167:AJ167"/>
-    <mergeCell ref="AE168:AJ168"/>
-    <mergeCell ref="AE169:AJ169"/>
-    <mergeCell ref="Y168:AD168"/>
-    <mergeCell ref="Y169:AD169"/>
-    <mergeCell ref="AE161:AJ161"/>
-    <mergeCell ref="AE162:AJ162"/>
-    <mergeCell ref="AE163:AJ163"/>
-    <mergeCell ref="AE164:AJ164"/>
-    <mergeCell ref="AE165:AJ165"/>
-    <mergeCell ref="AE160:AJ160"/>
-    <mergeCell ref="AE151:AJ151"/>
-    <mergeCell ref="AE152:AJ152"/>
-    <mergeCell ref="AE153:AJ153"/>
-    <mergeCell ref="AE154:AJ154"/>
-    <mergeCell ref="AE155:AJ155"/>
-    <mergeCell ref="AE156:AJ156"/>
-    <mergeCell ref="AE157:AJ157"/>
-    <mergeCell ref="AE158:AJ158"/>
-    <mergeCell ref="AE159:AJ159"/>
-    <mergeCell ref="AE148:AJ148"/>
-    <mergeCell ref="AE149:AJ149"/>
-    <mergeCell ref="AE150:AJ150"/>
-    <mergeCell ref="L44:AD44"/>
-    <mergeCell ref="Y151:AD151"/>
-    <mergeCell ref="Y152:AD152"/>
-    <mergeCell ref="Y153:AD153"/>
-    <mergeCell ref="Y154:AD154"/>
-    <mergeCell ref="Y155:AD155"/>
-    <mergeCell ref="S129:X129"/>
-    <mergeCell ref="S130:X130"/>
-    <mergeCell ref="S131:X131"/>
-    <mergeCell ref="S132:X132"/>
-    <mergeCell ref="S133:X133"/>
-    <mergeCell ref="S134:X134"/>
-    <mergeCell ref="S135:X135"/>
-    <mergeCell ref="S136:X136"/>
-    <mergeCell ref="S137:X137"/>
-    <mergeCell ref="S138:X138"/>
-    <mergeCell ref="S139:X139"/>
-    <mergeCell ref="S140:X140"/>
-    <mergeCell ref="S141:X141"/>
-    <mergeCell ref="S125:X125"/>
-    <mergeCell ref="L49:AD49"/>
-    <mergeCell ref="Y156:AD156"/>
-    <mergeCell ref="Y157:AD157"/>
-    <mergeCell ref="Y158:AD158"/>
-    <mergeCell ref="S142:X142"/>
-    <mergeCell ref="S143:X143"/>
-    <mergeCell ref="S144:X144"/>
-    <mergeCell ref="S145:X145"/>
-    <mergeCell ref="S146:X146"/>
-    <mergeCell ref="S147:X147"/>
-    <mergeCell ref="S148:X148"/>
-    <mergeCell ref="S149:X149"/>
-    <mergeCell ref="S150:X150"/>
-    <mergeCell ref="S151:X151"/>
-    <mergeCell ref="S152:X152"/>
-    <mergeCell ref="S153:X153"/>
-    <mergeCell ref="S154:X154"/>
-    <mergeCell ref="S155:X155"/>
-    <mergeCell ref="S156:X156"/>
-    <mergeCell ref="S157:X157"/>
-    <mergeCell ref="S158:X158"/>
-    <mergeCell ref="AL1:AP1"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="AL2:AP2"/>
-    <mergeCell ref="AD1:AH1"/>
-    <mergeCell ref="AD2:AH2"/>
-    <mergeCell ref="P1:Z1"/>
-    <mergeCell ref="P2:Z2"/>
-    <mergeCell ref="L47:AD47"/>
-    <mergeCell ref="L48:AD48"/>
-    <mergeCell ref="L18:AD18"/>
-    <mergeCell ref="L19:AD19"/>
-    <mergeCell ref="L20:AD20"/>
-    <mergeCell ref="L40:AD40"/>
-    <mergeCell ref="L41:AD41"/>
-    <mergeCell ref="L43:AD43"/>
-    <mergeCell ref="L39:AD39"/>
-    <mergeCell ref="L42:AD42"/>
+    <mergeCell ref="Y174:AD174"/>
+    <mergeCell ref="Y159:AD159"/>
+    <mergeCell ref="Y160:AD160"/>
+    <mergeCell ref="Y161:AD161"/>
+    <mergeCell ref="Y162:AD162"/>
+    <mergeCell ref="Y163:AD163"/>
+    <mergeCell ref="Y164:AD164"/>
+    <mergeCell ref="Y165:AD165"/>
+    <mergeCell ref="Y166:AD166"/>
+    <mergeCell ref="Y167:AD167"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a PDF download specific design doc.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/RequirementDefinition.xlsx
+++ b/skrum_docs/02_SpecificationDocs/RequirementDefinition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="27520" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="更新履歴" sheetId="2" r:id="rId1"/>
@@ -2838,13 +2838,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>　OKR削除、</t>
-    <rPh sb="4" eb="6">
-      <t>サク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>自投稿操作</t>
     <rPh sb="0" eb="1">
       <t>ジ</t>
@@ -3205,6 +3198,16 @@
     </rPh>
     <rPh sb="17" eb="19">
       <t>ハッシn</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　OKR削除、OKR追加、</t>
+    <rPh sb="4" eb="6">
+      <t>サク</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ツイk</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4330,21 +4333,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom style="dotted">
@@ -4516,13 +4504,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="250">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -4660,25 +4661,25 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="83" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="87" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="90" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="91" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="92" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="93" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -4714,7 +4715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4732,6 +4733,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4741,7 +4787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4768,24 +4814,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4795,42 +4823,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4838,9 +4830,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -4913,6 +4902,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6498,7 +6505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6729,13 +6736,13 @@
         <v>42979</v>
       </c>
       <c r="C12" s="71" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D12" s="71" t="s">
         <v>66</v>
       </c>
       <c r="E12" s="71" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F12" s="71"/>
     </row>
@@ -6748,13 +6755,13 @@
         <v>42991</v>
       </c>
       <c r="C13" s="71" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D13" s="71" t="s">
         <v>66</v>
       </c>
       <c r="E13" s="71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F13" s="71"/>
     </row>
@@ -7250,7 +7257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ293"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
@@ -7260,15 +7267,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="219" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="224"/>
-      <c r="C1" s="224"/>
-      <c r="D1" s="224"/>
-      <c r="E1" s="224"/>
-      <c r="F1" s="224"/>
-      <c r="G1" s="225"/>
+      <c r="B1" s="220"/>
+      <c r="C1" s="220"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="220"/>
+      <c r="F1" s="220"/>
+      <c r="G1" s="221"/>
       <c r="H1" s="47"/>
       <c r="I1" s="44" t="s">
         <v>72</v>
@@ -7279,53 +7286,53 @@
       <c r="M1" s="45"/>
       <c r="N1" s="45"/>
       <c r="O1" s="46"/>
-      <c r="P1" s="232" t="s">
+      <c r="P1" s="228" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="233"/>
-      <c r="R1" s="233"/>
-      <c r="S1" s="233"/>
-      <c r="T1" s="233"/>
-      <c r="U1" s="233"/>
-      <c r="V1" s="233"/>
-      <c r="W1" s="233"/>
-      <c r="X1" s="233"/>
-      <c r="Y1" s="233"/>
-      <c r="Z1" s="234"/>
+      <c r="Q1" s="229"/>
+      <c r="R1" s="229"/>
+      <c r="S1" s="229"/>
+      <c r="T1" s="229"/>
+      <c r="U1" s="229"/>
+      <c r="V1" s="229"/>
+      <c r="W1" s="229"/>
+      <c r="X1" s="229"/>
+      <c r="Y1" s="229"/>
+      <c r="Z1" s="230"/>
       <c r="AA1" s="44" t="s">
         <v>67</v>
       </c>
       <c r="AB1" s="42"/>
       <c r="AC1" s="43"/>
-      <c r="AD1" s="229">
+      <c r="AD1" s="225">
         <v>42760</v>
       </c>
-      <c r="AE1" s="230"/>
-      <c r="AF1" s="230"/>
-      <c r="AG1" s="230"/>
-      <c r="AH1" s="231"/>
+      <c r="AE1" s="226"/>
+      <c r="AF1" s="226"/>
+      <c r="AG1" s="226"/>
+      <c r="AH1" s="227"/>
       <c r="AI1" s="44" t="s">
         <v>69</v>
       </c>
       <c r="AJ1" s="45"/>
       <c r="AK1" s="46"/>
-      <c r="AL1" s="220" t="s">
+      <c r="AL1" s="216" t="s">
         <v>71</v>
       </c>
-      <c r="AM1" s="221"/>
-      <c r="AN1" s="221"/>
-      <c r="AO1" s="221"/>
-      <c r="AP1" s="222"/>
+      <c r="AM1" s="217"/>
+      <c r="AN1" s="217"/>
+      <c r="AO1" s="217"/>
+      <c r="AP1" s="218"/>
       <c r="AQ1" s="2"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A2" s="226"/>
-      <c r="B2" s="227"/>
-      <c r="C2" s="227"/>
-      <c r="D2" s="227"/>
-      <c r="E2" s="227"/>
-      <c r="F2" s="227"/>
-      <c r="G2" s="228"/>
+      <c r="A2" s="222"/>
+      <c r="B2" s="223"/>
+      <c r="C2" s="223"/>
+      <c r="D2" s="223"/>
+      <c r="E2" s="223"/>
+      <c r="F2" s="223"/>
+      <c r="G2" s="224"/>
       <c r="H2" s="48"/>
       <c r="I2" s="44" t="s">
         <v>73</v>
@@ -7336,41 +7343,41 @@
       <c r="M2" s="45"/>
       <c r="N2" s="45"/>
       <c r="O2" s="46"/>
-      <c r="P2" s="232"/>
-      <c r="Q2" s="233"/>
-      <c r="R2" s="233"/>
-      <c r="S2" s="233"/>
-      <c r="T2" s="233"/>
-      <c r="U2" s="233"/>
-      <c r="V2" s="233"/>
-      <c r="W2" s="233"/>
-      <c r="X2" s="233"/>
-      <c r="Y2" s="233"/>
-      <c r="Z2" s="234"/>
+      <c r="P2" s="228"/>
+      <c r="Q2" s="229"/>
+      <c r="R2" s="229"/>
+      <c r="S2" s="229"/>
+      <c r="T2" s="229"/>
+      <c r="U2" s="229"/>
+      <c r="V2" s="229"/>
+      <c r="W2" s="229"/>
+      <c r="X2" s="229"/>
+      <c r="Y2" s="229"/>
+      <c r="Z2" s="230"/>
       <c r="AA2" s="44" t="s">
         <v>68</v>
       </c>
       <c r="AB2" s="42"/>
       <c r="AC2" s="43"/>
-      <c r="AD2" s="229">
+      <c r="AD2" s="225">
         <v>42991</v>
       </c>
-      <c r="AE2" s="230"/>
-      <c r="AF2" s="230"/>
-      <c r="AG2" s="230"/>
-      <c r="AH2" s="231"/>
+      <c r="AE2" s="226"/>
+      <c r="AF2" s="226"/>
+      <c r="AG2" s="226"/>
+      <c r="AH2" s="227"/>
       <c r="AI2" s="44" t="s">
         <v>70</v>
       </c>
       <c r="AJ2" s="45"/>
       <c r="AK2" s="46"/>
-      <c r="AL2" s="220" t="s">
+      <c r="AL2" s="216" t="s">
         <v>71</v>
       </c>
-      <c r="AM2" s="221"/>
-      <c r="AN2" s="221"/>
-      <c r="AO2" s="221"/>
-      <c r="AP2" s="222"/>
+      <c r="AM2" s="217"/>
+      <c r="AN2" s="217"/>
+      <c r="AO2" s="217"/>
+      <c r="AP2" s="218"/>
       <c r="AQ2" s="2"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
@@ -7908,27 +7915,27 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="34"/>
-      <c r="L19" s="216" t="s">
+      <c r="L19" s="213" t="s">
         <v>47</v>
       </c>
-      <c r="M19" s="217"/>
-      <c r="N19" s="217"/>
-      <c r="O19" s="217"/>
-      <c r="P19" s="217"/>
-      <c r="Q19" s="217"/>
-      <c r="R19" s="217"/>
-      <c r="S19" s="217"/>
-      <c r="T19" s="217"/>
-      <c r="U19" s="217"/>
-      <c r="V19" s="217"/>
-      <c r="W19" s="217"/>
-      <c r="X19" s="217"/>
-      <c r="Y19" s="217"/>
-      <c r="Z19" s="217"/>
-      <c r="AA19" s="217"/>
-      <c r="AB19" s="217"/>
-      <c r="AC19" s="217"/>
-      <c r="AD19" s="218"/>
+      <c r="M19" s="214"/>
+      <c r="N19" s="214"/>
+      <c r="O19" s="214"/>
+      <c r="P19" s="214"/>
+      <c r="Q19" s="214"/>
+      <c r="R19" s="214"/>
+      <c r="S19" s="214"/>
+      <c r="T19" s="214"/>
+      <c r="U19" s="214"/>
+      <c r="V19" s="214"/>
+      <c r="W19" s="214"/>
+      <c r="X19" s="214"/>
+      <c r="Y19" s="214"/>
+      <c r="Z19" s="214"/>
+      <c r="AA19" s="214"/>
+      <c r="AB19" s="214"/>
+      <c r="AC19" s="214"/>
+      <c r="AD19" s="215"/>
       <c r="AE19" s="2"/>
       <c r="AP19" s="5"/>
       <c r="AQ19" s="2"/>
@@ -7944,27 +7951,27 @@
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="34"/>
-      <c r="L20" s="216" t="s">
+      <c r="L20" s="213" t="s">
         <v>48</v>
       </c>
-      <c r="M20" s="217"/>
-      <c r="N20" s="217"/>
-      <c r="O20" s="217"/>
-      <c r="P20" s="217"/>
-      <c r="Q20" s="217"/>
-      <c r="R20" s="217"/>
-      <c r="S20" s="217"/>
-      <c r="T20" s="217"/>
-      <c r="U20" s="217"/>
-      <c r="V20" s="217"/>
-      <c r="W20" s="217"/>
-      <c r="X20" s="217"/>
-      <c r="Y20" s="217"/>
-      <c r="Z20" s="217"/>
-      <c r="AA20" s="217"/>
-      <c r="AB20" s="217"/>
-      <c r="AC20" s="217"/>
-      <c r="AD20" s="218"/>
+      <c r="M20" s="214"/>
+      <c r="N20" s="214"/>
+      <c r="O20" s="214"/>
+      <c r="P20" s="214"/>
+      <c r="Q20" s="214"/>
+      <c r="R20" s="214"/>
+      <c r="S20" s="214"/>
+      <c r="T20" s="214"/>
+      <c r="U20" s="214"/>
+      <c r="V20" s="214"/>
+      <c r="W20" s="214"/>
+      <c r="X20" s="214"/>
+      <c r="Y20" s="214"/>
+      <c r="Z20" s="214"/>
+      <c r="AA20" s="214"/>
+      <c r="AB20" s="214"/>
+      <c r="AC20" s="214"/>
+      <c r="AD20" s="215"/>
       <c r="AE20" s="2"/>
       <c r="AP20" s="5"/>
       <c r="AQ20" s="2"/>
@@ -7980,27 +7987,27 @@
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
       <c r="K21" s="35"/>
-      <c r="L21" s="216" t="s">
+      <c r="L21" s="213" t="s">
         <v>49</v>
       </c>
-      <c r="M21" s="217"/>
-      <c r="N21" s="217"/>
-      <c r="O21" s="217"/>
-      <c r="P21" s="217"/>
-      <c r="Q21" s="217"/>
-      <c r="R21" s="217"/>
-      <c r="S21" s="217"/>
-      <c r="T21" s="217"/>
-      <c r="U21" s="217"/>
-      <c r="V21" s="217"/>
-      <c r="W21" s="217"/>
-      <c r="X21" s="217"/>
-      <c r="Y21" s="217"/>
-      <c r="Z21" s="217"/>
-      <c r="AA21" s="217"/>
-      <c r="AB21" s="217"/>
-      <c r="AC21" s="217"/>
-      <c r="AD21" s="218"/>
+      <c r="M21" s="214"/>
+      <c r="N21" s="214"/>
+      <c r="O21" s="214"/>
+      <c r="P21" s="214"/>
+      <c r="Q21" s="214"/>
+      <c r="R21" s="214"/>
+      <c r="S21" s="214"/>
+      <c r="T21" s="214"/>
+      <c r="U21" s="214"/>
+      <c r="V21" s="214"/>
+      <c r="W21" s="214"/>
+      <c r="X21" s="214"/>
+      <c r="Y21" s="214"/>
+      <c r="Z21" s="214"/>
+      <c r="AA21" s="214"/>
+      <c r="AB21" s="214"/>
+      <c r="AC21" s="214"/>
+      <c r="AD21" s="215"/>
       <c r="AE21" s="2"/>
       <c r="AP21" s="5"/>
       <c r="AQ21" s="2"/>
@@ -8454,27 +8461,27 @@
       <c r="I40" s="53"/>
       <c r="J40" s="53"/>
       <c r="K40" s="54"/>
-      <c r="L40" s="192" t="s">
+      <c r="L40" s="207" t="s">
         <v>52</v>
       </c>
-      <c r="M40" s="193"/>
-      <c r="N40" s="193"/>
-      <c r="O40" s="193"/>
-      <c r="P40" s="193"/>
-      <c r="Q40" s="193"/>
-      <c r="R40" s="193"/>
-      <c r="S40" s="193"/>
-      <c r="T40" s="193"/>
-      <c r="U40" s="193"/>
-      <c r="V40" s="193"/>
-      <c r="W40" s="193"/>
-      <c r="X40" s="193"/>
-      <c r="Y40" s="193"/>
-      <c r="Z40" s="193"/>
-      <c r="AA40" s="193"/>
-      <c r="AB40" s="193"/>
-      <c r="AC40" s="193"/>
-      <c r="AD40" s="194"/>
+      <c r="M40" s="208"/>
+      <c r="N40" s="208"/>
+      <c r="O40" s="208"/>
+      <c r="P40" s="208"/>
+      <c r="Q40" s="208"/>
+      <c r="R40" s="208"/>
+      <c r="S40" s="208"/>
+      <c r="T40" s="208"/>
+      <c r="U40" s="208"/>
+      <c r="V40" s="208"/>
+      <c r="W40" s="208"/>
+      <c r="X40" s="208"/>
+      <c r="Y40" s="208"/>
+      <c r="Z40" s="208"/>
+      <c r="AA40" s="208"/>
+      <c r="AB40" s="208"/>
+      <c r="AC40" s="208"/>
+      <c r="AD40" s="209"/>
       <c r="AE40" s="2"/>
       <c r="AP40" s="5"/>
       <c r="AQ40" s="2"/>
@@ -8490,27 +8497,27 @@
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="13"/>
-      <c r="L41" s="216" t="s">
+      <c r="L41" s="213" t="s">
         <v>50</v>
       </c>
-      <c r="M41" s="217"/>
-      <c r="N41" s="217"/>
-      <c r="O41" s="217"/>
-      <c r="P41" s="217"/>
-      <c r="Q41" s="217"/>
-      <c r="R41" s="217"/>
-      <c r="S41" s="217"/>
-      <c r="T41" s="217"/>
-      <c r="U41" s="217"/>
-      <c r="V41" s="217"/>
-      <c r="W41" s="217"/>
-      <c r="X41" s="217"/>
-      <c r="Y41" s="217"/>
-      <c r="Z41" s="217"/>
-      <c r="AA41" s="217"/>
-      <c r="AB41" s="217"/>
-      <c r="AC41" s="217"/>
-      <c r="AD41" s="218"/>
+      <c r="M41" s="214"/>
+      <c r="N41" s="214"/>
+      <c r="O41" s="214"/>
+      <c r="P41" s="214"/>
+      <c r="Q41" s="214"/>
+      <c r="R41" s="214"/>
+      <c r="S41" s="214"/>
+      <c r="T41" s="214"/>
+      <c r="U41" s="214"/>
+      <c r="V41" s="214"/>
+      <c r="W41" s="214"/>
+      <c r="X41" s="214"/>
+      <c r="Y41" s="214"/>
+      <c r="Z41" s="214"/>
+      <c r="AA41" s="214"/>
+      <c r="AB41" s="214"/>
+      <c r="AC41" s="214"/>
+      <c r="AD41" s="215"/>
       <c r="AE41" s="2"/>
       <c r="AP41" s="5"/>
       <c r="AQ41" s="2"/>
@@ -8526,27 +8533,27 @@
       <c r="I42" s="32"/>
       <c r="J42" s="32"/>
       <c r="K42" s="33"/>
-      <c r="L42" s="216" t="s">
+      <c r="L42" s="213" t="s">
         <v>63</v>
       </c>
-      <c r="M42" s="217"/>
-      <c r="N42" s="217"/>
-      <c r="O42" s="217"/>
-      <c r="P42" s="217"/>
-      <c r="Q42" s="217"/>
-      <c r="R42" s="217"/>
-      <c r="S42" s="217"/>
-      <c r="T42" s="217"/>
-      <c r="U42" s="217"/>
-      <c r="V42" s="217"/>
-      <c r="W42" s="217"/>
-      <c r="X42" s="217"/>
-      <c r="Y42" s="217"/>
-      <c r="Z42" s="217"/>
-      <c r="AA42" s="217"/>
-      <c r="AB42" s="217"/>
-      <c r="AC42" s="217"/>
-      <c r="AD42" s="218"/>
+      <c r="M42" s="214"/>
+      <c r="N42" s="214"/>
+      <c r="O42" s="214"/>
+      <c r="P42" s="214"/>
+      <c r="Q42" s="214"/>
+      <c r="R42" s="214"/>
+      <c r="S42" s="214"/>
+      <c r="T42" s="214"/>
+      <c r="U42" s="214"/>
+      <c r="V42" s="214"/>
+      <c r="W42" s="214"/>
+      <c r="X42" s="214"/>
+      <c r="Y42" s="214"/>
+      <c r="Z42" s="214"/>
+      <c r="AA42" s="214"/>
+      <c r="AB42" s="214"/>
+      <c r="AC42" s="214"/>
+      <c r="AD42" s="215"/>
       <c r="AE42" s="2"/>
       <c r="AP42" s="5"/>
       <c r="AQ42" s="2"/>
@@ -8562,27 +8569,27 @@
       <c r="I43" s="32"/>
       <c r="J43" s="32"/>
       <c r="K43" s="33"/>
-      <c r="L43" s="216" t="s">
+      <c r="L43" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="M43" s="217"/>
-      <c r="N43" s="217"/>
-      <c r="O43" s="217"/>
-      <c r="P43" s="217"/>
-      <c r="Q43" s="217"/>
-      <c r="R43" s="217"/>
-      <c r="S43" s="217"/>
-      <c r="T43" s="217"/>
-      <c r="U43" s="217"/>
-      <c r="V43" s="217"/>
-      <c r="W43" s="217"/>
-      <c r="X43" s="217"/>
-      <c r="Y43" s="217"/>
-      <c r="Z43" s="217"/>
-      <c r="AA43" s="217"/>
-      <c r="AB43" s="217"/>
-      <c r="AC43" s="217"/>
-      <c r="AD43" s="218"/>
+      <c r="M43" s="214"/>
+      <c r="N43" s="214"/>
+      <c r="O43" s="214"/>
+      <c r="P43" s="214"/>
+      <c r="Q43" s="214"/>
+      <c r="R43" s="214"/>
+      <c r="S43" s="214"/>
+      <c r="T43" s="214"/>
+      <c r="U43" s="214"/>
+      <c r="V43" s="214"/>
+      <c r="W43" s="214"/>
+      <c r="X43" s="214"/>
+      <c r="Y43" s="214"/>
+      <c r="Z43" s="214"/>
+      <c r="AA43" s="214"/>
+      <c r="AB43" s="214"/>
+      <c r="AC43" s="214"/>
+      <c r="AD43" s="215"/>
       <c r="AE43" s="2"/>
       <c r="AP43" s="5"/>
       <c r="AQ43" s="2"/>
@@ -8598,27 +8605,27 @@
       <c r="I44" s="32"/>
       <c r="J44" s="32"/>
       <c r="K44" s="33"/>
-      <c r="L44" s="216" t="s">
+      <c r="L44" s="213" t="s">
         <v>64</v>
       </c>
-      <c r="M44" s="217"/>
-      <c r="N44" s="217"/>
-      <c r="O44" s="217"/>
-      <c r="P44" s="217"/>
-      <c r="Q44" s="217"/>
-      <c r="R44" s="217"/>
-      <c r="S44" s="217"/>
-      <c r="T44" s="217"/>
-      <c r="U44" s="217"/>
-      <c r="V44" s="217"/>
-      <c r="W44" s="217"/>
-      <c r="X44" s="217"/>
-      <c r="Y44" s="217"/>
-      <c r="Z44" s="217"/>
-      <c r="AA44" s="217"/>
-      <c r="AB44" s="217"/>
-      <c r="AC44" s="217"/>
-      <c r="AD44" s="218"/>
+      <c r="M44" s="214"/>
+      <c r="N44" s="214"/>
+      <c r="O44" s="214"/>
+      <c r="P44" s="214"/>
+      <c r="Q44" s="214"/>
+      <c r="R44" s="214"/>
+      <c r="S44" s="214"/>
+      <c r="T44" s="214"/>
+      <c r="U44" s="214"/>
+      <c r="V44" s="214"/>
+      <c r="W44" s="214"/>
+      <c r="X44" s="214"/>
+      <c r="Y44" s="214"/>
+      <c r="Z44" s="214"/>
+      <c r="AA44" s="214"/>
+      <c r="AB44" s="214"/>
+      <c r="AC44" s="214"/>
+      <c r="AD44" s="215"/>
       <c r="AE44" s="2"/>
       <c r="AP44" s="5"/>
       <c r="AQ44" s="2"/>
@@ -8634,27 +8641,27 @@
       <c r="I45" s="32"/>
       <c r="J45" s="32"/>
       <c r="K45" s="33"/>
-      <c r="L45" s="216" t="s">
+      <c r="L45" s="213" t="s">
         <v>61</v>
       </c>
-      <c r="M45" s="217"/>
-      <c r="N45" s="217"/>
-      <c r="O45" s="217"/>
-      <c r="P45" s="217"/>
-      <c r="Q45" s="217"/>
-      <c r="R45" s="217"/>
-      <c r="S45" s="217"/>
-      <c r="T45" s="217"/>
-      <c r="U45" s="217"/>
-      <c r="V45" s="217"/>
-      <c r="W45" s="217"/>
-      <c r="X45" s="217"/>
-      <c r="Y45" s="217"/>
-      <c r="Z45" s="217"/>
-      <c r="AA45" s="217"/>
-      <c r="AB45" s="217"/>
-      <c r="AC45" s="217"/>
-      <c r="AD45" s="218"/>
+      <c r="M45" s="214"/>
+      <c r="N45" s="214"/>
+      <c r="O45" s="214"/>
+      <c r="P45" s="214"/>
+      <c r="Q45" s="214"/>
+      <c r="R45" s="214"/>
+      <c r="S45" s="214"/>
+      <c r="T45" s="214"/>
+      <c r="U45" s="214"/>
+      <c r="V45" s="214"/>
+      <c r="W45" s="214"/>
+      <c r="X45" s="214"/>
+      <c r="Y45" s="214"/>
+      <c r="Z45" s="214"/>
+      <c r="AA45" s="214"/>
+      <c r="AB45" s="214"/>
+      <c r="AC45" s="214"/>
+      <c r="AD45" s="215"/>
       <c r="AE45" s="2"/>
       <c r="AP45" s="5"/>
       <c r="AQ45" s="2"/>
@@ -8729,27 +8736,27 @@
       <c r="I48" s="53"/>
       <c r="J48" s="53"/>
       <c r="K48" s="54"/>
-      <c r="L48" s="192" t="s">
+      <c r="L48" s="207" t="s">
         <v>52</v>
       </c>
-      <c r="M48" s="193"/>
-      <c r="N48" s="193"/>
-      <c r="O48" s="193"/>
-      <c r="P48" s="193"/>
-      <c r="Q48" s="193"/>
-      <c r="R48" s="193"/>
-      <c r="S48" s="193"/>
-      <c r="T48" s="193"/>
-      <c r="U48" s="193"/>
-      <c r="V48" s="193"/>
-      <c r="W48" s="193"/>
-      <c r="X48" s="193"/>
-      <c r="Y48" s="193"/>
-      <c r="Z48" s="193"/>
-      <c r="AA48" s="193"/>
-      <c r="AB48" s="193"/>
-      <c r="AC48" s="193"/>
-      <c r="AD48" s="194"/>
+      <c r="M48" s="208"/>
+      <c r="N48" s="208"/>
+      <c r="O48" s="208"/>
+      <c r="P48" s="208"/>
+      <c r="Q48" s="208"/>
+      <c r="R48" s="208"/>
+      <c r="S48" s="208"/>
+      <c r="T48" s="208"/>
+      <c r="U48" s="208"/>
+      <c r="V48" s="208"/>
+      <c r="W48" s="208"/>
+      <c r="X48" s="208"/>
+      <c r="Y48" s="208"/>
+      <c r="Z48" s="208"/>
+      <c r="AA48" s="208"/>
+      <c r="AB48" s="208"/>
+      <c r="AC48" s="208"/>
+      <c r="AD48" s="209"/>
       <c r="AP48" s="5"/>
       <c r="AQ48" s="2"/>
     </row>
@@ -8763,27 +8770,27 @@
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="13"/>
-      <c r="L49" s="216" t="s">
+      <c r="L49" s="213" t="s">
         <v>50</v>
       </c>
-      <c r="M49" s="217"/>
-      <c r="N49" s="217"/>
-      <c r="O49" s="217"/>
-      <c r="P49" s="217"/>
-      <c r="Q49" s="217"/>
-      <c r="R49" s="217"/>
-      <c r="S49" s="217"/>
-      <c r="T49" s="217"/>
-      <c r="U49" s="217"/>
-      <c r="V49" s="217"/>
-      <c r="W49" s="217"/>
-      <c r="X49" s="217"/>
-      <c r="Y49" s="217"/>
-      <c r="Z49" s="217"/>
-      <c r="AA49" s="217"/>
-      <c r="AB49" s="217"/>
-      <c r="AC49" s="217"/>
-      <c r="AD49" s="218"/>
+      <c r="M49" s="214"/>
+      <c r="N49" s="214"/>
+      <c r="O49" s="214"/>
+      <c r="P49" s="214"/>
+      <c r="Q49" s="214"/>
+      <c r="R49" s="214"/>
+      <c r="S49" s="214"/>
+      <c r="T49" s="214"/>
+      <c r="U49" s="214"/>
+      <c r="V49" s="214"/>
+      <c r="W49" s="214"/>
+      <c r="X49" s="214"/>
+      <c r="Y49" s="214"/>
+      <c r="Z49" s="214"/>
+      <c r="AA49" s="214"/>
+      <c r="AB49" s="214"/>
+      <c r="AC49" s="214"/>
+      <c r="AD49" s="215"/>
       <c r="AP49" s="5"/>
       <c r="AQ49" s="2"/>
     </row>
@@ -8797,27 +8804,27 @@
       <c r="I50" s="32"/>
       <c r="J50" s="32"/>
       <c r="K50" s="33"/>
-      <c r="L50" s="216" t="s">
+      <c r="L50" s="213" t="s">
         <v>190</v>
       </c>
-      <c r="M50" s="217"/>
-      <c r="N50" s="217"/>
-      <c r="O50" s="217"/>
-      <c r="P50" s="217"/>
-      <c r="Q50" s="217"/>
-      <c r="R50" s="217"/>
-      <c r="S50" s="217"/>
-      <c r="T50" s="217"/>
-      <c r="U50" s="217"/>
-      <c r="V50" s="217"/>
-      <c r="W50" s="217"/>
-      <c r="X50" s="217"/>
-      <c r="Y50" s="217"/>
-      <c r="Z50" s="217"/>
-      <c r="AA50" s="217"/>
-      <c r="AB50" s="217"/>
-      <c r="AC50" s="217"/>
-      <c r="AD50" s="218"/>
+      <c r="M50" s="214"/>
+      <c r="N50" s="214"/>
+      <c r="O50" s="214"/>
+      <c r="P50" s="214"/>
+      <c r="Q50" s="214"/>
+      <c r="R50" s="214"/>
+      <c r="S50" s="214"/>
+      <c r="T50" s="214"/>
+      <c r="U50" s="214"/>
+      <c r="V50" s="214"/>
+      <c r="W50" s="214"/>
+      <c r="X50" s="214"/>
+      <c r="Y50" s="214"/>
+      <c r="Z50" s="214"/>
+      <c r="AA50" s="214"/>
+      <c r="AB50" s="214"/>
+      <c r="AC50" s="214"/>
+      <c r="AD50" s="215"/>
       <c r="AP50" s="5"/>
       <c r="AQ50" s="2"/>
     </row>
@@ -11420,30 +11427,30 @@
       <c r="P125" s="53"/>
       <c r="Q125" s="53"/>
       <c r="R125" s="54"/>
-      <c r="S125" s="192" t="s">
+      <c r="S125" s="207" t="s">
         <v>6</v>
       </c>
-      <c r="T125" s="193"/>
-      <c r="U125" s="193"/>
-      <c r="V125" s="193"/>
-      <c r="W125" s="193"/>
-      <c r="X125" s="194"/>
-      <c r="Y125" s="192" t="s">
+      <c r="T125" s="208"/>
+      <c r="U125" s="208"/>
+      <c r="V125" s="208"/>
+      <c r="W125" s="208"/>
+      <c r="X125" s="209"/>
+      <c r="Y125" s="207" t="s">
         <v>7</v>
       </c>
-      <c r="Z125" s="193"/>
-      <c r="AA125" s="193"/>
-      <c r="AB125" s="193"/>
-      <c r="AC125" s="193"/>
-      <c r="AD125" s="194"/>
-      <c r="AE125" s="192" t="s">
+      <c r="Z125" s="208"/>
+      <c r="AA125" s="208"/>
+      <c r="AB125" s="208"/>
+      <c r="AC125" s="208"/>
+      <c r="AD125" s="209"/>
+      <c r="AE125" s="207" t="s">
         <v>26</v>
       </c>
-      <c r="AF125" s="193"/>
-      <c r="AG125" s="193"/>
-      <c r="AH125" s="193"/>
-      <c r="AI125" s="193"/>
-      <c r="AJ125" s="194"/>
+      <c r="AF125" s="208"/>
+      <c r="AG125" s="208"/>
+      <c r="AH125" s="208"/>
+      <c r="AI125" s="208"/>
+      <c r="AJ125" s="209"/>
       <c r="AP125" s="5"/>
       <c r="AQ125" s="2"/>
     </row>
@@ -11465,30 +11472,30 @@
       <c r="P126" s="98"/>
       <c r="Q126" s="98"/>
       <c r="R126" s="102"/>
-      <c r="S126" s="216" t="s">
+      <c r="S126" s="213" t="s">
         <v>16</v>
       </c>
-      <c r="T126" s="217"/>
-      <c r="U126" s="217"/>
-      <c r="V126" s="217"/>
-      <c r="W126" s="217"/>
-      <c r="X126" s="218"/>
-      <c r="Y126" s="216" t="s">
+      <c r="T126" s="214"/>
+      <c r="U126" s="214"/>
+      <c r="V126" s="214"/>
+      <c r="W126" s="214"/>
+      <c r="X126" s="215"/>
+      <c r="Y126" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="Z126" s="217"/>
-      <c r="AA126" s="217"/>
-      <c r="AB126" s="217"/>
-      <c r="AC126" s="217"/>
-      <c r="AD126" s="218"/>
-      <c r="AE126" s="216" t="s">
+      <c r="Z126" s="214"/>
+      <c r="AA126" s="214"/>
+      <c r="AB126" s="214"/>
+      <c r="AC126" s="214"/>
+      <c r="AD126" s="215"/>
+      <c r="AE126" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="AF126" s="217"/>
-      <c r="AG126" s="217"/>
-      <c r="AH126" s="217"/>
-      <c r="AI126" s="217"/>
-      <c r="AJ126" s="218"/>
+      <c r="AF126" s="214"/>
+      <c r="AG126" s="214"/>
+      <c r="AH126" s="214"/>
+      <c r="AI126" s="214"/>
+      <c r="AJ126" s="215"/>
       <c r="AP126" s="5"/>
       <c r="AQ126" s="2"/>
     </row>
@@ -11549,30 +11556,30 @@
       <c r="P128" s="130"/>
       <c r="Q128" s="130"/>
       <c r="R128" s="131"/>
-      <c r="S128" s="195" t="s">
+      <c r="S128" s="249" t="s">
         <v>8</v>
       </c>
-      <c r="T128" s="196"/>
-      <c r="U128" s="196"/>
-      <c r="V128" s="196"/>
-      <c r="W128" s="196"/>
-      <c r="X128" s="197"/>
-      <c r="Y128" s="195" t="s">
+      <c r="T128" s="250"/>
+      <c r="U128" s="250"/>
+      <c r="V128" s="250"/>
+      <c r="W128" s="250"/>
+      <c r="X128" s="251"/>
+      <c r="Y128" s="249" t="s">
         <v>14</v>
       </c>
-      <c r="Z128" s="196"/>
-      <c r="AA128" s="196"/>
-      <c r="AB128" s="196"/>
-      <c r="AC128" s="196"/>
-      <c r="AD128" s="197"/>
-      <c r="AE128" s="195" t="s">
+      <c r="Z128" s="250"/>
+      <c r="AA128" s="250"/>
+      <c r="AB128" s="250"/>
+      <c r="AC128" s="250"/>
+      <c r="AD128" s="251"/>
+      <c r="AE128" s="249" t="s">
         <v>15</v>
       </c>
-      <c r="AF128" s="196"/>
-      <c r="AG128" s="196"/>
-      <c r="AH128" s="196"/>
-      <c r="AI128" s="196"/>
-      <c r="AJ128" s="197"/>
+      <c r="AF128" s="250"/>
+      <c r="AG128" s="250"/>
+      <c r="AH128" s="250"/>
+      <c r="AI128" s="250"/>
+      <c r="AJ128" s="251"/>
       <c r="AP128" s="5"/>
       <c r="AQ128" s="2"/>
     </row>
@@ -11594,30 +11601,30 @@
       <c r="P129" s="127"/>
       <c r="Q129" s="127"/>
       <c r="R129" s="132"/>
-      <c r="S129" s="219" t="s">
+      <c r="S129" s="246" t="s">
         <v>8</v>
       </c>
-      <c r="T129" s="219"/>
-      <c r="U129" s="219"/>
-      <c r="V129" s="219"/>
-      <c r="W129" s="219"/>
-      <c r="X129" s="219"/>
-      <c r="Y129" s="219" t="s">
+      <c r="T129" s="247"/>
+      <c r="U129" s="247"/>
+      <c r="V129" s="247"/>
+      <c r="W129" s="247"/>
+      <c r="X129" s="248"/>
+      <c r="Y129" s="246" t="s">
         <v>14</v>
       </c>
-      <c r="Z129" s="219"/>
-      <c r="AA129" s="219"/>
-      <c r="AB129" s="219"/>
-      <c r="AC129" s="219"/>
-      <c r="AD129" s="219"/>
-      <c r="AE129" s="219" t="s">
+      <c r="Z129" s="247"/>
+      <c r="AA129" s="247"/>
+      <c r="AB129" s="247"/>
+      <c r="AC129" s="247"/>
+      <c r="AD129" s="248"/>
+      <c r="AE129" s="246" t="s">
         <v>15</v>
       </c>
-      <c r="AF129" s="219"/>
-      <c r="AG129" s="219"/>
-      <c r="AH129" s="219"/>
-      <c r="AI129" s="219"/>
-      <c r="AJ129" s="219"/>
+      <c r="AF129" s="247"/>
+      <c r="AG129" s="247"/>
+      <c r="AH129" s="247"/>
+      <c r="AI129" s="247"/>
+      <c r="AJ129" s="248"/>
       <c r="AP129" s="5"/>
       <c r="AQ129" s="2"/>
     </row>
@@ -11641,30 +11648,30 @@
       <c r="P130" s="75"/>
       <c r="Q130" s="75"/>
       <c r="R130" s="133"/>
-      <c r="S130" s="198" t="s">
+      <c r="S130" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T130" s="199"/>
-      <c r="U130" s="199"/>
-      <c r="V130" s="199"/>
-      <c r="W130" s="199"/>
-      <c r="X130" s="200"/>
-      <c r="Y130" s="198" t="s">
+      <c r="T130" s="190"/>
+      <c r="U130" s="190"/>
+      <c r="V130" s="190"/>
+      <c r="W130" s="190"/>
+      <c r="X130" s="191"/>
+      <c r="Y130" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="Z130" s="199"/>
-      <c r="AA130" s="199"/>
-      <c r="AB130" s="199"/>
-      <c r="AC130" s="199"/>
-      <c r="AD130" s="200"/>
-      <c r="AE130" s="198" t="s">
+      <c r="Z130" s="190"/>
+      <c r="AA130" s="190"/>
+      <c r="AB130" s="190"/>
+      <c r="AC130" s="190"/>
+      <c r="AD130" s="191"/>
+      <c r="AE130" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="AF130" s="199"/>
-      <c r="AG130" s="199"/>
-      <c r="AH130" s="199"/>
-      <c r="AI130" s="199"/>
-      <c r="AJ130" s="200"/>
+      <c r="AF130" s="190"/>
+      <c r="AG130" s="190"/>
+      <c r="AH130" s="190"/>
+      <c r="AI130" s="190"/>
+      <c r="AJ130" s="191"/>
       <c r="AP130" s="5"/>
       <c r="AQ130" s="2"/>
     </row>
@@ -11682,30 +11689,30 @@
       <c r="P131" s="75"/>
       <c r="Q131" s="75"/>
       <c r="R131" s="133"/>
-      <c r="S131" s="198" t="s">
+      <c r="S131" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T131" s="199"/>
-      <c r="U131" s="199"/>
-      <c r="V131" s="199"/>
-      <c r="W131" s="199"/>
-      <c r="X131" s="200"/>
-      <c r="Y131" s="198" t="s">
+      <c r="T131" s="190"/>
+      <c r="U131" s="190"/>
+      <c r="V131" s="190"/>
+      <c r="W131" s="190"/>
+      <c r="X131" s="191"/>
+      <c r="Y131" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z131" s="199"/>
-      <c r="AA131" s="199"/>
-      <c r="AB131" s="199"/>
-      <c r="AC131" s="199"/>
-      <c r="AD131" s="200"/>
-      <c r="AE131" s="198" t="s">
+      <c r="Z131" s="190"/>
+      <c r="AA131" s="190"/>
+      <c r="AB131" s="190"/>
+      <c r="AC131" s="190"/>
+      <c r="AD131" s="191"/>
+      <c r="AE131" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="AF131" s="199"/>
-      <c r="AG131" s="199"/>
-      <c r="AH131" s="199"/>
-      <c r="AI131" s="199"/>
-      <c r="AJ131" s="200"/>
+      <c r="AF131" s="190"/>
+      <c r="AG131" s="190"/>
+      <c r="AH131" s="190"/>
+      <c r="AI131" s="190"/>
+      <c r="AJ131" s="191"/>
       <c r="AP131" s="5"/>
       <c r="AQ131" s="2"/>
     </row>
@@ -11727,30 +11734,30 @@
       <c r="P132" s="75"/>
       <c r="Q132" s="75"/>
       <c r="R132" s="133"/>
-      <c r="S132" s="198" t="s">
+      <c r="S132" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T132" s="199"/>
-      <c r="U132" s="199"/>
-      <c r="V132" s="199"/>
-      <c r="W132" s="199"/>
-      <c r="X132" s="200"/>
-      <c r="Y132" s="198" t="s">
+      <c r="T132" s="190"/>
+      <c r="U132" s="190"/>
+      <c r="V132" s="190"/>
+      <c r="W132" s="190"/>
+      <c r="X132" s="191"/>
+      <c r="Y132" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z132" s="199"/>
-      <c r="AA132" s="199"/>
-      <c r="AB132" s="199"/>
-      <c r="AC132" s="199"/>
-      <c r="AD132" s="200"/>
-      <c r="AE132" s="198" t="s">
+      <c r="Z132" s="190"/>
+      <c r="AA132" s="190"/>
+      <c r="AB132" s="190"/>
+      <c r="AC132" s="190"/>
+      <c r="AD132" s="191"/>
+      <c r="AE132" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="AF132" s="199"/>
-      <c r="AG132" s="199"/>
-      <c r="AH132" s="199"/>
-      <c r="AI132" s="199"/>
-      <c r="AJ132" s="200"/>
+      <c r="AF132" s="190"/>
+      <c r="AG132" s="190"/>
+      <c r="AH132" s="190"/>
+      <c r="AI132" s="190"/>
+      <c r="AJ132" s="191"/>
       <c r="AP132" s="5"/>
       <c r="AQ132" s="2"/>
     </row>
@@ -11772,30 +11779,30 @@
       <c r="P133" s="75"/>
       <c r="Q133" s="75"/>
       <c r="R133" s="76"/>
-      <c r="S133" s="207" t="s">
+      <c r="S133" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="T133" s="208"/>
-      <c r="U133" s="208"/>
-      <c r="V133" s="208"/>
-      <c r="W133" s="208"/>
-      <c r="X133" s="209"/>
-      <c r="Y133" s="207" t="s">
+      <c r="T133" s="187"/>
+      <c r="U133" s="187"/>
+      <c r="V133" s="187"/>
+      <c r="W133" s="187"/>
+      <c r="X133" s="188"/>
+      <c r="Y133" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="Z133" s="208"/>
-      <c r="AA133" s="208"/>
-      <c r="AB133" s="208"/>
-      <c r="AC133" s="208"/>
-      <c r="AD133" s="209"/>
-      <c r="AE133" s="207" t="s">
+      <c r="Z133" s="187"/>
+      <c r="AA133" s="187"/>
+      <c r="AB133" s="187"/>
+      <c r="AC133" s="187"/>
+      <c r="AD133" s="188"/>
+      <c r="AE133" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="AF133" s="208"/>
-      <c r="AG133" s="208"/>
-      <c r="AH133" s="208"/>
-      <c r="AI133" s="208"/>
-      <c r="AJ133" s="209"/>
+      <c r="AF133" s="187"/>
+      <c r="AG133" s="187"/>
+      <c r="AH133" s="187"/>
+      <c r="AI133" s="187"/>
+      <c r="AJ133" s="188"/>
       <c r="AP133" s="5"/>
       <c r="AQ133" s="2"/>
     </row>
@@ -11819,30 +11826,30 @@
       <c r="P134" s="75"/>
       <c r="Q134" s="75"/>
       <c r="R134" s="76"/>
-      <c r="S134" s="207" t="s">
+      <c r="S134" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T134" s="208"/>
-      <c r="U134" s="208"/>
-      <c r="V134" s="208"/>
-      <c r="W134" s="208"/>
-      <c r="X134" s="209"/>
-      <c r="Y134" s="207" t="s">
+      <c r="T134" s="187"/>
+      <c r="U134" s="187"/>
+      <c r="V134" s="187"/>
+      <c r="W134" s="187"/>
+      <c r="X134" s="188"/>
+      <c r="Y134" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="Z134" s="208"/>
-      <c r="AA134" s="208"/>
-      <c r="AB134" s="208"/>
-      <c r="AC134" s="208"/>
-      <c r="AD134" s="209"/>
-      <c r="AE134" s="207" t="s">
+      <c r="Z134" s="187"/>
+      <c r="AA134" s="187"/>
+      <c r="AB134" s="187"/>
+      <c r="AC134" s="187"/>
+      <c r="AD134" s="188"/>
+      <c r="AE134" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="AF134" s="208"/>
-      <c r="AG134" s="208"/>
-      <c r="AH134" s="208"/>
-      <c r="AI134" s="208"/>
-      <c r="AJ134" s="209"/>
+      <c r="AF134" s="187"/>
+      <c r="AG134" s="187"/>
+      <c r="AH134" s="187"/>
+      <c r="AI134" s="187"/>
+      <c r="AJ134" s="188"/>
       <c r="AP134" s="5"/>
       <c r="AQ134" s="2"/>
     </row>
@@ -11860,30 +11867,30 @@
       <c r="P135" s="75"/>
       <c r="Q135" s="75"/>
       <c r="R135" s="76"/>
-      <c r="S135" s="207" t="s">
+      <c r="S135" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T135" s="208"/>
-      <c r="U135" s="208"/>
-      <c r="V135" s="208"/>
-      <c r="W135" s="208"/>
-      <c r="X135" s="209"/>
-      <c r="Y135" s="207" t="s">
+      <c r="T135" s="187"/>
+      <c r="U135" s="187"/>
+      <c r="V135" s="187"/>
+      <c r="W135" s="187"/>
+      <c r="X135" s="188"/>
+      <c r="Y135" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z135" s="208"/>
-      <c r="AA135" s="208"/>
-      <c r="AB135" s="208"/>
-      <c r="AC135" s="208"/>
-      <c r="AD135" s="209"/>
-      <c r="AE135" s="207" t="s">
+      <c r="Z135" s="187"/>
+      <c r="AA135" s="187"/>
+      <c r="AB135" s="187"/>
+      <c r="AC135" s="187"/>
+      <c r="AD135" s="188"/>
+      <c r="AE135" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="AF135" s="208"/>
-      <c r="AG135" s="208"/>
-      <c r="AH135" s="208"/>
-      <c r="AI135" s="208"/>
-      <c r="AJ135" s="209"/>
+      <c r="AF135" s="187"/>
+      <c r="AG135" s="187"/>
+      <c r="AH135" s="187"/>
+      <c r="AI135" s="187"/>
+      <c r="AJ135" s="188"/>
       <c r="AP135" s="5"/>
       <c r="AQ135" s="2"/>
     </row>
@@ -11905,30 +11912,30 @@
       <c r="P136" s="75"/>
       <c r="Q136" s="75"/>
       <c r="R136" s="76"/>
-      <c r="S136" s="207" t="s">
+      <c r="S136" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T136" s="208"/>
-      <c r="U136" s="208"/>
-      <c r="V136" s="208"/>
-      <c r="W136" s="208"/>
-      <c r="X136" s="209"/>
-      <c r="Y136" s="207" t="s">
+      <c r="T136" s="187"/>
+      <c r="U136" s="187"/>
+      <c r="V136" s="187"/>
+      <c r="W136" s="187"/>
+      <c r="X136" s="188"/>
+      <c r="Y136" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z136" s="208"/>
-      <c r="AA136" s="208"/>
-      <c r="AB136" s="208"/>
-      <c r="AC136" s="208"/>
-      <c r="AD136" s="209"/>
-      <c r="AE136" s="207" t="s">
+      <c r="Z136" s="187"/>
+      <c r="AA136" s="187"/>
+      <c r="AB136" s="187"/>
+      <c r="AC136" s="187"/>
+      <c r="AD136" s="188"/>
+      <c r="AE136" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="AF136" s="208"/>
-      <c r="AG136" s="208"/>
-      <c r="AH136" s="208"/>
-      <c r="AI136" s="208"/>
-      <c r="AJ136" s="209"/>
+      <c r="AF136" s="187"/>
+      <c r="AG136" s="187"/>
+      <c r="AH136" s="187"/>
+      <c r="AI136" s="187"/>
+      <c r="AJ136" s="188"/>
       <c r="AP136" s="5"/>
       <c r="AQ136" s="2"/>
     </row>
@@ -11950,30 +11957,30 @@
       <c r="P137" s="75"/>
       <c r="Q137" s="75"/>
       <c r="R137" s="76"/>
-      <c r="S137" s="204" t="s">
+      <c r="S137" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="T137" s="205"/>
-      <c r="U137" s="205"/>
-      <c r="V137" s="205"/>
-      <c r="W137" s="205"/>
-      <c r="X137" s="206"/>
-      <c r="Y137" s="204" t="s">
+      <c r="T137" s="184"/>
+      <c r="U137" s="184"/>
+      <c r="V137" s="184"/>
+      <c r="W137" s="184"/>
+      <c r="X137" s="185"/>
+      <c r="Y137" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="Z137" s="205"/>
-      <c r="AA137" s="205"/>
-      <c r="AB137" s="205"/>
-      <c r="AC137" s="205"/>
-      <c r="AD137" s="206"/>
-      <c r="AE137" s="207" t="s">
+      <c r="Z137" s="184"/>
+      <c r="AA137" s="184"/>
+      <c r="AB137" s="184"/>
+      <c r="AC137" s="184"/>
+      <c r="AD137" s="185"/>
+      <c r="AE137" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="AF137" s="208"/>
-      <c r="AG137" s="208"/>
-      <c r="AH137" s="208"/>
-      <c r="AI137" s="208"/>
-      <c r="AJ137" s="209"/>
+      <c r="AF137" s="187"/>
+      <c r="AG137" s="187"/>
+      <c r="AH137" s="187"/>
+      <c r="AI137" s="187"/>
+      <c r="AJ137" s="188"/>
       <c r="AP137" s="5"/>
       <c r="AQ137" s="2"/>
     </row>
@@ -11997,30 +12004,30 @@
       <c r="P138" s="75"/>
       <c r="Q138" s="75"/>
       <c r="R138" s="76"/>
-      <c r="S138" s="207" t="s">
+      <c r="S138" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T138" s="208"/>
-      <c r="U138" s="208"/>
-      <c r="V138" s="208"/>
-      <c r="W138" s="208"/>
-      <c r="X138" s="209"/>
-      <c r="Y138" s="207" t="s">
+      <c r="T138" s="187"/>
+      <c r="U138" s="187"/>
+      <c r="V138" s="187"/>
+      <c r="W138" s="187"/>
+      <c r="X138" s="188"/>
+      <c r="Y138" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="Z138" s="208"/>
-      <c r="AA138" s="208"/>
-      <c r="AB138" s="208"/>
-      <c r="AC138" s="208"/>
-      <c r="AD138" s="209"/>
-      <c r="AE138" s="207" t="s">
+      <c r="Z138" s="187"/>
+      <c r="AA138" s="187"/>
+      <c r="AB138" s="187"/>
+      <c r="AC138" s="187"/>
+      <c r="AD138" s="188"/>
+      <c r="AE138" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="AF138" s="208"/>
-      <c r="AG138" s="208"/>
-      <c r="AH138" s="208"/>
-      <c r="AI138" s="208"/>
-      <c r="AJ138" s="209"/>
+      <c r="AF138" s="187"/>
+      <c r="AG138" s="187"/>
+      <c r="AH138" s="187"/>
+      <c r="AI138" s="187"/>
+      <c r="AJ138" s="188"/>
       <c r="AP138" s="5"/>
       <c r="AQ138" s="2"/>
     </row>
@@ -12038,30 +12045,30 @@
       <c r="P139" s="75"/>
       <c r="Q139" s="75"/>
       <c r="R139" s="76"/>
-      <c r="S139" s="207" t="s">
+      <c r="S139" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T139" s="208"/>
-      <c r="U139" s="208"/>
-      <c r="V139" s="208"/>
-      <c r="W139" s="208"/>
-      <c r="X139" s="209"/>
-      <c r="Y139" s="207" t="s">
+      <c r="T139" s="187"/>
+      <c r="U139" s="187"/>
+      <c r="V139" s="187"/>
+      <c r="W139" s="187"/>
+      <c r="X139" s="188"/>
+      <c r="Y139" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z139" s="208"/>
-      <c r="AA139" s="208"/>
-      <c r="AB139" s="208"/>
-      <c r="AC139" s="208"/>
-      <c r="AD139" s="209"/>
-      <c r="AE139" s="207" t="s">
+      <c r="Z139" s="187"/>
+      <c r="AA139" s="187"/>
+      <c r="AB139" s="187"/>
+      <c r="AC139" s="187"/>
+      <c r="AD139" s="188"/>
+      <c r="AE139" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="AF139" s="208"/>
-      <c r="AG139" s="208"/>
-      <c r="AH139" s="208"/>
-      <c r="AI139" s="208"/>
-      <c r="AJ139" s="209"/>
+      <c r="AF139" s="187"/>
+      <c r="AG139" s="187"/>
+      <c r="AH139" s="187"/>
+      <c r="AI139" s="187"/>
+      <c r="AJ139" s="188"/>
       <c r="AP139" s="5"/>
       <c r="AQ139" s="2"/>
     </row>
@@ -12083,30 +12090,30 @@
       <c r="P140" s="75"/>
       <c r="Q140" s="75"/>
       <c r="R140" s="76"/>
-      <c r="S140" s="207" t="s">
+      <c r="S140" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T140" s="208"/>
-      <c r="U140" s="208"/>
-      <c r="V140" s="208"/>
-      <c r="W140" s="208"/>
-      <c r="X140" s="209"/>
-      <c r="Y140" s="207" t="s">
+      <c r="T140" s="187"/>
+      <c r="U140" s="187"/>
+      <c r="V140" s="187"/>
+      <c r="W140" s="187"/>
+      <c r="X140" s="188"/>
+      <c r="Y140" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z140" s="208"/>
-      <c r="AA140" s="208"/>
-      <c r="AB140" s="208"/>
-      <c r="AC140" s="208"/>
-      <c r="AD140" s="209"/>
-      <c r="AE140" s="207" t="s">
+      <c r="Z140" s="187"/>
+      <c r="AA140" s="187"/>
+      <c r="AB140" s="187"/>
+      <c r="AC140" s="187"/>
+      <c r="AD140" s="188"/>
+      <c r="AE140" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="AF140" s="208"/>
-      <c r="AG140" s="208"/>
-      <c r="AH140" s="208"/>
-      <c r="AI140" s="208"/>
-      <c r="AJ140" s="209"/>
+      <c r="AF140" s="187"/>
+      <c r="AG140" s="187"/>
+      <c r="AH140" s="187"/>
+      <c r="AI140" s="187"/>
+      <c r="AJ140" s="188"/>
       <c r="AP140" s="5"/>
       <c r="AQ140" s="2"/>
     </row>
@@ -12128,30 +12135,30 @@
       <c r="P141" s="75"/>
       <c r="Q141" s="75"/>
       <c r="R141" s="76"/>
-      <c r="S141" s="207" t="s">
+      <c r="S141" s="186" t="s">
         <v>39</v>
       </c>
-      <c r="T141" s="208"/>
-      <c r="U141" s="208"/>
-      <c r="V141" s="208"/>
-      <c r="W141" s="208"/>
-      <c r="X141" s="209"/>
-      <c r="Y141" s="207" t="s">
+      <c r="T141" s="187"/>
+      <c r="U141" s="187"/>
+      <c r="V141" s="187"/>
+      <c r="W141" s="187"/>
+      <c r="X141" s="188"/>
+      <c r="Y141" s="186" t="s">
         <v>218</v>
       </c>
-      <c r="Z141" s="208"/>
-      <c r="AA141" s="208"/>
-      <c r="AB141" s="208"/>
-      <c r="AC141" s="208"/>
-      <c r="AD141" s="209"/>
-      <c r="AE141" s="207" t="s">
+      <c r="Z141" s="187"/>
+      <c r="AA141" s="187"/>
+      <c r="AB141" s="187"/>
+      <c r="AC141" s="187"/>
+      <c r="AD141" s="188"/>
+      <c r="AE141" s="186" t="s">
         <v>218</v>
       </c>
-      <c r="AF141" s="208"/>
-      <c r="AG141" s="208"/>
-      <c r="AH141" s="208"/>
-      <c r="AI141" s="208"/>
-      <c r="AJ141" s="209"/>
+      <c r="AF141" s="187"/>
+      <c r="AG141" s="187"/>
+      <c r="AH141" s="187"/>
+      <c r="AI141" s="187"/>
+      <c r="AJ141" s="188"/>
       <c r="AP141" s="5"/>
       <c r="AQ141" s="2"/>
     </row>
@@ -12175,30 +12182,30 @@
       <c r="P142" s="134"/>
       <c r="Q142" s="134"/>
       <c r="R142" s="135"/>
-      <c r="S142" s="207" t="s">
+      <c r="S142" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T142" s="208"/>
-      <c r="U142" s="208"/>
-      <c r="V142" s="208"/>
-      <c r="W142" s="208"/>
-      <c r="X142" s="209"/>
-      <c r="Y142" s="207" t="s">
+      <c r="T142" s="187"/>
+      <c r="U142" s="187"/>
+      <c r="V142" s="187"/>
+      <c r="W142" s="187"/>
+      <c r="X142" s="188"/>
+      <c r="Y142" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="Z142" s="208"/>
-      <c r="AA142" s="208"/>
-      <c r="AB142" s="208"/>
-      <c r="AC142" s="208"/>
-      <c r="AD142" s="209"/>
-      <c r="AE142" s="207" t="s">
+      <c r="Z142" s="187"/>
+      <c r="AA142" s="187"/>
+      <c r="AB142" s="187"/>
+      <c r="AC142" s="187"/>
+      <c r="AD142" s="188"/>
+      <c r="AE142" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="AF142" s="208"/>
-      <c r="AG142" s="208"/>
-      <c r="AH142" s="208"/>
-      <c r="AI142" s="208"/>
-      <c r="AJ142" s="209"/>
+      <c r="AF142" s="187"/>
+      <c r="AG142" s="187"/>
+      <c r="AH142" s="187"/>
+      <c r="AI142" s="187"/>
+      <c r="AJ142" s="188"/>
       <c r="AP142" s="5"/>
       <c r="AQ142" s="2"/>
     </row>
@@ -12216,30 +12223,30 @@
       <c r="P143" s="75"/>
       <c r="Q143" s="75"/>
       <c r="R143" s="76"/>
-      <c r="S143" s="207" t="s">
+      <c r="S143" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T143" s="208"/>
-      <c r="U143" s="208"/>
-      <c r="V143" s="208"/>
-      <c r="W143" s="208"/>
-      <c r="X143" s="209"/>
-      <c r="Y143" s="207" t="s">
+      <c r="T143" s="187"/>
+      <c r="U143" s="187"/>
+      <c r="V143" s="187"/>
+      <c r="W143" s="187"/>
+      <c r="X143" s="188"/>
+      <c r="Y143" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z143" s="208"/>
-      <c r="AA143" s="208"/>
-      <c r="AB143" s="208"/>
-      <c r="AC143" s="208"/>
-      <c r="AD143" s="209"/>
-      <c r="AE143" s="207" t="s">
+      <c r="Z143" s="187"/>
+      <c r="AA143" s="187"/>
+      <c r="AB143" s="187"/>
+      <c r="AC143" s="187"/>
+      <c r="AD143" s="188"/>
+      <c r="AE143" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="AF143" s="208"/>
-      <c r="AG143" s="208"/>
-      <c r="AH143" s="208"/>
-      <c r="AI143" s="208"/>
-      <c r="AJ143" s="209"/>
+      <c r="AF143" s="187"/>
+      <c r="AG143" s="187"/>
+      <c r="AH143" s="187"/>
+      <c r="AI143" s="187"/>
+      <c r="AJ143" s="188"/>
       <c r="AP143" s="5"/>
       <c r="AQ143" s="2"/>
     </row>
@@ -12261,30 +12268,30 @@
       <c r="P144" s="75"/>
       <c r="Q144" s="75"/>
       <c r="R144" s="76"/>
-      <c r="S144" s="198" t="s">
+      <c r="S144" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T144" s="199"/>
-      <c r="U144" s="199"/>
-      <c r="V144" s="199"/>
-      <c r="W144" s="199"/>
-      <c r="X144" s="200"/>
-      <c r="Y144" s="198" t="s">
+      <c r="T144" s="190"/>
+      <c r="U144" s="190"/>
+      <c r="V144" s="190"/>
+      <c r="W144" s="190"/>
+      <c r="X144" s="191"/>
+      <c r="Y144" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z144" s="199"/>
-      <c r="AA144" s="199"/>
-      <c r="AB144" s="199"/>
-      <c r="AC144" s="199"/>
-      <c r="AD144" s="200"/>
-      <c r="AE144" s="198" t="s">
+      <c r="Z144" s="190"/>
+      <c r="AA144" s="190"/>
+      <c r="AB144" s="190"/>
+      <c r="AC144" s="190"/>
+      <c r="AD144" s="191"/>
+      <c r="AE144" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="AF144" s="199"/>
-      <c r="AG144" s="199"/>
-      <c r="AH144" s="199"/>
-      <c r="AI144" s="199"/>
-      <c r="AJ144" s="200"/>
+      <c r="AF144" s="190"/>
+      <c r="AG144" s="190"/>
+      <c r="AH144" s="190"/>
+      <c r="AI144" s="190"/>
+      <c r="AJ144" s="191"/>
       <c r="AP144" s="5"/>
       <c r="AQ144" s="2"/>
     </row>
@@ -12306,30 +12313,30 @@
       <c r="P145" s="75"/>
       <c r="Q145" s="75"/>
       <c r="R145" s="76"/>
-      <c r="S145" s="207" t="s">
+      <c r="S145" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T145" s="208"/>
-      <c r="U145" s="208"/>
-      <c r="V145" s="208"/>
-      <c r="W145" s="208"/>
-      <c r="X145" s="209"/>
-      <c r="Y145" s="207" t="s">
+      <c r="T145" s="187"/>
+      <c r="U145" s="187"/>
+      <c r="V145" s="187"/>
+      <c r="W145" s="187"/>
+      <c r="X145" s="188"/>
+      <c r="Y145" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z145" s="208"/>
-      <c r="AA145" s="208"/>
-      <c r="AB145" s="208"/>
-      <c r="AC145" s="208"/>
-      <c r="AD145" s="209"/>
-      <c r="AE145" s="207" t="s">
+      <c r="Z145" s="187"/>
+      <c r="AA145" s="187"/>
+      <c r="AB145" s="187"/>
+      <c r="AC145" s="187"/>
+      <c r="AD145" s="188"/>
+      <c r="AE145" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="AF145" s="208"/>
-      <c r="AG145" s="208"/>
-      <c r="AH145" s="208"/>
-      <c r="AI145" s="208"/>
-      <c r="AJ145" s="209"/>
+      <c r="AF145" s="187"/>
+      <c r="AG145" s="187"/>
+      <c r="AH145" s="187"/>
+      <c r="AI145" s="187"/>
+      <c r="AJ145" s="188"/>
       <c r="AP145" s="5"/>
       <c r="AQ145" s="2"/>
     </row>
@@ -12353,30 +12360,30 @@
       <c r="P146" s="75"/>
       <c r="Q146" s="75"/>
       <c r="R146" s="76"/>
-      <c r="S146" s="207" t="s">
+      <c r="S146" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T146" s="208"/>
-      <c r="U146" s="208"/>
-      <c r="V146" s="208"/>
-      <c r="W146" s="208"/>
-      <c r="X146" s="209"/>
-      <c r="Y146" s="204" t="s">
+      <c r="T146" s="187"/>
+      <c r="U146" s="187"/>
+      <c r="V146" s="187"/>
+      <c r="W146" s="187"/>
+      <c r="X146" s="188"/>
+      <c r="Y146" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="Z146" s="205"/>
-      <c r="AA146" s="205"/>
-      <c r="AB146" s="205"/>
-      <c r="AC146" s="205"/>
-      <c r="AD146" s="206"/>
-      <c r="AE146" s="204" t="s">
+      <c r="Z146" s="184"/>
+      <c r="AA146" s="184"/>
+      <c r="AB146" s="184"/>
+      <c r="AC146" s="184"/>
+      <c r="AD146" s="185"/>
+      <c r="AE146" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF146" s="205"/>
-      <c r="AG146" s="205"/>
-      <c r="AH146" s="205"/>
-      <c r="AI146" s="205"/>
-      <c r="AJ146" s="206"/>
+      <c r="AF146" s="184"/>
+      <c r="AG146" s="184"/>
+      <c r="AH146" s="184"/>
+      <c r="AI146" s="184"/>
+      <c r="AJ146" s="185"/>
       <c r="AP146" s="5"/>
       <c r="AQ146" s="2"/>
     </row>
@@ -12394,30 +12401,30 @@
       <c r="P147" s="75"/>
       <c r="Q147" s="75"/>
       <c r="R147" s="76"/>
-      <c r="S147" s="207" t="s">
+      <c r="S147" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T147" s="208"/>
-      <c r="U147" s="208"/>
-      <c r="V147" s="208"/>
-      <c r="W147" s="208"/>
-      <c r="X147" s="209"/>
-      <c r="Y147" s="207" t="s">
+      <c r="T147" s="187"/>
+      <c r="U147" s="187"/>
+      <c r="V147" s="187"/>
+      <c r="W147" s="187"/>
+      <c r="X147" s="188"/>
+      <c r="Y147" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z147" s="208"/>
-      <c r="AA147" s="208"/>
-      <c r="AB147" s="208"/>
-      <c r="AC147" s="208"/>
-      <c r="AD147" s="209"/>
-      <c r="AE147" s="204" t="s">
+      <c r="Z147" s="187"/>
+      <c r="AA147" s="187"/>
+      <c r="AB147" s="187"/>
+      <c r="AC147" s="187"/>
+      <c r="AD147" s="188"/>
+      <c r="AE147" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF147" s="205"/>
-      <c r="AG147" s="205"/>
-      <c r="AH147" s="205"/>
-      <c r="AI147" s="205"/>
-      <c r="AJ147" s="206"/>
+      <c r="AF147" s="184"/>
+      <c r="AG147" s="184"/>
+      <c r="AH147" s="184"/>
+      <c r="AI147" s="184"/>
+      <c r="AJ147" s="185"/>
       <c r="AP147" s="5"/>
       <c r="AQ147" s="2"/>
     </row>
@@ -12439,30 +12446,30 @@
       <c r="P148" s="75"/>
       <c r="Q148" s="75"/>
       <c r="R148" s="76"/>
-      <c r="S148" s="207" t="s">
+      <c r="S148" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T148" s="208"/>
-      <c r="U148" s="208"/>
-      <c r="V148" s="208"/>
-      <c r="W148" s="208"/>
-      <c r="X148" s="209"/>
-      <c r="Y148" s="207" t="s">
+      <c r="T148" s="187"/>
+      <c r="U148" s="187"/>
+      <c r="V148" s="187"/>
+      <c r="W148" s="187"/>
+      <c r="X148" s="188"/>
+      <c r="Y148" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z148" s="208"/>
-      <c r="AA148" s="208"/>
-      <c r="AB148" s="208"/>
-      <c r="AC148" s="208"/>
-      <c r="AD148" s="209"/>
-      <c r="AE148" s="204" t="s">
+      <c r="Z148" s="187"/>
+      <c r="AA148" s="187"/>
+      <c r="AB148" s="187"/>
+      <c r="AC148" s="187"/>
+      <c r="AD148" s="188"/>
+      <c r="AE148" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF148" s="205"/>
-      <c r="AG148" s="205"/>
-      <c r="AH148" s="205"/>
-      <c r="AI148" s="205"/>
-      <c r="AJ148" s="206"/>
+      <c r="AF148" s="184"/>
+      <c r="AG148" s="184"/>
+      <c r="AH148" s="184"/>
+      <c r="AI148" s="184"/>
+      <c r="AJ148" s="185"/>
       <c r="AP148" s="5"/>
       <c r="AQ148" s="2"/>
     </row>
@@ -12486,30 +12493,30 @@
       <c r="P149" s="75"/>
       <c r="Q149" s="75"/>
       <c r="R149" s="76"/>
-      <c r="S149" s="198" t="s">
+      <c r="S149" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T149" s="199"/>
-      <c r="U149" s="199"/>
-      <c r="V149" s="199"/>
-      <c r="W149" s="199"/>
-      <c r="X149" s="200"/>
-      <c r="Y149" s="198" t="s">
+      <c r="T149" s="190"/>
+      <c r="U149" s="190"/>
+      <c r="V149" s="190"/>
+      <c r="W149" s="190"/>
+      <c r="X149" s="191"/>
+      <c r="Y149" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z149" s="199"/>
-      <c r="AA149" s="199"/>
-      <c r="AB149" s="199"/>
-      <c r="AC149" s="199"/>
-      <c r="AD149" s="200"/>
-      <c r="AE149" s="198" t="s">
+      <c r="Z149" s="190"/>
+      <c r="AA149" s="190"/>
+      <c r="AB149" s="190"/>
+      <c r="AC149" s="190"/>
+      <c r="AD149" s="191"/>
+      <c r="AE149" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="AF149" s="199"/>
-      <c r="AG149" s="199"/>
-      <c r="AH149" s="199"/>
-      <c r="AI149" s="199"/>
-      <c r="AJ149" s="200"/>
+      <c r="AF149" s="190"/>
+      <c r="AG149" s="190"/>
+      <c r="AH149" s="190"/>
+      <c r="AI149" s="190"/>
+      <c r="AJ149" s="191"/>
       <c r="AP149" s="5"/>
       <c r="AQ149" s="2"/>
     </row>
@@ -12531,30 +12538,30 @@
       <c r="P150" s="75"/>
       <c r="Q150" s="75"/>
       <c r="R150" s="76"/>
-      <c r="S150" s="198" t="s">
+      <c r="S150" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T150" s="199"/>
-      <c r="U150" s="199"/>
-      <c r="V150" s="199"/>
-      <c r="W150" s="199"/>
-      <c r="X150" s="200"/>
-      <c r="Y150" s="198" t="s">
+      <c r="T150" s="190"/>
+      <c r="U150" s="190"/>
+      <c r="V150" s="190"/>
+      <c r="W150" s="190"/>
+      <c r="X150" s="191"/>
+      <c r="Y150" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z150" s="199"/>
-      <c r="AA150" s="199"/>
-      <c r="AB150" s="199"/>
-      <c r="AC150" s="199"/>
-      <c r="AD150" s="200"/>
-      <c r="AE150" s="198" t="s">
+      <c r="Z150" s="190"/>
+      <c r="AA150" s="190"/>
+      <c r="AB150" s="190"/>
+      <c r="AC150" s="190"/>
+      <c r="AD150" s="191"/>
+      <c r="AE150" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF150" s="199"/>
-      <c r="AG150" s="199"/>
-      <c r="AH150" s="199"/>
-      <c r="AI150" s="199"/>
-      <c r="AJ150" s="200"/>
+      <c r="AF150" s="190"/>
+      <c r="AG150" s="190"/>
+      <c r="AH150" s="190"/>
+      <c r="AI150" s="190"/>
+      <c r="AJ150" s="191"/>
       <c r="AP150" s="5"/>
       <c r="AQ150" s="2"/>
     </row>
@@ -12578,30 +12585,30 @@
       <c r="P151" s="75"/>
       <c r="Q151" s="75"/>
       <c r="R151" s="76"/>
-      <c r="S151" s="198" t="s">
+      <c r="S151" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T151" s="199"/>
-      <c r="U151" s="199"/>
-      <c r="V151" s="199"/>
-      <c r="W151" s="199"/>
-      <c r="X151" s="200"/>
-      <c r="Y151" s="198" t="s">
+      <c r="T151" s="190"/>
+      <c r="U151" s="190"/>
+      <c r="V151" s="190"/>
+      <c r="W151" s="190"/>
+      <c r="X151" s="191"/>
+      <c r="Y151" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z151" s="199"/>
-      <c r="AA151" s="199"/>
-      <c r="AB151" s="199"/>
-      <c r="AC151" s="199"/>
-      <c r="AD151" s="200"/>
-      <c r="AE151" s="198" t="s">
+      <c r="Z151" s="190"/>
+      <c r="AA151" s="190"/>
+      <c r="AB151" s="190"/>
+      <c r="AC151" s="190"/>
+      <c r="AD151" s="191"/>
+      <c r="AE151" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF151" s="199"/>
-      <c r="AG151" s="199"/>
-      <c r="AH151" s="199"/>
-      <c r="AI151" s="199"/>
-      <c r="AJ151" s="200"/>
+      <c r="AF151" s="190"/>
+      <c r="AG151" s="190"/>
+      <c r="AH151" s="190"/>
+      <c r="AI151" s="190"/>
+      <c r="AJ151" s="191"/>
       <c r="AP151" s="5"/>
       <c r="AQ151" s="2"/>
     </row>
@@ -12623,30 +12630,30 @@
       <c r="P152" s="75"/>
       <c r="Q152" s="75"/>
       <c r="R152" s="76"/>
-      <c r="S152" s="198" t="s">
+      <c r="S152" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T152" s="199"/>
-      <c r="U152" s="199"/>
-      <c r="V152" s="199"/>
-      <c r="W152" s="199"/>
-      <c r="X152" s="200"/>
-      <c r="Y152" s="198" t="s">
+      <c r="T152" s="190"/>
+      <c r="U152" s="190"/>
+      <c r="V152" s="190"/>
+      <c r="W152" s="190"/>
+      <c r="X152" s="191"/>
+      <c r="Y152" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z152" s="199"/>
-      <c r="AA152" s="199"/>
-      <c r="AB152" s="199"/>
-      <c r="AC152" s="199"/>
-      <c r="AD152" s="200"/>
-      <c r="AE152" s="198" t="s">
+      <c r="Z152" s="190"/>
+      <c r="AA152" s="190"/>
+      <c r="AB152" s="190"/>
+      <c r="AC152" s="190"/>
+      <c r="AD152" s="191"/>
+      <c r="AE152" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF152" s="199"/>
-      <c r="AG152" s="199"/>
-      <c r="AH152" s="199"/>
-      <c r="AI152" s="199"/>
-      <c r="AJ152" s="200"/>
+      <c r="AF152" s="190"/>
+      <c r="AG152" s="190"/>
+      <c r="AH152" s="190"/>
+      <c r="AI152" s="190"/>
+      <c r="AJ152" s="191"/>
       <c r="AP152" s="5"/>
       <c r="AQ152" s="2"/>
     </row>
@@ -12670,30 +12677,30 @@
       <c r="P153" s="75"/>
       <c r="Q153" s="75"/>
       <c r="R153" s="76"/>
-      <c r="S153" s="198" t="s">
+      <c r="S153" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T153" s="199"/>
-      <c r="U153" s="199"/>
-      <c r="V153" s="199"/>
-      <c r="W153" s="199"/>
-      <c r="X153" s="200"/>
-      <c r="Y153" s="198" t="s">
+      <c r="T153" s="190"/>
+      <c r="U153" s="190"/>
+      <c r="V153" s="190"/>
+      <c r="W153" s="190"/>
+      <c r="X153" s="191"/>
+      <c r="Y153" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z153" s="199"/>
-      <c r="AA153" s="199"/>
-      <c r="AB153" s="199"/>
-      <c r="AC153" s="199"/>
-      <c r="AD153" s="200"/>
-      <c r="AE153" s="210" t="s">
+      <c r="Z153" s="190"/>
+      <c r="AA153" s="190"/>
+      <c r="AB153" s="190"/>
+      <c r="AC153" s="190"/>
+      <c r="AD153" s="191"/>
+      <c r="AE153" s="189" t="s">
         <v>39</v>
       </c>
-      <c r="AF153" s="211"/>
-      <c r="AG153" s="211"/>
-      <c r="AH153" s="211"/>
-      <c r="AI153" s="211"/>
-      <c r="AJ153" s="212"/>
+      <c r="AF153" s="190"/>
+      <c r="AG153" s="190"/>
+      <c r="AH153" s="190"/>
+      <c r="AI153" s="190"/>
+      <c r="AJ153" s="191"/>
       <c r="AP153" s="5"/>
       <c r="AQ153" s="2"/>
     </row>
@@ -12717,30 +12724,30 @@
       <c r="P154" s="75"/>
       <c r="Q154" s="75"/>
       <c r="R154" s="76"/>
-      <c r="S154" s="198" t="s">
+      <c r="S154" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T154" s="199"/>
-      <c r="U154" s="199"/>
-      <c r="V154" s="199"/>
-      <c r="W154" s="199"/>
-      <c r="X154" s="200"/>
-      <c r="Y154" s="198" t="s">
+      <c r="T154" s="190"/>
+      <c r="U154" s="190"/>
+      <c r="V154" s="190"/>
+      <c r="W154" s="190"/>
+      <c r="X154" s="191"/>
+      <c r="Y154" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z154" s="199"/>
-      <c r="AA154" s="199"/>
-      <c r="AB154" s="199"/>
-      <c r="AC154" s="199"/>
-      <c r="AD154" s="200"/>
-      <c r="AE154" s="198" t="s">
+      <c r="Z154" s="190"/>
+      <c r="AA154" s="190"/>
+      <c r="AB154" s="190"/>
+      <c r="AC154" s="190"/>
+      <c r="AD154" s="191"/>
+      <c r="AE154" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF154" s="199"/>
-      <c r="AG154" s="199"/>
-      <c r="AH154" s="199"/>
-      <c r="AI154" s="199"/>
-      <c r="AJ154" s="200"/>
+      <c r="AF154" s="190"/>
+      <c r="AG154" s="190"/>
+      <c r="AH154" s="190"/>
+      <c r="AI154" s="190"/>
+      <c r="AJ154" s="191"/>
       <c r="AP154" s="5"/>
       <c r="AQ154" s="2"/>
     </row>
@@ -12764,30 +12771,30 @@
       <c r="P155" s="75"/>
       <c r="Q155" s="75"/>
       <c r="R155" s="76"/>
-      <c r="S155" s="198" t="s">
+      <c r="S155" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T155" s="199"/>
-      <c r="U155" s="199"/>
-      <c r="V155" s="199"/>
-      <c r="W155" s="199"/>
-      <c r="X155" s="200"/>
-      <c r="Y155" s="198" t="s">
+      <c r="T155" s="190"/>
+      <c r="U155" s="190"/>
+      <c r="V155" s="190"/>
+      <c r="W155" s="190"/>
+      <c r="X155" s="191"/>
+      <c r="Y155" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z155" s="199"/>
-      <c r="AA155" s="199"/>
-      <c r="AB155" s="199"/>
-      <c r="AC155" s="199"/>
-      <c r="AD155" s="200"/>
-      <c r="AE155" s="210" t="s">
+      <c r="Z155" s="190"/>
+      <c r="AA155" s="190"/>
+      <c r="AB155" s="190"/>
+      <c r="AC155" s="190"/>
+      <c r="AD155" s="191"/>
+      <c r="AE155" s="189" t="s">
         <v>39</v>
       </c>
-      <c r="AF155" s="211"/>
-      <c r="AG155" s="211"/>
-      <c r="AH155" s="211"/>
-      <c r="AI155" s="211"/>
-      <c r="AJ155" s="212"/>
+      <c r="AF155" s="190"/>
+      <c r="AG155" s="190"/>
+      <c r="AH155" s="190"/>
+      <c r="AI155" s="190"/>
+      <c r="AJ155" s="191"/>
       <c r="AP155" s="5"/>
       <c r="AQ155" s="2"/>
     </row>
@@ -12811,30 +12818,30 @@
       <c r="P156" s="75"/>
       <c r="Q156" s="75"/>
       <c r="R156" s="76"/>
-      <c r="S156" s="198" t="s">
+      <c r="S156" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T156" s="199"/>
-      <c r="U156" s="199"/>
-      <c r="V156" s="199"/>
-      <c r="W156" s="199"/>
-      <c r="X156" s="200"/>
-      <c r="Y156" s="198" t="s">
+      <c r="T156" s="190"/>
+      <c r="U156" s="190"/>
+      <c r="V156" s="190"/>
+      <c r="W156" s="190"/>
+      <c r="X156" s="191"/>
+      <c r="Y156" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z156" s="199"/>
-      <c r="AA156" s="199"/>
-      <c r="AB156" s="199"/>
-      <c r="AC156" s="199"/>
-      <c r="AD156" s="200"/>
-      <c r="AE156" s="198" t="s">
+      <c r="Z156" s="190"/>
+      <c r="AA156" s="190"/>
+      <c r="AB156" s="190"/>
+      <c r="AC156" s="190"/>
+      <c r="AD156" s="191"/>
+      <c r="AE156" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF156" s="199"/>
-      <c r="AG156" s="199"/>
-      <c r="AH156" s="199"/>
-      <c r="AI156" s="199"/>
-      <c r="AJ156" s="200"/>
+      <c r="AF156" s="190"/>
+      <c r="AG156" s="190"/>
+      <c r="AH156" s="190"/>
+      <c r="AI156" s="190"/>
+      <c r="AJ156" s="191"/>
       <c r="AP156" s="5"/>
       <c r="AQ156" s="2"/>
     </row>
@@ -12858,30 +12865,30 @@
       <c r="P157" s="75"/>
       <c r="Q157" s="75"/>
       <c r="R157" s="76"/>
-      <c r="S157" s="198" t="s">
+      <c r="S157" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T157" s="199"/>
-      <c r="U157" s="199"/>
-      <c r="V157" s="199"/>
-      <c r="W157" s="199"/>
-      <c r="X157" s="200"/>
-      <c r="Y157" s="198" t="s">
+      <c r="T157" s="190"/>
+      <c r="U157" s="190"/>
+      <c r="V157" s="190"/>
+      <c r="W157" s="190"/>
+      <c r="X157" s="191"/>
+      <c r="Y157" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z157" s="199"/>
-      <c r="AA157" s="199"/>
-      <c r="AB157" s="199"/>
-      <c r="AC157" s="199"/>
-      <c r="AD157" s="200"/>
-      <c r="AE157" s="198" t="s">
+      <c r="Z157" s="190"/>
+      <c r="AA157" s="190"/>
+      <c r="AB157" s="190"/>
+      <c r="AC157" s="190"/>
+      <c r="AD157" s="191"/>
+      <c r="AE157" s="189" t="s">
         <v>39</v>
       </c>
-      <c r="AF157" s="199"/>
-      <c r="AG157" s="199"/>
-      <c r="AH157" s="199"/>
-      <c r="AI157" s="199"/>
-      <c r="AJ157" s="200"/>
+      <c r="AF157" s="190"/>
+      <c r="AG157" s="190"/>
+      <c r="AH157" s="190"/>
+      <c r="AI157" s="190"/>
+      <c r="AJ157" s="191"/>
       <c r="AP157" s="5"/>
       <c r="AQ157" s="2"/>
     </row>
@@ -12903,30 +12910,30 @@
       <c r="P158" s="75"/>
       <c r="Q158" s="75"/>
       <c r="R158" s="76"/>
-      <c r="S158" s="198" t="s">
+      <c r="S158" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T158" s="199"/>
-      <c r="U158" s="199"/>
-      <c r="V158" s="199"/>
-      <c r="W158" s="199"/>
-      <c r="X158" s="200"/>
-      <c r="Y158" s="198" t="s">
+      <c r="T158" s="190"/>
+      <c r="U158" s="190"/>
+      <c r="V158" s="190"/>
+      <c r="W158" s="190"/>
+      <c r="X158" s="191"/>
+      <c r="Y158" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z158" s="199"/>
-      <c r="AA158" s="199"/>
-      <c r="AB158" s="199"/>
-      <c r="AC158" s="199"/>
-      <c r="AD158" s="200"/>
-      <c r="AE158" s="198" t="s">
+      <c r="Z158" s="190"/>
+      <c r="AA158" s="190"/>
+      <c r="AB158" s="190"/>
+      <c r="AC158" s="190"/>
+      <c r="AD158" s="191"/>
+      <c r="AE158" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF158" s="199"/>
-      <c r="AG158" s="199"/>
-      <c r="AH158" s="199"/>
-      <c r="AI158" s="199"/>
-      <c r="AJ158" s="200"/>
+      <c r="AF158" s="190"/>
+      <c r="AG158" s="190"/>
+      <c r="AH158" s="190"/>
+      <c r="AI158" s="190"/>
+      <c r="AJ158" s="191"/>
       <c r="AP158" s="5"/>
       <c r="AQ158" s="2"/>
     </row>
@@ -12948,30 +12955,30 @@
       <c r="P159" s="134"/>
       <c r="Q159" s="134"/>
       <c r="R159" s="135"/>
-      <c r="S159" s="195" t="s">
+      <c r="S159" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T159" s="196"/>
-      <c r="U159" s="196"/>
-      <c r="V159" s="196"/>
-      <c r="W159" s="196"/>
-      <c r="X159" s="197"/>
-      <c r="Y159" s="195" t="s">
+      <c r="T159" s="190"/>
+      <c r="U159" s="190"/>
+      <c r="V159" s="190"/>
+      <c r="W159" s="190"/>
+      <c r="X159" s="191"/>
+      <c r="Y159" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z159" s="196"/>
-      <c r="AA159" s="196"/>
-      <c r="AB159" s="196"/>
-      <c r="AC159" s="196"/>
-      <c r="AD159" s="197"/>
-      <c r="AE159" s="195" t="s">
+      <c r="Z159" s="190"/>
+      <c r="AA159" s="190"/>
+      <c r="AB159" s="190"/>
+      <c r="AC159" s="190"/>
+      <c r="AD159" s="191"/>
+      <c r="AE159" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF159" s="196"/>
-      <c r="AG159" s="196"/>
-      <c r="AH159" s="196"/>
-      <c r="AI159" s="196"/>
-      <c r="AJ159" s="197"/>
+      <c r="AF159" s="190"/>
+      <c r="AG159" s="190"/>
+      <c r="AH159" s="190"/>
+      <c r="AI159" s="190"/>
+      <c r="AJ159" s="191"/>
       <c r="AP159" s="5"/>
       <c r="AQ159" s="2"/>
     </row>
@@ -12993,30 +13000,30 @@
       <c r="P160" s="75"/>
       <c r="Q160" s="75"/>
       <c r="R160" s="76"/>
-      <c r="S160" s="198" t="s">
+      <c r="S160" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T160" s="199"/>
-      <c r="U160" s="199"/>
-      <c r="V160" s="199"/>
-      <c r="W160" s="199"/>
-      <c r="X160" s="200"/>
-      <c r="Y160" s="198" t="s">
+      <c r="T160" s="190"/>
+      <c r="U160" s="190"/>
+      <c r="V160" s="190"/>
+      <c r="W160" s="190"/>
+      <c r="X160" s="191"/>
+      <c r="Y160" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z160" s="199"/>
-      <c r="AA160" s="199"/>
-      <c r="AB160" s="199"/>
-      <c r="AC160" s="199"/>
-      <c r="AD160" s="200"/>
-      <c r="AE160" s="198" t="s">
+      <c r="Z160" s="190"/>
+      <c r="AA160" s="190"/>
+      <c r="AB160" s="190"/>
+      <c r="AC160" s="190"/>
+      <c r="AD160" s="191"/>
+      <c r="AE160" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF160" s="199"/>
-      <c r="AG160" s="199"/>
-      <c r="AH160" s="199"/>
-      <c r="AI160" s="199"/>
-      <c r="AJ160" s="200"/>
+      <c r="AF160" s="190"/>
+      <c r="AG160" s="190"/>
+      <c r="AH160" s="190"/>
+      <c r="AI160" s="190"/>
+      <c r="AJ160" s="191"/>
       <c r="AP160" s="5"/>
       <c r="AQ160" s="2"/>
     </row>
@@ -13040,30 +13047,30 @@
       <c r="P161" s="75"/>
       <c r="Q161" s="75"/>
       <c r="R161" s="76"/>
-      <c r="S161" s="198" t="s">
+      <c r="S161" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T161" s="199"/>
-      <c r="U161" s="199"/>
-      <c r="V161" s="199"/>
-      <c r="W161" s="199"/>
-      <c r="X161" s="200"/>
-      <c r="Y161" s="210" t="s">
+      <c r="T161" s="190"/>
+      <c r="U161" s="190"/>
+      <c r="V161" s="190"/>
+      <c r="W161" s="190"/>
+      <c r="X161" s="191"/>
+      <c r="Y161" s="192" t="s">
         <v>39</v>
       </c>
-      <c r="Z161" s="211"/>
-      <c r="AA161" s="211"/>
-      <c r="AB161" s="211"/>
-      <c r="AC161" s="211"/>
-      <c r="AD161" s="212"/>
-      <c r="AE161" s="213" t="s">
+      <c r="Z161" s="193"/>
+      <c r="AA161" s="193"/>
+      <c r="AB161" s="193"/>
+      <c r="AC161" s="193"/>
+      <c r="AD161" s="194"/>
+      <c r="AE161" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="AF161" s="214"/>
-      <c r="AG161" s="214"/>
-      <c r="AH161" s="214"/>
-      <c r="AI161" s="214"/>
-      <c r="AJ161" s="215"/>
+      <c r="AF161" s="196"/>
+      <c r="AG161" s="196"/>
+      <c r="AH161" s="196"/>
+      <c r="AI161" s="196"/>
+      <c r="AJ161" s="197"/>
       <c r="AP161" s="5"/>
       <c r="AQ161" s="2"/>
     </row>
@@ -13087,30 +13094,30 @@
       <c r="P162" s="75"/>
       <c r="Q162" s="75"/>
       <c r="R162" s="76"/>
-      <c r="S162" s="198" t="s">
+      <c r="S162" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T162" s="199"/>
-      <c r="U162" s="199"/>
-      <c r="V162" s="199"/>
-      <c r="W162" s="199"/>
-      <c r="X162" s="200"/>
-      <c r="Y162" s="198" t="s">
+      <c r="T162" s="190"/>
+      <c r="U162" s="190"/>
+      <c r="V162" s="190"/>
+      <c r="W162" s="190"/>
+      <c r="X162" s="191"/>
+      <c r="Y162" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z162" s="199"/>
-      <c r="AA162" s="199"/>
-      <c r="AB162" s="199"/>
-      <c r="AC162" s="199"/>
-      <c r="AD162" s="200"/>
-      <c r="AE162" s="213" t="s">
+      <c r="Z162" s="190"/>
+      <c r="AA162" s="190"/>
+      <c r="AB162" s="190"/>
+      <c r="AC162" s="190"/>
+      <c r="AD162" s="191"/>
+      <c r="AE162" s="195" t="s">
         <v>39</v>
       </c>
-      <c r="AF162" s="214"/>
-      <c r="AG162" s="214"/>
-      <c r="AH162" s="214"/>
-      <c r="AI162" s="214"/>
-      <c r="AJ162" s="215"/>
+      <c r="AF162" s="196"/>
+      <c r="AG162" s="196"/>
+      <c r="AH162" s="196"/>
+      <c r="AI162" s="196"/>
+      <c r="AJ162" s="197"/>
       <c r="AP162" s="5"/>
       <c r="AQ162" s="2"/>
     </row>
@@ -13134,30 +13141,30 @@
       <c r="P163" s="75"/>
       <c r="Q163" s="75"/>
       <c r="R163" s="76"/>
-      <c r="S163" s="198" t="s">
+      <c r="S163" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T163" s="199"/>
-      <c r="U163" s="199"/>
-      <c r="V163" s="199"/>
-      <c r="W163" s="199"/>
-      <c r="X163" s="200"/>
-      <c r="Y163" s="198" t="s">
+      <c r="T163" s="190"/>
+      <c r="U163" s="190"/>
+      <c r="V163" s="190"/>
+      <c r="W163" s="190"/>
+      <c r="X163" s="191"/>
+      <c r="Y163" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z163" s="199"/>
-      <c r="AA163" s="199"/>
-      <c r="AB163" s="199"/>
-      <c r="AC163" s="199"/>
-      <c r="AD163" s="200"/>
-      <c r="AE163" s="213" t="s">
+      <c r="Z163" s="190"/>
+      <c r="AA163" s="190"/>
+      <c r="AB163" s="190"/>
+      <c r="AC163" s="190"/>
+      <c r="AD163" s="191"/>
+      <c r="AE163" s="195" t="s">
         <v>39</v>
       </c>
-      <c r="AF163" s="214"/>
-      <c r="AG163" s="214"/>
-      <c r="AH163" s="214"/>
-      <c r="AI163" s="214"/>
-      <c r="AJ163" s="215"/>
+      <c r="AF163" s="196"/>
+      <c r="AG163" s="196"/>
+      <c r="AH163" s="196"/>
+      <c r="AI163" s="196"/>
+      <c r="AJ163" s="197"/>
       <c r="AP163" s="5"/>
       <c r="AQ163" s="2"/>
     </row>
@@ -13181,30 +13188,30 @@
       <c r="P164" s="75"/>
       <c r="Q164" s="75"/>
       <c r="R164" s="76"/>
-      <c r="S164" s="198" t="s">
+      <c r="S164" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T164" s="199"/>
-      <c r="U164" s="199"/>
-      <c r="V164" s="199"/>
-      <c r="W164" s="199"/>
-      <c r="X164" s="200"/>
-      <c r="Y164" s="198" t="s">
+      <c r="T164" s="190"/>
+      <c r="U164" s="190"/>
+      <c r="V164" s="190"/>
+      <c r="W164" s="190"/>
+      <c r="X164" s="191"/>
+      <c r="Y164" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z164" s="199"/>
-      <c r="AA164" s="199"/>
-      <c r="AB164" s="199"/>
-      <c r="AC164" s="199"/>
-      <c r="AD164" s="200"/>
-      <c r="AE164" s="213" t="s">
+      <c r="Z164" s="190"/>
+      <c r="AA164" s="190"/>
+      <c r="AB164" s="190"/>
+      <c r="AC164" s="190"/>
+      <c r="AD164" s="191"/>
+      <c r="AE164" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="AF164" s="214"/>
-      <c r="AG164" s="214"/>
-      <c r="AH164" s="214"/>
-      <c r="AI164" s="214"/>
-      <c r="AJ164" s="215"/>
+      <c r="AF164" s="196"/>
+      <c r="AG164" s="196"/>
+      <c r="AH164" s="196"/>
+      <c r="AI164" s="196"/>
+      <c r="AJ164" s="197"/>
       <c r="AP164" s="5"/>
       <c r="AQ164" s="2"/>
     </row>
@@ -13213,7 +13220,7 @@
       <c r="E165" s="9"/>
       <c r="F165" s="15"/>
       <c r="G165" s="139" t="s">
-        <v>268</v>
+        <v>296</v>
       </c>
       <c r="H165" s="92"/>
       <c r="I165" s="92"/>
@@ -13228,30 +13235,30 @@
       <c r="P165" s="75"/>
       <c r="Q165" s="75"/>
       <c r="R165" s="76"/>
-      <c r="S165" s="198" t="s">
+      <c r="S165" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T165" s="199"/>
-      <c r="U165" s="199"/>
-      <c r="V165" s="199"/>
-      <c r="W165" s="199"/>
-      <c r="X165" s="200"/>
-      <c r="Y165" s="198" t="s">
+      <c r="T165" s="190"/>
+      <c r="U165" s="190"/>
+      <c r="V165" s="190"/>
+      <c r="W165" s="190"/>
+      <c r="X165" s="191"/>
+      <c r="Y165" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z165" s="199"/>
-      <c r="AA165" s="199"/>
-      <c r="AB165" s="199"/>
-      <c r="AC165" s="199"/>
-      <c r="AD165" s="200"/>
-      <c r="AE165" s="198" t="s">
+      <c r="Z165" s="190"/>
+      <c r="AA165" s="190"/>
+      <c r="AB165" s="190"/>
+      <c r="AC165" s="190"/>
+      <c r="AD165" s="191"/>
+      <c r="AE165" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="AF165" s="199"/>
-      <c r="AG165" s="199"/>
-      <c r="AH165" s="199"/>
-      <c r="AI165" s="199"/>
-      <c r="AJ165" s="200"/>
+      <c r="AF165" s="190"/>
+      <c r="AG165" s="190"/>
+      <c r="AH165" s="190"/>
+      <c r="AI165" s="190"/>
+      <c r="AJ165" s="191"/>
       <c r="AP165" s="5"/>
       <c r="AQ165" s="2"/>
     </row>
@@ -13260,7 +13267,7 @@
       <c r="E166" s="9"/>
       <c r="F166" s="15"/>
       <c r="G166" s="136" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H166" s="134"/>
       <c r="I166" s="134"/>
@@ -13275,30 +13282,30 @@
       <c r="P166" s="75"/>
       <c r="Q166" s="75"/>
       <c r="R166" s="76"/>
-      <c r="S166" s="198" t="s">
+      <c r="S166" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T166" s="199"/>
-      <c r="U166" s="199"/>
-      <c r="V166" s="199"/>
-      <c r="W166" s="199"/>
-      <c r="X166" s="200"/>
-      <c r="Y166" s="198" t="s">
+      <c r="T166" s="190"/>
+      <c r="U166" s="190"/>
+      <c r="V166" s="190"/>
+      <c r="W166" s="190"/>
+      <c r="X166" s="191"/>
+      <c r="Y166" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z166" s="199"/>
-      <c r="AA166" s="199"/>
-      <c r="AB166" s="199"/>
-      <c r="AC166" s="199"/>
-      <c r="AD166" s="200"/>
-      <c r="AE166" s="213" t="s">
+      <c r="Z166" s="190"/>
+      <c r="AA166" s="190"/>
+      <c r="AB166" s="190"/>
+      <c r="AC166" s="190"/>
+      <c r="AD166" s="191"/>
+      <c r="AE166" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="AF166" s="214"/>
-      <c r="AG166" s="214"/>
-      <c r="AH166" s="214"/>
-      <c r="AI166" s="214"/>
-      <c r="AJ166" s="215"/>
+      <c r="AF166" s="196"/>
+      <c r="AG166" s="196"/>
+      <c r="AH166" s="196"/>
+      <c r="AI166" s="196"/>
+      <c r="AJ166" s="197"/>
       <c r="AP166" s="5"/>
       <c r="AQ166" s="2"/>
     </row>
@@ -13320,30 +13327,30 @@
       <c r="P167" s="75"/>
       <c r="Q167" s="75"/>
       <c r="R167" s="76"/>
-      <c r="S167" s="198" t="s">
+      <c r="S167" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T167" s="199"/>
-      <c r="U167" s="199"/>
-      <c r="V167" s="199"/>
-      <c r="W167" s="199"/>
-      <c r="X167" s="200"/>
-      <c r="Y167" s="198" t="s">
+      <c r="T167" s="190"/>
+      <c r="U167" s="190"/>
+      <c r="V167" s="190"/>
+      <c r="W167" s="190"/>
+      <c r="X167" s="191"/>
+      <c r="Y167" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z167" s="199"/>
-      <c r="AA167" s="199"/>
-      <c r="AB167" s="199"/>
-      <c r="AC167" s="199"/>
-      <c r="AD167" s="200"/>
-      <c r="AE167" s="198" t="s">
+      <c r="Z167" s="190"/>
+      <c r="AA167" s="190"/>
+      <c r="AB167" s="190"/>
+      <c r="AC167" s="190"/>
+      <c r="AD167" s="191"/>
+      <c r="AE167" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF167" s="199"/>
-      <c r="AG167" s="199"/>
-      <c r="AH167" s="199"/>
-      <c r="AI167" s="199"/>
-      <c r="AJ167" s="200"/>
+      <c r="AF167" s="190"/>
+      <c r="AG167" s="190"/>
+      <c r="AH167" s="190"/>
+      <c r="AI167" s="190"/>
+      <c r="AJ167" s="191"/>
       <c r="AP167" s="5"/>
       <c r="AQ167" s="2"/>
     </row>
@@ -13367,30 +13374,30 @@
       <c r="P168" s="134"/>
       <c r="Q168" s="134"/>
       <c r="R168" s="135"/>
-      <c r="S168" s="198" t="s">
+      <c r="S168" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T168" s="199"/>
-      <c r="U168" s="199"/>
-      <c r="V168" s="199"/>
-      <c r="W168" s="199"/>
-      <c r="X168" s="200"/>
-      <c r="Y168" s="210" t="s">
+      <c r="T168" s="190"/>
+      <c r="U168" s="190"/>
+      <c r="V168" s="190"/>
+      <c r="W168" s="190"/>
+      <c r="X168" s="191"/>
+      <c r="Y168" s="192" t="s">
         <v>39</v>
       </c>
-      <c r="Z168" s="211"/>
-      <c r="AA168" s="211"/>
-      <c r="AB168" s="211"/>
-      <c r="AC168" s="211"/>
-      <c r="AD168" s="212"/>
-      <c r="AE168" s="210" t="s">
+      <c r="Z168" s="193"/>
+      <c r="AA168" s="193"/>
+      <c r="AB168" s="193"/>
+      <c r="AC168" s="193"/>
+      <c r="AD168" s="194"/>
+      <c r="AE168" s="192" t="s">
         <v>14</v>
       </c>
-      <c r="AF168" s="211"/>
-      <c r="AG168" s="211"/>
-      <c r="AH168" s="211"/>
-      <c r="AI168" s="211"/>
-      <c r="AJ168" s="212"/>
+      <c r="AF168" s="193"/>
+      <c r="AG168" s="193"/>
+      <c r="AH168" s="193"/>
+      <c r="AI168" s="193"/>
+      <c r="AJ168" s="194"/>
       <c r="AP168" s="5"/>
       <c r="AQ168" s="2"/>
     </row>
@@ -13412,30 +13419,30 @@
       <c r="P169" s="75"/>
       <c r="Q169" s="75"/>
       <c r="R169" s="76"/>
-      <c r="S169" s="198" t="s">
+      <c r="S169" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T169" s="199"/>
-      <c r="U169" s="199"/>
-      <c r="V169" s="199"/>
-      <c r="W169" s="199"/>
-      <c r="X169" s="200"/>
-      <c r="Y169" s="198" t="s">
+      <c r="T169" s="190"/>
+      <c r="U169" s="190"/>
+      <c r="V169" s="190"/>
+      <c r="W169" s="190"/>
+      <c r="X169" s="191"/>
+      <c r="Y169" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z169" s="199"/>
-      <c r="AA169" s="199"/>
-      <c r="AB169" s="199"/>
-      <c r="AC169" s="199"/>
-      <c r="AD169" s="200"/>
-      <c r="AE169" s="210" t="s">
+      <c r="Z169" s="190"/>
+      <c r="AA169" s="190"/>
+      <c r="AB169" s="190"/>
+      <c r="AC169" s="190"/>
+      <c r="AD169" s="191"/>
+      <c r="AE169" s="192" t="s">
         <v>39</v>
       </c>
-      <c r="AF169" s="211"/>
-      <c r="AG169" s="211"/>
-      <c r="AH169" s="211"/>
-      <c r="AI169" s="211"/>
-      <c r="AJ169" s="212"/>
+      <c r="AF169" s="193"/>
+      <c r="AG169" s="193"/>
+      <c r="AH169" s="193"/>
+      <c r="AI169" s="193"/>
+      <c r="AJ169" s="194"/>
       <c r="AP169" s="5"/>
       <c r="AQ169" s="2"/>
     </row>
@@ -13457,30 +13464,30 @@
       <c r="P170" s="75"/>
       <c r="Q170" s="75"/>
       <c r="R170" s="76"/>
-      <c r="S170" s="198" t="s">
+      <c r="S170" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T170" s="199"/>
-      <c r="U170" s="199"/>
-      <c r="V170" s="199"/>
-      <c r="W170" s="199"/>
-      <c r="X170" s="200"/>
-      <c r="Y170" s="198" t="s">
+      <c r="T170" s="190"/>
+      <c r="U170" s="190"/>
+      <c r="V170" s="190"/>
+      <c r="W170" s="190"/>
+      <c r="X170" s="191"/>
+      <c r="Y170" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z170" s="199"/>
-      <c r="AA170" s="199"/>
-      <c r="AB170" s="199"/>
-      <c r="AC170" s="199"/>
-      <c r="AD170" s="200"/>
-      <c r="AE170" s="210" t="s">
+      <c r="Z170" s="190"/>
+      <c r="AA170" s="190"/>
+      <c r="AB170" s="190"/>
+      <c r="AC170" s="190"/>
+      <c r="AD170" s="191"/>
+      <c r="AE170" s="192" t="s">
         <v>39</v>
       </c>
-      <c r="AF170" s="211"/>
-      <c r="AG170" s="211"/>
-      <c r="AH170" s="211"/>
-      <c r="AI170" s="211"/>
-      <c r="AJ170" s="212"/>
+      <c r="AF170" s="193"/>
+      <c r="AG170" s="193"/>
+      <c r="AH170" s="193"/>
+      <c r="AI170" s="193"/>
+      <c r="AJ170" s="194"/>
       <c r="AP170" s="5"/>
       <c r="AQ170" s="2"/>
     </row>
@@ -13502,30 +13509,30 @@
       <c r="P171" s="75"/>
       <c r="Q171" s="75"/>
       <c r="R171" s="76"/>
-      <c r="S171" s="198" t="s">
+      <c r="S171" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T171" s="199"/>
-      <c r="U171" s="199"/>
-      <c r="V171" s="199"/>
-      <c r="W171" s="199"/>
-      <c r="X171" s="200"/>
-      <c r="Y171" s="198" t="s">
+      <c r="T171" s="190"/>
+      <c r="U171" s="190"/>
+      <c r="V171" s="190"/>
+      <c r="W171" s="190"/>
+      <c r="X171" s="191"/>
+      <c r="Y171" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z171" s="199"/>
-      <c r="AA171" s="199"/>
-      <c r="AB171" s="199"/>
-      <c r="AC171" s="199"/>
-      <c r="AD171" s="200"/>
-      <c r="AE171" s="210" t="s">
+      <c r="Z171" s="190"/>
+      <c r="AA171" s="190"/>
+      <c r="AB171" s="190"/>
+      <c r="AC171" s="190"/>
+      <c r="AD171" s="191"/>
+      <c r="AE171" s="192" t="s">
         <v>14</v>
       </c>
-      <c r="AF171" s="211"/>
-      <c r="AG171" s="211"/>
-      <c r="AH171" s="211"/>
-      <c r="AI171" s="211"/>
-      <c r="AJ171" s="212"/>
+      <c r="AF171" s="193"/>
+      <c r="AG171" s="193"/>
+      <c r="AH171" s="193"/>
+      <c r="AI171" s="193"/>
+      <c r="AJ171" s="194"/>
       <c r="AP171" s="5"/>
       <c r="AQ171" s="2"/>
     </row>
@@ -13547,30 +13554,30 @@
       <c r="P172" s="75"/>
       <c r="Q172" s="75"/>
       <c r="R172" s="76"/>
-      <c r="S172" s="198" t="s">
+      <c r="S172" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T172" s="199"/>
-      <c r="U172" s="199"/>
-      <c r="V172" s="199"/>
-      <c r="W172" s="199"/>
-      <c r="X172" s="200"/>
-      <c r="Y172" s="198" t="s">
+      <c r="T172" s="190"/>
+      <c r="U172" s="190"/>
+      <c r="V172" s="190"/>
+      <c r="W172" s="190"/>
+      <c r="X172" s="191"/>
+      <c r="Y172" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z172" s="199"/>
-      <c r="AA172" s="199"/>
-      <c r="AB172" s="199"/>
-      <c r="AC172" s="199"/>
-      <c r="AD172" s="200"/>
-      <c r="AE172" s="198" t="s">
+      <c r="Z172" s="190"/>
+      <c r="AA172" s="190"/>
+      <c r="AB172" s="190"/>
+      <c r="AC172" s="190"/>
+      <c r="AD172" s="191"/>
+      <c r="AE172" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="AF172" s="199"/>
-      <c r="AG172" s="199"/>
-      <c r="AH172" s="199"/>
-      <c r="AI172" s="199"/>
-      <c r="AJ172" s="200"/>
+      <c r="AF172" s="190"/>
+      <c r="AG172" s="190"/>
+      <c r="AH172" s="190"/>
+      <c r="AI172" s="190"/>
+      <c r="AJ172" s="191"/>
       <c r="AP172" s="5"/>
       <c r="AQ172" s="2"/>
     </row>
@@ -13592,30 +13599,30 @@
       <c r="P173" s="75"/>
       <c r="Q173" s="75"/>
       <c r="R173" s="76"/>
-      <c r="S173" s="198" t="s">
+      <c r="S173" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T173" s="199"/>
-      <c r="U173" s="199"/>
-      <c r="V173" s="199"/>
-      <c r="W173" s="199"/>
-      <c r="X173" s="200"/>
-      <c r="Y173" s="198" t="s">
+      <c r="T173" s="190"/>
+      <c r="U173" s="190"/>
+      <c r="V173" s="190"/>
+      <c r="W173" s="190"/>
+      <c r="X173" s="191"/>
+      <c r="Y173" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z173" s="199"/>
-      <c r="AA173" s="199"/>
-      <c r="AB173" s="199"/>
-      <c r="AC173" s="199"/>
-      <c r="AD173" s="200"/>
-      <c r="AE173" s="210" t="s">
+      <c r="Z173" s="190"/>
+      <c r="AA173" s="190"/>
+      <c r="AB173" s="190"/>
+      <c r="AC173" s="190"/>
+      <c r="AD173" s="191"/>
+      <c r="AE173" s="192" t="s">
         <v>14</v>
       </c>
-      <c r="AF173" s="211"/>
-      <c r="AG173" s="211"/>
-      <c r="AH173" s="211"/>
-      <c r="AI173" s="211"/>
-      <c r="AJ173" s="212"/>
+      <c r="AF173" s="193"/>
+      <c r="AG173" s="193"/>
+      <c r="AH173" s="193"/>
+      <c r="AI173" s="193"/>
+      <c r="AJ173" s="194"/>
       <c r="AP173" s="5"/>
       <c r="AQ173" s="2"/>
     </row>
@@ -13624,7 +13631,7 @@
       <c r="E174" s="9"/>
       <c r="F174" s="15"/>
       <c r="G174" s="74" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H174" s="75"/>
       <c r="I174" s="75"/>
@@ -13637,30 +13644,30 @@
       <c r="P174" s="75"/>
       <c r="Q174" s="75"/>
       <c r="R174" s="76"/>
-      <c r="S174" s="198" t="s">
+      <c r="S174" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T174" s="199"/>
-      <c r="U174" s="199"/>
-      <c r="V174" s="199"/>
-      <c r="W174" s="199"/>
-      <c r="X174" s="200"/>
-      <c r="Y174" s="198" t="s">
+      <c r="T174" s="190"/>
+      <c r="U174" s="190"/>
+      <c r="V174" s="190"/>
+      <c r="W174" s="190"/>
+      <c r="X174" s="191"/>
+      <c r="Y174" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="Z174" s="199"/>
-      <c r="AA174" s="199"/>
-      <c r="AB174" s="199"/>
-      <c r="AC174" s="199"/>
-      <c r="AD174" s="200"/>
-      <c r="AE174" s="198" t="s">
+      <c r="Z174" s="190"/>
+      <c r="AA174" s="190"/>
+      <c r="AB174" s="190"/>
+      <c r="AC174" s="190"/>
+      <c r="AD174" s="191"/>
+      <c r="AE174" s="189" t="s">
         <v>165</v>
       </c>
-      <c r="AF174" s="199"/>
-      <c r="AG174" s="199"/>
-      <c r="AH174" s="199"/>
-      <c r="AI174" s="199"/>
-      <c r="AJ174" s="200"/>
+      <c r="AF174" s="190"/>
+      <c r="AG174" s="190"/>
+      <c r="AH174" s="190"/>
+      <c r="AI174" s="190"/>
+      <c r="AJ174" s="191"/>
       <c r="AP174" s="5"/>
       <c r="AQ174" s="2"/>
     </row>
@@ -13669,7 +13676,7 @@
       <c r="E175" s="9"/>
       <c r="F175" s="15"/>
       <c r="G175" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H175" s="23"/>
       <c r="I175" s="23"/>
@@ -13684,30 +13691,30 @@
       <c r="P175" s="134"/>
       <c r="Q175" s="134"/>
       <c r="R175" s="135"/>
-      <c r="S175" s="198" t="s">
+      <c r="S175" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T175" s="199"/>
-      <c r="U175" s="199"/>
-      <c r="V175" s="199"/>
-      <c r="W175" s="199"/>
-      <c r="X175" s="200"/>
-      <c r="Y175" s="198" t="s">
+      <c r="T175" s="190"/>
+      <c r="U175" s="190"/>
+      <c r="V175" s="190"/>
+      <c r="W175" s="190"/>
+      <c r="X175" s="191"/>
+      <c r="Y175" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="Z175" s="199"/>
-      <c r="AA175" s="199"/>
-      <c r="AB175" s="199"/>
-      <c r="AC175" s="199"/>
-      <c r="AD175" s="200"/>
-      <c r="AE175" s="198" t="s">
+      <c r="Z175" s="190"/>
+      <c r="AA175" s="190"/>
+      <c r="AB175" s="190"/>
+      <c r="AC175" s="190"/>
+      <c r="AD175" s="191"/>
+      <c r="AE175" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="AF175" s="199"/>
-      <c r="AG175" s="199"/>
-      <c r="AH175" s="199"/>
-      <c r="AI175" s="199"/>
-      <c r="AJ175" s="200"/>
+      <c r="AF175" s="190"/>
+      <c r="AG175" s="190"/>
+      <c r="AH175" s="190"/>
+      <c r="AI175" s="190"/>
+      <c r="AJ175" s="191"/>
       <c r="AP175" s="5"/>
       <c r="AQ175" s="2"/>
     </row>
@@ -13716,7 +13723,7 @@
       <c r="E176" s="9"/>
       <c r="F176" s="15"/>
       <c r="G176" s="49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H176" s="10"/>
       <c r="I176" s="10"/>
@@ -13731,30 +13738,30 @@
       <c r="P176" s="75"/>
       <c r="Q176" s="75"/>
       <c r="R176" s="76"/>
-      <c r="S176" s="198" t="s">
+      <c r="S176" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T176" s="199"/>
-      <c r="U176" s="199"/>
-      <c r="V176" s="199"/>
-      <c r="W176" s="199"/>
-      <c r="X176" s="200"/>
-      <c r="Y176" s="210" t="s">
+      <c r="T176" s="190"/>
+      <c r="U176" s="190"/>
+      <c r="V176" s="190"/>
+      <c r="W176" s="190"/>
+      <c r="X176" s="191"/>
+      <c r="Y176" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="Z176" s="211"/>
-      <c r="AA176" s="211"/>
-      <c r="AB176" s="211"/>
-      <c r="AC176" s="211"/>
-      <c r="AD176" s="212"/>
-      <c r="AE176" s="198" t="s">
+      <c r="Z176" s="193"/>
+      <c r="AA176" s="193"/>
+      <c r="AB176" s="193"/>
+      <c r="AC176" s="193"/>
+      <c r="AD176" s="194"/>
+      <c r="AE176" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="AF176" s="199"/>
-      <c r="AG176" s="199"/>
-      <c r="AH176" s="199"/>
-      <c r="AI176" s="199"/>
-      <c r="AJ176" s="200"/>
+      <c r="AF176" s="190"/>
+      <c r="AG176" s="190"/>
+      <c r="AH176" s="190"/>
+      <c r="AI176" s="190"/>
+      <c r="AJ176" s="191"/>
       <c r="AP176" s="5"/>
       <c r="AQ176" s="2"/>
     </row>
@@ -13763,7 +13770,7 @@
       <c r="E177" s="9"/>
       <c r="F177" s="15"/>
       <c r="G177" s="49" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H177" s="16"/>
       <c r="I177" s="16"/>
@@ -13778,30 +13785,30 @@
       <c r="P177" s="75"/>
       <c r="Q177" s="75"/>
       <c r="R177" s="76"/>
-      <c r="S177" s="198" t="s">
+      <c r="S177" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T177" s="199"/>
-      <c r="U177" s="199"/>
-      <c r="V177" s="199"/>
-      <c r="W177" s="199"/>
-      <c r="X177" s="200"/>
-      <c r="Y177" s="210" t="s">
+      <c r="T177" s="190"/>
+      <c r="U177" s="190"/>
+      <c r="V177" s="190"/>
+      <c r="W177" s="190"/>
+      <c r="X177" s="191"/>
+      <c r="Y177" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="Z177" s="211"/>
-      <c r="AA177" s="211"/>
-      <c r="AB177" s="211"/>
-      <c r="AC177" s="211"/>
-      <c r="AD177" s="212"/>
-      <c r="AE177" s="198" t="s">
+      <c r="Z177" s="193"/>
+      <c r="AA177" s="193"/>
+      <c r="AB177" s="193"/>
+      <c r="AC177" s="193"/>
+      <c r="AD177" s="194"/>
+      <c r="AE177" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="AF177" s="199"/>
-      <c r="AG177" s="199"/>
-      <c r="AH177" s="199"/>
-      <c r="AI177" s="199"/>
-      <c r="AJ177" s="200"/>
+      <c r="AF177" s="190"/>
+      <c r="AG177" s="190"/>
+      <c r="AH177" s="190"/>
+      <c r="AI177" s="190"/>
+      <c r="AJ177" s="191"/>
       <c r="AP177" s="5"/>
       <c r="AQ177" s="2"/>
     </row>
@@ -13823,30 +13830,30 @@
       <c r="P178" s="75"/>
       <c r="Q178" s="75"/>
       <c r="R178" s="76"/>
-      <c r="S178" s="198" t="s">
+      <c r="S178" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T178" s="199"/>
-      <c r="U178" s="199"/>
-      <c r="V178" s="199"/>
-      <c r="W178" s="199"/>
-      <c r="X178" s="200"/>
-      <c r="Y178" s="210" t="s">
+      <c r="T178" s="190"/>
+      <c r="U178" s="190"/>
+      <c r="V178" s="190"/>
+      <c r="W178" s="190"/>
+      <c r="X178" s="191"/>
+      <c r="Y178" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="Z178" s="211"/>
-      <c r="AA178" s="211"/>
-      <c r="AB178" s="211"/>
-      <c r="AC178" s="211"/>
-      <c r="AD178" s="212"/>
-      <c r="AE178" s="198" t="s">
+      <c r="Z178" s="193"/>
+      <c r="AA178" s="193"/>
+      <c r="AB178" s="193"/>
+      <c r="AC178" s="193"/>
+      <c r="AD178" s="194"/>
+      <c r="AE178" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="AF178" s="199"/>
-      <c r="AG178" s="199"/>
-      <c r="AH178" s="199"/>
-      <c r="AI178" s="199"/>
-      <c r="AJ178" s="200"/>
+      <c r="AF178" s="190"/>
+      <c r="AG178" s="190"/>
+      <c r="AH178" s="190"/>
+      <c r="AI178" s="190"/>
+      <c r="AJ178" s="191"/>
       <c r="AP178" s="5"/>
       <c r="AQ178" s="2"/>
     </row>
@@ -13868,30 +13875,30 @@
       <c r="P179" s="75"/>
       <c r="Q179" s="75"/>
       <c r="R179" s="76"/>
-      <c r="S179" s="198" t="s">
+      <c r="S179" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T179" s="199"/>
-      <c r="U179" s="199"/>
-      <c r="V179" s="199"/>
-      <c r="W179" s="199"/>
-      <c r="X179" s="200"/>
-      <c r="Y179" s="210" t="s">
+      <c r="T179" s="190"/>
+      <c r="U179" s="190"/>
+      <c r="V179" s="190"/>
+      <c r="W179" s="190"/>
+      <c r="X179" s="191"/>
+      <c r="Y179" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="Z179" s="211"/>
-      <c r="AA179" s="211"/>
-      <c r="AB179" s="211"/>
-      <c r="AC179" s="211"/>
-      <c r="AD179" s="212"/>
-      <c r="AE179" s="210" t="s">
+      <c r="Z179" s="193"/>
+      <c r="AA179" s="193"/>
+      <c r="AB179" s="193"/>
+      <c r="AC179" s="193"/>
+      <c r="AD179" s="194"/>
+      <c r="AE179" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AF179" s="211"/>
-      <c r="AG179" s="211"/>
-      <c r="AH179" s="211"/>
-      <c r="AI179" s="211"/>
-      <c r="AJ179" s="212"/>
+      <c r="AF179" s="193"/>
+      <c r="AG179" s="193"/>
+      <c r="AH179" s="193"/>
+      <c r="AI179" s="193"/>
+      <c r="AJ179" s="194"/>
       <c r="AP179" s="5"/>
       <c r="AQ179" s="2"/>
     </row>
@@ -13913,30 +13920,30 @@
       <c r="P180" s="75"/>
       <c r="Q180" s="75"/>
       <c r="R180" s="76"/>
-      <c r="S180" s="210" t="s">
+      <c r="S180" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="T180" s="211"/>
-      <c r="U180" s="211"/>
-      <c r="V180" s="211"/>
-      <c r="W180" s="211"/>
-      <c r="X180" s="212"/>
-      <c r="Y180" s="210" t="s">
+      <c r="T180" s="193"/>
+      <c r="U180" s="193"/>
+      <c r="V180" s="193"/>
+      <c r="W180" s="193"/>
+      <c r="X180" s="194"/>
+      <c r="Y180" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="Z180" s="211"/>
-      <c r="AA180" s="211"/>
-      <c r="AB180" s="211"/>
-      <c r="AC180" s="211"/>
-      <c r="AD180" s="212"/>
-      <c r="AE180" s="210" t="s">
+      <c r="Z180" s="193"/>
+      <c r="AA180" s="193"/>
+      <c r="AB180" s="193"/>
+      <c r="AC180" s="193"/>
+      <c r="AD180" s="194"/>
+      <c r="AE180" s="192" t="s">
         <v>14</v>
       </c>
-      <c r="AF180" s="211"/>
-      <c r="AG180" s="211"/>
-      <c r="AH180" s="211"/>
-      <c r="AI180" s="211"/>
-      <c r="AJ180" s="212"/>
+      <c r="AF180" s="193"/>
+      <c r="AG180" s="193"/>
+      <c r="AH180" s="193"/>
+      <c r="AI180" s="193"/>
+      <c r="AJ180" s="194"/>
       <c r="AP180" s="5"/>
       <c r="AQ180" s="2"/>
     </row>
@@ -13958,30 +13965,30 @@
       <c r="P181" s="149"/>
       <c r="Q181" s="149"/>
       <c r="R181" s="150"/>
-      <c r="S181" s="201" t="s">
+      <c r="S181" s="210" t="s">
         <v>8</v>
       </c>
-      <c r="T181" s="202"/>
-      <c r="U181" s="202"/>
-      <c r="V181" s="202"/>
-      <c r="W181" s="202"/>
-      <c r="X181" s="203"/>
-      <c r="Y181" s="201" t="s">
+      <c r="T181" s="211"/>
+      <c r="U181" s="211"/>
+      <c r="V181" s="211"/>
+      <c r="W181" s="211"/>
+      <c r="X181" s="212"/>
+      <c r="Y181" s="210" t="s">
         <v>8</v>
       </c>
-      <c r="Z181" s="202"/>
-      <c r="AA181" s="202"/>
-      <c r="AB181" s="202"/>
-      <c r="AC181" s="202"/>
-      <c r="AD181" s="203"/>
-      <c r="AE181" s="201" t="s">
+      <c r="Z181" s="211"/>
+      <c r="AA181" s="211"/>
+      <c r="AB181" s="211"/>
+      <c r="AC181" s="211"/>
+      <c r="AD181" s="212"/>
+      <c r="AE181" s="210" t="s">
         <v>14</v>
       </c>
-      <c r="AF181" s="202"/>
-      <c r="AG181" s="202"/>
-      <c r="AH181" s="202"/>
-      <c r="AI181" s="202"/>
-      <c r="AJ181" s="203"/>
+      <c r="AF181" s="211"/>
+      <c r="AG181" s="211"/>
+      <c r="AH181" s="211"/>
+      <c r="AI181" s="211"/>
+      <c r="AJ181" s="212"/>
       <c r="AP181" s="5"/>
       <c r="AQ181" s="2"/>
     </row>
@@ -14003,30 +14010,30 @@
       <c r="P182" s="75"/>
       <c r="Q182" s="75"/>
       <c r="R182" s="76"/>
-      <c r="S182" s="198" t="s">
+      <c r="S182" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="T182" s="199"/>
-      <c r="U182" s="199"/>
-      <c r="V182" s="199"/>
-      <c r="W182" s="199"/>
-      <c r="X182" s="200"/>
-      <c r="Y182" s="198" t="s">
+      <c r="T182" s="190"/>
+      <c r="U182" s="190"/>
+      <c r="V182" s="190"/>
+      <c r="W182" s="190"/>
+      <c r="X182" s="191"/>
+      <c r="Y182" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="Z182" s="199"/>
-      <c r="AA182" s="199"/>
-      <c r="AB182" s="199"/>
-      <c r="AC182" s="199"/>
-      <c r="AD182" s="200"/>
-      <c r="AE182" s="198" t="s">
+      <c r="Z182" s="190"/>
+      <c r="AA182" s="190"/>
+      <c r="AB182" s="190"/>
+      <c r="AC182" s="190"/>
+      <c r="AD182" s="191"/>
+      <c r="AE182" s="189" t="s">
         <v>39</v>
       </c>
-      <c r="AF182" s="199"/>
-      <c r="AG182" s="199"/>
-      <c r="AH182" s="199"/>
-      <c r="AI182" s="199"/>
-      <c r="AJ182" s="200"/>
+      <c r="AF182" s="190"/>
+      <c r="AG182" s="190"/>
+      <c r="AH182" s="190"/>
+      <c r="AI182" s="190"/>
+      <c r="AJ182" s="191"/>
       <c r="AP182" s="5"/>
       <c r="AQ182" s="2"/>
     </row>
@@ -14048,30 +14055,30 @@
       <c r="P183" s="149"/>
       <c r="Q183" s="149"/>
       <c r="R183" s="150"/>
-      <c r="S183" s="201" t="s">
+      <c r="S183" s="210" t="s">
         <v>8</v>
       </c>
-      <c r="T183" s="202"/>
-      <c r="U183" s="202"/>
-      <c r="V183" s="202"/>
-      <c r="W183" s="202"/>
-      <c r="X183" s="203"/>
-      <c r="Y183" s="201" t="s">
+      <c r="T183" s="211"/>
+      <c r="U183" s="211"/>
+      <c r="V183" s="211"/>
+      <c r="W183" s="211"/>
+      <c r="X183" s="212"/>
+      <c r="Y183" s="210" t="s">
         <v>14</v>
       </c>
-      <c r="Z183" s="202"/>
-      <c r="AA183" s="202"/>
-      <c r="AB183" s="202"/>
-      <c r="AC183" s="202"/>
-      <c r="AD183" s="203"/>
-      <c r="AE183" s="201" t="s">
+      <c r="Z183" s="211"/>
+      <c r="AA183" s="211"/>
+      <c r="AB183" s="211"/>
+      <c r="AC183" s="211"/>
+      <c r="AD183" s="212"/>
+      <c r="AE183" s="210" t="s">
         <v>14</v>
       </c>
-      <c r="AF183" s="202"/>
-      <c r="AG183" s="202"/>
-      <c r="AH183" s="202"/>
-      <c r="AI183" s="202"/>
-      <c r="AJ183" s="203"/>
+      <c r="AF183" s="211"/>
+      <c r="AG183" s="211"/>
+      <c r="AH183" s="211"/>
+      <c r="AI183" s="211"/>
+      <c r="AJ183" s="212"/>
       <c r="AP183" s="5"/>
       <c r="AQ183" s="2"/>
     </row>
@@ -14093,30 +14100,30 @@
       <c r="P184" s="152"/>
       <c r="Q184" s="152"/>
       <c r="R184" s="153"/>
-      <c r="S184" s="247" t="s">
+      <c r="S184" s="243" t="s">
         <v>8</v>
       </c>
-      <c r="T184" s="248"/>
-      <c r="U184" s="248"/>
-      <c r="V184" s="248"/>
-      <c r="W184" s="248"/>
-      <c r="X184" s="249"/>
-      <c r="Y184" s="247" t="s">
+      <c r="T184" s="244"/>
+      <c r="U184" s="244"/>
+      <c r="V184" s="244"/>
+      <c r="W184" s="244"/>
+      <c r="X184" s="245"/>
+      <c r="Y184" s="243" t="s">
         <v>14</v>
       </c>
-      <c r="Z184" s="248"/>
-      <c r="AA184" s="248"/>
-      <c r="AB184" s="248"/>
-      <c r="AC184" s="248"/>
-      <c r="AD184" s="249"/>
-      <c r="AE184" s="247" t="s">
+      <c r="Z184" s="244"/>
+      <c r="AA184" s="244"/>
+      <c r="AB184" s="244"/>
+      <c r="AC184" s="244"/>
+      <c r="AD184" s="245"/>
+      <c r="AE184" s="243" t="s">
         <v>14</v>
       </c>
-      <c r="AF184" s="248"/>
-      <c r="AG184" s="248"/>
-      <c r="AH184" s="248"/>
-      <c r="AI184" s="248"/>
-      <c r="AJ184" s="249"/>
+      <c r="AF184" s="244"/>
+      <c r="AG184" s="244"/>
+      <c r="AH184" s="244"/>
+      <c r="AI184" s="244"/>
+      <c r="AJ184" s="245"/>
       <c r="AP184" s="5"/>
       <c r="AQ184" s="2"/>
     </row>
@@ -14510,7 +14517,7 @@
       <c r="AK199" s="98"/>
       <c r="AL199" s="102"/>
       <c r="AM199" s="169" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN199" s="170"/>
       <c r="AO199" s="171"/>
@@ -14559,7 +14566,7 @@
       <c r="AK200" s="99"/>
       <c r="AL200" s="103"/>
       <c r="AM200" s="125" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN200" s="105"/>
       <c r="AO200" s="116"/>
@@ -14606,7 +14613,7 @@
       <c r="AK201" s="100"/>
       <c r="AL201" s="104"/>
       <c r="AM201" s="160" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN201" s="161"/>
       <c r="AO201" s="162"/>
@@ -14696,7 +14703,7 @@
       <c r="AK203" s="99"/>
       <c r="AL203" s="103"/>
       <c r="AM203" s="169" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN203" s="164"/>
       <c r="AO203" s="165"/>
@@ -14869,7 +14876,7 @@
       <c r="AK207" s="40"/>
       <c r="AL207" s="17"/>
       <c r="AM207" s="125" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN207" s="155"/>
       <c r="AO207" s="51"/>
@@ -14916,7 +14923,7 @@
       <c r="AK208" s="90"/>
       <c r="AL208" s="97"/>
       <c r="AM208" s="160" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN208" s="161"/>
       <c r="AO208" s="162"/>
@@ -15006,7 +15013,7 @@
       <c r="AK210" s="91"/>
       <c r="AL210" s="33"/>
       <c r="AM210" s="169" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN210" s="164"/>
       <c r="AO210" s="165"/>
@@ -15055,7 +15062,7 @@
       <c r="AK211" s="40"/>
       <c r="AL211" s="17"/>
       <c r="AM211" s="125" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN211" s="155"/>
       <c r="AO211" s="51"/>
@@ -15102,7 +15109,7 @@
       <c r="AK212" s="90"/>
       <c r="AL212" s="97"/>
       <c r="AM212" s="160" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN212" s="161"/>
       <c r="AO212" s="162"/>
@@ -15192,7 +15199,7 @@
       <c r="AK214" s="91"/>
       <c r="AL214" s="33"/>
       <c r="AM214" s="169" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AN214" s="164"/>
       <c r="AO214" s="165"/>
@@ -16029,7 +16036,7 @@
         <v>11</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F233" s="92"/>
       <c r="G233" s="92"/>
@@ -16142,17 +16149,17 @@
       <c r="AA235" s="62"/>
       <c r="AB235" s="62"/>
       <c r="AC235" s="63"/>
-      <c r="AD235" s="192" t="s">
+      <c r="AD235" s="207" t="s">
         <v>239</v>
       </c>
-      <c r="AE235" s="193"/>
-      <c r="AF235" s="193"/>
-      <c r="AG235" s="193"/>
-      <c r="AH235" s="193"/>
-      <c r="AI235" s="193"/>
-      <c r="AJ235" s="193"/>
-      <c r="AK235" s="193"/>
-      <c r="AL235" s="194"/>
+      <c r="AE235" s="208"/>
+      <c r="AF235" s="208"/>
+      <c r="AG235" s="208"/>
+      <c r="AH235" s="208"/>
+      <c r="AI235" s="208"/>
+      <c r="AJ235" s="208"/>
+      <c r="AK235" s="208"/>
+      <c r="AL235" s="209"/>
       <c r="AM235" s="92"/>
       <c r="AN235" s="2"/>
       <c r="AP235" s="5"/>
@@ -16210,7 +16217,7 @@
     <row r="237" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A237" s="4"/>
       <c r="C237" s="93" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D237" s="94"/>
       <c r="E237" s="94"/>
@@ -16220,7 +16227,7 @@
       <c r="I237" s="96"/>
       <c r="J237" s="104"/>
       <c r="K237" s="100" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L237" s="100"/>
       <c r="M237" s="100"/>
@@ -16240,21 +16247,21 @@
       <c r="AA237" s="100"/>
       <c r="AB237" s="100"/>
       <c r="AC237" s="104"/>
-      <c r="AD237" s="183" t="s">
+      <c r="AD237" s="198" t="s">
         <v>8</v>
       </c>
-      <c r="AE237" s="184"/>
-      <c r="AF237" s="184"/>
-      <c r="AG237" s="185"/>
-      <c r="AH237" s="183" t="s">
+      <c r="AE237" s="199"/>
+      <c r="AF237" s="199"/>
+      <c r="AG237" s="200"/>
+      <c r="AH237" s="198" t="s">
         <v>8</v>
       </c>
-      <c r="AI237" s="185"/>
-      <c r="AJ237" s="183" t="s">
+      <c r="AI237" s="200"/>
+      <c r="AJ237" s="198" t="s">
         <v>8</v>
       </c>
-      <c r="AK237" s="184"/>
-      <c r="AL237" s="185"/>
+      <c r="AK237" s="199"/>
+      <c r="AL237" s="200"/>
       <c r="AM237" s="92"/>
       <c r="AN237" s="2"/>
       <c r="AP237" s="5"/>
@@ -16271,7 +16278,7 @@
       <c r="I238" s="90"/>
       <c r="J238" s="128"/>
       <c r="K238" s="92" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L238" s="92"/>
       <c r="M238" s="92"/>
@@ -16291,15 +16298,15 @@
       <c r="AA238" s="92"/>
       <c r="AB238" s="92"/>
       <c r="AC238" s="128"/>
-      <c r="AD238" s="186"/>
-      <c r="AE238" s="187"/>
-      <c r="AF238" s="187"/>
-      <c r="AG238" s="188"/>
-      <c r="AH238" s="186"/>
-      <c r="AI238" s="188"/>
-      <c r="AJ238" s="186"/>
-      <c r="AK238" s="187"/>
-      <c r="AL238" s="188"/>
+      <c r="AD238" s="201"/>
+      <c r="AE238" s="202"/>
+      <c r="AF238" s="202"/>
+      <c r="AG238" s="203"/>
+      <c r="AH238" s="201"/>
+      <c r="AI238" s="203"/>
+      <c r="AJ238" s="201"/>
+      <c r="AK238" s="202"/>
+      <c r="AL238" s="203"/>
       <c r="AM238" s="92"/>
       <c r="AN238" s="2"/>
       <c r="AP238" s="5"/>
@@ -16316,7 +16323,7 @@
       <c r="I239" s="90"/>
       <c r="J239" s="128"/>
       <c r="K239" s="119" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L239" s="92"/>
       <c r="M239" s="92"/>
@@ -16336,15 +16343,15 @@
       <c r="AA239" s="92"/>
       <c r="AB239" s="92"/>
       <c r="AC239" s="128"/>
-      <c r="AD239" s="186"/>
-      <c r="AE239" s="187"/>
-      <c r="AF239" s="187"/>
-      <c r="AG239" s="188"/>
-      <c r="AH239" s="186"/>
-      <c r="AI239" s="188"/>
-      <c r="AJ239" s="186"/>
-      <c r="AK239" s="187"/>
-      <c r="AL239" s="188"/>
+      <c r="AD239" s="201"/>
+      <c r="AE239" s="202"/>
+      <c r="AF239" s="202"/>
+      <c r="AG239" s="203"/>
+      <c r="AH239" s="201"/>
+      <c r="AI239" s="203"/>
+      <c r="AJ239" s="201"/>
+      <c r="AK239" s="202"/>
+      <c r="AL239" s="203"/>
       <c r="AM239" s="92"/>
       <c r="AN239" s="2"/>
       <c r="AP239" s="5"/>
@@ -16361,7 +16368,7 @@
       <c r="I240" s="172"/>
       <c r="J240" s="121"/>
       <c r="K240" s="113" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L240" s="113"/>
       <c r="M240" s="113"/>
@@ -16381,15 +16388,15 @@
       <c r="AA240" s="113"/>
       <c r="AB240" s="113"/>
       <c r="AC240" s="121"/>
-      <c r="AD240" s="189"/>
-      <c r="AE240" s="190"/>
-      <c r="AF240" s="190"/>
-      <c r="AG240" s="191"/>
-      <c r="AH240" s="189"/>
-      <c r="AI240" s="191"/>
-      <c r="AJ240" s="189"/>
-      <c r="AK240" s="190"/>
-      <c r="AL240" s="191"/>
+      <c r="AD240" s="204"/>
+      <c r="AE240" s="205"/>
+      <c r="AF240" s="205"/>
+      <c r="AG240" s="206"/>
+      <c r="AH240" s="204"/>
+      <c r="AI240" s="206"/>
+      <c r="AJ240" s="204"/>
+      <c r="AK240" s="205"/>
+      <c r="AL240" s="206"/>
       <c r="AM240" s="92"/>
       <c r="AN240" s="2"/>
       <c r="AP240" s="5"/>
@@ -16398,7 +16405,7 @@
     <row r="241" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A241" s="4"/>
       <c r="C241" s="93" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D241" s="94"/>
       <c r="E241" s="94"/>
@@ -16408,7 +16415,7 @@
       <c r="I241" s="117"/>
       <c r="J241" s="173"/>
       <c r="K241" s="117" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L241" s="117"/>
       <c r="M241" s="117"/>
@@ -16459,7 +16466,7 @@
       <c r="I242" s="119"/>
       <c r="J242" s="120"/>
       <c r="K242" s="119" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L242" s="119"/>
       <c r="M242" s="119"/>
@@ -16504,7 +16511,7 @@
       <c r="I243" s="119"/>
       <c r="J243" s="120"/>
       <c r="K243" s="119" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L243" s="119"/>
       <c r="M243" s="119"/>
@@ -16549,7 +16556,7 @@
       <c r="I244" s="113"/>
       <c r="J244" s="121"/>
       <c r="K244" s="113" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L244" s="113"/>
       <c r="M244" s="113"/>
@@ -16586,7 +16593,7 @@
     <row r="245" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A245" s="4"/>
       <c r="C245" s="93" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D245" s="94"/>
       <c r="E245" s="94"/>
@@ -16596,7 +16603,7 @@
       <c r="I245" s="117"/>
       <c r="J245" s="173"/>
       <c r="K245" s="117" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L245" s="117"/>
       <c r="M245" s="117"/>
@@ -16647,7 +16654,7 @@
       <c r="I246" s="119"/>
       <c r="J246" s="120"/>
       <c r="K246" s="119" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L246" s="119"/>
       <c r="M246" s="119"/>
@@ -16692,7 +16699,7 @@
       <c r="I247" s="90"/>
       <c r="J247" s="128"/>
       <c r="K247" s="119" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L247" s="92"/>
       <c r="M247" s="92"/>
@@ -16737,7 +16744,7 @@
       <c r="I248" s="172"/>
       <c r="J248" s="121"/>
       <c r="K248" s="113" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L248" s="113"/>
       <c r="M248" s="113"/>
@@ -16774,7 +16781,7 @@
     <row r="249" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A249" s="4"/>
       <c r="C249" s="93" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D249" s="94"/>
       <c r="E249" s="94"/>
@@ -16784,7 +16791,7 @@
       <c r="I249" s="117"/>
       <c r="J249" s="173"/>
       <c r="K249" s="117" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L249" s="117"/>
       <c r="M249" s="117"/>
@@ -16835,7 +16842,7 @@
       <c r="I250" s="113"/>
       <c r="J250" s="121"/>
       <c r="K250" s="113" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L250" s="113"/>
       <c r="M250" s="113"/>
@@ -17077,17 +17084,17 @@
       <c r="AA255" s="62"/>
       <c r="AB255" s="62"/>
       <c r="AC255" s="63"/>
-      <c r="AD255" s="192" t="s">
+      <c r="AD255" s="207" t="s">
         <v>239</v>
       </c>
-      <c r="AE255" s="193"/>
-      <c r="AF255" s="193"/>
-      <c r="AG255" s="193"/>
-      <c r="AH255" s="193"/>
-      <c r="AI255" s="193"/>
-      <c r="AJ255" s="193"/>
-      <c r="AK255" s="193"/>
-      <c r="AL255" s="194"/>
+      <c r="AE255" s="208"/>
+      <c r="AF255" s="208"/>
+      <c r="AG255" s="208"/>
+      <c r="AH255" s="208"/>
+      <c r="AI255" s="208"/>
+      <c r="AJ255" s="208"/>
+      <c r="AK255" s="208"/>
+      <c r="AL255" s="209"/>
       <c r="AM255" s="92"/>
       <c r="AN255" s="2"/>
       <c r="AP255" s="5"/>
@@ -17179,21 +17186,21 @@
       <c r="AA257" s="100"/>
       <c r="AB257" s="100"/>
       <c r="AC257" s="104"/>
-      <c r="AD257" s="235" t="s">
+      <c r="AD257" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="AE257" s="241"/>
-      <c r="AF257" s="241"/>
-      <c r="AG257" s="236"/>
-      <c r="AH257" s="235" t="s">
+      <c r="AE257" s="237"/>
+      <c r="AF257" s="237"/>
+      <c r="AG257" s="232"/>
+      <c r="AH257" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="AI257" s="236"/>
-      <c r="AJ257" s="235" t="s">
+      <c r="AI257" s="232"/>
+      <c r="AJ257" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="AK257" s="241"/>
-      <c r="AL257" s="236"/>
+      <c r="AK257" s="237"/>
+      <c r="AL257" s="232"/>
       <c r="AM257" s="92"/>
       <c r="AN257" s="2"/>
       <c r="AP257" s="5"/>
@@ -17231,15 +17238,15 @@
       <c r="AA258" s="99"/>
       <c r="AB258" s="99"/>
       <c r="AC258" s="103"/>
-      <c r="AD258" s="237"/>
-      <c r="AE258" s="242"/>
-      <c r="AF258" s="242"/>
-      <c r="AG258" s="238"/>
-      <c r="AH258" s="237"/>
-      <c r="AI258" s="238"/>
-      <c r="AJ258" s="237"/>
-      <c r="AK258" s="242"/>
-      <c r="AL258" s="238"/>
+      <c r="AD258" s="233"/>
+      <c r="AE258" s="238"/>
+      <c r="AF258" s="238"/>
+      <c r="AG258" s="234"/>
+      <c r="AH258" s="233"/>
+      <c r="AI258" s="234"/>
+      <c r="AJ258" s="233"/>
+      <c r="AK258" s="238"/>
+      <c r="AL258" s="234"/>
       <c r="AM258" s="92"/>
       <c r="AN258" s="2"/>
       <c r="AP258" s="5"/>
@@ -17279,21 +17286,21 @@
       <c r="AA259" s="98"/>
       <c r="AB259" s="98"/>
       <c r="AC259" s="102"/>
-      <c r="AD259" s="235" t="s">
+      <c r="AD259" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="AE259" s="241"/>
-      <c r="AF259" s="241"/>
-      <c r="AG259" s="236"/>
-      <c r="AH259" s="235" t="s">
+      <c r="AE259" s="237"/>
+      <c r="AF259" s="237"/>
+      <c r="AG259" s="232"/>
+      <c r="AH259" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="AI259" s="236"/>
-      <c r="AJ259" s="235" t="s">
+      <c r="AI259" s="232"/>
+      <c r="AJ259" s="231" t="s">
         <v>8</v>
       </c>
-      <c r="AK259" s="241"/>
-      <c r="AL259" s="236"/>
+      <c r="AK259" s="237"/>
+      <c r="AL259" s="232"/>
       <c r="AM259" s="92"/>
       <c r="AN259" s="2"/>
       <c r="AP259" s="5"/>
@@ -17333,21 +17340,21 @@
       <c r="AA260" s="105"/>
       <c r="AB260" s="105"/>
       <c r="AC260" s="116"/>
-      <c r="AD260" s="239" t="s">
+      <c r="AD260" s="235" t="s">
         <v>8</v>
       </c>
-      <c r="AE260" s="243"/>
-      <c r="AF260" s="243"/>
-      <c r="AG260" s="240"/>
-      <c r="AH260" s="239" t="s">
+      <c r="AE260" s="239"/>
+      <c r="AF260" s="239"/>
+      <c r="AG260" s="236"/>
+      <c r="AH260" s="235" t="s">
         <v>8</v>
       </c>
-      <c r="AI260" s="240"/>
-      <c r="AJ260" s="239" t="s">
+      <c r="AI260" s="236"/>
+      <c r="AJ260" s="235" t="s">
         <v>8</v>
       </c>
-      <c r="AK260" s="243"/>
-      <c r="AL260" s="240"/>
+      <c r="AK260" s="239"/>
+      <c r="AL260" s="236"/>
       <c r="AM260" s="92"/>
       <c r="AN260" s="2"/>
       <c r="AP260" s="5"/>
@@ -17389,21 +17396,21 @@
       <c r="AA261" s="105"/>
       <c r="AB261" s="105"/>
       <c r="AC261" s="116"/>
-      <c r="AD261" s="239" t="s">
+      <c r="AD261" s="235" t="s">
         <v>8</v>
       </c>
-      <c r="AE261" s="243"/>
-      <c r="AF261" s="243"/>
-      <c r="AG261" s="240"/>
-      <c r="AH261" s="239" t="s">
+      <c r="AE261" s="239"/>
+      <c r="AF261" s="239"/>
+      <c r="AG261" s="236"/>
+      <c r="AH261" s="235" t="s">
         <v>8</v>
       </c>
-      <c r="AI261" s="240"/>
-      <c r="AJ261" s="239" t="s">
+      <c r="AI261" s="236"/>
+      <c r="AJ261" s="235" t="s">
         <v>14</v>
       </c>
-      <c r="AK261" s="243"/>
-      <c r="AL261" s="240"/>
+      <c r="AK261" s="239"/>
+      <c r="AL261" s="236"/>
       <c r="AM261" s="92"/>
       <c r="AN261" s="2"/>
       <c r="AP261" s="5"/>
@@ -17443,21 +17450,21 @@
       <c r="AA262" s="105"/>
       <c r="AB262" s="105"/>
       <c r="AC262" s="116"/>
-      <c r="AD262" s="239" t="s">
+      <c r="AD262" s="235" t="s">
         <v>14</v>
       </c>
-      <c r="AE262" s="243"/>
-      <c r="AF262" s="243"/>
-      <c r="AG262" s="240"/>
-      <c r="AH262" s="239" t="s">
+      <c r="AE262" s="239"/>
+      <c r="AF262" s="239"/>
+      <c r="AG262" s="236"/>
+      <c r="AH262" s="235" t="s">
         <v>14</v>
       </c>
-      <c r="AI262" s="240"/>
-      <c r="AJ262" s="239" t="s">
+      <c r="AI262" s="236"/>
+      <c r="AJ262" s="235" t="s">
         <v>8</v>
       </c>
-      <c r="AK262" s="243"/>
-      <c r="AL262" s="240"/>
+      <c r="AK262" s="239"/>
+      <c r="AL262" s="236"/>
       <c r="AM262" s="92"/>
       <c r="AN262" s="2"/>
       <c r="AP262" s="5"/>
@@ -17497,21 +17504,21 @@
       <c r="AA263" s="105"/>
       <c r="AB263" s="105"/>
       <c r="AC263" s="116"/>
-      <c r="AD263" s="244" t="s">
+      <c r="AD263" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="AE263" s="245"/>
-      <c r="AF263" s="245"/>
-      <c r="AG263" s="246"/>
-      <c r="AH263" s="244" t="s">
+      <c r="AE263" s="241"/>
+      <c r="AF263" s="241"/>
+      <c r="AG263" s="242"/>
+      <c r="AH263" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="AI263" s="246"/>
-      <c r="AJ263" s="239" t="s">
+      <c r="AI263" s="242"/>
+      <c r="AJ263" s="235" t="s">
         <v>14</v>
       </c>
-      <c r="AK263" s="243"/>
-      <c r="AL263" s="240"/>
+      <c r="AK263" s="239"/>
+      <c r="AL263" s="236"/>
       <c r="AM263" s="92"/>
       <c r="AN263" s="2"/>
       <c r="AP263" s="5"/>
@@ -17553,21 +17560,21 @@
       <c r="AA264" s="98"/>
       <c r="AB264" s="98"/>
       <c r="AC264" s="102"/>
-      <c r="AD264" s="216" t="s">
+      <c r="AD264" s="213" t="s">
         <v>8</v>
       </c>
-      <c r="AE264" s="217"/>
-      <c r="AF264" s="217"/>
-      <c r="AG264" s="218"/>
-      <c r="AH264" s="216" t="s">
+      <c r="AE264" s="214"/>
+      <c r="AF264" s="214"/>
+      <c r="AG264" s="215"/>
+      <c r="AH264" s="213" t="s">
         <v>8</v>
       </c>
-      <c r="AI264" s="218"/>
-      <c r="AJ264" s="216" t="s">
+      <c r="AI264" s="215"/>
+      <c r="AJ264" s="213" t="s">
         <v>8</v>
       </c>
-      <c r="AK264" s="217"/>
-      <c r="AL264" s="218"/>
+      <c r="AK264" s="214"/>
+      <c r="AL264" s="215"/>
       <c r="AM264" s="92"/>
       <c r="AN264" s="2"/>
       <c r="AP264" s="5"/>
@@ -18169,6 +18176,19 @@
     </row>
   </sheetData>
   <mergeCells count="234">
+    <mergeCell ref="Y129:AD129"/>
+    <mergeCell ref="S129:X129"/>
+    <mergeCell ref="Y128:AD128"/>
+    <mergeCell ref="S128:X128"/>
+    <mergeCell ref="S160:X160"/>
+    <mergeCell ref="Y159:AD159"/>
+    <mergeCell ref="S159:X159"/>
+    <mergeCell ref="Y158:AD158"/>
+    <mergeCell ref="Y157:AD157"/>
+    <mergeCell ref="Y151:AD151"/>
+    <mergeCell ref="Y150:AD150"/>
+    <mergeCell ref="AE149:AJ149"/>
+    <mergeCell ref="Y149:AD149"/>
     <mergeCell ref="S184:X184"/>
     <mergeCell ref="Y184:AD184"/>
     <mergeCell ref="AE184:AJ184"/>
@@ -18204,15 +18224,11 @@
     <mergeCell ref="S167:X167"/>
     <mergeCell ref="S165:X165"/>
     <mergeCell ref="S169:X169"/>
-    <mergeCell ref="AD255:AL255"/>
-    <mergeCell ref="AD257:AG257"/>
-    <mergeCell ref="AD258:AG258"/>
-    <mergeCell ref="AD259:AG259"/>
+    <mergeCell ref="Y170:AD170"/>
+    <mergeCell ref="S168:X168"/>
     <mergeCell ref="AD260:AG260"/>
     <mergeCell ref="AD261:AG261"/>
     <mergeCell ref="AD262:AG262"/>
-    <mergeCell ref="Y157:AD157"/>
-    <mergeCell ref="Y158:AD158"/>
     <mergeCell ref="AE162:AJ162"/>
     <mergeCell ref="AE163:AJ163"/>
     <mergeCell ref="AE167:AJ167"/>
@@ -18228,6 +18244,8 @@
     <mergeCell ref="AE170:AJ170"/>
     <mergeCell ref="Y166:AD166"/>
     <mergeCell ref="Y165:AD165"/>
+    <mergeCell ref="L50:AD50"/>
+    <mergeCell ref="AE133:AJ133"/>
     <mergeCell ref="AD264:AG264"/>
     <mergeCell ref="AH257:AI257"/>
     <mergeCell ref="AH258:AI258"/>
@@ -18246,7 +18264,10 @@
     <mergeCell ref="AD263:AG263"/>
     <mergeCell ref="AH263:AI263"/>
     <mergeCell ref="AJ263:AL263"/>
-    <mergeCell ref="S135:X135"/>
+    <mergeCell ref="AD255:AL255"/>
+    <mergeCell ref="AD257:AG257"/>
+    <mergeCell ref="AD258:AG258"/>
+    <mergeCell ref="AD259:AG259"/>
     <mergeCell ref="AL1:AP1"/>
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="AL2:AP2"/>
@@ -18265,24 +18286,6 @@
     <mergeCell ref="L40:AD40"/>
     <mergeCell ref="L43:AD43"/>
     <mergeCell ref="L45:AD45"/>
-    <mergeCell ref="S133:X133"/>
-    <mergeCell ref="L50:AD50"/>
-    <mergeCell ref="AE160:AJ160"/>
-    <mergeCell ref="AE154:AJ154"/>
-    <mergeCell ref="AE155:AJ155"/>
-    <mergeCell ref="AE156:AJ156"/>
-    <mergeCell ref="AE157:AJ157"/>
-    <mergeCell ref="AE158:AJ158"/>
-    <mergeCell ref="AE159:AJ159"/>
-    <mergeCell ref="S125:X125"/>
-    <mergeCell ref="Y125:AD125"/>
-    <mergeCell ref="Y126:AD126"/>
-    <mergeCell ref="AE125:AJ125"/>
-    <mergeCell ref="AE126:AJ126"/>
-    <mergeCell ref="S128:X128"/>
-    <mergeCell ref="S129:X129"/>
-    <mergeCell ref="Y128:AD128"/>
-    <mergeCell ref="Y129:AD129"/>
     <mergeCell ref="S156:X156"/>
     <mergeCell ref="S157:X157"/>
     <mergeCell ref="S130:X130"/>
@@ -18291,8 +18294,14 @@
     <mergeCell ref="S134:X134"/>
     <mergeCell ref="Y143:AD143"/>
     <mergeCell ref="Y144:AD144"/>
-    <mergeCell ref="S152:X152"/>
-    <mergeCell ref="Y152:AD152"/>
+    <mergeCell ref="S135:X135"/>
+    <mergeCell ref="S133:X133"/>
+    <mergeCell ref="Y148:AD148"/>
+    <mergeCell ref="S125:X125"/>
+    <mergeCell ref="Y125:AD125"/>
+    <mergeCell ref="Y126:AD126"/>
+    <mergeCell ref="AE125:AJ125"/>
+    <mergeCell ref="AE126:AJ126"/>
     <mergeCell ref="S153:X153"/>
     <mergeCell ref="S154:X154"/>
     <mergeCell ref="Y155:AD155"/>
@@ -18315,9 +18324,8 @@
     <mergeCell ref="AE145:AJ145"/>
     <mergeCell ref="AE146:AJ146"/>
     <mergeCell ref="AE147:AJ147"/>
-    <mergeCell ref="AE148:AJ148"/>
-    <mergeCell ref="S142:X142"/>
-    <mergeCell ref="AE151:AJ151"/>
+    <mergeCell ref="AE154:AJ154"/>
+    <mergeCell ref="AE155:AJ155"/>
     <mergeCell ref="Y132:AD132"/>
     <mergeCell ref="Y134:AD134"/>
     <mergeCell ref="Y135:AD135"/>
@@ -18327,8 +18335,6 @@
     <mergeCell ref="S148:X148"/>
     <mergeCell ref="S143:X143"/>
     <mergeCell ref="S144:X144"/>
-    <mergeCell ref="S149:X149"/>
-    <mergeCell ref="S150:X150"/>
     <mergeCell ref="S136:X136"/>
     <mergeCell ref="S145:X145"/>
     <mergeCell ref="S146:X146"/>
@@ -18339,7 +18345,6 @@
     <mergeCell ref="S141:X141"/>
     <mergeCell ref="Y145:AD145"/>
     <mergeCell ref="Y146:AD146"/>
-    <mergeCell ref="Y147:AD147"/>
     <mergeCell ref="Y133:AD133"/>
     <mergeCell ref="Y138:AD138"/>
     <mergeCell ref="Y139:AD139"/>
@@ -18348,36 +18353,30 @@
     <mergeCell ref="Y142:AD142"/>
     <mergeCell ref="Y164:AD164"/>
     <mergeCell ref="Y169:AD169"/>
-    <mergeCell ref="Y170:AD170"/>
-    <mergeCell ref="S168:X168"/>
-    <mergeCell ref="AE133:AJ133"/>
+    <mergeCell ref="AE148:AJ148"/>
+    <mergeCell ref="AE151:AJ151"/>
+    <mergeCell ref="Y152:AD152"/>
+    <mergeCell ref="AE160:AJ160"/>
+    <mergeCell ref="AE156:AJ156"/>
+    <mergeCell ref="AE157:AJ157"/>
+    <mergeCell ref="AE158:AJ158"/>
+    <mergeCell ref="AE159:AJ159"/>
+    <mergeCell ref="Y160:AD160"/>
+    <mergeCell ref="AE144:AJ144"/>
+    <mergeCell ref="AE143:AJ143"/>
+    <mergeCell ref="AE142:AJ142"/>
+    <mergeCell ref="AE141:AJ141"/>
+    <mergeCell ref="AE140:AJ140"/>
+    <mergeCell ref="AE139:AJ139"/>
     <mergeCell ref="AE138:AJ138"/>
-    <mergeCell ref="AE139:AJ139"/>
-    <mergeCell ref="AE140:AJ140"/>
-    <mergeCell ref="AE141:AJ141"/>
-    <mergeCell ref="Y159:AD159"/>
-    <mergeCell ref="Y160:AD160"/>
-    <mergeCell ref="Y161:AD161"/>
-    <mergeCell ref="Y162:AD162"/>
-    <mergeCell ref="AE142:AJ142"/>
-    <mergeCell ref="AE143:AJ143"/>
-    <mergeCell ref="AE144:AJ144"/>
-    <mergeCell ref="AE149:AJ149"/>
-    <mergeCell ref="Y149:AD149"/>
-    <mergeCell ref="AE161:AJ161"/>
-    <mergeCell ref="Y148:AD148"/>
-    <mergeCell ref="Y150:AD150"/>
-    <mergeCell ref="Y153:AD153"/>
-    <mergeCell ref="Y154:AD154"/>
-    <mergeCell ref="S161:X161"/>
     <mergeCell ref="AD237:AG240"/>
     <mergeCell ref="AJ237:AL240"/>
     <mergeCell ref="AH237:AI240"/>
     <mergeCell ref="AD235:AL235"/>
-    <mergeCell ref="S159:X159"/>
-    <mergeCell ref="S160:X160"/>
     <mergeCell ref="S183:X183"/>
-    <mergeCell ref="Y151:AD151"/>
+    <mergeCell ref="Y161:AD161"/>
+    <mergeCell ref="Y162:AD162"/>
+    <mergeCell ref="AE161:AJ161"/>
     <mergeCell ref="S137:X137"/>
     <mergeCell ref="Y137:AD137"/>
     <mergeCell ref="AE137:AJ137"/>
@@ -18394,6 +18393,14 @@
     <mergeCell ref="AE165:AJ165"/>
     <mergeCell ref="AE166:AJ166"/>
     <mergeCell ref="S164:X164"/>
+    <mergeCell ref="S161:X161"/>
+    <mergeCell ref="Y153:AD153"/>
+    <mergeCell ref="Y154:AD154"/>
+    <mergeCell ref="Y147:AD147"/>
+    <mergeCell ref="S142:X142"/>
+    <mergeCell ref="S149:X149"/>
+    <mergeCell ref="S150:X150"/>
+    <mergeCell ref="S152:X152"/>
     <mergeCell ref="AD245:AG248"/>
     <mergeCell ref="AH245:AI248"/>
     <mergeCell ref="AJ245:AL248"/>

</xml_diff>

<commit_message>
OwnerSearchAPI - Added ownerUserRoleLevel and ownerGroupType.
</commit_message>
<xml_diff>
--- a/skrum_docs/02_SpecificationDocs/RequirementDefinition.xlsx
+++ b/skrum_docs/02_SpecificationDocs/RequirementDefinition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="460" windowWidth="27520" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="更新履歴" sheetId="2" r:id="rId1"/>
@@ -3283,7 +3283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3305,12 +3305,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4523,7 +4517,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -4692,18 +4686,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4733,22 +4727,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4769,13 +4754,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4785,15 +4797,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4859,15 +4862,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4893,33 +4887,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="85" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5022,8 +4989,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3162300" y="15468600"/>
-          <a:ext cx="1714500" cy="1981200"/>
+          <a:off x="3619500" y="15468600"/>
+          <a:ext cx="1981200" cy="1981200"/>
           <a:chOff x="3479800" y="21310600"/>
           <a:chExt cx="1981200" cy="1981200"/>
         </a:xfrm>
@@ -5141,8 +5108,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5867400" y="15468600"/>
-          <a:ext cx="1752600" cy="1981200"/>
+          <a:off x="6743700" y="15468600"/>
+          <a:ext cx="1981200" cy="1981200"/>
           <a:chOff x="6743700" y="21310600"/>
           <a:chExt cx="1981200" cy="1981200"/>
         </a:xfrm>
@@ -6509,12 +6476,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="13" style="69" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="48.5" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -7261,21 +7228,21 @@
       <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="3.33203125" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="3.28515625" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="3.33203125" style="1"/>
+    <col min="1" max="16384" width="3.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="222" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="223"/>
+      <c r="E1" s="223"/>
+      <c r="F1" s="223"/>
+      <c r="G1" s="224"/>
       <c r="H1" s="47"/>
       <c r="I1" s="44" t="s">
         <v>72</v>
@@ -7286,53 +7253,53 @@
       <c r="M1" s="45"/>
       <c r="N1" s="45"/>
       <c r="O1" s="46"/>
-      <c r="P1" s="228" t="s">
+      <c r="P1" s="231" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="229"/>
-      <c r="R1" s="229"/>
-      <c r="S1" s="229"/>
-      <c r="T1" s="229"/>
-      <c r="U1" s="229"/>
-      <c r="V1" s="229"/>
-      <c r="W1" s="229"/>
-      <c r="X1" s="229"/>
-      <c r="Y1" s="229"/>
-      <c r="Z1" s="230"/>
+      <c r="Q1" s="232"/>
+      <c r="R1" s="232"/>
+      <c r="S1" s="232"/>
+      <c r="T1" s="232"/>
+      <c r="U1" s="232"/>
+      <c r="V1" s="232"/>
+      <c r="W1" s="232"/>
+      <c r="X1" s="232"/>
+      <c r="Y1" s="232"/>
+      <c r="Z1" s="233"/>
       <c r="AA1" s="44" t="s">
         <v>67</v>
       </c>
       <c r="AB1" s="42"/>
       <c r="AC1" s="43"/>
-      <c r="AD1" s="225">
+      <c r="AD1" s="228">
         <v>42760</v>
       </c>
-      <c r="AE1" s="226"/>
-      <c r="AF1" s="226"/>
-      <c r="AG1" s="226"/>
-      <c r="AH1" s="227"/>
+      <c r="AE1" s="229"/>
+      <c r="AF1" s="229"/>
+      <c r="AG1" s="229"/>
+      <c r="AH1" s="230"/>
       <c r="AI1" s="44" t="s">
         <v>69</v>
       </c>
       <c r="AJ1" s="45"/>
       <c r="AK1" s="46"/>
-      <c r="AL1" s="216" t="s">
+      <c r="AL1" s="219" t="s">
         <v>71</v>
       </c>
-      <c r="AM1" s="217"/>
-      <c r="AN1" s="217"/>
-      <c r="AO1" s="217"/>
-      <c r="AP1" s="218"/>
+      <c r="AM1" s="220"/>
+      <c r="AN1" s="220"/>
+      <c r="AO1" s="220"/>
+      <c r="AP1" s="221"/>
       <c r="AQ1" s="2"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A2" s="222"/>
-      <c r="B2" s="223"/>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="224"/>
+      <c r="A2" s="225"/>
+      <c r="B2" s="226"/>
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="227"/>
       <c r="H2" s="48"/>
       <c r="I2" s="44" t="s">
         <v>73</v>
@@ -7343,41 +7310,41 @@
       <c r="M2" s="45"/>
       <c r="N2" s="45"/>
       <c r="O2" s="46"/>
-      <c r="P2" s="228"/>
-      <c r="Q2" s="229"/>
-      <c r="R2" s="229"/>
-      <c r="S2" s="229"/>
-      <c r="T2" s="229"/>
-      <c r="U2" s="229"/>
-      <c r="V2" s="229"/>
-      <c r="W2" s="229"/>
-      <c r="X2" s="229"/>
-      <c r="Y2" s="229"/>
-      <c r="Z2" s="230"/>
+      <c r="P2" s="231"/>
+      <c r="Q2" s="232"/>
+      <c r="R2" s="232"/>
+      <c r="S2" s="232"/>
+      <c r="T2" s="232"/>
+      <c r="U2" s="232"/>
+      <c r="V2" s="232"/>
+      <c r="W2" s="232"/>
+      <c r="X2" s="232"/>
+      <c r="Y2" s="232"/>
+      <c r="Z2" s="233"/>
       <c r="AA2" s="44" t="s">
         <v>68</v>
       </c>
       <c r="AB2" s="42"/>
       <c r="AC2" s="43"/>
-      <c r="AD2" s="225">
+      <c r="AD2" s="228">
         <v>42991</v>
       </c>
-      <c r="AE2" s="226"/>
-      <c r="AF2" s="226"/>
-      <c r="AG2" s="226"/>
-      <c r="AH2" s="227"/>
+      <c r="AE2" s="229"/>
+      <c r="AF2" s="229"/>
+      <c r="AG2" s="229"/>
+      <c r="AH2" s="230"/>
       <c r="AI2" s="44" t="s">
         <v>70</v>
       </c>
       <c r="AJ2" s="45"/>
       <c r="AK2" s="46"/>
-      <c r="AL2" s="216" t="s">
+      <c r="AL2" s="219" t="s">
         <v>71</v>
       </c>
-      <c r="AM2" s="217"/>
-      <c r="AN2" s="217"/>
-      <c r="AO2" s="217"/>
-      <c r="AP2" s="218"/>
+      <c r="AM2" s="220"/>
+      <c r="AN2" s="220"/>
+      <c r="AO2" s="220"/>
+      <c r="AP2" s="221"/>
       <c r="AQ2" s="2"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
@@ -7915,27 +7882,27 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="34"/>
-      <c r="L19" s="198" t="s">
+      <c r="L19" s="204" t="s">
         <v>47</v>
       </c>
-      <c r="M19" s="199"/>
-      <c r="N19" s="199"/>
-      <c r="O19" s="199"/>
-      <c r="P19" s="199"/>
-      <c r="Q19" s="199"/>
-      <c r="R19" s="199"/>
-      <c r="S19" s="199"/>
-      <c r="T19" s="199"/>
-      <c r="U19" s="199"/>
-      <c r="V19" s="199"/>
-      <c r="W19" s="199"/>
-      <c r="X19" s="199"/>
-      <c r="Y19" s="199"/>
-      <c r="Z19" s="199"/>
-      <c r="AA19" s="199"/>
-      <c r="AB19" s="199"/>
-      <c r="AC19" s="199"/>
-      <c r="AD19" s="200"/>
+      <c r="M19" s="205"/>
+      <c r="N19" s="205"/>
+      <c r="O19" s="205"/>
+      <c r="P19" s="205"/>
+      <c r="Q19" s="205"/>
+      <c r="R19" s="205"/>
+      <c r="S19" s="205"/>
+      <c r="T19" s="205"/>
+      <c r="U19" s="205"/>
+      <c r="V19" s="205"/>
+      <c r="W19" s="205"/>
+      <c r="X19" s="205"/>
+      <c r="Y19" s="205"/>
+      <c r="Z19" s="205"/>
+      <c r="AA19" s="205"/>
+      <c r="AB19" s="205"/>
+      <c r="AC19" s="205"/>
+      <c r="AD19" s="206"/>
       <c r="AE19" s="2"/>
       <c r="AP19" s="5"/>
       <c r="AQ19" s="2"/>
@@ -7951,27 +7918,27 @@
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="34"/>
-      <c r="L20" s="198" t="s">
+      <c r="L20" s="204" t="s">
         <v>48</v>
       </c>
-      <c r="M20" s="199"/>
-      <c r="N20" s="199"/>
-      <c r="O20" s="199"/>
-      <c r="P20" s="199"/>
-      <c r="Q20" s="199"/>
-      <c r="R20" s="199"/>
-      <c r="S20" s="199"/>
-      <c r="T20" s="199"/>
-      <c r="U20" s="199"/>
-      <c r="V20" s="199"/>
-      <c r="W20" s="199"/>
-      <c r="X20" s="199"/>
-      <c r="Y20" s="199"/>
-      <c r="Z20" s="199"/>
-      <c r="AA20" s="199"/>
-      <c r="AB20" s="199"/>
-      <c r="AC20" s="199"/>
-      <c r="AD20" s="200"/>
+      <c r="M20" s="205"/>
+      <c r="N20" s="205"/>
+      <c r="O20" s="205"/>
+      <c r="P20" s="205"/>
+      <c r="Q20" s="205"/>
+      <c r="R20" s="205"/>
+      <c r="S20" s="205"/>
+      <c r="T20" s="205"/>
+      <c r="U20" s="205"/>
+      <c r="V20" s="205"/>
+      <c r="W20" s="205"/>
+      <c r="X20" s="205"/>
+      <c r="Y20" s="205"/>
+      <c r="Z20" s="205"/>
+      <c r="AA20" s="205"/>
+      <c r="AB20" s="205"/>
+      <c r="AC20" s="205"/>
+      <c r="AD20" s="206"/>
       <c r="AE20" s="2"/>
       <c r="AP20" s="5"/>
       <c r="AQ20" s="2"/>
@@ -7987,27 +7954,27 @@
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
       <c r="K21" s="35"/>
-      <c r="L21" s="198" t="s">
+      <c r="L21" s="204" t="s">
         <v>49</v>
       </c>
-      <c r="M21" s="199"/>
-      <c r="N21" s="199"/>
-      <c r="O21" s="199"/>
-      <c r="P21" s="199"/>
-      <c r="Q21" s="199"/>
-      <c r="R21" s="199"/>
-      <c r="S21" s="199"/>
-      <c r="T21" s="199"/>
-      <c r="U21" s="199"/>
-      <c r="V21" s="199"/>
-      <c r="W21" s="199"/>
-      <c r="X21" s="199"/>
-      <c r="Y21" s="199"/>
-      <c r="Z21" s="199"/>
-      <c r="AA21" s="199"/>
-      <c r="AB21" s="199"/>
-      <c r="AC21" s="199"/>
-      <c r="AD21" s="200"/>
+      <c r="M21" s="205"/>
+      <c r="N21" s="205"/>
+      <c r="O21" s="205"/>
+      <c r="P21" s="205"/>
+      <c r="Q21" s="205"/>
+      <c r="R21" s="205"/>
+      <c r="S21" s="205"/>
+      <c r="T21" s="205"/>
+      <c r="U21" s="205"/>
+      <c r="V21" s="205"/>
+      <c r="W21" s="205"/>
+      <c r="X21" s="205"/>
+      <c r="Y21" s="205"/>
+      <c r="Z21" s="205"/>
+      <c r="AA21" s="205"/>
+      <c r="AB21" s="205"/>
+      <c r="AC21" s="205"/>
+      <c r="AD21" s="206"/>
       <c r="AE21" s="2"/>
       <c r="AP21" s="5"/>
       <c r="AQ21" s="2"/>
@@ -8461,27 +8428,27 @@
       <c r="I40" s="53"/>
       <c r="J40" s="53"/>
       <c r="K40" s="54"/>
-      <c r="L40" s="213" t="s">
+      <c r="L40" s="216" t="s">
         <v>52</v>
       </c>
-      <c r="M40" s="214"/>
-      <c r="N40" s="214"/>
-      <c r="O40" s="214"/>
-      <c r="P40" s="214"/>
-      <c r="Q40" s="214"/>
-      <c r="R40" s="214"/>
-      <c r="S40" s="214"/>
-      <c r="T40" s="214"/>
-      <c r="U40" s="214"/>
-      <c r="V40" s="214"/>
-      <c r="W40" s="214"/>
-      <c r="X40" s="214"/>
-      <c r="Y40" s="214"/>
-      <c r="Z40" s="214"/>
-      <c r="AA40" s="214"/>
-      <c r="AB40" s="214"/>
-      <c r="AC40" s="214"/>
-      <c r="AD40" s="215"/>
+      <c r="M40" s="217"/>
+      <c r="N40" s="217"/>
+      <c r="O40" s="217"/>
+      <c r="P40" s="217"/>
+      <c r="Q40" s="217"/>
+      <c r="R40" s="217"/>
+      <c r="S40" s="217"/>
+      <c r="T40" s="217"/>
+      <c r="U40" s="217"/>
+      <c r="V40" s="217"/>
+      <c r="W40" s="217"/>
+      <c r="X40" s="217"/>
+      <c r="Y40" s="217"/>
+      <c r="Z40" s="217"/>
+      <c r="AA40" s="217"/>
+      <c r="AB40" s="217"/>
+      <c r="AC40" s="217"/>
+      <c r="AD40" s="218"/>
       <c r="AE40" s="2"/>
       <c r="AP40" s="5"/>
       <c r="AQ40" s="2"/>
@@ -8497,27 +8464,27 @@
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="13"/>
-      <c r="L41" s="198" t="s">
+      <c r="L41" s="204" t="s">
         <v>50</v>
       </c>
-      <c r="M41" s="199"/>
-      <c r="N41" s="199"/>
-      <c r="O41" s="199"/>
-      <c r="P41" s="199"/>
-      <c r="Q41" s="199"/>
-      <c r="R41" s="199"/>
-      <c r="S41" s="199"/>
-      <c r="T41" s="199"/>
-      <c r="U41" s="199"/>
-      <c r="V41" s="199"/>
-      <c r="W41" s="199"/>
-      <c r="X41" s="199"/>
-      <c r="Y41" s="199"/>
-      <c r="Z41" s="199"/>
-      <c r="AA41" s="199"/>
-      <c r="AB41" s="199"/>
-      <c r="AC41" s="199"/>
-      <c r="AD41" s="200"/>
+      <c r="M41" s="205"/>
+      <c r="N41" s="205"/>
+      <c r="O41" s="205"/>
+      <c r="P41" s="205"/>
+      <c r="Q41" s="205"/>
+      <c r="R41" s="205"/>
+      <c r="S41" s="205"/>
+      <c r="T41" s="205"/>
+      <c r="U41" s="205"/>
+      <c r="V41" s="205"/>
+      <c r="W41" s="205"/>
+      <c r="X41" s="205"/>
+      <c r="Y41" s="205"/>
+      <c r="Z41" s="205"/>
+      <c r="AA41" s="205"/>
+      <c r="AB41" s="205"/>
+      <c r="AC41" s="205"/>
+      <c r="AD41" s="206"/>
       <c r="AE41" s="2"/>
       <c r="AP41" s="5"/>
       <c r="AQ41" s="2"/>
@@ -8533,27 +8500,27 @@
       <c r="I42" s="32"/>
       <c r="J42" s="32"/>
       <c r="K42" s="33"/>
-      <c r="L42" s="198" t="s">
+      <c r="L42" s="204" t="s">
         <v>63</v>
       </c>
-      <c r="M42" s="199"/>
-      <c r="N42" s="199"/>
-      <c r="O42" s="199"/>
-      <c r="P42" s="199"/>
-      <c r="Q42" s="199"/>
-      <c r="R42" s="199"/>
-      <c r="S42" s="199"/>
-      <c r="T42" s="199"/>
-      <c r="U42" s="199"/>
-      <c r="V42" s="199"/>
-      <c r="W42" s="199"/>
-      <c r="X42" s="199"/>
-      <c r="Y42" s="199"/>
-      <c r="Z42" s="199"/>
-      <c r="AA42" s="199"/>
-      <c r="AB42" s="199"/>
-      <c r="AC42" s="199"/>
-      <c r="AD42" s="200"/>
+      <c r="M42" s="205"/>
+      <c r="N42" s="205"/>
+      <c r="O42" s="205"/>
+      <c r="P42" s="205"/>
+      <c r="Q42" s="205"/>
+      <c r="R42" s="205"/>
+      <c r="S42" s="205"/>
+      <c r="T42" s="205"/>
+      <c r="U42" s="205"/>
+      <c r="V42" s="205"/>
+      <c r="W42" s="205"/>
+      <c r="X42" s="205"/>
+      <c r="Y42" s="205"/>
+      <c r="Z42" s="205"/>
+      <c r="AA42" s="205"/>
+      <c r="AB42" s="205"/>
+      <c r="AC42" s="205"/>
+      <c r="AD42" s="206"/>
       <c r="AE42" s="2"/>
       <c r="AP42" s="5"/>
       <c r="AQ42" s="2"/>
@@ -8569,27 +8536,27 @@
       <c r="I43" s="32"/>
       <c r="J43" s="32"/>
       <c r="K43" s="33"/>
-      <c r="L43" s="198" t="s">
+      <c r="L43" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="M43" s="199"/>
-      <c r="N43" s="199"/>
-      <c r="O43" s="199"/>
-      <c r="P43" s="199"/>
-      <c r="Q43" s="199"/>
-      <c r="R43" s="199"/>
-      <c r="S43" s="199"/>
-      <c r="T43" s="199"/>
-      <c r="U43" s="199"/>
-      <c r="V43" s="199"/>
-      <c r="W43" s="199"/>
-      <c r="X43" s="199"/>
-      <c r="Y43" s="199"/>
-      <c r="Z43" s="199"/>
-      <c r="AA43" s="199"/>
-      <c r="AB43" s="199"/>
-      <c r="AC43" s="199"/>
-      <c r="AD43" s="200"/>
+      <c r="M43" s="205"/>
+      <c r="N43" s="205"/>
+      <c r="O43" s="205"/>
+      <c r="P43" s="205"/>
+      <c r="Q43" s="205"/>
+      <c r="R43" s="205"/>
+      <c r="S43" s="205"/>
+      <c r="T43" s="205"/>
+      <c r="U43" s="205"/>
+      <c r="V43" s="205"/>
+      <c r="W43" s="205"/>
+      <c r="X43" s="205"/>
+      <c r="Y43" s="205"/>
+      <c r="Z43" s="205"/>
+      <c r="AA43" s="205"/>
+      <c r="AB43" s="205"/>
+      <c r="AC43" s="205"/>
+      <c r="AD43" s="206"/>
       <c r="AE43" s="2"/>
       <c r="AP43" s="5"/>
       <c r="AQ43" s="2"/>
@@ -8605,27 +8572,27 @@
       <c r="I44" s="32"/>
       <c r="J44" s="32"/>
       <c r="K44" s="33"/>
-      <c r="L44" s="198" t="s">
+      <c r="L44" s="204" t="s">
         <v>64</v>
       </c>
-      <c r="M44" s="199"/>
-      <c r="N44" s="199"/>
-      <c r="O44" s="199"/>
-      <c r="P44" s="199"/>
-      <c r="Q44" s="199"/>
-      <c r="R44" s="199"/>
-      <c r="S44" s="199"/>
-      <c r="T44" s="199"/>
-      <c r="U44" s="199"/>
-      <c r="V44" s="199"/>
-      <c r="W44" s="199"/>
-      <c r="X44" s="199"/>
-      <c r="Y44" s="199"/>
-      <c r="Z44" s="199"/>
-      <c r="AA44" s="199"/>
-      <c r="AB44" s="199"/>
-      <c r="AC44" s="199"/>
-      <c r="AD44" s="200"/>
+      <c r="M44" s="205"/>
+      <c r="N44" s="205"/>
+      <c r="O44" s="205"/>
+      <c r="P44" s="205"/>
+      <c r="Q44" s="205"/>
+      <c r="R44" s="205"/>
+      <c r="S44" s="205"/>
+      <c r="T44" s="205"/>
+      <c r="U44" s="205"/>
+      <c r="V44" s="205"/>
+      <c r="W44" s="205"/>
+      <c r="X44" s="205"/>
+      <c r="Y44" s="205"/>
+      <c r="Z44" s="205"/>
+      <c r="AA44" s="205"/>
+      <c r="AB44" s="205"/>
+      <c r="AC44" s="205"/>
+      <c r="AD44" s="206"/>
       <c r="AE44" s="2"/>
       <c r="AP44" s="5"/>
       <c r="AQ44" s="2"/>
@@ -8641,27 +8608,27 @@
       <c r="I45" s="32"/>
       <c r="J45" s="32"/>
       <c r="K45" s="33"/>
-      <c r="L45" s="198" t="s">
+      <c r="L45" s="204" t="s">
         <v>61</v>
       </c>
-      <c r="M45" s="199"/>
-      <c r="N45" s="199"/>
-      <c r="O45" s="199"/>
-      <c r="P45" s="199"/>
-      <c r="Q45" s="199"/>
-      <c r="R45" s="199"/>
-      <c r="S45" s="199"/>
-      <c r="T45" s="199"/>
-      <c r="U45" s="199"/>
-      <c r="V45" s="199"/>
-      <c r="W45" s="199"/>
-      <c r="X45" s="199"/>
-      <c r="Y45" s="199"/>
-      <c r="Z45" s="199"/>
-      <c r="AA45" s="199"/>
-      <c r="AB45" s="199"/>
-      <c r="AC45" s="199"/>
-      <c r="AD45" s="200"/>
+      <c r="M45" s="205"/>
+      <c r="N45" s="205"/>
+      <c r="O45" s="205"/>
+      <c r="P45" s="205"/>
+      <c r="Q45" s="205"/>
+      <c r="R45" s="205"/>
+      <c r="S45" s="205"/>
+      <c r="T45" s="205"/>
+      <c r="U45" s="205"/>
+      <c r="V45" s="205"/>
+      <c r="W45" s="205"/>
+      <c r="X45" s="205"/>
+      <c r="Y45" s="205"/>
+      <c r="Z45" s="205"/>
+      <c r="AA45" s="205"/>
+      <c r="AB45" s="205"/>
+      <c r="AC45" s="205"/>
+      <c r="AD45" s="206"/>
       <c r="AE45" s="2"/>
       <c r="AP45" s="5"/>
       <c r="AQ45" s="2"/>
@@ -8736,27 +8703,27 @@
       <c r="I48" s="53"/>
       <c r="J48" s="53"/>
       <c r="K48" s="54"/>
-      <c r="L48" s="213" t="s">
+      <c r="L48" s="216" t="s">
         <v>52</v>
       </c>
-      <c r="M48" s="214"/>
-      <c r="N48" s="214"/>
-      <c r="O48" s="214"/>
-      <c r="P48" s="214"/>
-      <c r="Q48" s="214"/>
-      <c r="R48" s="214"/>
-      <c r="S48" s="214"/>
-      <c r="T48" s="214"/>
-      <c r="U48" s="214"/>
-      <c r="V48" s="214"/>
-      <c r="W48" s="214"/>
-      <c r="X48" s="214"/>
-      <c r="Y48" s="214"/>
-      <c r="Z48" s="214"/>
-      <c r="AA48" s="214"/>
-      <c r="AB48" s="214"/>
-      <c r="AC48" s="214"/>
-      <c r="AD48" s="215"/>
+      <c r="M48" s="217"/>
+      <c r="N48" s="217"/>
+      <c r="O48" s="217"/>
+      <c r="P48" s="217"/>
+      <c r="Q48" s="217"/>
+      <c r="R48" s="217"/>
+      <c r="S48" s="217"/>
+      <c r="T48" s="217"/>
+      <c r="U48" s="217"/>
+      <c r="V48" s="217"/>
+      <c r="W48" s="217"/>
+      <c r="X48" s="217"/>
+      <c r="Y48" s="217"/>
+      <c r="Z48" s="217"/>
+      <c r="AA48" s="217"/>
+      <c r="AB48" s="217"/>
+      <c r="AC48" s="217"/>
+      <c r="AD48" s="218"/>
       <c r="AP48" s="5"/>
       <c r="AQ48" s="2"/>
     </row>
@@ -8770,27 +8737,27 @@
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="13"/>
-      <c r="L49" s="198" t="s">
+      <c r="L49" s="204" t="s">
         <v>50</v>
       </c>
-      <c r="M49" s="199"/>
-      <c r="N49" s="199"/>
-      <c r="O49" s="199"/>
-      <c r="P49" s="199"/>
-      <c r="Q49" s="199"/>
-      <c r="R49" s="199"/>
-      <c r="S49" s="199"/>
-      <c r="T49" s="199"/>
-      <c r="U49" s="199"/>
-      <c r="V49" s="199"/>
-      <c r="W49" s="199"/>
-      <c r="X49" s="199"/>
-      <c r="Y49" s="199"/>
-      <c r="Z49" s="199"/>
-      <c r="AA49" s="199"/>
-      <c r="AB49" s="199"/>
-      <c r="AC49" s="199"/>
-      <c r="AD49" s="200"/>
+      <c r="M49" s="205"/>
+      <c r="N49" s="205"/>
+      <c r="O49" s="205"/>
+      <c r="P49" s="205"/>
+      <c r="Q49" s="205"/>
+      <c r="R49" s="205"/>
+      <c r="S49" s="205"/>
+      <c r="T49" s="205"/>
+      <c r="U49" s="205"/>
+      <c r="V49" s="205"/>
+      <c r="W49" s="205"/>
+      <c r="X49" s="205"/>
+      <c r="Y49" s="205"/>
+      <c r="Z49" s="205"/>
+      <c r="AA49" s="205"/>
+      <c r="AB49" s="205"/>
+      <c r="AC49" s="205"/>
+      <c r="AD49" s="206"/>
       <c r="AP49" s="5"/>
       <c r="AQ49" s="2"/>
     </row>
@@ -8804,27 +8771,27 @@
       <c r="I50" s="32"/>
       <c r="J50" s="32"/>
       <c r="K50" s="33"/>
-      <c r="L50" s="198" t="s">
+      <c r="L50" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="M50" s="199"/>
-      <c r="N50" s="199"/>
-      <c r="O50" s="199"/>
-      <c r="P50" s="199"/>
-      <c r="Q50" s="199"/>
-      <c r="R50" s="199"/>
-      <c r="S50" s="199"/>
-      <c r="T50" s="199"/>
-      <c r="U50" s="199"/>
-      <c r="V50" s="199"/>
-      <c r="W50" s="199"/>
-      <c r="X50" s="199"/>
-      <c r="Y50" s="199"/>
-      <c r="Z50" s="199"/>
-      <c r="AA50" s="199"/>
-      <c r="AB50" s="199"/>
-      <c r="AC50" s="199"/>
-      <c r="AD50" s="200"/>
+      <c r="M50" s="205"/>
+      <c r="N50" s="205"/>
+      <c r="O50" s="205"/>
+      <c r="P50" s="205"/>
+      <c r="Q50" s="205"/>
+      <c r="R50" s="205"/>
+      <c r="S50" s="205"/>
+      <c r="T50" s="205"/>
+      <c r="U50" s="205"/>
+      <c r="V50" s="205"/>
+      <c r="W50" s="205"/>
+      <c r="X50" s="205"/>
+      <c r="Y50" s="205"/>
+      <c r="Z50" s="205"/>
+      <c r="AA50" s="205"/>
+      <c r="AB50" s="205"/>
+      <c r="AC50" s="205"/>
+      <c r="AD50" s="206"/>
       <c r="AP50" s="5"/>
       <c r="AQ50" s="2"/>
     </row>
@@ -11427,30 +11394,30 @@
       <c r="P125" s="53"/>
       <c r="Q125" s="53"/>
       <c r="R125" s="54"/>
-      <c r="S125" s="213" t="s">
+      <c r="S125" s="216" t="s">
         <v>6</v>
       </c>
-      <c r="T125" s="214"/>
-      <c r="U125" s="214"/>
-      <c r="V125" s="214"/>
-      <c r="W125" s="214"/>
-      <c r="X125" s="215"/>
-      <c r="Y125" s="213" t="s">
+      <c r="T125" s="217"/>
+      <c r="U125" s="217"/>
+      <c r="V125" s="217"/>
+      <c r="W125" s="217"/>
+      <c r="X125" s="218"/>
+      <c r="Y125" s="216" t="s">
         <v>7</v>
       </c>
-      <c r="Z125" s="214"/>
-      <c r="AA125" s="214"/>
-      <c r="AB125" s="214"/>
-      <c r="AC125" s="214"/>
-      <c r="AD125" s="215"/>
-      <c r="AE125" s="213" t="s">
+      <c r="Z125" s="217"/>
+      <c r="AA125" s="217"/>
+      <c r="AB125" s="217"/>
+      <c r="AC125" s="217"/>
+      <c r="AD125" s="218"/>
+      <c r="AE125" s="216" t="s">
         <v>26</v>
       </c>
-      <c r="AF125" s="214"/>
-      <c r="AG125" s="214"/>
-      <c r="AH125" s="214"/>
-      <c r="AI125" s="214"/>
-      <c r="AJ125" s="215"/>
+      <c r="AF125" s="217"/>
+      <c r="AG125" s="217"/>
+      <c r="AH125" s="217"/>
+      <c r="AI125" s="217"/>
+      <c r="AJ125" s="218"/>
       <c r="AP125" s="5"/>
       <c r="AQ125" s="2"/>
     </row>
@@ -11472,30 +11439,30 @@
       <c r="P126" s="98"/>
       <c r="Q126" s="98"/>
       <c r="R126" s="102"/>
-      <c r="S126" s="198" t="s">
+      <c r="S126" s="204" t="s">
         <v>16</v>
       </c>
-      <c r="T126" s="199"/>
-      <c r="U126" s="199"/>
-      <c r="V126" s="199"/>
-      <c r="W126" s="199"/>
-      <c r="X126" s="200"/>
-      <c r="Y126" s="198" t="s">
+      <c r="T126" s="205"/>
+      <c r="U126" s="205"/>
+      <c r="V126" s="205"/>
+      <c r="W126" s="205"/>
+      <c r="X126" s="206"/>
+      <c r="Y126" s="204" t="s">
         <v>9</v>
       </c>
-      <c r="Z126" s="199"/>
-      <c r="AA126" s="199"/>
-      <c r="AB126" s="199"/>
-      <c r="AC126" s="199"/>
-      <c r="AD126" s="200"/>
-      <c r="AE126" s="198" t="s">
+      <c r="Z126" s="205"/>
+      <c r="AA126" s="205"/>
+      <c r="AB126" s="205"/>
+      <c r="AC126" s="205"/>
+      <c r="AD126" s="206"/>
+      <c r="AE126" s="204" t="s">
         <v>9</v>
       </c>
-      <c r="AF126" s="199"/>
-      <c r="AG126" s="199"/>
-      <c r="AH126" s="199"/>
-      <c r="AI126" s="199"/>
-      <c r="AJ126" s="200"/>
+      <c r="AF126" s="205"/>
+      <c r="AG126" s="205"/>
+      <c r="AH126" s="205"/>
+      <c r="AI126" s="205"/>
+      <c r="AJ126" s="206"/>
       <c r="AP126" s="5"/>
       <c r="AQ126" s="2"/>
     </row>
@@ -11779,30 +11746,30 @@
       <c r="P133" s="75"/>
       <c r="Q133" s="75"/>
       <c r="R133" s="76"/>
-      <c r="S133" s="201" t="s">
+      <c r="S133" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="T133" s="202"/>
-      <c r="U133" s="202"/>
-      <c r="V133" s="202"/>
-      <c r="W133" s="202"/>
-      <c r="X133" s="203"/>
-      <c r="Y133" s="201" t="s">
+      <c r="T133" s="184"/>
+      <c r="U133" s="184"/>
+      <c r="V133" s="184"/>
+      <c r="W133" s="184"/>
+      <c r="X133" s="185"/>
+      <c r="Y133" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="Z133" s="202"/>
-      <c r="AA133" s="202"/>
-      <c r="AB133" s="202"/>
-      <c r="AC133" s="202"/>
-      <c r="AD133" s="203"/>
-      <c r="AE133" s="201" t="s">
+      <c r="Z133" s="184"/>
+      <c r="AA133" s="184"/>
+      <c r="AB133" s="184"/>
+      <c r="AC133" s="184"/>
+      <c r="AD133" s="185"/>
+      <c r="AE133" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="AF133" s="202"/>
-      <c r="AG133" s="202"/>
-      <c r="AH133" s="202"/>
-      <c r="AI133" s="202"/>
-      <c r="AJ133" s="203"/>
+      <c r="AF133" s="184"/>
+      <c r="AG133" s="184"/>
+      <c r="AH133" s="184"/>
+      <c r="AI133" s="184"/>
+      <c r="AJ133" s="185"/>
       <c r="AP133" s="5"/>
       <c r="AQ133" s="2"/>
     </row>
@@ -11826,30 +11793,30 @@
       <c r="P134" s="75"/>
       <c r="Q134" s="75"/>
       <c r="R134" s="76"/>
-      <c r="S134" s="201" t="s">
+      <c r="S134" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T134" s="202"/>
-      <c r="U134" s="202"/>
-      <c r="V134" s="202"/>
-      <c r="W134" s="202"/>
-      <c r="X134" s="203"/>
-      <c r="Y134" s="201" t="s">
+      <c r="T134" s="184"/>
+      <c r="U134" s="184"/>
+      <c r="V134" s="184"/>
+      <c r="W134" s="184"/>
+      <c r="X134" s="185"/>
+      <c r="Y134" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="Z134" s="202"/>
-      <c r="AA134" s="202"/>
-      <c r="AB134" s="202"/>
-      <c r="AC134" s="202"/>
-      <c r="AD134" s="203"/>
-      <c r="AE134" s="201" t="s">
+      <c r="Z134" s="184"/>
+      <c r="AA134" s="184"/>
+      <c r="AB134" s="184"/>
+      <c r="AC134" s="184"/>
+      <c r="AD134" s="185"/>
+      <c r="AE134" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF134" s="202"/>
-      <c r="AG134" s="202"/>
-      <c r="AH134" s="202"/>
-      <c r="AI134" s="202"/>
-      <c r="AJ134" s="203"/>
+      <c r="AF134" s="184"/>
+      <c r="AG134" s="184"/>
+      <c r="AH134" s="184"/>
+      <c r="AI134" s="184"/>
+      <c r="AJ134" s="185"/>
       <c r="AP134" s="5"/>
       <c r="AQ134" s="2"/>
     </row>
@@ -11867,30 +11834,30 @@
       <c r="P135" s="75"/>
       <c r="Q135" s="75"/>
       <c r="R135" s="76"/>
-      <c r="S135" s="201" t="s">
+      <c r="S135" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T135" s="202"/>
-      <c r="U135" s="202"/>
-      <c r="V135" s="202"/>
-      <c r="W135" s="202"/>
-      <c r="X135" s="203"/>
-      <c r="Y135" s="201" t="s">
+      <c r="T135" s="184"/>
+      <c r="U135" s="184"/>
+      <c r="V135" s="184"/>
+      <c r="W135" s="184"/>
+      <c r="X135" s="185"/>
+      <c r="Y135" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="Z135" s="202"/>
-      <c r="AA135" s="202"/>
-      <c r="AB135" s="202"/>
-      <c r="AC135" s="202"/>
-      <c r="AD135" s="203"/>
-      <c r="AE135" s="201" t="s">
+      <c r="Z135" s="184"/>
+      <c r="AA135" s="184"/>
+      <c r="AB135" s="184"/>
+      <c r="AC135" s="184"/>
+      <c r="AD135" s="185"/>
+      <c r="AE135" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF135" s="202"/>
-      <c r="AG135" s="202"/>
-      <c r="AH135" s="202"/>
-      <c r="AI135" s="202"/>
-      <c r="AJ135" s="203"/>
+      <c r="AF135" s="184"/>
+      <c r="AG135" s="184"/>
+      <c r="AH135" s="184"/>
+      <c r="AI135" s="184"/>
+      <c r="AJ135" s="185"/>
       <c r="AP135" s="5"/>
       <c r="AQ135" s="2"/>
     </row>
@@ -11912,30 +11879,30 @@
       <c r="P136" s="75"/>
       <c r="Q136" s="75"/>
       <c r="R136" s="76"/>
-      <c r="S136" s="201" t="s">
+      <c r="S136" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T136" s="202"/>
-      <c r="U136" s="202"/>
-      <c r="V136" s="202"/>
-      <c r="W136" s="202"/>
-      <c r="X136" s="203"/>
-      <c r="Y136" s="201" t="s">
+      <c r="T136" s="184"/>
+      <c r="U136" s="184"/>
+      <c r="V136" s="184"/>
+      <c r="W136" s="184"/>
+      <c r="X136" s="185"/>
+      <c r="Y136" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="Z136" s="202"/>
-      <c r="AA136" s="202"/>
-      <c r="AB136" s="202"/>
-      <c r="AC136" s="202"/>
-      <c r="AD136" s="203"/>
-      <c r="AE136" s="201" t="s">
+      <c r="Z136" s="184"/>
+      <c r="AA136" s="184"/>
+      <c r="AB136" s="184"/>
+      <c r="AC136" s="184"/>
+      <c r="AD136" s="185"/>
+      <c r="AE136" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF136" s="202"/>
-      <c r="AG136" s="202"/>
-      <c r="AH136" s="202"/>
-      <c r="AI136" s="202"/>
-      <c r="AJ136" s="203"/>
+      <c r="AF136" s="184"/>
+      <c r="AG136" s="184"/>
+      <c r="AH136" s="184"/>
+      <c r="AI136" s="184"/>
+      <c r="AJ136" s="185"/>
       <c r="AP136" s="5"/>
       <c r="AQ136" s="2"/>
     </row>
@@ -11957,30 +11924,30 @@
       <c r="P137" s="75"/>
       <c r="Q137" s="75"/>
       <c r="R137" s="76"/>
-      <c r="S137" s="231" t="s">
+      <c r="S137" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="T137" s="232"/>
-      <c r="U137" s="232"/>
-      <c r="V137" s="232"/>
-      <c r="W137" s="232"/>
-      <c r="X137" s="233"/>
-      <c r="Y137" s="231" t="s">
+      <c r="T137" s="184"/>
+      <c r="U137" s="184"/>
+      <c r="V137" s="184"/>
+      <c r="W137" s="184"/>
+      <c r="X137" s="185"/>
+      <c r="Y137" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="Z137" s="232"/>
-      <c r="AA137" s="232"/>
-      <c r="AB137" s="232"/>
-      <c r="AC137" s="232"/>
-      <c r="AD137" s="233"/>
-      <c r="AE137" s="201" t="s">
+      <c r="Z137" s="184"/>
+      <c r="AA137" s="184"/>
+      <c r="AB137" s="184"/>
+      <c r="AC137" s="184"/>
+      <c r="AD137" s="185"/>
+      <c r="AE137" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="AF137" s="202"/>
-      <c r="AG137" s="202"/>
-      <c r="AH137" s="202"/>
-      <c r="AI137" s="202"/>
-      <c r="AJ137" s="203"/>
+      <c r="AF137" s="184"/>
+      <c r="AG137" s="184"/>
+      <c r="AH137" s="184"/>
+      <c r="AI137" s="184"/>
+      <c r="AJ137" s="185"/>
       <c r="AP137" s="5"/>
       <c r="AQ137" s="2"/>
     </row>
@@ -12004,30 +11971,30 @@
       <c r="P138" s="75"/>
       <c r="Q138" s="75"/>
       <c r="R138" s="76"/>
-      <c r="S138" s="201" t="s">
+      <c r="S138" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T138" s="202"/>
-      <c r="U138" s="202"/>
-      <c r="V138" s="202"/>
-      <c r="W138" s="202"/>
-      <c r="X138" s="203"/>
-      <c r="Y138" s="201" t="s">
+      <c r="T138" s="184"/>
+      <c r="U138" s="184"/>
+      <c r="V138" s="184"/>
+      <c r="W138" s="184"/>
+      <c r="X138" s="185"/>
+      <c r="Y138" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="Z138" s="202"/>
-      <c r="AA138" s="202"/>
-      <c r="AB138" s="202"/>
-      <c r="AC138" s="202"/>
-      <c r="AD138" s="203"/>
-      <c r="AE138" s="201" t="s">
+      <c r="Z138" s="184"/>
+      <c r="AA138" s="184"/>
+      <c r="AB138" s="184"/>
+      <c r="AC138" s="184"/>
+      <c r="AD138" s="185"/>
+      <c r="AE138" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF138" s="202"/>
-      <c r="AG138" s="202"/>
-      <c r="AH138" s="202"/>
-      <c r="AI138" s="202"/>
-      <c r="AJ138" s="203"/>
+      <c r="AF138" s="184"/>
+      <c r="AG138" s="184"/>
+      <c r="AH138" s="184"/>
+      <c r="AI138" s="184"/>
+      <c r="AJ138" s="185"/>
       <c r="AP138" s="5"/>
       <c r="AQ138" s="2"/>
     </row>
@@ -12045,30 +12012,30 @@
       <c r="P139" s="75"/>
       <c r="Q139" s="75"/>
       <c r="R139" s="76"/>
-      <c r="S139" s="201" t="s">
+      <c r="S139" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T139" s="202"/>
-      <c r="U139" s="202"/>
-      <c r="V139" s="202"/>
-      <c r="W139" s="202"/>
-      <c r="X139" s="203"/>
-      <c r="Y139" s="201" t="s">
+      <c r="T139" s="184"/>
+      <c r="U139" s="184"/>
+      <c r="V139" s="184"/>
+      <c r="W139" s="184"/>
+      <c r="X139" s="185"/>
+      <c r="Y139" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="Z139" s="202"/>
-      <c r="AA139" s="202"/>
-      <c r="AB139" s="202"/>
-      <c r="AC139" s="202"/>
-      <c r="AD139" s="203"/>
-      <c r="AE139" s="201" t="s">
+      <c r="Z139" s="184"/>
+      <c r="AA139" s="184"/>
+      <c r="AB139" s="184"/>
+      <c r="AC139" s="184"/>
+      <c r="AD139" s="185"/>
+      <c r="AE139" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF139" s="202"/>
-      <c r="AG139" s="202"/>
-      <c r="AH139" s="202"/>
-      <c r="AI139" s="202"/>
-      <c r="AJ139" s="203"/>
+      <c r="AF139" s="184"/>
+      <c r="AG139" s="184"/>
+      <c r="AH139" s="184"/>
+      <c r="AI139" s="184"/>
+      <c r="AJ139" s="185"/>
       <c r="AP139" s="5"/>
       <c r="AQ139" s="2"/>
     </row>
@@ -12090,30 +12057,30 @@
       <c r="P140" s="75"/>
       <c r="Q140" s="75"/>
       <c r="R140" s="76"/>
-      <c r="S140" s="201" t="s">
+      <c r="S140" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T140" s="202"/>
-      <c r="U140" s="202"/>
-      <c r="V140" s="202"/>
-      <c r="W140" s="202"/>
-      <c r="X140" s="203"/>
-      <c r="Y140" s="201" t="s">
+      <c r="T140" s="184"/>
+      <c r="U140" s="184"/>
+      <c r="V140" s="184"/>
+      <c r="W140" s="184"/>
+      <c r="X140" s="185"/>
+      <c r="Y140" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="Z140" s="202"/>
-      <c r="AA140" s="202"/>
-      <c r="AB140" s="202"/>
-      <c r="AC140" s="202"/>
-      <c r="AD140" s="203"/>
-      <c r="AE140" s="201" t="s">
+      <c r="Z140" s="184"/>
+      <c r="AA140" s="184"/>
+      <c r="AB140" s="184"/>
+      <c r="AC140" s="184"/>
+      <c r="AD140" s="185"/>
+      <c r="AE140" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF140" s="202"/>
-      <c r="AG140" s="202"/>
-      <c r="AH140" s="202"/>
-      <c r="AI140" s="202"/>
-      <c r="AJ140" s="203"/>
+      <c r="AF140" s="184"/>
+      <c r="AG140" s="184"/>
+      <c r="AH140" s="184"/>
+      <c r="AI140" s="184"/>
+      <c r="AJ140" s="185"/>
       <c r="AP140" s="5"/>
       <c r="AQ140" s="2"/>
     </row>
@@ -12135,30 +12102,30 @@
       <c r="P141" s="75"/>
       <c r="Q141" s="75"/>
       <c r="R141" s="76"/>
-      <c r="S141" s="201" t="s">
+      <c r="S141" s="183" t="s">
         <v>39</v>
       </c>
-      <c r="T141" s="202"/>
-      <c r="U141" s="202"/>
-      <c r="V141" s="202"/>
-      <c r="W141" s="202"/>
-      <c r="X141" s="203"/>
-      <c r="Y141" s="201" t="s">
+      <c r="T141" s="184"/>
+      <c r="U141" s="184"/>
+      <c r="V141" s="184"/>
+      <c r="W141" s="184"/>
+      <c r="X141" s="185"/>
+      <c r="Y141" s="183" t="s">
         <v>218</v>
       </c>
-      <c r="Z141" s="202"/>
-      <c r="AA141" s="202"/>
-      <c r="AB141" s="202"/>
-      <c r="AC141" s="202"/>
-      <c r="AD141" s="203"/>
-      <c r="AE141" s="201" t="s">
+      <c r="Z141" s="184"/>
+      <c r="AA141" s="184"/>
+      <c r="AB141" s="184"/>
+      <c r="AC141" s="184"/>
+      <c r="AD141" s="185"/>
+      <c r="AE141" s="183" t="s">
         <v>218</v>
       </c>
-      <c r="AF141" s="202"/>
-      <c r="AG141" s="202"/>
-      <c r="AH141" s="202"/>
-      <c r="AI141" s="202"/>
-      <c r="AJ141" s="203"/>
+      <c r="AF141" s="184"/>
+      <c r="AG141" s="184"/>
+      <c r="AH141" s="184"/>
+      <c r="AI141" s="184"/>
+      <c r="AJ141" s="185"/>
       <c r="AP141" s="5"/>
       <c r="AQ141" s="2"/>
     </row>
@@ -12182,30 +12149,30 @@
       <c r="P142" s="134"/>
       <c r="Q142" s="134"/>
       <c r="R142" s="135"/>
-      <c r="S142" s="201" t="s">
+      <c r="S142" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T142" s="202"/>
-      <c r="U142" s="202"/>
-      <c r="V142" s="202"/>
-      <c r="W142" s="202"/>
-      <c r="X142" s="203"/>
-      <c r="Y142" s="201" t="s">
+      <c r="T142" s="184"/>
+      <c r="U142" s="184"/>
+      <c r="V142" s="184"/>
+      <c r="W142" s="184"/>
+      <c r="X142" s="185"/>
+      <c r="Y142" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="Z142" s="202"/>
-      <c r="AA142" s="202"/>
-      <c r="AB142" s="202"/>
-      <c r="AC142" s="202"/>
-      <c r="AD142" s="203"/>
-      <c r="AE142" s="201" t="s">
+      <c r="Z142" s="184"/>
+      <c r="AA142" s="184"/>
+      <c r="AB142" s="184"/>
+      <c r="AC142" s="184"/>
+      <c r="AD142" s="185"/>
+      <c r="AE142" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF142" s="202"/>
-      <c r="AG142" s="202"/>
-      <c r="AH142" s="202"/>
-      <c r="AI142" s="202"/>
-      <c r="AJ142" s="203"/>
+      <c r="AF142" s="184"/>
+      <c r="AG142" s="184"/>
+      <c r="AH142" s="184"/>
+      <c r="AI142" s="184"/>
+      <c r="AJ142" s="185"/>
       <c r="AP142" s="5"/>
       <c r="AQ142" s="2"/>
     </row>
@@ -12223,30 +12190,30 @@
       <c r="P143" s="75"/>
       <c r="Q143" s="75"/>
       <c r="R143" s="76"/>
-      <c r="S143" s="201" t="s">
+      <c r="S143" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T143" s="202"/>
-      <c r="U143" s="202"/>
-      <c r="V143" s="202"/>
-      <c r="W143" s="202"/>
-      <c r="X143" s="203"/>
-      <c r="Y143" s="201" t="s">
+      <c r="T143" s="184"/>
+      <c r="U143" s="184"/>
+      <c r="V143" s="184"/>
+      <c r="W143" s="184"/>
+      <c r="X143" s="185"/>
+      <c r="Y143" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="Z143" s="202"/>
-      <c r="AA143" s="202"/>
-      <c r="AB143" s="202"/>
-      <c r="AC143" s="202"/>
-      <c r="AD143" s="203"/>
-      <c r="AE143" s="201" t="s">
+      <c r="Z143" s="184"/>
+      <c r="AA143" s="184"/>
+      <c r="AB143" s="184"/>
+      <c r="AC143" s="184"/>
+      <c r="AD143" s="185"/>
+      <c r="AE143" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF143" s="202"/>
-      <c r="AG143" s="202"/>
-      <c r="AH143" s="202"/>
-      <c r="AI143" s="202"/>
-      <c r="AJ143" s="203"/>
+      <c r="AF143" s="184"/>
+      <c r="AG143" s="184"/>
+      <c r="AH143" s="184"/>
+      <c r="AI143" s="184"/>
+      <c r="AJ143" s="185"/>
       <c r="AP143" s="5"/>
       <c r="AQ143" s="2"/>
     </row>
@@ -12313,30 +12280,30 @@
       <c r="P145" s="75"/>
       <c r="Q145" s="75"/>
       <c r="R145" s="76"/>
-      <c r="S145" s="201" t="s">
+      <c r="S145" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T145" s="202"/>
-      <c r="U145" s="202"/>
-      <c r="V145" s="202"/>
-      <c r="W145" s="202"/>
-      <c r="X145" s="203"/>
-      <c r="Y145" s="201" t="s">
+      <c r="T145" s="184"/>
+      <c r="U145" s="184"/>
+      <c r="V145" s="184"/>
+      <c r="W145" s="184"/>
+      <c r="X145" s="185"/>
+      <c r="Y145" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="Z145" s="202"/>
-      <c r="AA145" s="202"/>
-      <c r="AB145" s="202"/>
-      <c r="AC145" s="202"/>
-      <c r="AD145" s="203"/>
-      <c r="AE145" s="201" t="s">
+      <c r="Z145" s="184"/>
+      <c r="AA145" s="184"/>
+      <c r="AB145" s="184"/>
+      <c r="AC145" s="184"/>
+      <c r="AD145" s="185"/>
+      <c r="AE145" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="AF145" s="202"/>
-      <c r="AG145" s="202"/>
-      <c r="AH145" s="202"/>
-      <c r="AI145" s="202"/>
-      <c r="AJ145" s="203"/>
+      <c r="AF145" s="184"/>
+      <c r="AG145" s="184"/>
+      <c r="AH145" s="184"/>
+      <c r="AI145" s="184"/>
+      <c r="AJ145" s="185"/>
       <c r="AP145" s="5"/>
       <c r="AQ145" s="2"/>
     </row>
@@ -12360,30 +12327,30 @@
       <c r="P146" s="75"/>
       <c r="Q146" s="75"/>
       <c r="R146" s="76"/>
-      <c r="S146" s="201" t="s">
+      <c r="S146" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T146" s="202"/>
-      <c r="U146" s="202"/>
-      <c r="V146" s="202"/>
-      <c r="W146" s="202"/>
-      <c r="X146" s="203"/>
-      <c r="Y146" s="231" t="s">
+      <c r="T146" s="184"/>
+      <c r="U146" s="184"/>
+      <c r="V146" s="184"/>
+      <c r="W146" s="184"/>
+      <c r="X146" s="185"/>
+      <c r="Y146" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="Z146" s="232"/>
-      <c r="AA146" s="232"/>
-      <c r="AB146" s="232"/>
-      <c r="AC146" s="232"/>
-      <c r="AD146" s="233"/>
-      <c r="AE146" s="231" t="s">
+      <c r="Z146" s="184"/>
+      <c r="AA146" s="184"/>
+      <c r="AB146" s="184"/>
+      <c r="AC146" s="184"/>
+      <c r="AD146" s="185"/>
+      <c r="AE146" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF146" s="232"/>
-      <c r="AG146" s="232"/>
-      <c r="AH146" s="232"/>
-      <c r="AI146" s="232"/>
-      <c r="AJ146" s="233"/>
+      <c r="AF146" s="184"/>
+      <c r="AG146" s="184"/>
+      <c r="AH146" s="184"/>
+      <c r="AI146" s="184"/>
+      <c r="AJ146" s="185"/>
       <c r="AP146" s="5"/>
       <c r="AQ146" s="2"/>
     </row>
@@ -12401,30 +12368,30 @@
       <c r="P147" s="75"/>
       <c r="Q147" s="75"/>
       <c r="R147" s="76"/>
-      <c r="S147" s="201" t="s">
+      <c r="S147" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T147" s="202"/>
-      <c r="U147" s="202"/>
-      <c r="V147" s="202"/>
-      <c r="W147" s="202"/>
-      <c r="X147" s="203"/>
-      <c r="Y147" s="201" t="s">
+      <c r="T147" s="184"/>
+      <c r="U147" s="184"/>
+      <c r="V147" s="184"/>
+      <c r="W147" s="184"/>
+      <c r="X147" s="185"/>
+      <c r="Y147" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="Z147" s="202"/>
-      <c r="AA147" s="202"/>
-      <c r="AB147" s="202"/>
-      <c r="AC147" s="202"/>
-      <c r="AD147" s="203"/>
-      <c r="AE147" s="231" t="s">
+      <c r="Z147" s="184"/>
+      <c r="AA147" s="184"/>
+      <c r="AB147" s="184"/>
+      <c r="AC147" s="184"/>
+      <c r="AD147" s="185"/>
+      <c r="AE147" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF147" s="232"/>
-      <c r="AG147" s="232"/>
-      <c r="AH147" s="232"/>
-      <c r="AI147" s="232"/>
-      <c r="AJ147" s="233"/>
+      <c r="AF147" s="184"/>
+      <c r="AG147" s="184"/>
+      <c r="AH147" s="184"/>
+      <c r="AI147" s="184"/>
+      <c r="AJ147" s="185"/>
       <c r="AP147" s="5"/>
       <c r="AQ147" s="2"/>
     </row>
@@ -12446,30 +12413,30 @@
       <c r="P148" s="75"/>
       <c r="Q148" s="75"/>
       <c r="R148" s="76"/>
-      <c r="S148" s="201" t="s">
+      <c r="S148" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="T148" s="202"/>
-      <c r="U148" s="202"/>
-      <c r="V148" s="202"/>
-      <c r="W148" s="202"/>
-      <c r="X148" s="203"/>
-      <c r="Y148" s="201" t="s">
+      <c r="T148" s="184"/>
+      <c r="U148" s="184"/>
+      <c r="V148" s="184"/>
+      <c r="W148" s="184"/>
+      <c r="X148" s="185"/>
+      <c r="Y148" s="183" t="s">
         <v>8</v>
       </c>
-      <c r="Z148" s="202"/>
-      <c r="AA148" s="202"/>
-      <c r="AB148" s="202"/>
-      <c r="AC148" s="202"/>
-      <c r="AD148" s="203"/>
-      <c r="AE148" s="231" t="s">
+      <c r="Z148" s="184"/>
+      <c r="AA148" s="184"/>
+      <c r="AB148" s="184"/>
+      <c r="AC148" s="184"/>
+      <c r="AD148" s="185"/>
+      <c r="AE148" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="AF148" s="232"/>
-      <c r="AG148" s="232"/>
-      <c r="AH148" s="232"/>
-      <c r="AI148" s="232"/>
-      <c r="AJ148" s="233"/>
+      <c r="AF148" s="184"/>
+      <c r="AG148" s="184"/>
+      <c r="AH148" s="184"/>
+      <c r="AI148" s="184"/>
+      <c r="AJ148" s="185"/>
       <c r="AP148" s="5"/>
       <c r="AQ148" s="2"/>
     </row>
@@ -13055,22 +13022,22 @@
       <c r="V161" s="181"/>
       <c r="W161" s="181"/>
       <c r="X161" s="182"/>
-      <c r="Y161" s="186" t="s">
+      <c r="Y161" s="180" t="s">
         <v>39</v>
       </c>
-      <c r="Z161" s="187"/>
-      <c r="AA161" s="187"/>
-      <c r="AB161" s="187"/>
-      <c r="AC161" s="187"/>
-      <c r="AD161" s="188"/>
-      <c r="AE161" s="195" t="s">
+      <c r="Z161" s="181"/>
+      <c r="AA161" s="181"/>
+      <c r="AB161" s="181"/>
+      <c r="AC161" s="181"/>
+      <c r="AD161" s="182"/>
+      <c r="AE161" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="AF161" s="196"/>
-      <c r="AG161" s="196"/>
-      <c r="AH161" s="196"/>
-      <c r="AI161" s="196"/>
-      <c r="AJ161" s="197"/>
+      <c r="AF161" s="181"/>
+      <c r="AG161" s="181"/>
+      <c r="AH161" s="181"/>
+      <c r="AI161" s="181"/>
+      <c r="AJ161" s="182"/>
       <c r="AP161" s="5"/>
       <c r="AQ161" s="2"/>
     </row>
@@ -13110,14 +13077,14 @@
       <c r="AB162" s="181"/>
       <c r="AC162" s="181"/>
       <c r="AD162" s="182"/>
-      <c r="AE162" s="195" t="s">
+      <c r="AE162" s="180" t="s">
         <v>39</v>
       </c>
-      <c r="AF162" s="196"/>
-      <c r="AG162" s="196"/>
-      <c r="AH162" s="196"/>
-      <c r="AI162" s="196"/>
-      <c r="AJ162" s="197"/>
+      <c r="AF162" s="181"/>
+      <c r="AG162" s="181"/>
+      <c r="AH162" s="181"/>
+      <c r="AI162" s="181"/>
+      <c r="AJ162" s="182"/>
       <c r="AP162" s="5"/>
       <c r="AQ162" s="2"/>
     </row>
@@ -13157,14 +13124,14 @@
       <c r="AB163" s="181"/>
       <c r="AC163" s="181"/>
       <c r="AD163" s="182"/>
-      <c r="AE163" s="195" t="s">
+      <c r="AE163" s="180" t="s">
         <v>39</v>
       </c>
-      <c r="AF163" s="196"/>
-      <c r="AG163" s="196"/>
-      <c r="AH163" s="196"/>
-      <c r="AI163" s="196"/>
-      <c r="AJ163" s="197"/>
+      <c r="AF163" s="181"/>
+      <c r="AG163" s="181"/>
+      <c r="AH163" s="181"/>
+      <c r="AI163" s="181"/>
+      <c r="AJ163" s="182"/>
       <c r="AP163" s="5"/>
       <c r="AQ163" s="2"/>
     </row>
@@ -13204,14 +13171,14 @@
       <c r="AB164" s="181"/>
       <c r="AC164" s="181"/>
       <c r="AD164" s="182"/>
-      <c r="AE164" s="195" t="s">
+      <c r="AE164" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="AF164" s="196"/>
-      <c r="AG164" s="196"/>
-      <c r="AH164" s="196"/>
-      <c r="AI164" s="196"/>
-      <c r="AJ164" s="197"/>
+      <c r="AF164" s="181"/>
+      <c r="AG164" s="181"/>
+      <c r="AH164" s="181"/>
+      <c r="AI164" s="181"/>
+      <c r="AJ164" s="182"/>
       <c r="AP164" s="5"/>
       <c r="AQ164" s="2"/>
     </row>
@@ -13298,14 +13265,14 @@
       <c r="AB166" s="181"/>
       <c r="AC166" s="181"/>
       <c r="AD166" s="182"/>
-      <c r="AE166" s="195" t="s">
+      <c r="AE166" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="AF166" s="196"/>
-      <c r="AG166" s="196"/>
-      <c r="AH166" s="196"/>
-      <c r="AI166" s="196"/>
-      <c r="AJ166" s="197"/>
+      <c r="AF166" s="181"/>
+      <c r="AG166" s="181"/>
+      <c r="AH166" s="181"/>
+      <c r="AI166" s="181"/>
+      <c r="AJ166" s="182"/>
       <c r="AP166" s="5"/>
       <c r="AQ166" s="2"/>
     </row>
@@ -13382,22 +13349,22 @@
       <c r="V168" s="181"/>
       <c r="W168" s="181"/>
       <c r="X168" s="182"/>
-      <c r="Y168" s="186" t="s">
+      <c r="Y168" s="180" t="s">
         <v>39</v>
       </c>
-      <c r="Z168" s="187"/>
-      <c r="AA168" s="187"/>
-      <c r="AB168" s="187"/>
-      <c r="AC168" s="187"/>
-      <c r="AD168" s="188"/>
-      <c r="AE168" s="186" t="s">
+      <c r="Z168" s="181"/>
+      <c r="AA168" s="181"/>
+      <c r="AB168" s="181"/>
+      <c r="AC168" s="181"/>
+      <c r="AD168" s="182"/>
+      <c r="AE168" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="AF168" s="187"/>
-      <c r="AG168" s="187"/>
-      <c r="AH168" s="187"/>
-      <c r="AI168" s="187"/>
-      <c r="AJ168" s="188"/>
+      <c r="AF168" s="181"/>
+      <c r="AG168" s="181"/>
+      <c r="AH168" s="181"/>
+      <c r="AI168" s="181"/>
+      <c r="AJ168" s="182"/>
       <c r="AP168" s="5"/>
       <c r="AQ168" s="2"/>
     </row>
@@ -13435,14 +13402,14 @@
       <c r="AB169" s="181"/>
       <c r="AC169" s="181"/>
       <c r="AD169" s="182"/>
-      <c r="AE169" s="186" t="s">
+      <c r="AE169" s="180" t="s">
         <v>39</v>
       </c>
-      <c r="AF169" s="187"/>
-      <c r="AG169" s="187"/>
-      <c r="AH169" s="187"/>
-      <c r="AI169" s="187"/>
-      <c r="AJ169" s="188"/>
+      <c r="AF169" s="181"/>
+      <c r="AG169" s="181"/>
+      <c r="AH169" s="181"/>
+      <c r="AI169" s="181"/>
+      <c r="AJ169" s="182"/>
       <c r="AP169" s="5"/>
       <c r="AQ169" s="2"/>
     </row>
@@ -13480,14 +13447,14 @@
       <c r="AB170" s="181"/>
       <c r="AC170" s="181"/>
       <c r="AD170" s="182"/>
-      <c r="AE170" s="186" t="s">
+      <c r="AE170" s="180" t="s">
         <v>39</v>
       </c>
-      <c r="AF170" s="187"/>
-      <c r="AG170" s="187"/>
-      <c r="AH170" s="187"/>
-      <c r="AI170" s="187"/>
-      <c r="AJ170" s="188"/>
+      <c r="AF170" s="181"/>
+      <c r="AG170" s="181"/>
+      <c r="AH170" s="181"/>
+      <c r="AI170" s="181"/>
+      <c r="AJ170" s="182"/>
       <c r="AP170" s="5"/>
       <c r="AQ170" s="2"/>
     </row>
@@ -13525,14 +13492,14 @@
       <c r="AB171" s="181"/>
       <c r="AC171" s="181"/>
       <c r="AD171" s="182"/>
-      <c r="AE171" s="186" t="s">
+      <c r="AE171" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="AF171" s="187"/>
-      <c r="AG171" s="187"/>
-      <c r="AH171" s="187"/>
-      <c r="AI171" s="187"/>
-      <c r="AJ171" s="188"/>
+      <c r="AF171" s="181"/>
+      <c r="AG171" s="181"/>
+      <c r="AH171" s="181"/>
+      <c r="AI171" s="181"/>
+      <c r="AJ171" s="182"/>
       <c r="AP171" s="5"/>
       <c r="AQ171" s="2"/>
     </row>
@@ -13615,14 +13582,14 @@
       <c r="AB173" s="181"/>
       <c r="AC173" s="181"/>
       <c r="AD173" s="182"/>
-      <c r="AE173" s="186" t="s">
+      <c r="AE173" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="AF173" s="187"/>
-      <c r="AG173" s="187"/>
-      <c r="AH173" s="187"/>
-      <c r="AI173" s="187"/>
-      <c r="AJ173" s="188"/>
+      <c r="AF173" s="181"/>
+      <c r="AG173" s="181"/>
+      <c r="AH173" s="181"/>
+      <c r="AI173" s="181"/>
+      <c r="AJ173" s="182"/>
       <c r="AP173" s="5"/>
       <c r="AQ173" s="2"/>
     </row>
@@ -13746,14 +13713,14 @@
       <c r="V176" s="181"/>
       <c r="W176" s="181"/>
       <c r="X176" s="182"/>
-      <c r="Y176" s="186" t="s">
+      <c r="Y176" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="Z176" s="187"/>
-      <c r="AA176" s="187"/>
-      <c r="AB176" s="187"/>
-      <c r="AC176" s="187"/>
-      <c r="AD176" s="188"/>
+      <c r="Z176" s="181"/>
+      <c r="AA176" s="181"/>
+      <c r="AB176" s="181"/>
+      <c r="AC176" s="181"/>
+      <c r="AD176" s="182"/>
       <c r="AE176" s="180" t="s">
         <v>14</v>
       </c>
@@ -13793,14 +13760,14 @@
       <c r="V177" s="181"/>
       <c r="W177" s="181"/>
       <c r="X177" s="182"/>
-      <c r="Y177" s="186" t="s">
+      <c r="Y177" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="Z177" s="187"/>
-      <c r="AA177" s="187"/>
-      <c r="AB177" s="187"/>
-      <c r="AC177" s="187"/>
-      <c r="AD177" s="188"/>
+      <c r="Z177" s="181"/>
+      <c r="AA177" s="181"/>
+      <c r="AB177" s="181"/>
+      <c r="AC177" s="181"/>
+      <c r="AD177" s="182"/>
       <c r="AE177" s="180" t="s">
         <v>14</v>
       </c>
@@ -13838,14 +13805,14 @@
       <c r="V178" s="181"/>
       <c r="W178" s="181"/>
       <c r="X178" s="182"/>
-      <c r="Y178" s="186" t="s">
+      <c r="Y178" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="Z178" s="187"/>
-      <c r="AA178" s="187"/>
-      <c r="AB178" s="187"/>
-      <c r="AC178" s="187"/>
-      <c r="AD178" s="188"/>
+      <c r="Z178" s="181"/>
+      <c r="AA178" s="181"/>
+      <c r="AB178" s="181"/>
+      <c r="AC178" s="181"/>
+      <c r="AD178" s="182"/>
       <c r="AE178" s="180" t="s">
         <v>14</v>
       </c>
@@ -13883,22 +13850,22 @@
       <c r="V179" s="181"/>
       <c r="W179" s="181"/>
       <c r="X179" s="182"/>
-      <c r="Y179" s="186" t="s">
+      <c r="Y179" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="Z179" s="187"/>
-      <c r="AA179" s="187"/>
-      <c r="AB179" s="187"/>
-      <c r="AC179" s="187"/>
-      <c r="AD179" s="188"/>
-      <c r="AE179" s="186" t="s">
+      <c r="Z179" s="181"/>
+      <c r="AA179" s="181"/>
+      <c r="AB179" s="181"/>
+      <c r="AC179" s="181"/>
+      <c r="AD179" s="182"/>
+      <c r="AE179" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="AF179" s="187"/>
-      <c r="AG179" s="187"/>
-      <c r="AH179" s="187"/>
-      <c r="AI179" s="187"/>
-      <c r="AJ179" s="188"/>
+      <c r="AF179" s="181"/>
+      <c r="AG179" s="181"/>
+      <c r="AH179" s="181"/>
+      <c r="AI179" s="181"/>
+      <c r="AJ179" s="182"/>
       <c r="AP179" s="5"/>
       <c r="AQ179" s="2"/>
     </row>
@@ -13920,30 +13887,30 @@
       <c r="P180" s="75"/>
       <c r="Q180" s="75"/>
       <c r="R180" s="76"/>
-      <c r="S180" s="186" t="s">
+      <c r="S180" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="T180" s="187"/>
-      <c r="U180" s="187"/>
-      <c r="V180" s="187"/>
-      <c r="W180" s="187"/>
-      <c r="X180" s="188"/>
-      <c r="Y180" s="186" t="s">
+      <c r="T180" s="181"/>
+      <c r="U180" s="181"/>
+      <c r="V180" s="181"/>
+      <c r="W180" s="181"/>
+      <c r="X180" s="182"/>
+      <c r="Y180" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="Z180" s="187"/>
-      <c r="AA180" s="187"/>
-      <c r="AB180" s="187"/>
-      <c r="AC180" s="187"/>
-      <c r="AD180" s="188"/>
-      <c r="AE180" s="186" t="s">
+      <c r="Z180" s="181"/>
+      <c r="AA180" s="181"/>
+      <c r="AB180" s="181"/>
+      <c r="AC180" s="181"/>
+      <c r="AD180" s="182"/>
+      <c r="AE180" s="180" t="s">
         <v>14</v>
       </c>
-      <c r="AF180" s="187"/>
-      <c r="AG180" s="187"/>
-      <c r="AH180" s="187"/>
-      <c r="AI180" s="187"/>
-      <c r="AJ180" s="188"/>
+      <c r="AF180" s="181"/>
+      <c r="AG180" s="181"/>
+      <c r="AH180" s="181"/>
+      <c r="AI180" s="181"/>
+      <c r="AJ180" s="182"/>
       <c r="AP180" s="5"/>
       <c r="AQ180" s="2"/>
     </row>
@@ -13965,30 +13932,30 @@
       <c r="P181" s="149"/>
       <c r="Q181" s="149"/>
       <c r="R181" s="150"/>
-      <c r="S181" s="189" t="s">
+      <c r="S181" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T181" s="190"/>
-      <c r="U181" s="190"/>
-      <c r="V181" s="190"/>
-      <c r="W181" s="190"/>
-      <c r="X181" s="191"/>
-      <c r="Y181" s="189" t="s">
+      <c r="T181" s="187"/>
+      <c r="U181" s="187"/>
+      <c r="V181" s="187"/>
+      <c r="W181" s="187"/>
+      <c r="X181" s="188"/>
+      <c r="Y181" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="Z181" s="190"/>
-      <c r="AA181" s="190"/>
-      <c r="AB181" s="190"/>
-      <c r="AC181" s="190"/>
-      <c r="AD181" s="191"/>
-      <c r="AE181" s="189" t="s">
+      <c r="Z181" s="187"/>
+      <c r="AA181" s="187"/>
+      <c r="AB181" s="187"/>
+      <c r="AC181" s="187"/>
+      <c r="AD181" s="188"/>
+      <c r="AE181" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="AF181" s="190"/>
-      <c r="AG181" s="190"/>
-      <c r="AH181" s="190"/>
-      <c r="AI181" s="190"/>
-      <c r="AJ181" s="191"/>
+      <c r="AF181" s="187"/>
+      <c r="AG181" s="187"/>
+      <c r="AH181" s="187"/>
+      <c r="AI181" s="187"/>
+      <c r="AJ181" s="188"/>
       <c r="AP181" s="5"/>
       <c r="AQ181" s="2"/>
     </row>
@@ -14055,30 +14022,30 @@
       <c r="P183" s="149"/>
       <c r="Q183" s="149"/>
       <c r="R183" s="150"/>
-      <c r="S183" s="189" t="s">
+      <c r="S183" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="T183" s="190"/>
-      <c r="U183" s="190"/>
-      <c r="V183" s="190"/>
-      <c r="W183" s="190"/>
-      <c r="X183" s="191"/>
-      <c r="Y183" s="189" t="s">
+      <c r="T183" s="187"/>
+      <c r="U183" s="187"/>
+      <c r="V183" s="187"/>
+      <c r="W183" s="187"/>
+      <c r="X183" s="188"/>
+      <c r="Y183" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="Z183" s="190"/>
-      <c r="AA183" s="190"/>
-      <c r="AB183" s="190"/>
-      <c r="AC183" s="190"/>
-      <c r="AD183" s="191"/>
-      <c r="AE183" s="189" t="s">
+      <c r="Z183" s="187"/>
+      <c r="AA183" s="187"/>
+      <c r="AB183" s="187"/>
+      <c r="AC183" s="187"/>
+      <c r="AD183" s="188"/>
+      <c r="AE183" s="186" t="s">
         <v>14</v>
       </c>
-      <c r="AF183" s="190"/>
-      <c r="AG183" s="190"/>
-      <c r="AH183" s="190"/>
-      <c r="AI183" s="190"/>
-      <c r="AJ183" s="191"/>
+      <c r="AF183" s="187"/>
+      <c r="AG183" s="187"/>
+      <c r="AH183" s="187"/>
+      <c r="AI183" s="187"/>
+      <c r="AJ183" s="188"/>
       <c r="AP183" s="5"/>
       <c r="AQ183" s="2"/>
     </row>
@@ -14100,30 +14067,30 @@
       <c r="P184" s="152"/>
       <c r="Q184" s="152"/>
       <c r="R184" s="153"/>
-      <c r="S184" s="183" t="s">
+      <c r="S184" s="201" t="s">
         <v>8</v>
       </c>
-      <c r="T184" s="184"/>
-      <c r="U184" s="184"/>
-      <c r="V184" s="184"/>
-      <c r="W184" s="184"/>
-      <c r="X184" s="185"/>
-      <c r="Y184" s="183" t="s">
+      <c r="T184" s="202"/>
+      <c r="U184" s="202"/>
+      <c r="V184" s="202"/>
+      <c r="W184" s="202"/>
+      <c r="X184" s="203"/>
+      <c r="Y184" s="201" t="s">
         <v>14</v>
       </c>
-      <c r="Z184" s="184"/>
-      <c r="AA184" s="184"/>
-      <c r="AB184" s="184"/>
-      <c r="AC184" s="184"/>
-      <c r="AD184" s="185"/>
-      <c r="AE184" s="183" t="s">
+      <c r="Z184" s="202"/>
+      <c r="AA184" s="202"/>
+      <c r="AB184" s="202"/>
+      <c r="AC184" s="202"/>
+      <c r="AD184" s="203"/>
+      <c r="AE184" s="201" t="s">
         <v>14</v>
       </c>
-      <c r="AF184" s="184"/>
-      <c r="AG184" s="184"/>
-      <c r="AH184" s="184"/>
-      <c r="AI184" s="184"/>
-      <c r="AJ184" s="185"/>
+      <c r="AF184" s="202"/>
+      <c r="AG184" s="202"/>
+      <c r="AH184" s="202"/>
+      <c r="AI184" s="202"/>
+      <c r="AJ184" s="203"/>
       <c r="AP184" s="5"/>
       <c r="AQ184" s="2"/>
     </row>
@@ -16149,17 +16116,17 @@
       <c r="AA235" s="62"/>
       <c r="AB235" s="62"/>
       <c r="AC235" s="63"/>
-      <c r="AD235" s="213" t="s">
+      <c r="AD235" s="216" t="s">
         <v>239</v>
       </c>
-      <c r="AE235" s="214"/>
-      <c r="AF235" s="214"/>
-      <c r="AG235" s="214"/>
-      <c r="AH235" s="214"/>
-      <c r="AI235" s="214"/>
-      <c r="AJ235" s="214"/>
-      <c r="AK235" s="214"/>
-      <c r="AL235" s="215"/>
+      <c r="AE235" s="217"/>
+      <c r="AF235" s="217"/>
+      <c r="AG235" s="217"/>
+      <c r="AH235" s="217"/>
+      <c r="AI235" s="217"/>
+      <c r="AJ235" s="217"/>
+      <c r="AK235" s="217"/>
+      <c r="AL235" s="218"/>
       <c r="AM235" s="92"/>
       <c r="AN235" s="2"/>
       <c r="AP235" s="5"/>
@@ -16435,21 +16402,21 @@
       <c r="AA241" s="117"/>
       <c r="AB241" s="117"/>
       <c r="AC241" s="173"/>
-      <c r="AD241" s="243" t="s">
+      <c r="AD241" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AE241" s="244"/>
-      <c r="AF241" s="244"/>
-      <c r="AG241" s="245"/>
-      <c r="AH241" s="243" t="s">
+      <c r="AE241" s="193"/>
+      <c r="AF241" s="193"/>
+      <c r="AG241" s="194"/>
+      <c r="AH241" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AI241" s="245"/>
-      <c r="AJ241" s="243" t="s">
+      <c r="AI241" s="194"/>
+      <c r="AJ241" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AK241" s="244"/>
-      <c r="AL241" s="245"/>
+      <c r="AK241" s="193"/>
+      <c r="AL241" s="194"/>
       <c r="AM241" s="92"/>
       <c r="AN241" s="2"/>
       <c r="AP241" s="5"/>
@@ -16486,15 +16453,15 @@
       <c r="AA242" s="119"/>
       <c r="AB242" s="119"/>
       <c r="AC242" s="120"/>
-      <c r="AD242" s="246"/>
-      <c r="AE242" s="247"/>
-      <c r="AF242" s="247"/>
-      <c r="AG242" s="248"/>
-      <c r="AH242" s="246"/>
-      <c r="AI242" s="248"/>
-      <c r="AJ242" s="246"/>
-      <c r="AK242" s="247"/>
-      <c r="AL242" s="248"/>
+      <c r="AD242" s="195"/>
+      <c r="AE242" s="196"/>
+      <c r="AF242" s="196"/>
+      <c r="AG242" s="197"/>
+      <c r="AH242" s="195"/>
+      <c r="AI242" s="197"/>
+      <c r="AJ242" s="195"/>
+      <c r="AK242" s="196"/>
+      <c r="AL242" s="197"/>
       <c r="AM242" s="92"/>
       <c r="AN242" s="2"/>
       <c r="AP242" s="5"/>
@@ -16531,15 +16498,15 @@
       <c r="AA243" s="119"/>
       <c r="AB243" s="119"/>
       <c r="AC243" s="120"/>
-      <c r="AD243" s="246"/>
-      <c r="AE243" s="247"/>
-      <c r="AF243" s="247"/>
-      <c r="AG243" s="248"/>
-      <c r="AH243" s="246"/>
-      <c r="AI243" s="248"/>
-      <c r="AJ243" s="246"/>
-      <c r="AK243" s="247"/>
-      <c r="AL243" s="248"/>
+      <c r="AD243" s="195"/>
+      <c r="AE243" s="196"/>
+      <c r="AF243" s="196"/>
+      <c r="AG243" s="197"/>
+      <c r="AH243" s="195"/>
+      <c r="AI243" s="197"/>
+      <c r="AJ243" s="195"/>
+      <c r="AK243" s="196"/>
+      <c r="AL243" s="197"/>
       <c r="AM243" s="92"/>
       <c r="AN243" s="2"/>
       <c r="AP243" s="5"/>
@@ -16576,15 +16543,15 @@
       <c r="AA244" s="113"/>
       <c r="AB244" s="113"/>
       <c r="AC244" s="121"/>
-      <c r="AD244" s="249"/>
-      <c r="AE244" s="250"/>
-      <c r="AF244" s="250"/>
-      <c r="AG244" s="251"/>
-      <c r="AH244" s="249"/>
-      <c r="AI244" s="251"/>
-      <c r="AJ244" s="249"/>
-      <c r="AK244" s="250"/>
-      <c r="AL244" s="251"/>
+      <c r="AD244" s="198"/>
+      <c r="AE244" s="199"/>
+      <c r="AF244" s="199"/>
+      <c r="AG244" s="200"/>
+      <c r="AH244" s="198"/>
+      <c r="AI244" s="200"/>
+      <c r="AJ244" s="198"/>
+      <c r="AK244" s="199"/>
+      <c r="AL244" s="200"/>
       <c r="AM244" s="92"/>
       <c r="AN244" s="2"/>
       <c r="AP244" s="5"/>
@@ -16623,21 +16590,21 @@
       <c r="AA245" s="117"/>
       <c r="AB245" s="117"/>
       <c r="AC245" s="173"/>
-      <c r="AD245" s="243" t="s">
+      <c r="AD245" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AE245" s="244"/>
-      <c r="AF245" s="244"/>
-      <c r="AG245" s="245"/>
-      <c r="AH245" s="243" t="s">
+      <c r="AE245" s="193"/>
+      <c r="AF245" s="193"/>
+      <c r="AG245" s="194"/>
+      <c r="AH245" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AI245" s="245"/>
-      <c r="AJ245" s="243" t="s">
+      <c r="AI245" s="194"/>
+      <c r="AJ245" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AK245" s="244"/>
-      <c r="AL245" s="245"/>
+      <c r="AK245" s="193"/>
+      <c r="AL245" s="194"/>
       <c r="AM245" s="92"/>
       <c r="AN245" s="2"/>
       <c r="AP245" s="5"/>
@@ -16674,15 +16641,15 @@
       <c r="AA246" s="119"/>
       <c r="AB246" s="119"/>
       <c r="AC246" s="120"/>
-      <c r="AD246" s="246"/>
-      <c r="AE246" s="247"/>
-      <c r="AF246" s="247"/>
-      <c r="AG246" s="248"/>
-      <c r="AH246" s="246"/>
-      <c r="AI246" s="248"/>
-      <c r="AJ246" s="246"/>
-      <c r="AK246" s="247"/>
-      <c r="AL246" s="248"/>
+      <c r="AD246" s="195"/>
+      <c r="AE246" s="196"/>
+      <c r="AF246" s="196"/>
+      <c r="AG246" s="197"/>
+      <c r="AH246" s="195"/>
+      <c r="AI246" s="197"/>
+      <c r="AJ246" s="195"/>
+      <c r="AK246" s="196"/>
+      <c r="AL246" s="197"/>
       <c r="AM246" s="92"/>
       <c r="AN246" s="2"/>
       <c r="AP246" s="5"/>
@@ -16719,15 +16686,15 @@
       <c r="AA247" s="92"/>
       <c r="AB247" s="92"/>
       <c r="AC247" s="128"/>
-      <c r="AD247" s="246"/>
-      <c r="AE247" s="247"/>
-      <c r="AF247" s="247"/>
-      <c r="AG247" s="248"/>
-      <c r="AH247" s="246"/>
-      <c r="AI247" s="248"/>
-      <c r="AJ247" s="246"/>
-      <c r="AK247" s="247"/>
-      <c r="AL247" s="248"/>
+      <c r="AD247" s="195"/>
+      <c r="AE247" s="196"/>
+      <c r="AF247" s="196"/>
+      <c r="AG247" s="197"/>
+      <c r="AH247" s="195"/>
+      <c r="AI247" s="197"/>
+      <c r="AJ247" s="195"/>
+      <c r="AK247" s="196"/>
+      <c r="AL247" s="197"/>
       <c r="AM247" s="92"/>
       <c r="AN247" s="2"/>
       <c r="AP247" s="5"/>
@@ -16764,15 +16731,15 @@
       <c r="AA248" s="113"/>
       <c r="AB248" s="113"/>
       <c r="AC248" s="121"/>
-      <c r="AD248" s="249"/>
-      <c r="AE248" s="250"/>
-      <c r="AF248" s="250"/>
-      <c r="AG248" s="251"/>
-      <c r="AH248" s="249"/>
-      <c r="AI248" s="251"/>
-      <c r="AJ248" s="249"/>
-      <c r="AK248" s="250"/>
-      <c r="AL248" s="251"/>
+      <c r="AD248" s="198"/>
+      <c r="AE248" s="199"/>
+      <c r="AF248" s="199"/>
+      <c r="AG248" s="200"/>
+      <c r="AH248" s="198"/>
+      <c r="AI248" s="200"/>
+      <c r="AJ248" s="198"/>
+      <c r="AK248" s="199"/>
+      <c r="AL248" s="200"/>
       <c r="AM248" s="92"/>
       <c r="AN248" s="2"/>
       <c r="AP248" s="5"/>
@@ -16811,21 +16778,21 @@
       <c r="AA249" s="117"/>
       <c r="AB249" s="117"/>
       <c r="AC249" s="173"/>
-      <c r="AD249" s="243" t="s">
+      <c r="AD249" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AE249" s="244"/>
-      <c r="AF249" s="244"/>
-      <c r="AG249" s="245"/>
-      <c r="AH249" s="243" t="s">
+      <c r="AE249" s="193"/>
+      <c r="AF249" s="193"/>
+      <c r="AG249" s="194"/>
+      <c r="AH249" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AI249" s="245"/>
-      <c r="AJ249" s="243" t="s">
+      <c r="AI249" s="194"/>
+      <c r="AJ249" s="192" t="s">
         <v>8</v>
       </c>
-      <c r="AK249" s="244"/>
-      <c r="AL249" s="245"/>
+      <c r="AK249" s="193"/>
+      <c r="AL249" s="194"/>
       <c r="AM249" s="92"/>
       <c r="AN249" s="2"/>
       <c r="AP249" s="5"/>
@@ -16862,15 +16829,15 @@
       <c r="AA250" s="113"/>
       <c r="AB250" s="113"/>
       <c r="AC250" s="121"/>
-      <c r="AD250" s="249"/>
-      <c r="AE250" s="250"/>
-      <c r="AF250" s="250"/>
-      <c r="AG250" s="251"/>
-      <c r="AH250" s="249"/>
-      <c r="AI250" s="251"/>
-      <c r="AJ250" s="249"/>
-      <c r="AK250" s="250"/>
-      <c r="AL250" s="251"/>
+      <c r="AD250" s="198"/>
+      <c r="AE250" s="199"/>
+      <c r="AF250" s="199"/>
+      <c r="AG250" s="200"/>
+      <c r="AH250" s="198"/>
+      <c r="AI250" s="200"/>
+      <c r="AJ250" s="198"/>
+      <c r="AK250" s="199"/>
+      <c r="AL250" s="200"/>
       <c r="AM250" s="92"/>
       <c r="AN250" s="2"/>
       <c r="AP250" s="5"/>
@@ -17084,17 +17051,17 @@
       <c r="AA255" s="62"/>
       <c r="AB255" s="62"/>
       <c r="AC255" s="63"/>
-      <c r="AD255" s="213" t="s">
+      <c r="AD255" s="216" t="s">
         <v>239</v>
       </c>
-      <c r="AE255" s="214"/>
-      <c r="AF255" s="214"/>
-      <c r="AG255" s="214"/>
-      <c r="AH255" s="214"/>
-      <c r="AI255" s="214"/>
-      <c r="AJ255" s="214"/>
-      <c r="AK255" s="214"/>
-      <c r="AL255" s="215"/>
+      <c r="AE255" s="217"/>
+      <c r="AF255" s="217"/>
+      <c r="AG255" s="217"/>
+      <c r="AH255" s="217"/>
+      <c r="AI255" s="217"/>
+      <c r="AJ255" s="217"/>
+      <c r="AK255" s="217"/>
+      <c r="AL255" s="218"/>
       <c r="AM255" s="92"/>
       <c r="AN255" s="2"/>
       <c r="AP255" s="5"/>
@@ -17186,21 +17153,21 @@
       <c r="AA257" s="100"/>
       <c r="AB257" s="100"/>
       <c r="AC257" s="104"/>
-      <c r="AD257" s="204" t="s">
+      <c r="AD257" s="207" t="s">
         <v>8</v>
       </c>
-      <c r="AE257" s="208"/>
-      <c r="AF257" s="208"/>
-      <c r="AG257" s="205"/>
-      <c r="AH257" s="204" t="s">
+      <c r="AE257" s="211"/>
+      <c r="AF257" s="211"/>
+      <c r="AG257" s="208"/>
+      <c r="AH257" s="207" t="s">
         <v>8</v>
       </c>
-      <c r="AI257" s="205"/>
-      <c r="AJ257" s="204" t="s">
+      <c r="AI257" s="208"/>
+      <c r="AJ257" s="207" t="s">
         <v>8</v>
       </c>
-      <c r="AK257" s="208"/>
-      <c r="AL257" s="205"/>
+      <c r="AK257" s="211"/>
+      <c r="AL257" s="208"/>
       <c r="AM257" s="92"/>
       <c r="AN257" s="2"/>
       <c r="AP257" s="5"/>
@@ -17238,15 +17205,15 @@
       <c r="AA258" s="99"/>
       <c r="AB258" s="99"/>
       <c r="AC258" s="103"/>
-      <c r="AD258" s="206"/>
-      <c r="AE258" s="209"/>
-      <c r="AF258" s="209"/>
-      <c r="AG258" s="207"/>
-      <c r="AH258" s="206"/>
-      <c r="AI258" s="207"/>
-      <c r="AJ258" s="206"/>
-      <c r="AK258" s="209"/>
-      <c r="AL258" s="207"/>
+      <c r="AD258" s="209"/>
+      <c r="AE258" s="212"/>
+      <c r="AF258" s="212"/>
+      <c r="AG258" s="210"/>
+      <c r="AH258" s="209"/>
+      <c r="AI258" s="210"/>
+      <c r="AJ258" s="209"/>
+      <c r="AK258" s="212"/>
+      <c r="AL258" s="210"/>
       <c r="AM258" s="92"/>
       <c r="AN258" s="2"/>
       <c r="AP258" s="5"/>
@@ -17286,21 +17253,21 @@
       <c r="AA259" s="98"/>
       <c r="AB259" s="98"/>
       <c r="AC259" s="102"/>
-      <c r="AD259" s="204" t="s">
+      <c r="AD259" s="207" t="s">
         <v>8</v>
       </c>
-      <c r="AE259" s="208"/>
-      <c r="AF259" s="208"/>
-      <c r="AG259" s="205"/>
-      <c r="AH259" s="204" t="s">
+      <c r="AE259" s="211"/>
+      <c r="AF259" s="211"/>
+      <c r="AG259" s="208"/>
+      <c r="AH259" s="207" t="s">
         <v>8</v>
       </c>
-      <c r="AI259" s="205"/>
-      <c r="AJ259" s="204" t="s">
+      <c r="AI259" s="208"/>
+      <c r="AJ259" s="207" t="s">
         <v>8</v>
       </c>
-      <c r="AK259" s="208"/>
-      <c r="AL259" s="205"/>
+      <c r="AK259" s="211"/>
+      <c r="AL259" s="208"/>
       <c r="AM259" s="92"/>
       <c r="AN259" s="2"/>
       <c r="AP259" s="5"/>
@@ -17340,21 +17307,21 @@
       <c r="AA260" s="105"/>
       <c r="AB260" s="105"/>
       <c r="AC260" s="116"/>
-      <c r="AD260" s="192" t="s">
+      <c r="AD260" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="AE260" s="193"/>
-      <c r="AF260" s="193"/>
-      <c r="AG260" s="194"/>
-      <c r="AH260" s="192" t="s">
+      <c r="AE260" s="190"/>
+      <c r="AF260" s="190"/>
+      <c r="AG260" s="191"/>
+      <c r="AH260" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="AI260" s="194"/>
-      <c r="AJ260" s="192" t="s">
+      <c r="AI260" s="191"/>
+      <c r="AJ260" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="AK260" s="193"/>
-      <c r="AL260" s="194"/>
+      <c r="AK260" s="190"/>
+      <c r="AL260" s="191"/>
       <c r="AM260" s="92"/>
       <c r="AN260" s="2"/>
       <c r="AP260" s="5"/>
@@ -17396,21 +17363,21 @@
       <c r="AA261" s="105"/>
       <c r="AB261" s="105"/>
       <c r="AC261" s="116"/>
-      <c r="AD261" s="192" t="s">
+      <c r="AD261" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="AE261" s="193"/>
-      <c r="AF261" s="193"/>
-      <c r="AG261" s="194"/>
-      <c r="AH261" s="192" t="s">
+      <c r="AE261" s="190"/>
+      <c r="AF261" s="190"/>
+      <c r="AG261" s="191"/>
+      <c r="AH261" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="AI261" s="194"/>
-      <c r="AJ261" s="192" t="s">
+      <c r="AI261" s="191"/>
+      <c r="AJ261" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="AK261" s="193"/>
-      <c r="AL261" s="194"/>
+      <c r="AK261" s="190"/>
+      <c r="AL261" s="191"/>
       <c r="AM261" s="92"/>
       <c r="AN261" s="2"/>
       <c r="AP261" s="5"/>
@@ -17450,21 +17417,21 @@
       <c r="AA262" s="105"/>
       <c r="AB262" s="105"/>
       <c r="AC262" s="116"/>
-      <c r="AD262" s="192" t="s">
+      <c r="AD262" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="AE262" s="193"/>
-      <c r="AF262" s="193"/>
-      <c r="AG262" s="194"/>
-      <c r="AH262" s="192" t="s">
+      <c r="AE262" s="190"/>
+      <c r="AF262" s="190"/>
+      <c r="AG262" s="191"/>
+      <c r="AH262" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="AI262" s="194"/>
-      <c r="AJ262" s="192" t="s">
+      <c r="AI262" s="191"/>
+      <c r="AJ262" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="AK262" s="193"/>
-      <c r="AL262" s="194"/>
+      <c r="AK262" s="190"/>
+      <c r="AL262" s="191"/>
       <c r="AM262" s="92"/>
       <c r="AN262" s="2"/>
       <c r="AP262" s="5"/>
@@ -17504,21 +17471,21 @@
       <c r="AA263" s="105"/>
       <c r="AB263" s="105"/>
       <c r="AC263" s="116"/>
-      <c r="AD263" s="210" t="s">
+      <c r="AD263" s="213" t="s">
         <v>8</v>
       </c>
-      <c r="AE263" s="211"/>
-      <c r="AF263" s="211"/>
-      <c r="AG263" s="212"/>
-      <c r="AH263" s="210" t="s">
+      <c r="AE263" s="214"/>
+      <c r="AF263" s="214"/>
+      <c r="AG263" s="215"/>
+      <c r="AH263" s="213" t="s">
         <v>8</v>
       </c>
-      <c r="AI263" s="212"/>
-      <c r="AJ263" s="192" t="s">
+      <c r="AI263" s="215"/>
+      <c r="AJ263" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="AK263" s="193"/>
-      <c r="AL263" s="194"/>
+      <c r="AK263" s="190"/>
+      <c r="AL263" s="191"/>
       <c r="AM263" s="92"/>
       <c r="AN263" s="2"/>
       <c r="AP263" s="5"/>
@@ -17560,21 +17527,21 @@
       <c r="AA264" s="98"/>
       <c r="AB264" s="98"/>
       <c r="AC264" s="102"/>
-      <c r="AD264" s="198" t="s">
+      <c r="AD264" s="204" t="s">
         <v>8</v>
       </c>
-      <c r="AE264" s="199"/>
-      <c r="AF264" s="199"/>
-      <c r="AG264" s="200"/>
-      <c r="AH264" s="198" t="s">
+      <c r="AE264" s="205"/>
+      <c r="AF264" s="205"/>
+      <c r="AG264" s="206"/>
+      <c r="AH264" s="204" t="s">
         <v>8</v>
       </c>
-      <c r="AI264" s="200"/>
-      <c r="AJ264" s="198" t="s">
+      <c r="AI264" s="206"/>
+      <c r="AJ264" s="204" t="s">
         <v>8</v>
       </c>
-      <c r="AK264" s="199"/>
-      <c r="AL264" s="200"/>
+      <c r="AK264" s="205"/>
+      <c r="AL264" s="206"/>
       <c r="AM264" s="92"/>
       <c r="AN264" s="2"/>
       <c r="AP264" s="5"/>
@@ -18176,6 +18143,27 @@
     </row>
   </sheetData>
   <mergeCells count="234">
+    <mergeCell ref="AE137:AJ137"/>
+    <mergeCell ref="AE164:AJ164"/>
+    <mergeCell ref="AE165:AJ165"/>
+    <mergeCell ref="AE166:AJ166"/>
+    <mergeCell ref="AE138:AJ138"/>
+    <mergeCell ref="AD237:AG240"/>
+    <mergeCell ref="AJ237:AL240"/>
+    <mergeCell ref="AH237:AI240"/>
+    <mergeCell ref="AD235:AL235"/>
+    <mergeCell ref="AE144:AJ144"/>
+    <mergeCell ref="AE143:AJ143"/>
+    <mergeCell ref="AE142:AJ142"/>
+    <mergeCell ref="AE146:AJ146"/>
+    <mergeCell ref="AE147:AJ147"/>
+    <mergeCell ref="AE154:AJ154"/>
+    <mergeCell ref="S171:X171"/>
+    <mergeCell ref="Y171:AD171"/>
+    <mergeCell ref="AE171:AJ171"/>
+    <mergeCell ref="S172:X172"/>
+    <mergeCell ref="Y172:AD172"/>
+    <mergeCell ref="AE172:AJ172"/>
     <mergeCell ref="AH245:AI248"/>
     <mergeCell ref="AJ245:AL248"/>
     <mergeCell ref="AJ249:AL250"/>
@@ -18184,21 +18172,6 @@
     <mergeCell ref="AD241:AG244"/>
     <mergeCell ref="AH241:AI244"/>
     <mergeCell ref="AJ241:AL244"/>
-    <mergeCell ref="Y137:AD137"/>
-    <mergeCell ref="AE137:AJ137"/>
-    <mergeCell ref="S173:X173"/>
-    <mergeCell ref="Y173:AD173"/>
-    <mergeCell ref="AE173:AJ173"/>
-    <mergeCell ref="S171:X171"/>
-    <mergeCell ref="Y171:AD171"/>
-    <mergeCell ref="AE171:AJ171"/>
-    <mergeCell ref="S172:X172"/>
-    <mergeCell ref="Y172:AD172"/>
-    <mergeCell ref="AE172:AJ172"/>
-    <mergeCell ref="AE164:AJ164"/>
-    <mergeCell ref="AE165:AJ165"/>
-    <mergeCell ref="AE166:AJ166"/>
-    <mergeCell ref="S164:X164"/>
     <mergeCell ref="S161:X161"/>
     <mergeCell ref="Y153:AD153"/>
     <mergeCell ref="Y154:AD154"/>
@@ -18207,11 +18180,8 @@
     <mergeCell ref="S149:X149"/>
     <mergeCell ref="S150:X150"/>
     <mergeCell ref="S152:X152"/>
-    <mergeCell ref="AE138:AJ138"/>
-    <mergeCell ref="AD237:AG240"/>
-    <mergeCell ref="AJ237:AL240"/>
-    <mergeCell ref="AH237:AI240"/>
-    <mergeCell ref="AD235:AL235"/>
+    <mergeCell ref="S143:X143"/>
+    <mergeCell ref="S144:X144"/>
     <mergeCell ref="S183:X183"/>
     <mergeCell ref="Y161:AD161"/>
     <mergeCell ref="Y162:AD162"/>
@@ -18222,11 +18192,20 @@
     <mergeCell ref="AE158:AJ158"/>
     <mergeCell ref="AE159:AJ159"/>
     <mergeCell ref="Y160:AD160"/>
-    <mergeCell ref="AE144:AJ144"/>
-    <mergeCell ref="AE143:AJ143"/>
-    <mergeCell ref="AE142:AJ142"/>
-    <mergeCell ref="S143:X143"/>
-    <mergeCell ref="S144:X144"/>
+    <mergeCell ref="AE162:AJ162"/>
+    <mergeCell ref="AE163:AJ163"/>
+    <mergeCell ref="AE167:AJ167"/>
+    <mergeCell ref="AE168:AJ168"/>
+    <mergeCell ref="AE182:AJ182"/>
+    <mergeCell ref="AE183:AJ183"/>
+    <mergeCell ref="Y182:AD182"/>
+    <mergeCell ref="Y183:AD183"/>
+    <mergeCell ref="Y163:AD163"/>
+    <mergeCell ref="Y167:AD167"/>
+    <mergeCell ref="Y168:AD168"/>
+    <mergeCell ref="AE169:AJ169"/>
+    <mergeCell ref="AE170:AJ170"/>
+    <mergeCell ref="Y166:AD166"/>
     <mergeCell ref="S136:X136"/>
     <mergeCell ref="S145:X145"/>
     <mergeCell ref="S146:X146"/>
@@ -18236,9 +18215,6 @@
     <mergeCell ref="S140:X140"/>
     <mergeCell ref="S141:X141"/>
     <mergeCell ref="S137:X137"/>
-    <mergeCell ref="AE146:AJ146"/>
-    <mergeCell ref="AE147:AJ147"/>
-    <mergeCell ref="AE154:AJ154"/>
     <mergeCell ref="AE155:AJ155"/>
     <mergeCell ref="Y132:AD132"/>
     <mergeCell ref="Y134:AD134"/>
@@ -18260,6 +18236,9 @@
     <mergeCell ref="AE141:AJ141"/>
     <mergeCell ref="AE140:AJ140"/>
     <mergeCell ref="AE139:AJ139"/>
+    <mergeCell ref="AE149:AJ149"/>
+    <mergeCell ref="Y149:AD149"/>
+    <mergeCell ref="Y137:AD137"/>
     <mergeCell ref="S125:X125"/>
     <mergeCell ref="Y125:AD125"/>
     <mergeCell ref="Y126:AD126"/>
@@ -18326,29 +18305,6 @@
     <mergeCell ref="AD257:AG257"/>
     <mergeCell ref="AD258:AG258"/>
     <mergeCell ref="AD259:AG259"/>
-    <mergeCell ref="AE162:AJ162"/>
-    <mergeCell ref="AE163:AJ163"/>
-    <mergeCell ref="AE167:AJ167"/>
-    <mergeCell ref="AE168:AJ168"/>
-    <mergeCell ref="AE182:AJ182"/>
-    <mergeCell ref="AE183:AJ183"/>
-    <mergeCell ref="Y182:AD182"/>
-    <mergeCell ref="Y183:AD183"/>
-    <mergeCell ref="Y163:AD163"/>
-    <mergeCell ref="Y167:AD167"/>
-    <mergeCell ref="Y168:AD168"/>
-    <mergeCell ref="AE169:AJ169"/>
-    <mergeCell ref="AE170:AJ170"/>
-    <mergeCell ref="Y166:AD166"/>
-    <mergeCell ref="Y165:AD165"/>
-    <mergeCell ref="Y164:AD164"/>
-    <mergeCell ref="Y169:AD169"/>
-    <mergeCell ref="S163:X163"/>
-    <mergeCell ref="S167:X167"/>
-    <mergeCell ref="S165:X165"/>
-    <mergeCell ref="S169:X169"/>
-    <mergeCell ref="Y170:AD170"/>
-    <mergeCell ref="S168:X168"/>
     <mergeCell ref="AD260:AG260"/>
     <mergeCell ref="AD261:AG261"/>
     <mergeCell ref="AD262:AG262"/>
@@ -18360,10 +18316,6 @@
     <mergeCell ref="S176:X176"/>
     <mergeCell ref="Y176:AD176"/>
     <mergeCell ref="AE176:AJ176"/>
-    <mergeCell ref="S170:X170"/>
-    <mergeCell ref="S166:X166"/>
-    <mergeCell ref="AE149:AJ149"/>
-    <mergeCell ref="Y149:AD149"/>
     <mergeCell ref="S184:X184"/>
     <mergeCell ref="Y184:AD184"/>
     <mergeCell ref="AE184:AJ184"/>
@@ -18386,6 +18338,21 @@
     <mergeCell ref="S162:X162"/>
     <mergeCell ref="S174:X174"/>
     <mergeCell ref="Y174:AD174"/>
+    <mergeCell ref="Y165:AD165"/>
+    <mergeCell ref="Y164:AD164"/>
+    <mergeCell ref="Y169:AD169"/>
+    <mergeCell ref="S163:X163"/>
+    <mergeCell ref="S167:X167"/>
+    <mergeCell ref="S165:X165"/>
+    <mergeCell ref="S169:X169"/>
+    <mergeCell ref="Y170:AD170"/>
+    <mergeCell ref="S168:X168"/>
+    <mergeCell ref="S170:X170"/>
+    <mergeCell ref="S166:X166"/>
+    <mergeCell ref="S164:X164"/>
+    <mergeCell ref="S173:X173"/>
+    <mergeCell ref="Y173:AD173"/>
+    <mergeCell ref="AE173:AJ173"/>
     <mergeCell ref="Y129:AD129"/>
     <mergeCell ref="S129:X129"/>
     <mergeCell ref="Y128:AD128"/>

</xml_diff>